<commit_message>
Updating Leaderboard, Club history and README
</commit_message>
<xml_diff>
--- a/public/Data/HEMANPUNTERS.xlsx
+++ b/public/Data/HEMANPUNTERS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bturnor\source\repos\PersonalWork\seeMore\public\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4BB1737-FC95-4600-B233-C4B65E7D7BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF446B2C-75F3-4099-A001-A69BE1B38345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="86280" yWindow="45" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="4" xr2:uid="{525E8989-1938-4309-A4CF-8F1D15E362FB}"/>
+    <workbookView xWindow="0" yWindow="-192" windowWidth="23040" windowHeight="13872" firstSheet="3" activeTab="3" xr2:uid="{525E8989-1938-4309-A4CF-8F1D15E362FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Punters club" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Punters 2021" sheetId="6" r:id="rId3"/>
     <sheet name="Punters 2022" sheetId="7" r:id="rId4"/>
     <sheet name="Punters 2023" sheetId="8" r:id="rId5"/>
+    <sheet name="Punters 2024" sheetId="9" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="111">
   <si>
     <t>HE_MAN PUNTERS 2019</t>
   </si>
@@ -362,6 +363,39 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>B.JASKOLA</t>
+  </si>
+  <si>
+    <t>J.VELLIOU</t>
+  </si>
+  <si>
+    <t>S.CAPOZZI</t>
+  </si>
+  <si>
+    <t>K.HORNSEY</t>
+  </si>
+  <si>
+    <t>B.TURNOR</t>
+  </si>
+  <si>
+    <t>P.BLAKEY</t>
+  </si>
+  <si>
+    <t>S.BAMFORD</t>
+  </si>
+  <si>
+    <t>B.RAFFAELE</t>
+  </si>
+  <si>
+    <t>B.SPICER</t>
+  </si>
+  <si>
+    <t>Strikes for 2024 Season</t>
+  </si>
+  <si>
+    <t>Strikes</t>
   </si>
 </sst>
 </file>
@@ -945,6 +979,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -963,19 +1000,16 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3712,50 +3746,50 @@
   <sheetData>
     <row r="1" spans="2:27" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="2" spans="2:27" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63" t="s">
+      <c r="D2" s="57"/>
+      <c r="E2" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63" t="s">
+      <c r="F2" s="57"/>
+      <c r="G2" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63" t="s">
+      <c r="H2" s="57"/>
+      <c r="I2" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="63"/>
-      <c r="K2" s="63" t="s">
+      <c r="J2" s="57"/>
+      <c r="K2" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="63"/>
-      <c r="M2" s="63" t="s">
+      <c r="L2" s="57"/>
+      <c r="M2" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="63"/>
-      <c r="O2" s="63" t="s">
+      <c r="N2" s="57"/>
+      <c r="O2" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="63" t="s">
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="R2" s="63"/>
-      <c r="S2" s="63" t="s">
+      <c r="R2" s="57"/>
+      <c r="S2" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="T2" s="63"/>
-      <c r="U2" s="63" t="s">
+      <c r="T2" s="57"/>
+      <c r="U2" s="57" t="s">
         <v>27</v>
       </c>
       <c r="V2" s="64"/>
-      <c r="W2" s="62" t="s">
+      <c r="W2" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="X2" s="63"/>
+      <c r="X2" s="57"/>
     </row>
     <row r="3" spans="2:27" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B3" s="32" t="s">
@@ -5316,34 +5350,34 @@
       </c>
     </row>
     <row r="29" spans="2:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="F29" s="59" t="s">
+      <c r="F29" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="G29" s="60"/>
-      <c r="H29" s="61"/>
-      <c r="I29" s="57">
+      <c r="G29" s="61"/>
+      <c r="H29" s="62"/>
+      <c r="I29" s="58">
         <f>C27+E27+G27+I27+K27+M27+O27+Q27+S27+U27</f>
         <v>2469.42</v>
       </c>
-      <c r="J29" s="58"/>
+      <c r="J29" s="59"/>
     </row>
     <row r="30" spans="2:27" x14ac:dyDescent="0.55000000000000004">
       <c r="G30" s="65" t="s">
         <v>57</v>
       </c>
       <c r="H30" s="65"/>
-      <c r="I30" s="57">
+      <c r="I30" s="58">
         <f>+D27+F27+H27+J27+L27+N27+P27+R27+T27+V27</f>
         <v>1774.69</v>
       </c>
-      <c r="J30" s="58"/>
+      <c r="J30" s="59"/>
     </row>
     <row r="31" spans="2:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="I31" s="57">
+      <c r="I31" s="58">
         <f>I30-I29</f>
         <v>-694.73</v>
       </c>
-      <c r="J31" s="58"/>
+      <c r="J31" s="59"/>
     </row>
     <row r="32" spans="2:27" x14ac:dyDescent="0.55000000000000004">
       <c r="C32" s="1">
@@ -5392,11 +5426,11 @@
       </c>
     </row>
     <row r="34" spans="3:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="I34" s="58">
+      <c r="I34" s="59">
         <f>I33+I31</f>
         <v>505.27</v>
       </c>
-      <c r="J34" s="58"/>
+      <c r="J34" s="59"/>
     </row>
     <row r="38" spans="3:16" x14ac:dyDescent="0.55000000000000004">
       <c r="C38" s="1">
@@ -5440,11 +5474,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
     <mergeCell ref="I30:J30"/>
     <mergeCell ref="F29:H29"/>
     <mergeCell ref="I31:J31"/>
@@ -5457,6 +5486,11 @@
     <mergeCell ref="S2:T2"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="I29:J29"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5489,50 +5523,50 @@
   <sheetData>
     <row r="1" spans="2:27" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="2" spans="2:27" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63" t="s">
+      <c r="D2" s="57"/>
+      <c r="E2" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="63"/>
-      <c r="G2" s="66" t="s">
+      <c r="F2" s="57"/>
+      <c r="G2" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="62"/>
-      <c r="I2" s="63" t="s">
+      <c r="H2" s="63"/>
+      <c r="I2" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="63"/>
-      <c r="K2" s="63" t="s">
+      <c r="J2" s="57"/>
+      <c r="K2" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="63"/>
-      <c r="M2" s="63" t="s">
+      <c r="L2" s="57"/>
+      <c r="M2" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="63"/>
-      <c r="O2" s="63" t="s">
+      <c r="N2" s="57"/>
+      <c r="O2" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="63" t="s">
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="R2" s="63"/>
-      <c r="S2" s="63" t="s">
+      <c r="R2" s="57"/>
+      <c r="S2" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="T2" s="63"/>
-      <c r="U2" s="63" t="s">
+      <c r="T2" s="57"/>
+      <c r="U2" s="57" t="s">
         <v>27</v>
       </c>
       <c r="V2" s="64"/>
-      <c r="W2" s="62" t="s">
+      <c r="W2" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="X2" s="63"/>
+      <c r="X2" s="57"/>
     </row>
     <row r="3" spans="2:27" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B3" s="32" t="s">
@@ -6892,34 +6926,34 @@
       </c>
     </row>
     <row r="29" spans="2:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="F29" s="59" t="s">
+      <c r="F29" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="G29" s="60"/>
-      <c r="H29" s="61"/>
-      <c r="I29" s="57">
+      <c r="G29" s="61"/>
+      <c r="H29" s="62"/>
+      <c r="I29" s="58">
         <f>C27+E27+G27+I27+K27+M27+O27+Q27+S27+U27</f>
         <v>1788.24</v>
       </c>
-      <c r="J29" s="58"/>
+      <c r="J29" s="59"/>
     </row>
     <row r="30" spans="2:27" x14ac:dyDescent="0.55000000000000004">
       <c r="G30" s="65" t="s">
         <v>57</v>
       </c>
       <c r="H30" s="65"/>
-      <c r="I30" s="57">
+      <c r="I30" s="58">
         <f>+D27+F27+H27+J27+L27+N27+P27+R27+T27+V27</f>
         <v>2492.1999999999998</v>
       </c>
-      <c r="J30" s="58"/>
+      <c r="J30" s="59"/>
     </row>
     <row r="31" spans="2:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="I31" s="57">
+      <c r="I31" s="58">
         <f>I30-I29</f>
         <v>703.95999999999981</v>
       </c>
-      <c r="J31" s="58"/>
+      <c r="J31" s="59"/>
     </row>
     <row r="32" spans="2:27" x14ac:dyDescent="0.55000000000000004">
       <c r="C32" s="36">
@@ -6973,11 +7007,11 @@
         <v>64</v>
       </c>
       <c r="H34" s="42"/>
-      <c r="I34" s="67">
+      <c r="I34" s="66">
         <f>I33+I31</f>
         <v>1303.9599999999998</v>
       </c>
-      <c r="J34" s="67"/>
+      <c r="J34" s="66"/>
       <c r="M34" s="33"/>
     </row>
     <row r="38" spans="3:16" x14ac:dyDescent="0.55000000000000004">
@@ -7022,11 +7056,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
     <mergeCell ref="Q2:R2"/>
     <mergeCell ref="S2:T2"/>
     <mergeCell ref="U2:V2"/>
@@ -7034,11 +7068,11 @@
     <mergeCell ref="F29:H29"/>
     <mergeCell ref="I29:J29"/>
     <mergeCell ref="M2:N2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="O2:P2"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7051,10 +7085,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AH41"/>
+  <dimension ref="B1:AH58"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="T37" sqref="T37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -7063,7 +7097,8 @@
     <col min="2" max="2" width="5.68359375" customWidth="1"/>
     <col min="3" max="3" width="7.83984375" customWidth="1"/>
     <col min="4" max="4" width="9.15625" customWidth="1"/>
-    <col min="5" max="23" width="7.83984375" customWidth="1"/>
+    <col min="5" max="5" width="9.734375" customWidth="1"/>
+    <col min="6" max="23" width="7.83984375" customWidth="1"/>
     <col min="24" max="24" width="8.83984375" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="9.41796875" customWidth="1"/>
     <col min="26" max="26" width="9.68359375" customWidth="1"/>
@@ -7072,54 +7107,54 @@
   <sheetData>
     <row r="1" spans="2:34" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="2" spans="2:34" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63" t="s">
+      <c r="D2" s="57"/>
+      <c r="E2" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63" t="s">
+      <c r="F2" s="57"/>
+      <c r="G2" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63" t="s">
+      <c r="H2" s="57"/>
+      <c r="I2" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="63"/>
-      <c r="K2" s="63" t="s">
+      <c r="J2" s="57"/>
+      <c r="K2" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="63"/>
-      <c r="M2" s="63" t="s">
+      <c r="L2" s="57"/>
+      <c r="M2" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="N2" s="63"/>
-      <c r="O2" s="63" t="s">
+      <c r="N2" s="57"/>
+      <c r="O2" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="63" t="s">
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="R2" s="63"/>
-      <c r="S2" s="63" t="s">
+      <c r="R2" s="57"/>
+      <c r="S2" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="T2" s="63"/>
-      <c r="U2" s="63" t="s">
+      <c r="T2" s="57"/>
+      <c r="U2" s="57" t="s">
         <v>65</v>
       </c>
       <c r="V2" s="64"/>
-      <c r="W2" s="63" t="s">
+      <c r="W2" s="57" t="s">
         <v>66</v>
       </c>
       <c r="X2" s="64"/>
-      <c r="Y2" s="62" t="s">
+      <c r="Y2" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="Z2" s="63"/>
+      <c r="Z2" s="57"/>
     </row>
     <row r="3" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B3" s="32" t="s">
@@ -9173,34 +9208,34 @@
       </c>
     </row>
     <row r="31" spans="2:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="F31" s="59" t="s">
+      <c r="F31" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="G31" s="60"/>
-      <c r="H31" s="61"/>
-      <c r="I31" s="57">
+      <c r="G31" s="61"/>
+      <c r="H31" s="62"/>
+      <c r="I31" s="58">
         <f>C29+E29+G29+I29+K29+M29+O29+Q29+S29+U29+W29</f>
         <v>2521.33</v>
       </c>
-      <c r="J31" s="58"/>
+      <c r="J31" s="59"/>
     </row>
     <row r="32" spans="2:30" x14ac:dyDescent="0.55000000000000004">
       <c r="G32" s="65" t="s">
         <v>57</v>
       </c>
       <c r="H32" s="65"/>
-      <c r="I32" s="57">
+      <c r="I32" s="58">
         <f>+D29+F29+H29+J29+L29+N29+P29+R29+T29+V29+X29</f>
         <v>2997.5899999999997</v>
       </c>
-      <c r="J32" s="58"/>
+      <c r="J32" s="59"/>
     </row>
     <row r="33" spans="3:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="I33" s="57">
+      <c r="I33" s="58">
         <f>I32-I31</f>
         <v>476.25999999999976</v>
       </c>
-      <c r="J33" s="58"/>
+      <c r="J33" s="59"/>
     </row>
     <row r="34" spans="3:17" x14ac:dyDescent="0.55000000000000004">
       <c r="C34" s="36">
@@ -9253,11 +9288,11 @@
         <v>64</v>
       </c>
       <c r="H36" s="42"/>
-      <c r="I36" s="67">
+      <c r="I36" s="66">
         <f>I35+I33</f>
         <v>2476.2599999999998</v>
       </c>
-      <c r="J36" s="67"/>
+      <c r="J36" s="66"/>
       <c r="M36" s="33"/>
     </row>
     <row r="40" spans="3:17" x14ac:dyDescent="0.55000000000000004">
@@ -9300,13 +9335,125 @@
         <v>-291.55999999999995</v>
       </c>
     </row>
+    <row r="46" spans="3:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="D46" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="47" spans="3:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="D47" t="s">
+        <v>90</v>
+      </c>
+      <c r="E47" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="48" spans="3:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="D48" t="s">
+        <v>92</v>
+      </c>
+      <c r="E48" s="1">
+        <f>SUM(N29)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D49" t="s">
+        <v>12</v>
+      </c>
+      <c r="E49" s="1">
+        <f>SUM(F29)</f>
+        <v>222.44</v>
+      </c>
+    </row>
+    <row r="50" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D50" t="s">
+        <v>94</v>
+      </c>
+      <c r="E50" s="1">
+        <f>SUM(J29)</f>
+        <v>325.82</v>
+      </c>
+    </row>
+    <row r="51" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D51" t="s">
+        <v>95</v>
+      </c>
+      <c r="E51" s="1">
+        <f>SUM(D29)</f>
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="52" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D52" t="s">
+        <v>93</v>
+      </c>
+      <c r="E52" s="1">
+        <f>SUM(P29)</f>
+        <v>217.61</v>
+      </c>
+    </row>
+    <row r="53" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D53" t="s">
+        <v>97</v>
+      </c>
+      <c r="E53" s="1">
+        <f>SUM(R29)</f>
+        <v>120.83000000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D54" t="s">
+        <v>98</v>
+      </c>
+      <c r="E54" s="1">
+        <f>SUM(L29)</f>
+        <v>46.25</v>
+      </c>
+    </row>
+    <row r="55" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D55" t="s">
+        <v>89</v>
+      </c>
+      <c r="E55" s="1">
+        <f>SUM(V29)</f>
+        <v>86.25</v>
+      </c>
+    </row>
+    <row r="56" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D56" t="s">
+        <v>96</v>
+      </c>
+      <c r="E56" s="1">
+        <f>SUM(H29)</f>
+        <v>400.6</v>
+      </c>
+    </row>
+    <row r="57" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D57" t="s">
+        <v>9</v>
+      </c>
+      <c r="E57" s="1">
+        <f>SUM(T29)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D58" t="s">
+        <v>99</v>
+      </c>
+      <c r="E58" s="1">
+        <f>SUM(E48:E57)</f>
+        <v>1427.5500000000002</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
     <mergeCell ref="Q2:R2"/>
     <mergeCell ref="S2:T2"/>
     <mergeCell ref="U2:V2"/>
@@ -9315,11 +9462,11 @@
     <mergeCell ref="I31:J31"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="W2:X2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="O2:P2"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="54" orientation="landscape" r:id="rId1"/>
@@ -9333,8 +9480,8 @@
   </sheetPr>
   <dimension ref="B1:AH58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T14" sqref="T14"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="I54" sqref="I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -9353,54 +9500,54 @@
   <sheetData>
     <row r="1" spans="2:34" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="2" spans="2:34" ht="18.3" x14ac:dyDescent="0.7">
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="63"/>
-      <c r="E2" s="66" t="s">
+      <c r="D2" s="57"/>
+      <c r="E2" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="62"/>
-      <c r="G2" s="63" t="s">
+      <c r="F2" s="63"/>
+      <c r="G2" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63" t="s">
+      <c r="H2" s="57"/>
+      <c r="I2" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="63"/>
-      <c r="K2" s="63" t="s">
+      <c r="J2" s="57"/>
+      <c r="K2" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="63"/>
-      <c r="M2" s="66" t="s">
+      <c r="L2" s="57"/>
+      <c r="M2" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="62"/>
-      <c r="O2" s="63" t="s">
+      <c r="N2" s="63"/>
+      <c r="O2" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="63" t="s">
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="R2" s="63"/>
-      <c r="S2" s="63" t="s">
+      <c r="R2" s="57"/>
+      <c r="S2" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="T2" s="63"/>
-      <c r="U2" s="63" t="s">
+      <c r="T2" s="57"/>
+      <c r="U2" s="57" t="s">
         <v>65</v>
       </c>
       <c r="V2" s="64"/>
-      <c r="W2" s="63" t="s">
+      <c r="W2" s="57" t="s">
         <v>66</v>
       </c>
       <c r="X2" s="64"/>
-      <c r="Y2" s="62" t="s">
+      <c r="Y2" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="Z2" s="63"/>
+      <c r="Z2" s="57"/>
     </row>
     <row r="3" spans="2:34" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="32" t="s">
@@ -11409,34 +11556,34 @@
       </c>
     </row>
     <row r="31" spans="2:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="F31" s="59" t="s">
+      <c r="F31" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="G31" s="60"/>
-      <c r="H31" s="61"/>
-      <c r="I31" s="57">
+      <c r="G31" s="61"/>
+      <c r="H31" s="62"/>
+      <c r="I31" s="58">
         <f>C29+E29+G29+I29+K29+M29+O29+Q29+S29+U29+W29</f>
         <v>2462.73</v>
       </c>
-      <c r="J31" s="58"/>
+      <c r="J31" s="59"/>
     </row>
     <row r="32" spans="2:30" x14ac:dyDescent="0.55000000000000004">
       <c r="G32" s="65" t="s">
         <v>57</v>
       </c>
       <c r="H32" s="65"/>
-      <c r="I32" s="57">
+      <c r="I32" s="58">
         <f>+D29+F29+H29+J29+L29+N29+P29+R29+T29+V29+X29</f>
         <v>1004.25</v>
       </c>
-      <c r="J32" s="58"/>
+      <c r="J32" s="59"/>
     </row>
     <row r="33" spans="3:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="I33" s="57">
+      <c r="I33" s="58">
         <f>I32-I31</f>
         <v>-1458.48</v>
       </c>
-      <c r="J33" s="58"/>
+      <c r="J33" s="59"/>
       <c r="Y33">
         <f>2167+183+5*10</f>
         <v>2400</v>
@@ -11532,11 +11679,11 @@
         <v>64</v>
       </c>
       <c r="H38" s="42"/>
-      <c r="I38" s="67">
+      <c r="I38" s="66">
         <f>I36+I33+J37</f>
         <v>322.7800000000002</v>
       </c>
-      <c r="J38" s="67"/>
+      <c r="J38" s="66"/>
       <c r="M38" s="33"/>
     </row>
     <row r="40" spans="3:25" x14ac:dyDescent="0.55000000000000004">
@@ -11808,6 +11955,16 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
     <mergeCell ref="W2:X2"/>
     <mergeCell ref="Y2:Z2"/>
     <mergeCell ref="C2:D2"/>
@@ -11816,16 +11973,2179 @@
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="M2:N2"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="54" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7DF20FF-5D72-468B-A6CA-F6B5DE3B6E44}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B1:AH58"/>
+  <sheetViews>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="G61" sqref="G61"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="1.68359375" customWidth="1"/>
+    <col min="2" max="2" width="5.68359375" customWidth="1"/>
+    <col min="3" max="3" width="7.83984375" customWidth="1"/>
+    <col min="4" max="4" width="9.15625" customWidth="1"/>
+    <col min="5" max="23" width="7.83984375" customWidth="1"/>
+    <col min="24" max="24" width="8.83984375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.41796875" customWidth="1"/>
+    <col min="26" max="26" width="9.68359375" customWidth="1"/>
+    <col min="29" max="29" width="10.41796875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:34" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="2" spans="2:34" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="C2" s="57" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="57"/>
+      <c r="E2" s="67" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2" s="63"/>
+      <c r="G2" s="57" t="s">
+        <v>102</v>
+      </c>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57" t="s">
+        <v>103</v>
+      </c>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57" t="s">
+        <v>104</v>
+      </c>
+      <c r="L2" s="57"/>
+      <c r="M2" s="67" t="s">
+        <v>105</v>
+      </c>
+      <c r="N2" s="63"/>
+      <c r="O2" s="57" t="s">
+        <v>106</v>
+      </c>
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57" t="s">
+        <v>107</v>
+      </c>
+      <c r="R2" s="57"/>
+      <c r="S2" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="T2" s="57"/>
+      <c r="U2" s="57" t="s">
+        <v>108</v>
+      </c>
+      <c r="V2" s="64"/>
+      <c r="W2" s="57" t="s">
+        <v>66</v>
+      </c>
+      <c r="X2" s="64"/>
+      <c r="Y2" s="63" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z2" s="57"/>
+    </row>
+    <row r="3" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B3" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="M3" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="N3" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="O3" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="P3" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q3" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="R3" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="S3" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="T3" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="U3" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="V3" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="W3" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="X3" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y3" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z3" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA3" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB3" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC3" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD3" s="25"/>
+    </row>
+    <row r="4" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B4" s="54" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="12"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="13"/>
+      <c r="S4" s="14"/>
+      <c r="T4" s="13"/>
+      <c r="U4" s="12"/>
+      <c r="V4" s="19"/>
+      <c r="W4" s="12"/>
+      <c r="X4" s="19"/>
+      <c r="Y4" s="14">
+        <f t="shared" ref="Y4:Z25" si="0">U4+S4+Q4+O4+M4+K4+I4+G4+E4+C4</f>
+        <v>0</v>
+      </c>
+      <c r="Z4" s="48">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA4" s="1">
+        <f>Y4</f>
+        <v>0</v>
+      </c>
+      <c r="AB4" s="1">
+        <f>Z4</f>
+        <v>0</v>
+      </c>
+      <c r="AC4" s="1">
+        <f>AB4-AA4</f>
+        <v>0</v>
+      </c>
+      <c r="AD4" s="1"/>
+    </row>
+    <row r="5" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B5" s="52" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="15"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="17"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="17"/>
+      <c r="T5" s="16"/>
+      <c r="U5" s="15"/>
+      <c r="V5" s="20"/>
+      <c r="W5" s="15"/>
+      <c r="X5" s="20"/>
+      <c r="Y5" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z5" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA5" s="1">
+        <f>AA4+Y5</f>
+        <v>0</v>
+      </c>
+      <c r="AB5" s="1">
+        <f>AB4+Z5</f>
+        <v>0</v>
+      </c>
+      <c r="AC5" s="1">
+        <f t="shared" ref="AC5:AC26" si="1">AB5-AA5</f>
+        <v>0</v>
+      </c>
+      <c r="AD5" s="1"/>
+    </row>
+    <row r="6" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B6" s="51" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="15"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="17"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="17"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="15"/>
+      <c r="V6" s="20"/>
+      <c r="W6" s="15"/>
+      <c r="X6" s="20"/>
+      <c r="Y6" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z6" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA6" s="1">
+        <f t="shared" ref="AA6:AB21" si="2">AA5+Y6</f>
+        <v>0</v>
+      </c>
+      <c r="AB6" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AC6" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD6" s="1"/>
+      <c r="AE6" s="43" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF6" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG6" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="AH6" s="43" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B7" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="15"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="16"/>
+      <c r="S7" s="17"/>
+      <c r="T7" s="16"/>
+      <c r="U7" s="15"/>
+      <c r="V7" s="20"/>
+      <c r="W7" s="15"/>
+      <c r="X7" s="20"/>
+      <c r="Y7" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z7" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA7" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AB7" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AC7" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD7" s="44" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE7" s="44">
+        <f>+G29+'Punters 2021'!Q27+'Punters 2020'!M27+'Punters club'!J6+'Punters 2022'!C29</f>
+        <v>788</v>
+      </c>
+      <c r="AF7" s="44">
+        <f>+H29+'Punters 2021'!R27+'Punters 2020'!N27+'Punters club'!K6+'Punters 2022'!D29</f>
+        <v>534</v>
+      </c>
+      <c r="AG7" s="49">
+        <f>+AF7-AE7</f>
+        <v>-254</v>
+      </c>
+      <c r="AH7" s="47">
+        <f>(AF7-AE7)/AE7</f>
+        <v>-0.32233502538071068</v>
+      </c>
+    </row>
+    <row r="8" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B8" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="15"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="17"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="17"/>
+      <c r="R8" s="16"/>
+      <c r="S8" s="17"/>
+      <c r="T8" s="16"/>
+      <c r="U8" s="15"/>
+      <c r="V8" s="20"/>
+      <c r="W8" s="15"/>
+      <c r="X8" s="20"/>
+      <c r="Y8" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z8" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA8" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AB8" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AC8" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD8" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE8" s="44">
+        <f>+E29+'Punters 2021'!I27+'Punters 2020'!G27+'Punters club'!J7+'Punters 2022'!E29</f>
+        <v>923</v>
+      </c>
+      <c r="AF8" s="44">
+        <f>+F29+'Punters 2021'!J27+'Punters 2020'!H27+'Punters club'!K7+'Punters 2022'!F29</f>
+        <v>1019.77</v>
+      </c>
+      <c r="AG8" s="50">
+        <f t="shared" ref="AG8:AG16" si="3">+AF8-AE8</f>
+        <v>96.769999999999982</v>
+      </c>
+      <c r="AH8" s="47">
+        <f t="shared" ref="AH8:AH16" si="4">(AF8-AE8)/AE8</f>
+        <v>0.10484290357529792</v>
+      </c>
+    </row>
+    <row r="9" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B9" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="15"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="17"/>
+      <c r="R9" s="16"/>
+      <c r="S9" s="17"/>
+      <c r="T9" s="16"/>
+      <c r="U9" s="15"/>
+      <c r="V9" s="20"/>
+      <c r="W9" s="15"/>
+      <c r="X9" s="20"/>
+      <c r="Y9" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z9" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA9" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AB9" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AC9" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD9" s="44" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE9" s="44">
+        <f>+I29+'Punters 2021'!K27+'Punters 2020'!E27+'Punters club'!J11+'Punters 2022'!G29</f>
+        <v>896.48</v>
+      </c>
+      <c r="AF9" s="44">
+        <f>+J29+'Punters 2021'!L27+'Punters 2020'!F27+'Punters club'!K11+'Punters 2022'!H29</f>
+        <v>961.4</v>
+      </c>
+      <c r="AG9" s="50">
+        <f t="shared" si="3"/>
+        <v>64.919999999999959</v>
+      </c>
+      <c r="AH9" s="47">
+        <f t="shared" si="4"/>
+        <v>7.2416562555773639E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B10" s="53" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="15"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="17"/>
+      <c r="R10" s="16"/>
+      <c r="S10" s="17"/>
+      <c r="T10" s="16"/>
+      <c r="U10" s="15"/>
+      <c r="V10" s="20"/>
+      <c r="W10" s="15"/>
+      <c r="X10" s="20"/>
+      <c r="Y10" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z10" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA10" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AB10" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AC10" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD10" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE10" s="44">
+        <f>+Q29+'Punters 2021'!G27+'Punters 2020'!I27+'Punters club'!J10+'Punters 2022'!I29</f>
+        <v>899.9</v>
+      </c>
+      <c r="AF10" s="44">
+        <f>+R29+'Punters 2021'!H27+'Punters 2020'!J27+'Punters club'!K10+'Punters 2022'!J29</f>
+        <v>1459.8999999999999</v>
+      </c>
+      <c r="AG10" s="50">
+        <f t="shared" si="3"/>
+        <v>559.99999999999989</v>
+      </c>
+      <c r="AH10" s="45">
+        <f t="shared" si="4"/>
+        <v>0.6222913657073007</v>
+      </c>
+    </row>
+    <row r="11" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B11" s="52" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="15"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="17"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="17"/>
+      <c r="R11" s="16"/>
+      <c r="S11" s="17"/>
+      <c r="T11" s="16"/>
+      <c r="U11" s="15"/>
+      <c r="V11" s="20"/>
+      <c r="W11" s="15"/>
+      <c r="X11" s="20"/>
+      <c r="Y11" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z11" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA11" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AB11" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AC11" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD11" s="44" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE11" s="44">
+        <f>+M29+'Punters 2021'!E27+'Punters 2020'!K27+'Punters 2022'!K29</f>
+        <v>633</v>
+      </c>
+      <c r="AF11" s="44">
+        <f>+N29+'Punters 2021'!F27+'Punters 2020'!L27+'Punters 2022'!L29</f>
+        <v>58.25</v>
+      </c>
+      <c r="AG11" s="49">
+        <f t="shared" si="3"/>
+        <v>-574.75</v>
+      </c>
+      <c r="AH11" s="47">
+        <f t="shared" si="4"/>
+        <v>-0.90797788309636651</v>
+      </c>
+    </row>
+    <row r="12" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B12" s="51" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="15"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="17"/>
+      <c r="R12" s="16"/>
+      <c r="S12" s="17"/>
+      <c r="T12" s="16"/>
+      <c r="U12" s="15"/>
+      <c r="V12" s="20"/>
+      <c r="W12" s="15"/>
+      <c r="X12" s="20"/>
+      <c r="Y12" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z12" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA12" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AB12" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AC12" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD12" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE12" s="44">
+        <f>+C29+'Punters 2021'!S27+'Punters 2020'!S27+'Punters club'!J8+'Punters 2022'!M29</f>
+        <v>954.96</v>
+      </c>
+      <c r="AF12" s="44">
+        <f>+D29+'Punters 2021'!T27+'Punters 2020'!T27+'Punters club'!K8+'Punters 2022'!N29</f>
+        <v>564.32999999999993</v>
+      </c>
+      <c r="AG12" s="49">
+        <f t="shared" si="3"/>
+        <v>-390.63000000000011</v>
+      </c>
+      <c r="AH12" s="47">
+        <f t="shared" si="4"/>
+        <v>-0.40905378235737633</v>
+      </c>
+    </row>
+    <row r="13" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B13" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="15"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="17"/>
+      <c r="P13" s="16"/>
+      <c r="Q13" s="17"/>
+      <c r="R13" s="16"/>
+      <c r="S13" s="17"/>
+      <c r="T13" s="16"/>
+      <c r="U13" s="15"/>
+      <c r="V13" s="20"/>
+      <c r="W13" s="15"/>
+      <c r="X13" s="20"/>
+      <c r="Y13" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z13" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA13" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AB13" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AC13" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD13" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE13" s="44">
+        <f>+S29+'Punters 2021'!O27+'Punters 2020'!O27+'Punters club'!J9+'Punters 2022'!O29</f>
+        <v>881.34</v>
+      </c>
+      <c r="AF13" s="44">
+        <f>+T29+'Punters 2021'!P27+'Punters 2020'!P27+'Punters club'!K9+'Punters 2022'!P29</f>
+        <v>218.25</v>
+      </c>
+      <c r="AG13" s="49">
+        <f t="shared" si="3"/>
+        <v>-663.09</v>
+      </c>
+      <c r="AH13" s="47">
+        <f t="shared" si="4"/>
+        <v>-0.75236571584178635</v>
+      </c>
+    </row>
+    <row r="14" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B14" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="15"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="17"/>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="17"/>
+      <c r="R14" s="16"/>
+      <c r="S14" s="17"/>
+      <c r="T14" s="16"/>
+      <c r="U14" s="15"/>
+      <c r="V14" s="20"/>
+      <c r="W14" s="15"/>
+      <c r="X14" s="20"/>
+      <c r="Y14" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z14" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA14" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AB14" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AC14" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD14" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE14" s="44">
+        <f>+O29+'Punters 2021'!M27+'Punters 2020'!Q27+'Punters club'!J5+'Punters 2022'!Q29</f>
+        <v>883</v>
+      </c>
+      <c r="AF14" s="44">
+        <f>+P29+'Punters 2021'!N27+'Punters 2020'!R27+'Punters club'!K5+'Punters 2022'!R29</f>
+        <v>637.47</v>
+      </c>
+      <c r="AG14" s="49">
+        <f t="shared" si="3"/>
+        <v>-245.52999999999997</v>
+      </c>
+      <c r="AH14" s="47">
+        <f t="shared" si="4"/>
+        <v>-0.27806342015855035</v>
+      </c>
+    </row>
+    <row r="15" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B15" s="51" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="15"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="17"/>
+      <c r="P15" s="16"/>
+      <c r="Q15" s="17"/>
+      <c r="R15" s="16"/>
+      <c r="S15" s="17"/>
+      <c r="T15" s="16"/>
+      <c r="U15" s="15"/>
+      <c r="V15" s="20"/>
+      <c r="W15" s="15"/>
+      <c r="X15" s="20"/>
+      <c r="Y15" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z15" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA15" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AB15" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AC15" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD15" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE15" s="44">
+        <f>+K29+'Punters 2021'!C27+'Punters 2020'!C27+'Punters club'!J4+'Punters 2022'!S29</f>
+        <v>892.7</v>
+      </c>
+      <c r="AF15" s="44">
+        <f>+L29+'Punters 2021'!D27+'Punters 2020'!D27+'Punters club'!K4+'Punters 2022'!T29</f>
+        <v>1461.09</v>
+      </c>
+      <c r="AG15" s="50">
+        <f t="shared" si="3"/>
+        <v>568.38999999999987</v>
+      </c>
+      <c r="AH15" s="45">
+        <f t="shared" si="4"/>
+        <v>0.63670886075949351</v>
+      </c>
+    </row>
+    <row r="16" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B16" s="53" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="15"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="17"/>
+      <c r="R16" s="16"/>
+      <c r="S16" s="17"/>
+      <c r="T16" s="16"/>
+      <c r="U16" s="15"/>
+      <c r="V16" s="20"/>
+      <c r="W16" s="15"/>
+      <c r="X16" s="20"/>
+      <c r="Y16" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z16" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA16" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AB16" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AC16" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD16" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE16" s="44">
+        <f>+U29+'Punters 2022'!U29</f>
+        <v>200</v>
+      </c>
+      <c r="AF16" s="44">
+        <f>+V29+'Punters 2022'!V29</f>
+        <v>86.25</v>
+      </c>
+      <c r="AG16" s="49">
+        <f t="shared" si="3"/>
+        <v>-113.75</v>
+      </c>
+      <c r="AH16" s="47">
+        <f t="shared" si="4"/>
+        <v>-0.56874999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="2:30" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B17" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="15"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="17"/>
+      <c r="R17" s="16"/>
+      <c r="S17" s="17"/>
+      <c r="T17" s="16"/>
+      <c r="U17" s="15"/>
+      <c r="V17" s="20"/>
+      <c r="W17" s="15"/>
+      <c r="X17" s="20"/>
+      <c r="Y17" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z17" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA17" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AB17" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AC17" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD17" s="1"/>
+    </row>
+    <row r="18" spans="2:30" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B18" s="51" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="17"/>
+      <c r="P18" s="16"/>
+      <c r="Q18" s="17"/>
+      <c r="R18" s="16"/>
+      <c r="S18" s="17"/>
+      <c r="T18" s="16"/>
+      <c r="U18" s="15"/>
+      <c r="V18" s="20"/>
+      <c r="W18" s="15"/>
+      <c r="X18" s="20"/>
+      <c r="Y18" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z18" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA18" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AB18" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AC18" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD18" s="1"/>
+    </row>
+    <row r="19" spans="2:30" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B19" s="53" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="15"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="17"/>
+      <c r="P19" s="16"/>
+      <c r="Q19" s="17"/>
+      <c r="R19" s="16"/>
+      <c r="S19" s="17"/>
+      <c r="T19" s="16"/>
+      <c r="U19" s="15"/>
+      <c r="V19" s="20"/>
+      <c r="W19" s="15"/>
+      <c r="X19" s="20"/>
+      <c r="Y19" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z19" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA19" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AB19" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AC19" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD19" s="1"/>
+    </row>
+    <row r="20" spans="2:30" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B20" s="52" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="15"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="17"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="17"/>
+      <c r="P20" s="16"/>
+      <c r="Q20" s="17"/>
+      <c r="R20" s="16"/>
+      <c r="S20" s="17"/>
+      <c r="T20" s="16"/>
+      <c r="U20" s="15"/>
+      <c r="V20" s="20"/>
+      <c r="W20" s="15"/>
+      <c r="X20" s="20"/>
+      <c r="Y20" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z20" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA20" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AB20" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AC20" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD20" s="1"/>
+    </row>
+    <row r="21" spans="2:30" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B21" s="51" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="15"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="17"/>
+      <c r="N21" s="16"/>
+      <c r="O21" s="17"/>
+      <c r="P21" s="16"/>
+      <c r="Q21" s="17"/>
+      <c r="R21" s="16"/>
+      <c r="S21" s="17"/>
+      <c r="T21" s="16"/>
+      <c r="U21" s="15"/>
+      <c r="V21" s="20"/>
+      <c r="W21" s="15"/>
+      <c r="X21" s="20"/>
+      <c r="Y21" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z21" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA21" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AB21" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AC21" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD21" s="1"/>
+    </row>
+    <row r="22" spans="2:30" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B22" s="53" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="15"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="17"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="17"/>
+      <c r="N22" s="16"/>
+      <c r="O22" s="17"/>
+      <c r="P22" s="16"/>
+      <c r="Q22" s="17"/>
+      <c r="R22" s="16"/>
+      <c r="S22" s="17"/>
+      <c r="T22" s="16"/>
+      <c r="U22" s="15"/>
+      <c r="V22" s="20"/>
+      <c r="W22" s="15"/>
+      <c r="X22" s="20"/>
+      <c r="Y22" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z22" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA22" s="1">
+        <f t="shared" ref="AA22:AB26" si="5">AA21+Y22</f>
+        <v>0</v>
+      </c>
+      <c r="AB22" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AC22" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD22" s="1"/>
+    </row>
+    <row r="23" spans="2:30" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B23" s="52" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="15"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="16"/>
+      <c r="M23" s="17"/>
+      <c r="N23" s="16"/>
+      <c r="O23" s="17"/>
+      <c r="P23" s="16"/>
+      <c r="Q23" s="17"/>
+      <c r="R23" s="16"/>
+      <c r="S23" s="17"/>
+      <c r="T23" s="16"/>
+      <c r="U23" s="15"/>
+      <c r="V23" s="20"/>
+      <c r="W23" s="15"/>
+      <c r="X23" s="20"/>
+      <c r="Y23" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z23" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA23" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AB23" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AC23" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD23" s="1"/>
+    </row>
+    <row r="24" spans="2:30" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B24" s="51" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" s="15"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="16"/>
+      <c r="M24" s="17"/>
+      <c r="N24" s="16"/>
+      <c r="O24" s="17"/>
+      <c r="P24" s="16"/>
+      <c r="Q24" s="17"/>
+      <c r="R24" s="16"/>
+      <c r="S24" s="17"/>
+      <c r="T24" s="16"/>
+      <c r="U24" s="15"/>
+      <c r="V24" s="20"/>
+      <c r="W24" s="15"/>
+      <c r="X24" s="20"/>
+      <c r="Y24" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z24" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA24" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AB24" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AC24" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD24" s="1"/>
+    </row>
+    <row r="25" spans="2:30" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B25" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="15"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="17"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="17"/>
+      <c r="N25" s="16"/>
+      <c r="O25" s="17"/>
+      <c r="P25" s="16"/>
+      <c r="Q25" s="17"/>
+      <c r="R25" s="16"/>
+      <c r="S25" s="17"/>
+      <c r="T25" s="16"/>
+      <c r="U25" s="15"/>
+      <c r="V25" s="20"/>
+      <c r="W25" s="15"/>
+      <c r="X25" s="20"/>
+      <c r="Y25" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z25" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA25" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AB25" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AC25" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD25" s="1"/>
+    </row>
+    <row r="26" spans="2:30" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B26" s="54" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="15"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="17"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="17"/>
+      <c r="N26" s="16"/>
+      <c r="O26" s="17"/>
+      <c r="P26" s="16"/>
+      <c r="Q26" s="17"/>
+      <c r="R26" s="16"/>
+      <c r="S26" s="17"/>
+      <c r="T26" s="16"/>
+      <c r="U26" s="15"/>
+      <c r="V26" s="20"/>
+      <c r="W26" s="15"/>
+      <c r="X26" s="20"/>
+      <c r="Y26" s="17">
+        <f t="shared" ref="Y26:Z28" si="6">U26+S26+Q26+O26+M26+K26+I26+G26+E26+C26</f>
+        <v>0</v>
+      </c>
+      <c r="Z26" s="16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AA26" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AB26" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AC26" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD26" s="1"/>
+    </row>
+    <row r="27" spans="2:30" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B27" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" s="15"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="17"/>
+      <c r="N27" s="16"/>
+      <c r="O27" s="17"/>
+      <c r="P27" s="16"/>
+      <c r="Q27" s="17"/>
+      <c r="R27" s="16"/>
+      <c r="S27" s="17"/>
+      <c r="T27" s="16"/>
+      <c r="U27" s="15"/>
+      <c r="V27" s="20"/>
+      <c r="W27" s="15"/>
+      <c r="X27" s="20"/>
+      <c r="Y27" s="17">
+        <f>U27+S27+Q27+O27+M27+K27+I27+G27+E27+C27+W27</f>
+        <v>0</v>
+      </c>
+      <c r="Z27" s="16">
+        <f>V27+T27+R27+P27+N27+L27+J27+H27+F27+D27+X27</f>
+        <v>0</v>
+      </c>
+      <c r="AA27" s="1"/>
+      <c r="AB27" s="1"/>
+      <c r="AC27" s="1"/>
+      <c r="AD27" s="1"/>
+    </row>
+    <row r="28" spans="2:30" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B28" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="C28" s="15"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="17"/>
+      <c r="L28" s="16"/>
+      <c r="M28" s="17"/>
+      <c r="N28" s="16"/>
+      <c r="O28" s="17"/>
+      <c r="P28" s="16"/>
+      <c r="Q28" s="17"/>
+      <c r="R28" s="16"/>
+      <c r="S28" s="17"/>
+      <c r="T28" s="16"/>
+      <c r="U28" s="15"/>
+      <c r="V28" s="20"/>
+      <c r="W28" s="15"/>
+      <c r="X28" s="20"/>
+      <c r="Y28" s="17">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Z28" s="16">
+        <f>V28+T28+R28+P28+N28+L28+J28+H28+F28+D28+X28</f>
+        <v>0</v>
+      </c>
+      <c r="AA28" s="1"/>
+      <c r="AB28" s="1"/>
+      <c r="AC28" s="1"/>
+      <c r="AD28" s="1"/>
+    </row>
+    <row r="29" spans="2:30" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B29" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="18">
+        <f t="shared" ref="C29:Z29" si="7">SUM(C4:C28)</f>
+        <v>0</v>
+      </c>
+      <c r="D29" s="18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E29" s="18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F29" s="18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G29" s="18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H29" s="18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I29" s="18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J29" s="18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K29" s="18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L29" s="18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M29" s="18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N29" s="18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="O29" s="18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="P29" s="18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Q29" s="18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="R29" s="18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S29" s="18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="T29" s="18">
+        <f>SUM(T4:T28)</f>
+        <v>0</v>
+      </c>
+      <c r="U29" s="18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V29" s="21">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="W29" s="18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X29" s="21">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Y29" s="29">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Z29" s="18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:30" x14ac:dyDescent="0.55000000000000004">
+      <c r="D30" s="56" t="e">
+        <f>(D29-C29)/C29</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F30" s="34" t="e">
+        <f>(F29-E29)/E29</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H30" s="34" t="e">
+        <f>(H29-G29)/G29</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J30" s="34" t="e">
+        <f>(J29-I29)/I29</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L30" s="28" t="e">
+        <f>(L29-K29)/K29</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N30" s="28" t="e">
+        <f>(N29-M29)/M29</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P30" s="28" t="e">
+        <f>(P29-O29)/O29</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R30" s="28" t="e">
+        <f>(R29-Q29)/Q29</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T30" s="22" t="e">
+        <f>(T29-S29)/S29</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V30" s="28" t="e">
+        <f>(V29-U29)/U29</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="31" spans="2:30" x14ac:dyDescent="0.55000000000000004">
+      <c r="F31" s="60" t="s">
+        <v>56</v>
+      </c>
+      <c r="G31" s="61"/>
+      <c r="H31" s="62"/>
+      <c r="I31" s="58">
+        <f>C29+E29+G29+I29+K29+M29+O29+Q29+S29+U29+W29</f>
+        <v>0</v>
+      </c>
+      <c r="J31" s="59"/>
+    </row>
+    <row r="32" spans="2:30" x14ac:dyDescent="0.55000000000000004">
+      <c r="G32" s="65" t="s">
+        <v>57</v>
+      </c>
+      <c r="H32" s="65"/>
+      <c r="I32" s="58">
+        <f>+D29+F29+H29+J29+L29+N29+P29+R29+T29+V29+X29</f>
+        <v>0</v>
+      </c>
+      <c r="J32" s="59"/>
+    </row>
+    <row r="33" spans="3:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="I33" s="58">
+        <f>I32-I31</f>
+        <v>0</v>
+      </c>
+      <c r="J33" s="59"/>
+      <c r="Y33">
+        <f>2167+183+5*10</f>
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="34" spans="3:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="C34" s="36">
+        <f>C29+E29+G29+I29</f>
+        <v>0</v>
+      </c>
+      <c r="D34" s="36">
+        <f>D29+F29+H29+J29</f>
+        <v>0</v>
+      </c>
+      <c r="E34" s="37">
+        <f>D34-C34</f>
+        <v>0</v>
+      </c>
+      <c r="I34" s="38">
+        <f>O29+K29+M29</f>
+        <v>0</v>
+      </c>
+      <c r="J34" s="38">
+        <f>P29+L29+N29</f>
+        <v>0</v>
+      </c>
+      <c r="K34" s="39">
+        <f>J34-I34</f>
+        <v>0</v>
+      </c>
+      <c r="O34" s="40">
+        <f>U29+Q29+S29</f>
+        <v>0</v>
+      </c>
+      <c r="P34" s="40">
+        <f>V29+R29+T29</f>
+        <v>0</v>
+      </c>
+      <c r="Q34" s="41">
+        <f>P34-O34</f>
+        <v>0</v>
+      </c>
+      <c r="X34" s="55"/>
+      <c r="Y34">
+        <f>15*10</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="35" spans="3:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="C35" s="36"/>
+      <c r="D35" s="34" t="e">
+        <f>(D34-C34)/C34</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E35" s="37"/>
+      <c r="I35" s="38"/>
+      <c r="J35" s="34" t="e">
+        <f>(J34-I34)/I34</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K35" s="39"/>
+      <c r="O35" s="40"/>
+      <c r="P35" s="34" t="e">
+        <f>(P34-O34)/O34</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q35" s="41"/>
+      <c r="X35" s="55"/>
+    </row>
+    <row r="36" spans="3:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="G36" t="s">
+        <v>58</v>
+      </c>
+      <c r="I36" cm="1">
+        <f t="array" ref="I36:J36">2000+'Punters 2022'!I36:J36</f>
+        <v>4476.26</v>
+      </c>
+      <c r="J36">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="37" spans="3:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="G37" t="s">
+        <v>85</v>
+      </c>
+      <c r="J37">
+        <f>-269.5*10</f>
+        <v>-2695</v>
+      </c>
+    </row>
+    <row r="38" spans="3:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="G38" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="H38" s="42"/>
+      <c r="I38" s="66">
+        <f>I36+I33+J37</f>
+        <v>1781.2600000000002</v>
+      </c>
+      <c r="J38" s="66"/>
+      <c r="M38" s="33"/>
+    </row>
+    <row r="40" spans="3:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <f>10+15</f>
+        <v>25</v>
+      </c>
+      <c r="I40">
+        <v>10</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
+      <c r="M40">
+        <v>25</v>
+      </c>
+      <c r="O40">
+        <v>0</v>
+      </c>
+      <c r="Q40">
+        <v>0</v>
+      </c>
+      <c r="S40">
+        <v>0</v>
+      </c>
+      <c r="U40">
+        <v>13</v>
+      </c>
+      <c r="X40" s="55" t="s">
+        <v>86</v>
+      </c>
+      <c r="Y40">
+        <f>30+15+25+20+15+55+15+15+15+28</f>
+        <v>233</v>
+      </c>
+    </row>
+    <row r="41" spans="3:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="V41">
+        <f>3260-720</f>
+        <v>2540</v>
+      </c>
+    </row>
+    <row r="42" spans="3:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="C42" s="1">
+        <f>C29+E29+G29+I29</f>
+        <v>0</v>
+      </c>
+      <c r="D42" s="1">
+        <f>D29+F29+H29+J29</f>
+        <v>0</v>
+      </c>
+      <c r="I42" s="1">
+        <f>O29+K29+M29</f>
+        <v>0</v>
+      </c>
+      <c r="J42" s="1">
+        <f>P29+L29+N29</f>
+        <v>0</v>
+      </c>
+      <c r="O42" s="1">
+        <f>U29+Q29+S29</f>
+        <v>0</v>
+      </c>
+      <c r="P42" s="1">
+        <f>V29+R29+T29</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="3:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="D43" s="1">
+        <f>D42-C42</f>
+        <v>0</v>
+      </c>
+      <c r="J43" s="33">
+        <f>J42-I42</f>
+        <v>0</v>
+      </c>
+      <c r="P43" s="33">
+        <f>P42-O42</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="3:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="V45" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="46" spans="3:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="D46" t="s">
+        <v>88</v>
+      </c>
+      <c r="J46" t="s">
+        <v>109</v>
+      </c>
+      <c r="V46" t="s">
+        <v>89</v>
+      </c>
+      <c r="W46">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="3:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="D47" t="s">
+        <v>90</v>
+      </c>
+      <c r="E47" t="s">
+        <v>91</v>
+      </c>
+      <c r="J47" t="s">
+        <v>90</v>
+      </c>
+      <c r="K47" t="s">
+        <v>110</v>
+      </c>
+      <c r="V47" t="s">
+        <v>12</v>
+      </c>
+      <c r="W47">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="3:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="D48" t="s">
+        <v>92</v>
+      </c>
+      <c r="E48" s="1">
+        <f>SUM(V29)</f>
+        <v>0</v>
+      </c>
+      <c r="J48" t="s">
+        <v>92</v>
+      </c>
+      <c r="K48">
+        <v>0</v>
+      </c>
+      <c r="V48" t="s">
+        <v>93</v>
+      </c>
+      <c r="W48">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="4:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="D49" t="s">
+        <v>12</v>
+      </c>
+      <c r="E49" s="1">
+        <f>SUM(L29)</f>
+        <v>0</v>
+      </c>
+      <c r="J49" t="s">
+        <v>12</v>
+      </c>
+      <c r="K49">
+        <v>0</v>
+      </c>
+      <c r="V49" t="s">
+        <v>92</v>
+      </c>
+      <c r="W49">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="4:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="D50" t="s">
+        <v>94</v>
+      </c>
+      <c r="E50" s="1">
+        <f>SUM(D29)</f>
+        <v>0</v>
+      </c>
+      <c r="J50" t="s">
+        <v>94</v>
+      </c>
+      <c r="K50">
+        <v>0</v>
+      </c>
+      <c r="V50" t="s">
+        <v>9</v>
+      </c>
+      <c r="W50">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="4:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="D51" t="s">
+        <v>95</v>
+      </c>
+      <c r="E51" s="1">
+        <f>SUM(F29)</f>
+        <v>0</v>
+      </c>
+      <c r="J51" t="s">
+        <v>95</v>
+      </c>
+      <c r="K51">
+        <v>0</v>
+      </c>
+      <c r="V51" t="s">
+        <v>11</v>
+      </c>
+      <c r="W51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="4:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="D52" t="s">
+        <v>93</v>
+      </c>
+      <c r="E52" s="1">
+        <f>SUM(T29)</f>
+        <v>0</v>
+      </c>
+      <c r="J52" t="s">
+        <v>93</v>
+      </c>
+      <c r="K52">
+        <v>0</v>
+      </c>
+      <c r="V52" t="s">
+        <v>96</v>
+      </c>
+      <c r="W52">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="4:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="D53" t="s">
+        <v>97</v>
+      </c>
+      <c r="E53" s="1">
+        <f>SUM(R29)</f>
+        <v>0</v>
+      </c>
+      <c r="J53" t="s">
+        <v>97</v>
+      </c>
+      <c r="K53">
+        <v>0</v>
+      </c>
+      <c r="V53" t="s">
+        <v>98</v>
+      </c>
+      <c r="W53">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="4:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="D54" t="s">
+        <v>98</v>
+      </c>
+      <c r="E54" s="1">
+        <f>SUM(J29)</f>
+        <v>0</v>
+      </c>
+      <c r="J54" t="s">
+        <v>98</v>
+      </c>
+      <c r="K54">
+        <v>0</v>
+      </c>
+      <c r="V54" t="s">
+        <v>97</v>
+      </c>
+      <c r="W54">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="4:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="D55" t="s">
+        <v>89</v>
+      </c>
+      <c r="E55" s="1">
+        <f>SUM(H29)</f>
+        <v>0</v>
+      </c>
+      <c r="J55" t="s">
+        <v>89</v>
+      </c>
+      <c r="K55">
+        <v>0</v>
+      </c>
+      <c r="V55" t="s">
+        <v>94</v>
+      </c>
+      <c r="W55">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="4:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="D56" t="s">
+        <v>96</v>
+      </c>
+      <c r="E56" s="1">
+        <f>SUM(N29)</f>
+        <v>0</v>
+      </c>
+      <c r="J56" t="s">
+        <v>96</v>
+      </c>
+      <c r="K56">
+        <v>0</v>
+      </c>
+      <c r="W56">
+        <f>SUM(W46:W55)</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="4:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="D57" t="s">
+        <v>9</v>
+      </c>
+      <c r="E57" s="1">
+        <f>SUM(P29)</f>
+        <v>0</v>
+      </c>
+      <c r="J57" t="s">
+        <v>9</v>
+      </c>
+      <c r="K57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="4:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="D58" t="s">
+        <v>99</v>
+      </c>
+      <c r="E58" s="1">
+        <f>SUM(E48:E57)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="18">
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="I33:J33"/>
     <mergeCell ref="I38:J38"/>
     <mergeCell ref="O2:P2"/>
     <mergeCell ref="Q2:R2"/>
     <mergeCell ref="S2:T2"/>
     <mergeCell ref="U2:V2"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="54" orientation="landscape" r:id="rId1"/>
@@ -11833,6 +14153,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="3e1ffae5-f160-4019-9720-1b11bf1b81a3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002D8393059904904F9DB82DE4B9AFABF6" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f7bafc8adbaca2e93ffc3a1da3fd32d5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3e1ffae5-f160-4019-9720-1b11bf1b81a3" xmlns:ns4="21753bd8-bffc-4cd2-a328-982ee854c895" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f821f56a5d2247de677e71e73e5a99e" ns3:_="" ns4:_="">
     <xsd:import namespace="3e1ffae5-f160-4019-9720-1b11bf1b81a3"/>
@@ -12053,24 +14390,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4D7A62A-0CB5-48B0-A73A-0A91BCC8EAEF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3e1ffae5-f160-4019-9720-1b11bf1b81a3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="3e1ffae5-f160-4019-9720-1b11bf1b81a3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{948817D4-7F3F-493D-9D4C-B473DA03CC7E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22BA772B-ABF0-4278-9CEF-D9160BBA9E07}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12089,24 +14427,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{948817D4-7F3F-493D-9D4C-B473DA03CC7E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4D7A62A-0CB5-48B0-A73A-0A91BCC8EAEF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3e1ffae5-f160-4019-9720-1b11bf1b81a3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{0f7d30c2-cad0-4405-8153-25a6a3313da4}" enabled="1" method="Privileged" siteId="{6c637512-c417-4e78-9d62-b61258e4b619}" contentBits="0" removed="0"/>

</xml_diff>

<commit_message>
Updating leaderboard and betting round
</commit_message>
<xml_diff>
--- a/public/Data/HEMANPUNTERS.xlsx
+++ b/public/Data/HEMANPUNTERS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bturnor\source\repos\PersonalWork\seeMore\public\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF446B2C-75F3-4099-A001-A69BE1B38345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{515129D1-6049-4859-AA7B-8DC703CB0DD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-192" windowWidth="23040" windowHeight="13872" firstSheet="3" activeTab="3" xr2:uid="{525E8989-1938-4309-A4CF-8F1D15E362FB}"/>
+    <workbookView xWindow="57480" yWindow="45" windowWidth="29040" windowHeight="15720" firstSheet="5" activeTab="5" xr2:uid="{525E8989-1938-4309-A4CF-8F1D15E362FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Punters club" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="113">
   <si>
     <t>HE_MAN PUNTERS 2019</t>
   </si>
@@ -392,7 +392,13 @@
     <t>B.SPICER</t>
   </si>
   <si>
-    <t>Strikes for 2024 Season</t>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>1 leg losses @ 18th March 2024</t>
+  </si>
+  <si>
+    <t>Strikes for 2024 Season at 18th March 2024</t>
   </si>
   <si>
     <t>Strikes</t>
@@ -1030,6 +1036,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1329,9 +1339,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{389AE74A-6876-4CFE-8387-EE4223AB8F41}">
   <dimension ref="A1:M221"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:M66"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -7085,10 +7093,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AH58"/>
+  <dimension ref="B1:AH41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="T37" sqref="T37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -7097,8 +7105,7 @@
     <col min="2" max="2" width="5.68359375" customWidth="1"/>
     <col min="3" max="3" width="7.83984375" customWidth="1"/>
     <col min="4" max="4" width="9.15625" customWidth="1"/>
-    <col min="5" max="5" width="9.734375" customWidth="1"/>
-    <col min="6" max="23" width="7.83984375" customWidth="1"/>
+    <col min="5" max="23" width="7.83984375" customWidth="1"/>
     <col min="24" max="24" width="8.83984375" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="9.41796875" customWidth="1"/>
     <col min="26" max="26" width="9.68359375" customWidth="1"/>
@@ -9333,118 +9340,6 @@
       <c r="P41" s="33">
         <f>P40-O40</f>
         <v>-291.55999999999995</v>
-      </c>
-    </row>
-    <row r="46" spans="3:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="D46" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="47" spans="3:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="D47" t="s">
-        <v>90</v>
-      </c>
-      <c r="E47" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="48" spans="3:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="D48" t="s">
-        <v>92</v>
-      </c>
-      <c r="E48" s="1">
-        <f>SUM(N29)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="4:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="D49" t="s">
-        <v>12</v>
-      </c>
-      <c r="E49" s="1">
-        <f>SUM(F29)</f>
-        <v>222.44</v>
-      </c>
-    </row>
-    <row r="50" spans="4:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="D50" t="s">
-        <v>94</v>
-      </c>
-      <c r="E50" s="1">
-        <f>SUM(J29)</f>
-        <v>325.82</v>
-      </c>
-    </row>
-    <row r="51" spans="4:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="D51" t="s">
-        <v>95</v>
-      </c>
-      <c r="E51" s="1">
-        <f>SUM(D29)</f>
-        <v>7.75</v>
-      </c>
-    </row>
-    <row r="52" spans="4:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="D52" t="s">
-        <v>93</v>
-      </c>
-      <c r="E52" s="1">
-        <f>SUM(P29)</f>
-        <v>217.61</v>
-      </c>
-    </row>
-    <row r="53" spans="4:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="D53" t="s">
-        <v>97</v>
-      </c>
-      <c r="E53" s="1">
-        <f>SUM(R29)</f>
-        <v>120.83000000000001</v>
-      </c>
-    </row>
-    <row r="54" spans="4:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="D54" t="s">
-        <v>98</v>
-      </c>
-      <c r="E54" s="1">
-        <f>SUM(L29)</f>
-        <v>46.25</v>
-      </c>
-    </row>
-    <row r="55" spans="4:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="D55" t="s">
-        <v>89</v>
-      </c>
-      <c r="E55" s="1">
-        <f>SUM(V29)</f>
-        <v>86.25</v>
-      </c>
-    </row>
-    <row r="56" spans="4:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="D56" t="s">
-        <v>96</v>
-      </c>
-      <c r="E56" s="1">
-        <f>SUM(H29)</f>
-        <v>400.6</v>
-      </c>
-    </row>
-    <row r="57" spans="4:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="D57" t="s">
-        <v>9</v>
-      </c>
-      <c r="E57" s="1">
-        <f>SUM(T29)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="4:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="D58" t="s">
-        <v>99</v>
-      </c>
-      <c r="E58" s="1">
-        <f>SUM(E48:E57)</f>
-        <v>1427.5500000000002</v>
       </c>
     </row>
   </sheetData>
@@ -9480,8 +9375,8 @@
   </sheetPr>
   <dimension ref="B1:AH58"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="I54" sqref="I54"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I38" sqref="I38:J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -11986,8 +11881,8 @@
   </sheetPr>
   <dimension ref="B1:AH58"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="G61" sqref="G61"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="N54" sqref="N54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -11996,7 +11891,11 @@
     <col min="2" max="2" width="5.68359375" customWidth="1"/>
     <col min="3" max="3" width="7.83984375" customWidth="1"/>
     <col min="4" max="4" width="9.15625" customWidth="1"/>
-    <col min="5" max="23" width="7.83984375" customWidth="1"/>
+    <col min="5" max="7" width="7.83984375" customWidth="1"/>
+    <col min="8" max="8" width="8.68359375" customWidth="1"/>
+    <col min="9" max="19" width="7.83984375" customWidth="1"/>
+    <col min="20" max="20" width="8.578125" customWidth="1"/>
+    <col min="21" max="23" width="7.83984375" customWidth="1"/>
     <col min="24" max="24" width="8.83984375" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="9.41796875" customWidth="1"/>
     <col min="26" max="26" width="9.68359375" customWidth="1"/>
@@ -12144,7 +12043,7 @@
     </row>
     <row r="4" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B4" s="54" t="s">
-        <v>32</v>
+        <v>109</v>
       </c>
       <c r="C4" s="12"/>
       <c r="D4" s="13"/>
@@ -12191,65 +12090,122 @@
       <c r="AD4" s="1"/>
     </row>
     <row r="5" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B5" s="52" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="16"/>
-      <c r="S5" s="17"/>
-      <c r="T5" s="16"/>
-      <c r="U5" s="15"/>
-      <c r="V5" s="20"/>
+      <c r="B5" s="54" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="15">
+        <v>25</v>
+      </c>
+      <c r="D5" s="16">
+        <v>0</v>
+      </c>
+      <c r="E5" s="17">
+        <v>10</v>
+      </c>
+      <c r="F5" s="16">
+        <v>0</v>
+      </c>
+      <c r="G5" s="17">
+        <f>3+5+2+5+5+3</f>
+        <v>23</v>
+      </c>
+      <c r="H5" s="16">
+        <v>0</v>
+      </c>
+      <c r="I5" s="17">
+        <v>20</v>
+      </c>
+      <c r="J5" s="16">
+        <v>0</v>
+      </c>
+      <c r="K5" s="17">
+        <v>25</v>
+      </c>
+      <c r="L5" s="16">
+        <v>0</v>
+      </c>
+      <c r="M5" s="17">
+        <v>25</v>
+      </c>
+      <c r="N5" s="16">
+        <v>47.5</v>
+      </c>
+      <c r="O5" s="17">
+        <v>25</v>
+      </c>
+      <c r="P5" s="16">
+        <v>235</v>
+      </c>
+      <c r="Q5" s="17">
+        <v>25</v>
+      </c>
+      <c r="R5" s="16">
+        <v>0</v>
+      </c>
+      <c r="S5" s="17">
+        <v>25</v>
+      </c>
+      <c r="T5" s="16">
+        <v>0</v>
+      </c>
+      <c r="U5" s="15">
+        <v>20</v>
+      </c>
+      <c r="V5" s="20">
+        <v>0</v>
+      </c>
       <c r="W5" s="15"/>
       <c r="X5" s="20"/>
       <c r="Y5" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>223</v>
       </c>
       <c r="Z5" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>282.5</v>
       </c>
       <c r="AA5" s="1">
         <f>AA4+Y5</f>
-        <v>0</v>
+        <v>223</v>
       </c>
       <c r="AB5" s="1">
         <f>AB4+Z5</f>
-        <v>0</v>
+        <v>282.5</v>
       </c>
       <c r="AC5" s="1">
         <f t="shared" ref="AC5:AC26" si="1">AB5-AA5</f>
-        <v>0</v>
+        <v>59.5</v>
       </c>
       <c r="AD5" s="1"/>
     </row>
     <row r="6" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B6" s="51" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="16"/>
+      <c r="B6" s="52" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="15">
+        <v>25</v>
+      </c>
+      <c r="D6" s="16">
+        <v>0</v>
+      </c>
+      <c r="E6" s="17">
+        <v>40</v>
+      </c>
+      <c r="F6" s="16">
+        <v>0</v>
+      </c>
+      <c r="G6" s="17">
+        <v>25</v>
+      </c>
+      <c r="H6" s="16">
+        <v>0</v>
+      </c>
+      <c r="I6" s="17">
+        <v>30</v>
+      </c>
+      <c r="J6" s="16">
+        <v>0</v>
+      </c>
       <c r="K6" s="17"/>
       <c r="L6" s="16"/>
       <c r="M6" s="17"/>
@@ -12260,13 +12216,17 @@
       <c r="R6" s="16"/>
       <c r="S6" s="17"/>
       <c r="T6" s="16"/>
-      <c r="U6" s="15"/>
-      <c r="V6" s="20"/>
+      <c r="U6" s="15">
+        <v>5</v>
+      </c>
+      <c r="V6" s="20">
+        <v>0</v>
+      </c>
       <c r="W6" s="15"/>
       <c r="X6" s="20"/>
       <c r="Y6" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>125</v>
       </c>
       <c r="Z6" s="35">
         <f t="shared" si="0"/>
@@ -12274,15 +12234,15 @@
       </c>
       <c r="AA6" s="1">
         <f t="shared" ref="AA6:AB21" si="2">AA5+Y6</f>
-        <v>0</v>
+        <v>348</v>
       </c>
       <c r="AB6" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>282.5</v>
       </c>
       <c r="AC6" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-65.5</v>
       </c>
       <c r="AD6" s="1"/>
       <c r="AE6" s="43" t="s">
@@ -12299,8 +12259,8 @@
       </c>
     </row>
     <row r="7" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B7" s="53" t="s">
-        <v>36</v>
+      <c r="B7" s="51" t="s">
+        <v>35</v>
       </c>
       <c r="C7" s="15"/>
       <c r="D7" s="16"/>
@@ -12334,22 +12294,22 @@
       </c>
       <c r="AA7" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>348</v>
       </c>
       <c r="AB7" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>282.5</v>
       </c>
       <c r="AC7" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-65.5</v>
       </c>
       <c r="AD7" s="44" t="s">
         <v>71</v>
       </c>
       <c r="AE7" s="44">
         <f>+G29+'Punters 2021'!Q27+'Punters 2020'!M27+'Punters club'!J6+'Punters 2022'!C29</f>
-        <v>788</v>
+        <v>836</v>
       </c>
       <c r="AF7" s="44">
         <f>+H29+'Punters 2021'!R27+'Punters 2020'!N27+'Punters club'!K6+'Punters 2022'!D29</f>
@@ -12357,16 +12317,16 @@
       </c>
       <c r="AG7" s="49">
         <f>+AF7-AE7</f>
-        <v>-254</v>
+        <v>-302</v>
       </c>
       <c r="AH7" s="47">
         <f>(AF7-AE7)/AE7</f>
-        <v>-0.32233502538071068</v>
+        <v>-0.36124401913875598</v>
       </c>
     </row>
     <row r="8" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B8" s="52" t="s">
-        <v>37</v>
+      <c r="B8" s="53" t="s">
+        <v>36</v>
       </c>
       <c r="C8" s="15"/>
       <c r="D8" s="16"/>
@@ -12400,22 +12360,22 @@
       </c>
       <c r="AA8" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>348</v>
       </c>
       <c r="AB8" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>282.5</v>
       </c>
       <c r="AC8" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-65.5</v>
       </c>
       <c r="AD8" s="44" t="s">
         <v>72</v>
       </c>
       <c r="AE8" s="44">
         <f>+E29+'Punters 2021'!I27+'Punters 2020'!G27+'Punters club'!J7+'Punters 2022'!E29</f>
-        <v>923</v>
+        <v>973</v>
       </c>
       <c r="AF8" s="44">
         <f>+F29+'Punters 2021'!J27+'Punters 2020'!H27+'Punters club'!K7+'Punters 2022'!F29</f>
@@ -12423,16 +12383,16 @@
       </c>
       <c r="AG8" s="50">
         <f t="shared" ref="AG8:AG16" si="3">+AF8-AE8</f>
-        <v>96.769999999999982</v>
+        <v>46.769999999999982</v>
       </c>
       <c r="AH8" s="47">
         <f t="shared" ref="AH8:AH16" si="4">(AF8-AE8)/AE8</f>
-        <v>0.10484290357529792</v>
+        <v>4.8067831449126394E-2</v>
       </c>
     </row>
     <row r="9" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B9" s="51" t="s">
-        <v>38</v>
+      <c r="B9" s="52" t="s">
+        <v>37</v>
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="16"/>
@@ -12466,22 +12426,22 @@
       </c>
       <c r="AA9" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>348</v>
       </c>
       <c r="AB9" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>282.5</v>
       </c>
       <c r="AC9" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-65.5</v>
       </c>
       <c r="AD9" s="44" t="s">
         <v>73</v>
       </c>
       <c r="AE9" s="44">
         <f>+I29+'Punters 2021'!K27+'Punters 2020'!E27+'Punters club'!J11+'Punters 2022'!G29</f>
-        <v>896.48</v>
+        <v>946.48</v>
       </c>
       <c r="AF9" s="44">
         <f>+J29+'Punters 2021'!L27+'Punters 2020'!F27+'Punters club'!K11+'Punters 2022'!H29</f>
@@ -12489,16 +12449,16 @@
       </c>
       <c r="AG9" s="50">
         <f t="shared" si="3"/>
-        <v>64.919999999999959</v>
+        <v>14.919999999999959</v>
       </c>
       <c r="AH9" s="47">
         <f t="shared" si="4"/>
-        <v>7.2416562555773639E-2</v>
+        <v>1.5763671709914589E-2</v>
       </c>
     </row>
     <row r="10" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B10" s="53" t="s">
-        <v>39</v>
+      <c r="B10" s="51" t="s">
+        <v>38</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="16"/>
@@ -12532,22 +12492,22 @@
       </c>
       <c r="AA10" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>348</v>
       </c>
       <c r="AB10" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>282.5</v>
       </c>
       <c r="AC10" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-65.5</v>
       </c>
       <c r="AD10" s="44" t="s">
         <v>74</v>
       </c>
       <c r="AE10" s="44">
         <f>+Q29+'Punters 2021'!G27+'Punters 2020'!I27+'Punters club'!J10+'Punters 2022'!I29</f>
-        <v>899.9</v>
+        <v>924.9</v>
       </c>
       <c r="AF10" s="44">
         <f>+R29+'Punters 2021'!H27+'Punters 2020'!J27+'Punters club'!K10+'Punters 2022'!J29</f>
@@ -12555,16 +12515,16 @@
       </c>
       <c r="AG10" s="50">
         <f t="shared" si="3"/>
-        <v>559.99999999999989</v>
+        <v>534.99999999999989</v>
       </c>
       <c r="AH10" s="45">
         <f t="shared" si="4"/>
-        <v>0.6222913657073007</v>
+        <v>0.57844091253108432</v>
       </c>
     </row>
     <row r="11" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B11" s="52" t="s">
-        <v>40</v>
+      <c r="B11" s="53" t="s">
+        <v>39</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="16"/>
@@ -12598,39 +12558,39 @@
       </c>
       <c r="AA11" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>348</v>
       </c>
       <c r="AB11" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>282.5</v>
       </c>
       <c r="AC11" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-65.5</v>
       </c>
       <c r="AD11" s="44" t="s">
         <v>75</v>
       </c>
       <c r="AE11" s="44">
         <f>+M29+'Punters 2021'!E27+'Punters 2020'!K27+'Punters 2022'!K29</f>
-        <v>633</v>
+        <v>658</v>
       </c>
       <c r="AF11" s="44">
         <f>+N29+'Punters 2021'!F27+'Punters 2020'!L27+'Punters 2022'!L29</f>
-        <v>58.25</v>
+        <v>105.75</v>
       </c>
       <c r="AG11" s="49">
         <f t="shared" si="3"/>
-        <v>-574.75</v>
+        <v>-552.25</v>
       </c>
       <c r="AH11" s="47">
         <f t="shared" si="4"/>
-        <v>-0.90797788309636651</v>
+        <v>-0.8392857142857143</v>
       </c>
     </row>
     <row r="12" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B12" s="51" t="s">
-        <v>41</v>
+      <c r="B12" s="52" t="s">
+        <v>40</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="16"/>
@@ -12664,22 +12624,22 @@
       </c>
       <c r="AA12" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>348</v>
       </c>
       <c r="AB12" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>282.5</v>
       </c>
       <c r="AC12" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-65.5</v>
       </c>
       <c r="AD12" s="44" t="s">
         <v>76</v>
       </c>
       <c r="AE12" s="44">
         <f>+C29+'Punters 2021'!S27+'Punters 2020'!S27+'Punters club'!J8+'Punters 2022'!M29</f>
-        <v>954.96</v>
+        <v>1004.96</v>
       </c>
       <c r="AF12" s="44">
         <f>+D29+'Punters 2021'!T27+'Punters 2020'!T27+'Punters club'!K8+'Punters 2022'!N29</f>
@@ -12687,16 +12647,16 @@
       </c>
       <c r="AG12" s="49">
         <f t="shared" si="3"/>
-        <v>-390.63000000000011</v>
+        <v>-440.63000000000011</v>
       </c>
       <c r="AH12" s="47">
         <f t="shared" si="4"/>
-        <v>-0.40905378235737633</v>
+        <v>-0.43845526190097128</v>
       </c>
     </row>
     <row r="13" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B13" s="53" t="s">
-        <v>42</v>
+      <c r="B13" s="51" t="s">
+        <v>41</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="16"/>
@@ -12730,22 +12690,22 @@
       </c>
       <c r="AA13" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>348</v>
       </c>
       <c r="AB13" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>282.5</v>
       </c>
       <c r="AC13" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-65.5</v>
       </c>
       <c r="AD13" s="44" t="s">
         <v>77</v>
       </c>
       <c r="AE13" s="44">
         <f>+S29+'Punters 2021'!O27+'Punters 2020'!O27+'Punters club'!J9+'Punters 2022'!O29</f>
-        <v>881.34</v>
+        <v>906.34</v>
       </c>
       <c r="AF13" s="44">
         <f>+T29+'Punters 2021'!P27+'Punters 2020'!P27+'Punters club'!K9+'Punters 2022'!P29</f>
@@ -12753,16 +12713,16 @@
       </c>
       <c r="AG13" s="49">
         <f t="shared" si="3"/>
-        <v>-663.09</v>
+        <v>-688.09</v>
       </c>
       <c r="AH13" s="47">
         <f t="shared" si="4"/>
-        <v>-0.75236571584178635</v>
+        <v>-0.75919632808879667</v>
       </c>
     </row>
     <row r="14" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B14" s="52" t="s">
-        <v>43</v>
+      <c r="B14" s="53" t="s">
+        <v>42</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="16"/>
@@ -12796,39 +12756,39 @@
       </c>
       <c r="AA14" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>348</v>
       </c>
       <c r="AB14" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>282.5</v>
       </c>
       <c r="AC14" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-65.5</v>
       </c>
       <c r="AD14" s="44" t="s">
         <v>78</v>
       </c>
       <c r="AE14" s="44">
         <f>+O29+'Punters 2021'!M27+'Punters 2020'!Q27+'Punters club'!J5+'Punters 2022'!Q29</f>
-        <v>883</v>
+        <v>908</v>
       </c>
       <c r="AF14" s="44">
         <f>+P29+'Punters 2021'!N27+'Punters 2020'!R27+'Punters club'!K5+'Punters 2022'!R29</f>
-        <v>637.47</v>
+        <v>872.47000000000014</v>
       </c>
       <c r="AG14" s="49">
         <f t="shared" si="3"/>
-        <v>-245.52999999999997</v>
+        <v>-35.529999999999859</v>
       </c>
       <c r="AH14" s="47">
         <f t="shared" si="4"/>
-        <v>-0.27806342015855035</v>
+        <v>-3.9129955947136412E-2</v>
       </c>
     </row>
     <row r="15" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B15" s="51" t="s">
-        <v>44</v>
+      <c r="B15" s="52" t="s">
+        <v>43</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="16"/>
@@ -12862,22 +12822,22 @@
       </c>
       <c r="AA15" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>348</v>
       </c>
       <c r="AB15" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>282.5</v>
       </c>
       <c r="AC15" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-65.5</v>
       </c>
       <c r="AD15" s="44" t="s">
         <v>79</v>
       </c>
       <c r="AE15" s="44">
         <f>+K29+'Punters 2021'!C27+'Punters 2020'!C27+'Punters club'!J4+'Punters 2022'!S29</f>
-        <v>892.7</v>
+        <v>917.7</v>
       </c>
       <c r="AF15" s="44">
         <f>+L29+'Punters 2021'!D27+'Punters 2020'!D27+'Punters club'!K4+'Punters 2022'!T29</f>
@@ -12885,16 +12845,16 @@
       </c>
       <c r="AG15" s="50">
         <f t="shared" si="3"/>
-        <v>568.38999999999987</v>
+        <v>543.38999999999987</v>
       </c>
       <c r="AH15" s="45">
         <f t="shared" si="4"/>
-        <v>0.63670886075949351</v>
+        <v>0.59212160836874783</v>
       </c>
     </row>
     <row r="16" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B16" s="53" t="s">
-        <v>45</v>
+      <c r="B16" s="51" t="s">
+        <v>44</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="16"/>
@@ -12928,22 +12888,22 @@
       </c>
       <c r="AA16" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>348</v>
       </c>
       <c r="AB16" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>282.5</v>
       </c>
       <c r="AC16" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-65.5</v>
       </c>
       <c r="AD16" s="44" t="s">
         <v>80</v>
       </c>
       <c r="AE16" s="44">
         <f>+U29+'Punters 2022'!U29</f>
-        <v>200</v>
+        <v>225</v>
       </c>
       <c r="AF16" s="44">
         <f>+V29+'Punters 2022'!V29</f>
@@ -12951,16 +12911,16 @@
       </c>
       <c r="AG16" s="49">
         <f t="shared" si="3"/>
-        <v>-113.75</v>
+        <v>-138.75</v>
       </c>
       <c r="AH16" s="47">
         <f t="shared" si="4"/>
-        <v>-0.56874999999999998</v>
+        <v>-0.6166666666666667</v>
       </c>
     </row>
     <row r="17" spans="2:30" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B17" s="52" t="s">
-        <v>46</v>
+      <c r="B17" s="53" t="s">
+        <v>45</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="16"/>
@@ -12994,21 +12954,21 @@
       </c>
       <c r="AA17" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>348</v>
       </c>
       <c r="AB17" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>282.5</v>
       </c>
       <c r="AC17" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-65.5</v>
       </c>
       <c r="AD17" s="1"/>
     </row>
     <row r="18" spans="2:30" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B18" s="51" t="s">
-        <v>47</v>
+      <c r="B18" s="52" t="s">
+        <v>46</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="16"/>
@@ -13042,21 +13002,21 @@
       </c>
       <c r="AA18" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>348</v>
       </c>
       <c r="AB18" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>282.5</v>
       </c>
       <c r="AC18" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-65.5</v>
       </c>
       <c r="AD18" s="1"/>
     </row>
     <row r="19" spans="2:30" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B19" s="53" t="s">
-        <v>48</v>
+      <c r="B19" s="51" t="s">
+        <v>47</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="16"/>
@@ -13090,21 +13050,21 @@
       </c>
       <c r="AA19" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>348</v>
       </c>
       <c r="AB19" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>282.5</v>
       </c>
       <c r="AC19" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-65.5</v>
       </c>
       <c r="AD19" s="1"/>
     </row>
     <row r="20" spans="2:30" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B20" s="52" t="s">
-        <v>49</v>
+      <c r="B20" s="53" t="s">
+        <v>48</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="16"/>
@@ -13138,21 +13098,21 @@
       </c>
       <c r="AA20" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>348</v>
       </c>
       <c r="AB20" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>282.5</v>
       </c>
       <c r="AC20" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-65.5</v>
       </c>
       <c r="AD20" s="1"/>
     </row>
     <row r="21" spans="2:30" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B21" s="51" t="s">
-        <v>50</v>
+      <c r="B21" s="52" t="s">
+        <v>49</v>
       </c>
       <c r="C21" s="15"/>
       <c r="D21" s="16"/>
@@ -13186,21 +13146,21 @@
       </c>
       <c r="AA21" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>348</v>
       </c>
       <c r="AB21" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>282.5</v>
       </c>
       <c r="AC21" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-65.5</v>
       </c>
       <c r="AD21" s="1"/>
     </row>
     <row r="22" spans="2:30" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B22" s="53" t="s">
-        <v>59</v>
+      <c r="B22" s="51" t="s">
+        <v>50</v>
       </c>
       <c r="C22" s="15"/>
       <c r="D22" s="16"/>
@@ -13234,21 +13194,21 @@
       </c>
       <c r="AA22" s="1">
         <f t="shared" ref="AA22:AB26" si="5">AA21+Y22</f>
-        <v>0</v>
+        <v>348</v>
       </c>
       <c r="AB22" s="1">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>282.5</v>
       </c>
       <c r="AC22" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-65.5</v>
       </c>
       <c r="AD22" s="1"/>
     </row>
     <row r="23" spans="2:30" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B23" s="52" t="s">
-        <v>60</v>
+      <c r="B23" s="53" t="s">
+        <v>59</v>
       </c>
       <c r="C23" s="15"/>
       <c r="D23" s="16"/>
@@ -13282,21 +13242,21 @@
       </c>
       <c r="AA23" s="1">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>348</v>
       </c>
       <c r="AB23" s="1">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>282.5</v>
       </c>
       <c r="AC23" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-65.5</v>
       </c>
       <c r="AD23" s="1"/>
     </row>
     <row r="24" spans="2:30" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B24" s="51" t="s">
-        <v>61</v>
+      <c r="B24" s="52" t="s">
+        <v>60</v>
       </c>
       <c r="C24" s="15"/>
       <c r="D24" s="16"/>
@@ -13330,21 +13290,21 @@
       </c>
       <c r="AA24" s="1">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>348</v>
       </c>
       <c r="AB24" s="1">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>282.5</v>
       </c>
       <c r="AC24" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-65.5</v>
       </c>
       <c r="AD24" s="1"/>
     </row>
     <row r="25" spans="2:30" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B25" s="53" t="s">
-        <v>62</v>
+      <c r="B25" s="51" t="s">
+        <v>61</v>
       </c>
       <c r="C25" s="15"/>
       <c r="D25" s="16"/>
@@ -13378,21 +13338,21 @@
       </c>
       <c r="AA25" s="1">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>348</v>
       </c>
       <c r="AB25" s="1">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>282.5</v>
       </c>
       <c r="AC25" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-65.5</v>
       </c>
       <c r="AD25" s="1"/>
     </row>
     <row r="26" spans="2:30" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B26" s="54" t="s">
-        <v>63</v>
+      <c r="B26" s="53" t="s">
+        <v>62</v>
       </c>
       <c r="C26" s="15"/>
       <c r="D26" s="16"/>
@@ -13426,21 +13386,21 @@
       </c>
       <c r="AA26" s="1">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>348</v>
       </c>
       <c r="AB26" s="1">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>282.5</v>
       </c>
       <c r="AC26" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-65.5</v>
       </c>
       <c r="AD26" s="1"/>
     </row>
     <row r="27" spans="2:30" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B27" s="30" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="C27" s="15"/>
       <c r="D27" s="16"/>
@@ -13479,7 +13439,7 @@
     </row>
     <row r="28" spans="2:30" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B28" s="30" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C28" s="15"/>
       <c r="D28" s="16"/>
@@ -13522,7 +13482,7 @@
       </c>
       <c r="C29" s="18">
         <f t="shared" ref="C29:Z29" si="7">SUM(C4:C28)</f>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="D29" s="18">
         <f t="shared" si="7"/>
@@ -13530,7 +13490,7 @@
       </c>
       <c r="E29" s="18">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F29" s="18">
         <f t="shared" si="7"/>
@@ -13538,7 +13498,7 @@
       </c>
       <c r="G29" s="18">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="H29" s="18">
         <f t="shared" si="7"/>
@@ -13546,7 +13506,7 @@
       </c>
       <c r="I29" s="18">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="J29" s="18">
         <f t="shared" si="7"/>
@@ -13554,7 +13514,7 @@
       </c>
       <c r="K29" s="18">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="L29" s="18">
         <f t="shared" si="7"/>
@@ -13562,23 +13522,23 @@
       </c>
       <c r="M29" s="18">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="N29" s="18">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>47.5</v>
       </c>
       <c r="O29" s="18">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="P29" s="18">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>235</v>
       </c>
       <c r="Q29" s="18">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="R29" s="18">
         <f t="shared" si="7"/>
@@ -13586,7 +13546,7 @@
       </c>
       <c r="S29" s="18">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="T29" s="18">
         <f>SUM(T4:T28)</f>
@@ -13594,7 +13554,7 @@
       </c>
       <c r="U29" s="18">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="V29" s="21">
         <f t="shared" si="7"/>
@@ -13610,53 +13570,53 @@
       </c>
       <c r="Y29" s="29">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>348</v>
       </c>
       <c r="Z29" s="18">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>282.5</v>
       </c>
     </row>
     <row r="30" spans="2:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="D30" s="56" t="e">
+      <c r="D30" s="56">
         <f>(D29-C29)/C29</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F30" s="34" t="e">
+        <v>-1</v>
+      </c>
+      <c r="F30" s="34">
         <f>(F29-E29)/E29</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H30" s="34" t="e">
+        <v>-1</v>
+      </c>
+      <c r="H30" s="34">
         <f>(H29-G29)/G29</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J30" s="34" t="e">
+        <v>-1</v>
+      </c>
+      <c r="J30" s="34">
         <f>(J29-I29)/I29</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L30" s="28" t="e">
+        <v>-1</v>
+      </c>
+      <c r="L30" s="28">
         <f>(L29-K29)/K29</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N30" s="28" t="e">
+        <v>-1</v>
+      </c>
+      <c r="N30" s="28">
         <f>(N29-M29)/M29</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P30" s="28" t="e">
+        <v>0.9</v>
+      </c>
+      <c r="P30" s="28">
         <f>(P29-O29)/O29</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R30" s="28" t="e">
+        <v>8.4</v>
+      </c>
+      <c r="R30" s="28">
         <f>(R29-Q29)/Q29</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T30" s="22" t="e">
+        <v>-1</v>
+      </c>
+      <c r="T30" s="22">
         <f>(T29-S29)/S29</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V30" s="28" t="e">
+        <v>-1</v>
+      </c>
+      <c r="V30" s="28">
         <f>(V29-U29)/U29</f>
-        <v>#DIV/0!</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="31" spans="2:30" x14ac:dyDescent="0.55000000000000004">
@@ -13667,7 +13627,7 @@
       <c r="H31" s="62"/>
       <c r="I31" s="58">
         <f>C29+E29+G29+I29+K29+M29+O29+Q29+S29+U29+W29</f>
-        <v>0</v>
+        <v>348</v>
       </c>
       <c r="J31" s="59"/>
     </row>
@@ -13678,14 +13638,14 @@
       <c r="H32" s="65"/>
       <c r="I32" s="58">
         <f>+D29+F29+H29+J29+L29+N29+P29+R29+T29+V29+X29</f>
-        <v>0</v>
+        <v>282.5</v>
       </c>
       <c r="J32" s="59"/>
     </row>
     <row r="33" spans="3:25" x14ac:dyDescent="0.55000000000000004">
       <c r="I33" s="58">
         <f>I32-I31</f>
-        <v>0</v>
+        <v>-65.5</v>
       </c>
       <c r="J33" s="59"/>
       <c r="Y33">
@@ -13696,7 +13656,7 @@
     <row r="34" spans="3:25" x14ac:dyDescent="0.55000000000000004">
       <c r="C34" s="36">
         <f>C29+E29+G29+I29</f>
-        <v>0</v>
+        <v>198</v>
       </c>
       <c r="D34" s="36">
         <f>D29+F29+H29+J29</f>
@@ -13704,23 +13664,23 @@
       </c>
       <c r="E34" s="37">
         <f>D34-C34</f>
-        <v>0</v>
+        <v>-198</v>
       </c>
       <c r="I34" s="38">
         <f>O29+K29+M29</f>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="J34" s="38">
         <f>P29+L29+N29</f>
-        <v>0</v>
+        <v>282.5</v>
       </c>
       <c r="K34" s="39">
         <f>J34-I34</f>
-        <v>0</v>
+        <v>207.5</v>
       </c>
       <c r="O34" s="40">
         <f>U29+Q29+S29</f>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="P34" s="40">
         <f>V29+R29+T29</f>
@@ -13728,7 +13688,7 @@
       </c>
       <c r="Q34" s="41">
         <f>P34-O34</f>
-        <v>0</v>
+        <v>-75</v>
       </c>
       <c r="X34" s="55"/>
       <c r="Y34">
@@ -13738,21 +13698,21 @@
     </row>
     <row r="35" spans="3:25" x14ac:dyDescent="0.55000000000000004">
       <c r="C35" s="36"/>
-      <c r="D35" s="34" t="e">
+      <c r="D35" s="34">
         <f>(D34-C34)/C34</f>
-        <v>#DIV/0!</v>
+        <v>-1</v>
       </c>
       <c r="E35" s="37"/>
       <c r="I35" s="38"/>
-      <c r="J35" s="34" t="e">
+      <c r="J35" s="34">
         <f>(J34-I34)/I34</f>
-        <v>#DIV/0!</v>
+        <v>2.7666666666666666</v>
       </c>
       <c r="K35" s="39"/>
       <c r="O35" s="40"/>
-      <c r="P35" s="34" t="e">
+      <c r="P35" s="34">
         <f>(P34-O34)/O34</f>
-        <v>#DIV/0!</v>
+        <v>-1</v>
       </c>
       <c r="Q35" s="41"/>
       <c r="X35" s="55"/>
@@ -13761,22 +13721,15 @@
       <c r="G36" t="s">
         <v>58</v>
       </c>
-      <c r="I36" cm="1">
-        <f t="array" ref="I36:J36">2000+'Punters 2022'!I36:J36</f>
-        <v>4476.26</v>
-      </c>
-      <c r="J36">
-        <v>2000</v>
+      <c r="I36">
+        <f>2000+1.59</f>
+        <v>2001.59</v>
       </c>
     </row>
     <row r="37" spans="3:25" x14ac:dyDescent="0.55000000000000004">
       <c r="G37" t="s">
         <v>85</v>
       </c>
-      <c r="J37">
-        <f>-269.5*10</f>
-        <v>-2695</v>
-      </c>
     </row>
     <row r="38" spans="3:25" x14ac:dyDescent="0.55000000000000004">
       <c r="G38" s="42" t="s">
@@ -13784,8 +13737,8 @@
       </c>
       <c r="H38" s="42"/>
       <c r="I38" s="66">
-        <f>I36+I33+J37</f>
-        <v>1781.2600000000002</v>
+        <f>I36+I33</f>
+        <v>1936.09</v>
       </c>
       <c r="J38" s="66"/>
       <c r="M38" s="33"/>
@@ -13839,7 +13792,7 @@
     <row r="42" spans="3:25" x14ac:dyDescent="0.55000000000000004">
       <c r="C42" s="1">
         <f>C29+E29+G29+I29</f>
-        <v>0</v>
+        <v>198</v>
       </c>
       <c r="D42" s="1">
         <f>D29+F29+H29+J29</f>
@@ -13847,15 +13800,15 @@
       </c>
       <c r="I42" s="1">
         <f>O29+K29+M29</f>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="J42" s="1">
         <f>P29+L29+N29</f>
-        <v>0</v>
+        <v>282.5</v>
       </c>
       <c r="O42" s="1">
         <f>U29+Q29+S29</f>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="P42" s="1">
         <f>V29+R29+T29</f>
@@ -13865,20 +13818,20 @@
     <row r="43" spans="3:25" x14ac:dyDescent="0.55000000000000004">
       <c r="D43" s="1">
         <f>D42-C42</f>
-        <v>0</v>
+        <v>-198</v>
       </c>
       <c r="J43" s="33">
         <f>J42-I42</f>
-        <v>0</v>
+        <v>207.5</v>
       </c>
       <c r="P43" s="33">
         <f>P42-O42</f>
-        <v>0</v>
+        <v>-75</v>
       </c>
     </row>
     <row r="45" spans="3:25" x14ac:dyDescent="0.55000000000000004">
       <c r="V45" t="s">
-        <v>87</v>
+        <v>110</v>
       </c>
     </row>
     <row r="46" spans="3:25" x14ac:dyDescent="0.55000000000000004">
@@ -13886,13 +13839,13 @@
         <v>88</v>
       </c>
       <c r="J46" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="V46" t="s">
         <v>89</v>
       </c>
       <c r="W46">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="3:25" x14ac:dyDescent="0.55000000000000004">
@@ -13906,13 +13859,13 @@
         <v>90</v>
       </c>
       <c r="K47" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="V47" t="s">
         <v>12</v>
       </c>
       <c r="W47">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="3:25" x14ac:dyDescent="0.55000000000000004">
@@ -13927,13 +13880,10 @@
         <v>92</v>
       </c>
       <c r="K48">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V48" t="s">
         <v>93</v>
-      </c>
-      <c r="W48">
-        <v>7</v>
       </c>
     </row>
     <row r="49" spans="4:23" x14ac:dyDescent="0.55000000000000004">
@@ -13953,9 +13903,6 @@
       <c r="V49" t="s">
         <v>92</v>
       </c>
-      <c r="W49">
-        <v>4</v>
-      </c>
     </row>
     <row r="50" spans="4:23" x14ac:dyDescent="0.55000000000000004">
       <c r="D50" t="s">
@@ -13974,9 +13921,6 @@
       <c r="V50" t="s">
         <v>9</v>
       </c>
-      <c r="W50">
-        <v>4</v>
-      </c>
     </row>
     <row r="51" spans="4:23" x14ac:dyDescent="0.55000000000000004">
       <c r="D51" t="s">
@@ -13996,7 +13940,7 @@
         <v>11</v>
       </c>
       <c r="W51">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="4:23" x14ac:dyDescent="0.55000000000000004">
@@ -14017,7 +13961,7 @@
         <v>96</v>
       </c>
       <c r="W52">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="4:23" x14ac:dyDescent="0.55000000000000004">
@@ -14037,9 +13981,6 @@
       <c r="V53" t="s">
         <v>98</v>
       </c>
-      <c r="W53">
-        <v>3</v>
-      </c>
     </row>
     <row r="54" spans="4:23" x14ac:dyDescent="0.55000000000000004">
       <c r="D54" t="s">
@@ -14058,9 +13999,6 @@
       <c r="V54" t="s">
         <v>97</v>
       </c>
-      <c r="W54">
-        <v>6</v>
-      </c>
     </row>
     <row r="55" spans="4:23" x14ac:dyDescent="0.55000000000000004">
       <c r="D55" t="s">
@@ -14080,7 +14018,7 @@
         <v>94</v>
       </c>
       <c r="W55">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56" spans="4:23" x14ac:dyDescent="0.55000000000000004">
@@ -14089,7 +14027,7 @@
       </c>
       <c r="E56" s="1">
         <f>SUM(N29)</f>
-        <v>0</v>
+        <v>47.5</v>
       </c>
       <c r="J56" t="s">
         <v>96</v>
@@ -14099,7 +14037,7 @@
       </c>
       <c r="W56">
         <f>SUM(W46:W55)</f>
-        <v>55</v>
+        <v>10</v>
       </c>
     </row>
     <row r="57" spans="4:23" x14ac:dyDescent="0.55000000000000004">
@@ -14108,7 +14046,7 @@
       </c>
       <c r="E57" s="1">
         <f>SUM(P29)</f>
-        <v>0</v>
+        <v>235</v>
       </c>
       <c r="J57" t="s">
         <v>9</v>
@@ -14123,7 +14061,7 @@
       </c>
       <c r="E58" s="1">
         <f>SUM(E48:E57)</f>
-        <v>0</v>
+        <v>282.5</v>
       </c>
     </row>
   </sheetData>
@@ -14429,6 +14367,6 @@
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
-  <clbl:label id="{0f7d30c2-cad0-4405-8153-25a6a3313da4}" enabled="1" method="Privileged" siteId="{6c637512-c417-4e78-9d62-b61258e4b619}" contentBits="0" removed="0"/>
+  <clbl:label id="{0f7d30c2-cad0-4405-8153-25a6a3313da4}" enabled="1" method="Privileged" siteId="{6c637512-c417-4e78-9d62-b61258e4b619}" removed="0"/>
 </clbl:labelList>
 </file>
</xml_diff>

<commit_message>
Updating spreadsheet and homepage\
</commit_message>
<xml_diff>
--- a/public/Data/HEMANPUNTERS.xlsx
+++ b/public/Data/HEMANPUNTERS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bturnor\source\repos\PersonalWork\seeMore\public\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://insightonlineaus-my.sharepoint.com/personal/brenton_turnor_insight_com/Documents/Personal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{515129D1-6049-4859-AA7B-8DC703CB0DD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="155" documentId="13_ncr:1_{469677BE-0EE7-46CC-91C0-1B5E676F4187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{22CA198B-82D5-4D9D-9F12-1D1A8A6342EB}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="45" windowWidth="29040" windowHeight="15720" firstSheet="5" activeTab="5" xr2:uid="{525E8989-1938-4309-A4CF-8F1D15E362FB}"/>
   </bookViews>
@@ -395,13 +395,13 @@
     <t>OR</t>
   </si>
   <si>
-    <t>1 leg losses @ 18th March 2024</t>
+    <t>Strikes</t>
   </si>
   <si>
-    <t>Strikes for 2024 Season at 18th March 2024</t>
+    <t>Strikes for 2024 Season at 11th April 2024</t>
   </si>
   <si>
-    <t>Strikes</t>
+    <t>1 leg losses @ 11th April 2024</t>
   </si>
 </sst>
 </file>
@@ -11881,8 +11881,8 @@
   </sheetPr>
   <dimension ref="B1:AH58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="N54" sqref="N54"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="M50" sqref="M50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -12270,12 +12270,24 @@
       <c r="H7" s="16"/>
       <c r="I7" s="17"/>
       <c r="J7" s="16"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="17"/>
-      <c r="P7" s="16"/>
+      <c r="K7" s="17">
+        <v>25</v>
+      </c>
+      <c r="L7" s="16">
+        <v>0</v>
+      </c>
+      <c r="M7" s="17">
+        <v>30</v>
+      </c>
+      <c r="N7" s="16">
+        <v>0</v>
+      </c>
+      <c r="O7" s="17">
+        <v>25</v>
+      </c>
+      <c r="P7" s="16">
+        <v>0</v>
+      </c>
       <c r="Q7" s="17"/>
       <c r="R7" s="16"/>
       <c r="S7" s="17"/>
@@ -12286,7 +12298,7 @@
       <c r="X7" s="20"/>
       <c r="Y7" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="Z7" s="35">
         <f t="shared" si="0"/>
@@ -12294,7 +12306,7 @@
       </c>
       <c r="AA7" s="1">
         <f t="shared" si="2"/>
-        <v>348</v>
+        <v>428</v>
       </c>
       <c r="AB7" s="1">
         <f t="shared" si="2"/>
@@ -12302,14 +12314,14 @@
       </c>
       <c r="AC7" s="1">
         <f t="shared" si="1"/>
-        <v>-65.5</v>
+        <v>-145.5</v>
       </c>
       <c r="AD7" s="44" t="s">
         <v>71</v>
       </c>
       <c r="AE7" s="44">
         <f>+G29+'Punters 2021'!Q27+'Punters 2020'!M27+'Punters club'!J6+'Punters 2022'!C29</f>
-        <v>836</v>
+        <v>861</v>
       </c>
       <c r="AF7" s="44">
         <f>+H29+'Punters 2021'!R27+'Punters 2020'!N27+'Punters club'!K6+'Punters 2022'!D29</f>
@@ -12317,11 +12329,11 @@
       </c>
       <c r="AG7" s="49">
         <f>+AF7-AE7</f>
-        <v>-302</v>
+        <v>-327</v>
       </c>
       <c r="AH7" s="47">
         <f>(AF7-AE7)/AE7</f>
-        <v>-0.36124401913875598</v>
+        <v>-0.37979094076655051</v>
       </c>
     </row>
     <row r="8" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -12342,17 +12354,29 @@
       <c r="N8" s="16"/>
       <c r="O8" s="17"/>
       <c r="P8" s="16"/>
-      <c r="Q8" s="17"/>
-      <c r="R8" s="16"/>
-      <c r="S8" s="17"/>
-      <c r="T8" s="16"/>
-      <c r="U8" s="15"/>
-      <c r="V8" s="20"/>
+      <c r="Q8" s="17">
+        <v>30</v>
+      </c>
+      <c r="R8" s="16">
+        <v>0</v>
+      </c>
+      <c r="S8" s="17">
+        <v>30</v>
+      </c>
+      <c r="T8" s="16">
+        <v>0</v>
+      </c>
+      <c r="U8" s="15">
+        <v>10</v>
+      </c>
+      <c r="V8" s="20">
+        <v>0</v>
+      </c>
       <c r="W8" s="15"/>
       <c r="X8" s="20"/>
       <c r="Y8" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="Z8" s="35">
         <f t="shared" si="0"/>
@@ -12360,7 +12384,7 @@
       </c>
       <c r="AA8" s="1">
         <f t="shared" si="2"/>
-        <v>348</v>
+        <v>498</v>
       </c>
       <c r="AB8" s="1">
         <f t="shared" si="2"/>
@@ -12368,14 +12392,14 @@
       </c>
       <c r="AC8" s="1">
         <f t="shared" si="1"/>
-        <v>-65.5</v>
+        <v>-215.5</v>
       </c>
       <c r="AD8" s="44" t="s">
         <v>72</v>
       </c>
       <c r="AE8" s="44">
         <f>+E29+'Punters 2021'!I27+'Punters 2020'!G27+'Punters club'!J7+'Punters 2022'!E29</f>
-        <v>973</v>
+        <v>998</v>
       </c>
       <c r="AF8" s="44">
         <f>+F29+'Punters 2021'!J27+'Punters 2020'!H27+'Punters club'!K7+'Punters 2022'!F29</f>
@@ -12383,24 +12407,32 @@
       </c>
       <c r="AG8" s="50">
         <f t="shared" ref="AG8:AG16" si="3">+AF8-AE8</f>
-        <v>46.769999999999982</v>
+        <v>21.769999999999982</v>
       </c>
       <c r="AH8" s="47">
         <f t="shared" ref="AH8:AH16" si="4">(AF8-AE8)/AE8</f>
-        <v>4.8067831449126394E-2</v>
+        <v>2.1813627254508999E-2</v>
       </c>
     </row>
     <row r="9" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B9" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="15"/>
+      <c r="C9" s="15">
+        <v>30</v>
+      </c>
       <c r="D9" s="16"/>
-      <c r="E9" s="17"/>
+      <c r="E9" s="17">
+        <v>25</v>
+      </c>
       <c r="F9" s="16"/>
-      <c r="G9" s="17"/>
+      <c r="G9" s="17">
+        <v>25</v>
+      </c>
       <c r="H9" s="16"/>
-      <c r="I9" s="17"/>
+      <c r="I9" s="17">
+        <v>25</v>
+      </c>
       <c r="J9" s="16"/>
       <c r="K9" s="17"/>
       <c r="L9" s="16"/>
@@ -12418,7 +12450,7 @@
       <c r="X9" s="20"/>
       <c r="Y9" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="Z9" s="35">
         <f t="shared" si="0"/>
@@ -12426,7 +12458,7 @@
       </c>
       <c r="AA9" s="1">
         <f t="shared" si="2"/>
-        <v>348</v>
+        <v>603</v>
       </c>
       <c r="AB9" s="1">
         <f t="shared" si="2"/>
@@ -12434,14 +12466,14 @@
       </c>
       <c r="AC9" s="1">
         <f t="shared" si="1"/>
-        <v>-65.5</v>
+        <v>-320.5</v>
       </c>
       <c r="AD9" s="44" t="s">
         <v>73</v>
       </c>
       <c r="AE9" s="44">
         <f>+I29+'Punters 2021'!K27+'Punters 2020'!E27+'Punters club'!J11+'Punters 2022'!G29</f>
-        <v>946.48</v>
+        <v>971.48</v>
       </c>
       <c r="AF9" s="44">
         <f>+J29+'Punters 2021'!L27+'Punters 2020'!F27+'Punters club'!K11+'Punters 2022'!H29</f>
@@ -12449,11 +12481,11 @@
       </c>
       <c r="AG9" s="50">
         <f t="shared" si="3"/>
-        <v>14.919999999999959</v>
+        <v>-10.080000000000041</v>
       </c>
       <c r="AH9" s="47">
         <f t="shared" si="4"/>
-        <v>1.5763671709914589E-2</v>
+        <v>-1.0375921274756084E-2</v>
       </c>
     </row>
     <row r="10" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -12492,7 +12524,7 @@
       </c>
       <c r="AA10" s="1">
         <f t="shared" si="2"/>
-        <v>348</v>
+        <v>603</v>
       </c>
       <c r="AB10" s="1">
         <f t="shared" si="2"/>
@@ -12500,14 +12532,14 @@
       </c>
       <c r="AC10" s="1">
         <f t="shared" si="1"/>
-        <v>-65.5</v>
+        <v>-320.5</v>
       </c>
       <c r="AD10" s="44" t="s">
         <v>74</v>
       </c>
       <c r="AE10" s="44">
         <f>+Q29+'Punters 2021'!G27+'Punters 2020'!I27+'Punters club'!J10+'Punters 2022'!I29</f>
-        <v>924.9</v>
+        <v>954.9</v>
       </c>
       <c r="AF10" s="44">
         <f>+R29+'Punters 2021'!H27+'Punters 2020'!J27+'Punters club'!K10+'Punters 2022'!J29</f>
@@ -12515,11 +12547,11 @@
       </c>
       <c r="AG10" s="50">
         <f t="shared" si="3"/>
-        <v>534.99999999999989</v>
+        <v>504.99999999999989</v>
       </c>
       <c r="AH10" s="45">
         <f t="shared" si="4"/>
-        <v>0.57844091253108432</v>
+        <v>0.52885118860613667</v>
       </c>
     </row>
     <row r="11" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -12558,7 +12590,7 @@
       </c>
       <c r="AA11" s="1">
         <f t="shared" si="2"/>
-        <v>348</v>
+        <v>603</v>
       </c>
       <c r="AB11" s="1">
         <f t="shared" si="2"/>
@@ -12566,14 +12598,14 @@
       </c>
       <c r="AC11" s="1">
         <f t="shared" si="1"/>
-        <v>-65.5</v>
+        <v>-320.5</v>
       </c>
       <c r="AD11" s="44" t="s">
         <v>75</v>
       </c>
       <c r="AE11" s="44">
         <f>+M29+'Punters 2021'!E27+'Punters 2020'!K27+'Punters 2022'!K29</f>
-        <v>658</v>
+        <v>688</v>
       </c>
       <c r="AF11" s="44">
         <f>+N29+'Punters 2021'!F27+'Punters 2020'!L27+'Punters 2022'!L29</f>
@@ -12581,11 +12613,11 @@
       </c>
       <c r="AG11" s="49">
         <f t="shared" si="3"/>
-        <v>-552.25</v>
+        <v>-582.25</v>
       </c>
       <c r="AH11" s="47">
         <f t="shared" si="4"/>
-        <v>-0.8392857142857143</v>
+        <v>-0.84629360465116277</v>
       </c>
     </row>
     <row r="12" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -12624,7 +12656,7 @@
       </c>
       <c r="AA12" s="1">
         <f t="shared" si="2"/>
-        <v>348</v>
+        <v>603</v>
       </c>
       <c r="AB12" s="1">
         <f t="shared" si="2"/>
@@ -12632,14 +12664,14 @@
       </c>
       <c r="AC12" s="1">
         <f t="shared" si="1"/>
-        <v>-65.5</v>
+        <v>-320.5</v>
       </c>
       <c r="AD12" s="44" t="s">
         <v>76</v>
       </c>
       <c r="AE12" s="44">
         <f>+C29+'Punters 2021'!S27+'Punters 2020'!S27+'Punters club'!J8+'Punters 2022'!M29</f>
-        <v>1004.96</v>
+        <v>1034.96</v>
       </c>
       <c r="AF12" s="44">
         <f>+D29+'Punters 2021'!T27+'Punters 2020'!T27+'Punters club'!K8+'Punters 2022'!N29</f>
@@ -12647,11 +12679,11 @@
       </c>
       <c r="AG12" s="49">
         <f t="shared" si="3"/>
-        <v>-440.63000000000011</v>
+        <v>-470.63000000000011</v>
       </c>
       <c r="AH12" s="47">
         <f t="shared" si="4"/>
-        <v>-0.43845526190097128</v>
+        <v>-0.4547325500502436</v>
       </c>
     </row>
     <row r="13" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -12690,7 +12722,7 @@
       </c>
       <c r="AA13" s="1">
         <f t="shared" si="2"/>
-        <v>348</v>
+        <v>603</v>
       </c>
       <c r="AB13" s="1">
         <f t="shared" si="2"/>
@@ -12698,14 +12730,14 @@
       </c>
       <c r="AC13" s="1">
         <f t="shared" si="1"/>
-        <v>-65.5</v>
+        <v>-320.5</v>
       </c>
       <c r="AD13" s="44" t="s">
         <v>77</v>
       </c>
       <c r="AE13" s="44">
         <f>+S29+'Punters 2021'!O27+'Punters 2020'!O27+'Punters club'!J9+'Punters 2022'!O29</f>
-        <v>906.34</v>
+        <v>936.34</v>
       </c>
       <c r="AF13" s="44">
         <f>+T29+'Punters 2021'!P27+'Punters 2020'!P27+'Punters club'!K9+'Punters 2022'!P29</f>
@@ -12713,11 +12745,11 @@
       </c>
       <c r="AG13" s="49">
         <f t="shared" si="3"/>
-        <v>-688.09</v>
+        <v>-718.09</v>
       </c>
       <c r="AH13" s="47">
         <f t="shared" si="4"/>
-        <v>-0.75919632808879667</v>
+        <v>-0.76691159194309755</v>
       </c>
     </row>
     <row r="14" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -12756,7 +12788,7 @@
       </c>
       <c r="AA14" s="1">
         <f t="shared" si="2"/>
-        <v>348</v>
+        <v>603</v>
       </c>
       <c r="AB14" s="1">
         <f t="shared" si="2"/>
@@ -12764,14 +12796,14 @@
       </c>
       <c r="AC14" s="1">
         <f t="shared" si="1"/>
-        <v>-65.5</v>
+        <v>-320.5</v>
       </c>
       <c r="AD14" s="44" t="s">
         <v>78</v>
       </c>
       <c r="AE14" s="44">
         <f>+O29+'Punters 2021'!M27+'Punters 2020'!Q27+'Punters club'!J5+'Punters 2022'!Q29</f>
-        <v>908</v>
+        <v>933</v>
       </c>
       <c r="AF14" s="44">
         <f>+P29+'Punters 2021'!N27+'Punters 2020'!R27+'Punters club'!K5+'Punters 2022'!R29</f>
@@ -12779,11 +12811,11 @@
       </c>
       <c r="AG14" s="49">
         <f t="shared" si="3"/>
-        <v>-35.529999999999859</v>
+        <v>-60.529999999999859</v>
       </c>
       <c r="AH14" s="47">
         <f t="shared" si="4"/>
-        <v>-3.9129955947136412E-2</v>
+        <v>-6.4876741693461804E-2</v>
       </c>
     </row>
     <row r="15" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -12822,7 +12854,7 @@
       </c>
       <c r="AA15" s="1">
         <f t="shared" si="2"/>
-        <v>348</v>
+        <v>603</v>
       </c>
       <c r="AB15" s="1">
         <f t="shared" si="2"/>
@@ -12830,14 +12862,14 @@
       </c>
       <c r="AC15" s="1">
         <f t="shared" si="1"/>
-        <v>-65.5</v>
+        <v>-320.5</v>
       </c>
       <c r="AD15" s="44" t="s">
         <v>79</v>
       </c>
       <c r="AE15" s="44">
         <f>+K29+'Punters 2021'!C27+'Punters 2020'!C27+'Punters club'!J4+'Punters 2022'!S29</f>
-        <v>917.7</v>
+        <v>942.7</v>
       </c>
       <c r="AF15" s="44">
         <f>+L29+'Punters 2021'!D27+'Punters 2020'!D27+'Punters club'!K4+'Punters 2022'!T29</f>
@@ -12845,11 +12877,11 @@
       </c>
       <c r="AG15" s="50">
         <f t="shared" si="3"/>
-        <v>543.38999999999987</v>
+        <v>518.38999999999987</v>
       </c>
       <c r="AH15" s="45">
         <f t="shared" si="4"/>
-        <v>0.59212160836874783</v>
+        <v>0.54989922562851368</v>
       </c>
     </row>
     <row r="16" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -12888,7 +12920,7 @@
       </c>
       <c r="AA16" s="1">
         <f t="shared" si="2"/>
-        <v>348</v>
+        <v>603</v>
       </c>
       <c r="AB16" s="1">
         <f t="shared" si="2"/>
@@ -12896,14 +12928,14 @@
       </c>
       <c r="AC16" s="1">
         <f t="shared" si="1"/>
-        <v>-65.5</v>
+        <v>-320.5</v>
       </c>
       <c r="AD16" s="44" t="s">
         <v>80</v>
       </c>
       <c r="AE16" s="44">
         <f>+U29+'Punters 2022'!U29</f>
-        <v>225</v>
+        <v>235</v>
       </c>
       <c r="AF16" s="44">
         <f>+V29+'Punters 2022'!V29</f>
@@ -12911,11 +12943,11 @@
       </c>
       <c r="AG16" s="49">
         <f t="shared" si="3"/>
-        <v>-138.75</v>
+        <v>-148.75</v>
       </c>
       <c r="AH16" s="47">
         <f t="shared" si="4"/>
-        <v>-0.6166666666666667</v>
+        <v>-0.63297872340425532</v>
       </c>
     </row>
     <row r="17" spans="2:30" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -12954,7 +12986,7 @@
       </c>
       <c r="AA17" s="1">
         <f t="shared" si="2"/>
-        <v>348</v>
+        <v>603</v>
       </c>
       <c r="AB17" s="1">
         <f t="shared" si="2"/>
@@ -12962,7 +12994,7 @@
       </c>
       <c r="AC17" s="1">
         <f t="shared" si="1"/>
-        <v>-65.5</v>
+        <v>-320.5</v>
       </c>
       <c r="AD17" s="1"/>
     </row>
@@ -13002,7 +13034,7 @@
       </c>
       <c r="AA18" s="1">
         <f t="shared" si="2"/>
-        <v>348</v>
+        <v>603</v>
       </c>
       <c r="AB18" s="1">
         <f t="shared" si="2"/>
@@ -13010,7 +13042,7 @@
       </c>
       <c r="AC18" s="1">
         <f t="shared" si="1"/>
-        <v>-65.5</v>
+        <v>-320.5</v>
       </c>
       <c r="AD18" s="1"/>
     </row>
@@ -13050,7 +13082,7 @@
       </c>
       <c r="AA19" s="1">
         <f t="shared" si="2"/>
-        <v>348</v>
+        <v>603</v>
       </c>
       <c r="AB19" s="1">
         <f t="shared" si="2"/>
@@ -13058,7 +13090,7 @@
       </c>
       <c r="AC19" s="1">
         <f t="shared" si="1"/>
-        <v>-65.5</v>
+        <v>-320.5</v>
       </c>
       <c r="AD19" s="1"/>
     </row>
@@ -13098,7 +13130,7 @@
       </c>
       <c r="AA20" s="1">
         <f t="shared" si="2"/>
-        <v>348</v>
+        <v>603</v>
       </c>
       <c r="AB20" s="1">
         <f t="shared" si="2"/>
@@ -13106,7 +13138,7 @@
       </c>
       <c r="AC20" s="1">
         <f t="shared" si="1"/>
-        <v>-65.5</v>
+        <v>-320.5</v>
       </c>
       <c r="AD20" s="1"/>
     </row>
@@ -13146,7 +13178,7 @@
       </c>
       <c r="AA21" s="1">
         <f t="shared" si="2"/>
-        <v>348</v>
+        <v>603</v>
       </c>
       <c r="AB21" s="1">
         <f t="shared" si="2"/>
@@ -13154,7 +13186,7 @@
       </c>
       <c r="AC21" s="1">
         <f t="shared" si="1"/>
-        <v>-65.5</v>
+        <v>-320.5</v>
       </c>
       <c r="AD21" s="1"/>
     </row>
@@ -13194,7 +13226,7 @@
       </c>
       <c r="AA22" s="1">
         <f t="shared" ref="AA22:AB26" si="5">AA21+Y22</f>
-        <v>348</v>
+        <v>603</v>
       </c>
       <c r="AB22" s="1">
         <f t="shared" si="5"/>
@@ -13202,7 +13234,7 @@
       </c>
       <c r="AC22" s="1">
         <f t="shared" si="1"/>
-        <v>-65.5</v>
+        <v>-320.5</v>
       </c>
       <c r="AD22" s="1"/>
     </row>
@@ -13242,7 +13274,7 @@
       </c>
       <c r="AA23" s="1">
         <f t="shared" si="5"/>
-        <v>348</v>
+        <v>603</v>
       </c>
       <c r="AB23" s="1">
         <f t="shared" si="5"/>
@@ -13250,7 +13282,7 @@
       </c>
       <c r="AC23" s="1">
         <f t="shared" si="1"/>
-        <v>-65.5</v>
+        <v>-320.5</v>
       </c>
       <c r="AD23" s="1"/>
     </row>
@@ -13290,7 +13322,7 @@
       </c>
       <c r="AA24" s="1">
         <f t="shared" si="5"/>
-        <v>348</v>
+        <v>603</v>
       </c>
       <c r="AB24" s="1">
         <f t="shared" si="5"/>
@@ -13298,7 +13330,7 @@
       </c>
       <c r="AC24" s="1">
         <f t="shared" si="1"/>
-        <v>-65.5</v>
+        <v>-320.5</v>
       </c>
       <c r="AD24" s="1"/>
     </row>
@@ -13338,7 +13370,7 @@
       </c>
       <c r="AA25" s="1">
         <f t="shared" si="5"/>
-        <v>348</v>
+        <v>603</v>
       </c>
       <c r="AB25" s="1">
         <f t="shared" si="5"/>
@@ -13346,7 +13378,7 @@
       </c>
       <c r="AC25" s="1">
         <f t="shared" si="1"/>
-        <v>-65.5</v>
+        <v>-320.5</v>
       </c>
       <c r="AD25" s="1"/>
     </row>
@@ -13386,7 +13418,7 @@
       </c>
       <c r="AA26" s="1">
         <f t="shared" si="5"/>
-        <v>348</v>
+        <v>603</v>
       </c>
       <c r="AB26" s="1">
         <f t="shared" si="5"/>
@@ -13394,7 +13426,7 @@
       </c>
       <c r="AC26" s="1">
         <f t="shared" si="1"/>
-        <v>-65.5</v>
+        <v>-320.5</v>
       </c>
       <c r="AD26" s="1"/>
     </row>
@@ -13482,7 +13514,7 @@
       </c>
       <c r="C29" s="18">
         <f t="shared" ref="C29:Z29" si="7">SUM(C4:C28)</f>
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="D29" s="18">
         <f t="shared" si="7"/>
@@ -13490,7 +13522,7 @@
       </c>
       <c r="E29" s="18">
         <f t="shared" si="7"/>
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="F29" s="18">
         <f t="shared" si="7"/>
@@ -13498,7 +13530,7 @@
       </c>
       <c r="G29" s="18">
         <f t="shared" si="7"/>
-        <v>48</v>
+        <v>73</v>
       </c>
       <c r="H29" s="18">
         <f t="shared" si="7"/>
@@ -13506,7 +13538,7 @@
       </c>
       <c r="I29" s="18">
         <f t="shared" si="7"/>
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="J29" s="18">
         <f t="shared" si="7"/>
@@ -13514,7 +13546,7 @@
       </c>
       <c r="K29" s="18">
         <f t="shared" si="7"/>
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="L29" s="18">
         <f t="shared" si="7"/>
@@ -13522,7 +13554,7 @@
       </c>
       <c r="M29" s="18">
         <f t="shared" si="7"/>
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="N29" s="18">
         <f t="shared" si="7"/>
@@ -13530,7 +13562,7 @@
       </c>
       <c r="O29" s="18">
         <f t="shared" si="7"/>
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="P29" s="18">
         <f t="shared" si="7"/>
@@ -13538,7 +13570,7 @@
       </c>
       <c r="Q29" s="18">
         <f t="shared" si="7"/>
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="R29" s="18">
         <f t="shared" si="7"/>
@@ -13546,7 +13578,7 @@
       </c>
       <c r="S29" s="18">
         <f t="shared" si="7"/>
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="T29" s="18">
         <f>SUM(T4:T28)</f>
@@ -13554,7 +13586,7 @@
       </c>
       <c r="U29" s="18">
         <f t="shared" si="7"/>
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="V29" s="21">
         <f t="shared" si="7"/>
@@ -13570,7 +13602,7 @@
       </c>
       <c r="Y29" s="29">
         <f t="shared" si="7"/>
-        <v>348</v>
+        <v>603</v>
       </c>
       <c r="Z29" s="18">
         <f t="shared" si="7"/>
@@ -13600,11 +13632,11 @@
       </c>
       <c r="N30" s="28">
         <f>(N29-M29)/M29</f>
-        <v>0.9</v>
+        <v>-0.13636363636363635</v>
       </c>
       <c r="P30" s="28">
         <f>(P29-O29)/O29</f>
-        <v>8.4</v>
+        <v>3.7</v>
       </c>
       <c r="R30" s="28">
         <f>(R29-Q29)/Q29</f>
@@ -13627,7 +13659,7 @@
       <c r="H31" s="62"/>
       <c r="I31" s="58">
         <f>C29+E29+G29+I29+K29+M29+O29+Q29+S29+U29+W29</f>
-        <v>348</v>
+        <v>603</v>
       </c>
       <c r="J31" s="59"/>
     </row>
@@ -13645,7 +13677,7 @@
     <row r="33" spans="3:25" x14ac:dyDescent="0.55000000000000004">
       <c r="I33" s="58">
         <f>I32-I31</f>
-        <v>-65.5</v>
+        <v>-320.5</v>
       </c>
       <c r="J33" s="59"/>
       <c r="Y33">
@@ -13656,7 +13688,7 @@
     <row r="34" spans="3:25" x14ac:dyDescent="0.55000000000000004">
       <c r="C34" s="36">
         <f>C29+E29+G29+I29</f>
-        <v>198</v>
+        <v>303</v>
       </c>
       <c r="D34" s="36">
         <f>D29+F29+H29+J29</f>
@@ -13664,11 +13696,11 @@
       </c>
       <c r="E34" s="37">
         <f>D34-C34</f>
-        <v>-198</v>
+        <v>-303</v>
       </c>
       <c r="I34" s="38">
         <f>O29+K29+M29</f>
-        <v>75</v>
+        <v>155</v>
       </c>
       <c r="J34" s="38">
         <f>P29+L29+N29</f>
@@ -13676,11 +13708,11 @@
       </c>
       <c r="K34" s="39">
         <f>J34-I34</f>
-        <v>207.5</v>
+        <v>127.5</v>
       </c>
       <c r="O34" s="40">
         <f>U29+Q29+S29</f>
-        <v>75</v>
+        <v>145</v>
       </c>
       <c r="P34" s="40">
         <f>V29+R29+T29</f>
@@ -13688,7 +13720,7 @@
       </c>
       <c r="Q34" s="41">
         <f>P34-O34</f>
-        <v>-75</v>
+        <v>-145</v>
       </c>
       <c r="X34" s="55"/>
       <c r="Y34">
@@ -13706,7 +13738,7 @@
       <c r="I35" s="38"/>
       <c r="J35" s="34">
         <f>(J34-I34)/I34</f>
-        <v>2.7666666666666666</v>
+        <v>0.82258064516129037</v>
       </c>
       <c r="K35" s="39"/>
       <c r="O35" s="40"/>
@@ -13738,7 +13770,7 @@
       <c r="H38" s="42"/>
       <c r="I38" s="66">
         <f>I36+I33</f>
-        <v>1936.09</v>
+        <v>1681.09</v>
       </c>
       <c r="J38" s="66"/>
       <c r="M38" s="33"/>
@@ -13792,7 +13824,7 @@
     <row r="42" spans="3:25" x14ac:dyDescent="0.55000000000000004">
       <c r="C42" s="1">
         <f>C29+E29+G29+I29</f>
-        <v>198</v>
+        <v>303</v>
       </c>
       <c r="D42" s="1">
         <f>D29+F29+H29+J29</f>
@@ -13800,7 +13832,7 @@
       </c>
       <c r="I42" s="1">
         <f>O29+K29+M29</f>
-        <v>75</v>
+        <v>155</v>
       </c>
       <c r="J42" s="1">
         <f>P29+L29+N29</f>
@@ -13808,7 +13840,7 @@
       </c>
       <c r="O42" s="1">
         <f>U29+Q29+S29</f>
-        <v>75</v>
+        <v>145</v>
       </c>
       <c r="P42" s="1">
         <f>V29+R29+T29</f>
@@ -13818,20 +13850,20 @@
     <row r="43" spans="3:25" x14ac:dyDescent="0.55000000000000004">
       <c r="D43" s="1">
         <f>D42-C42</f>
-        <v>-198</v>
+        <v>-303</v>
       </c>
       <c r="J43" s="33">
         <f>J42-I42</f>
-        <v>207.5</v>
+        <v>127.5</v>
       </c>
       <c r="P43" s="33">
         <f>P42-O42</f>
-        <v>-75</v>
+        <v>-145</v>
       </c>
     </row>
     <row r="45" spans="3:25" x14ac:dyDescent="0.55000000000000004">
       <c r="V45" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="46" spans="3:25" x14ac:dyDescent="0.55000000000000004">
@@ -13859,13 +13891,13 @@
         <v>90</v>
       </c>
       <c r="K47" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="V47" t="s">
         <v>12</v>
       </c>
       <c r="W47">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="3:25" x14ac:dyDescent="0.55000000000000004">
@@ -13880,10 +13912,13 @@
         <v>92</v>
       </c>
       <c r="K48">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V48" t="s">
         <v>93</v>
+      </c>
+      <c r="W48">
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="4:23" x14ac:dyDescent="0.55000000000000004">
@@ -13898,7 +13933,7 @@
         <v>12</v>
       </c>
       <c r="K49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V49" t="s">
         <v>92</v>
@@ -13916,7 +13951,7 @@
         <v>94</v>
       </c>
       <c r="K50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V50" t="s">
         <v>9</v>
@@ -13955,13 +13990,13 @@
         <v>93</v>
       </c>
       <c r="K52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V52" t="s">
         <v>96</v>
       </c>
       <c r="W52">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="4:23" x14ac:dyDescent="0.55000000000000004">
@@ -13976,7 +14011,7 @@
         <v>97</v>
       </c>
       <c r="K53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V53" t="s">
         <v>98</v>
@@ -13999,6 +14034,9 @@
       <c r="V54" t="s">
         <v>97</v>
       </c>
+      <c r="W54">
+        <v>1</v>
+      </c>
     </row>
     <row r="55" spans="4:23" x14ac:dyDescent="0.55000000000000004">
       <c r="D55" t="s">
@@ -14033,11 +14071,11 @@
         <v>96</v>
       </c>
       <c r="K56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W56">
         <f>SUM(W46:W55)</f>
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="57" spans="4:23" x14ac:dyDescent="0.55000000000000004">
@@ -14367,6 +14405,6 @@
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
-  <clbl:label id="{0f7d30c2-cad0-4405-8153-25a6a3313da4}" enabled="1" method="Privileged" siteId="{6c637512-c417-4e78-9d62-b61258e4b619}" removed="0"/>
+  <clbl:label id="{0f7d30c2-cad0-4405-8153-25a6a3313da4}" enabled="1" method="Privileged" siteId="{6c637512-c417-4e78-9d62-b61258e4b619}" contentBits="0" removed="0"/>
 </clbl:labelList>
 </file>
</xml_diff>

<commit_message>
Fixed issue with leaderboard showing wrong data
</commit_message>
<xml_diff>
--- a/public/Data/HEMANPUNTERS.xlsx
+++ b/public/Data/HEMANPUNTERS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bturnor\source\repos\PersonalWork\seeMore\public\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A7CD420-4D11-4256-8848-3172309E6AEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC55E15-FCC0-4B26-BA90-FFFF711774D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="45" windowWidth="29040" windowHeight="15720" firstSheet="5" activeTab="5" xr2:uid="{525E8989-1938-4309-A4CF-8F1D15E362FB}"/>
   </bookViews>
@@ -985,9 +985,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1006,16 +1003,19 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3750,50 +3750,50 @@
   <sheetData>
     <row r="1" spans="2:27" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="2" spans="2:27" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57" t="s">
+      <c r="D2" s="63"/>
+      <c r="E2" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57" t="s">
+      <c r="F2" s="63"/>
+      <c r="G2" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57" t="s">
+      <c r="H2" s="63"/>
+      <c r="I2" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57" t="s">
+      <c r="J2" s="63"/>
+      <c r="K2" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="57"/>
-      <c r="M2" s="57" t="s">
+      <c r="L2" s="63"/>
+      <c r="M2" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="57"/>
-      <c r="O2" s="57" t="s">
+      <c r="N2" s="63"/>
+      <c r="O2" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="57"/>
-      <c r="Q2" s="57" t="s">
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="R2" s="57"/>
-      <c r="S2" s="57" t="s">
+      <c r="R2" s="63"/>
+      <c r="S2" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="T2" s="57"/>
-      <c r="U2" s="57" t="s">
+      <c r="T2" s="63"/>
+      <c r="U2" s="63" t="s">
         <v>27</v>
       </c>
       <c r="V2" s="64"/>
-      <c r="W2" s="63" t="s">
+      <c r="W2" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="X2" s="57"/>
+      <c r="X2" s="63"/>
     </row>
     <row r="3" spans="2:27" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B3" s="32" t="s">
@@ -5354,34 +5354,34 @@
       </c>
     </row>
     <row r="29" spans="2:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="F29" s="60" t="s">
+      <c r="F29" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="G29" s="61"/>
-      <c r="H29" s="62"/>
-      <c r="I29" s="58">
+      <c r="G29" s="60"/>
+      <c r="H29" s="61"/>
+      <c r="I29" s="57">
         <f>C27+E27+G27+I27+K27+M27+O27+Q27+S27+U27</f>
         <v>2469.42</v>
       </c>
-      <c r="J29" s="59"/>
+      <c r="J29" s="58"/>
     </row>
     <row r="30" spans="2:27" x14ac:dyDescent="0.55000000000000004">
       <c r="G30" s="65" t="s">
         <v>57</v>
       </c>
       <c r="H30" s="65"/>
-      <c r="I30" s="58">
+      <c r="I30" s="57">
         <f>+D27+F27+H27+J27+L27+N27+P27+R27+T27+V27</f>
         <v>1774.69</v>
       </c>
-      <c r="J30" s="59"/>
+      <c r="J30" s="58"/>
     </row>
     <row r="31" spans="2:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="I31" s="58">
+      <c r="I31" s="57">
         <f>I30-I29</f>
         <v>-694.73</v>
       </c>
-      <c r="J31" s="59"/>
+      <c r="J31" s="58"/>
     </row>
     <row r="32" spans="2:27" x14ac:dyDescent="0.55000000000000004">
       <c r="C32" s="1">
@@ -5430,11 +5430,11 @@
       </c>
     </row>
     <row r="34" spans="3:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="I34" s="59">
+      <c r="I34" s="58">
         <f>I33+I31</f>
         <v>505.27</v>
       </c>
-      <c r="J34" s="59"/>
+      <c r="J34" s="58"/>
     </row>
     <row r="38" spans="3:16" x14ac:dyDescent="0.55000000000000004">
       <c r="C38" s="1">
@@ -5478,6 +5478,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
     <mergeCell ref="I30:J30"/>
     <mergeCell ref="F29:H29"/>
     <mergeCell ref="I31:J31"/>
@@ -5490,11 +5495,6 @@
     <mergeCell ref="S2:T2"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="I29:J29"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5527,50 +5527,50 @@
   <sheetData>
     <row r="1" spans="2:27" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="2" spans="2:27" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57" t="s">
+      <c r="D2" s="63"/>
+      <c r="E2" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="57"/>
-      <c r="G2" s="67" t="s">
+      <c r="F2" s="63"/>
+      <c r="G2" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="57" t="s">
+      <c r="H2" s="62"/>
+      <c r="I2" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57" t="s">
+      <c r="J2" s="63"/>
+      <c r="K2" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="57"/>
-      <c r="M2" s="57" t="s">
+      <c r="L2" s="63"/>
+      <c r="M2" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="57"/>
-      <c r="O2" s="57" t="s">
+      <c r="N2" s="63"/>
+      <c r="O2" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="57"/>
-      <c r="Q2" s="57" t="s">
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="R2" s="57"/>
-      <c r="S2" s="57" t="s">
+      <c r="R2" s="63"/>
+      <c r="S2" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="T2" s="57"/>
-      <c r="U2" s="57" t="s">
+      <c r="T2" s="63"/>
+      <c r="U2" s="63" t="s">
         <v>27</v>
       </c>
       <c r="V2" s="64"/>
-      <c r="W2" s="63" t="s">
+      <c r="W2" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="X2" s="57"/>
+      <c r="X2" s="63"/>
     </row>
     <row r="3" spans="2:27" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B3" s="32" t="s">
@@ -6930,34 +6930,34 @@
       </c>
     </row>
     <row r="29" spans="2:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="F29" s="60" t="s">
+      <c r="F29" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="G29" s="61"/>
-      <c r="H29" s="62"/>
-      <c r="I29" s="58">
+      <c r="G29" s="60"/>
+      <c r="H29" s="61"/>
+      <c r="I29" s="57">
         <f>C27+E27+G27+I27+K27+M27+O27+Q27+S27+U27</f>
         <v>1788.24</v>
       </c>
-      <c r="J29" s="59"/>
+      <c r="J29" s="58"/>
     </row>
     <row r="30" spans="2:27" x14ac:dyDescent="0.55000000000000004">
       <c r="G30" s="65" t="s">
         <v>57</v>
       </c>
       <c r="H30" s="65"/>
-      <c r="I30" s="58">
+      <c r="I30" s="57">
         <f>+D27+F27+H27+J27+L27+N27+P27+R27+T27+V27</f>
         <v>2492.1999999999998</v>
       </c>
-      <c r="J30" s="59"/>
+      <c r="J30" s="58"/>
     </row>
     <row r="31" spans="2:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="I31" s="58">
+      <c r="I31" s="57">
         <f>I30-I29</f>
         <v>703.95999999999981</v>
       </c>
-      <c r="J31" s="59"/>
+      <c r="J31" s="58"/>
     </row>
     <row r="32" spans="2:27" x14ac:dyDescent="0.55000000000000004">
       <c r="C32" s="36">
@@ -7011,11 +7011,11 @@
         <v>64</v>
       </c>
       <c r="H34" s="42"/>
-      <c r="I34" s="66">
+      <c r="I34" s="67">
         <f>I33+I31</f>
         <v>1303.9599999999998</v>
       </c>
-      <c r="J34" s="66"/>
+      <c r="J34" s="67"/>
       <c r="M34" s="33"/>
     </row>
     <row r="38" spans="3:16" x14ac:dyDescent="0.55000000000000004">
@@ -7060,11 +7060,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="O2:P2"/>
     <mergeCell ref="Q2:R2"/>
     <mergeCell ref="S2:T2"/>
     <mergeCell ref="U2:V2"/>
@@ -7072,11 +7072,11 @@
     <mergeCell ref="F29:H29"/>
     <mergeCell ref="I29:J29"/>
     <mergeCell ref="M2:N2"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7110,54 +7110,54 @@
   <sheetData>
     <row r="1" spans="2:34" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="2" spans="2:34" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57" t="s">
+      <c r="D2" s="63"/>
+      <c r="E2" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57" t="s">
+      <c r="F2" s="63"/>
+      <c r="G2" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57" t="s">
+      <c r="H2" s="63"/>
+      <c r="I2" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57" t="s">
+      <c r="J2" s="63"/>
+      <c r="K2" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="57"/>
-      <c r="M2" s="57" t="s">
+      <c r="L2" s="63"/>
+      <c r="M2" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="N2" s="57"/>
-      <c r="O2" s="57" t="s">
+      <c r="N2" s="63"/>
+      <c r="O2" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="57"/>
-      <c r="Q2" s="57" t="s">
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="R2" s="57"/>
-      <c r="S2" s="57" t="s">
+      <c r="R2" s="63"/>
+      <c r="S2" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="T2" s="57"/>
-      <c r="U2" s="57" t="s">
+      <c r="T2" s="63"/>
+      <c r="U2" s="63" t="s">
         <v>65</v>
       </c>
       <c r="V2" s="64"/>
-      <c r="W2" s="57" t="s">
+      <c r="W2" s="63" t="s">
         <v>66</v>
       </c>
       <c r="X2" s="64"/>
-      <c r="Y2" s="63" t="s">
+      <c r="Y2" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="Z2" s="57"/>
+      <c r="Z2" s="63"/>
     </row>
     <row r="3" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B3" s="32" t="s">
@@ -9211,34 +9211,34 @@
       </c>
     </row>
     <row r="31" spans="2:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="F31" s="60" t="s">
+      <c r="F31" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="G31" s="61"/>
-      <c r="H31" s="62"/>
-      <c r="I31" s="58">
+      <c r="G31" s="60"/>
+      <c r="H31" s="61"/>
+      <c r="I31" s="57">
         <f>C29+E29+G29+I29+K29+M29+O29+Q29+S29+U29+W29</f>
         <v>2521.33</v>
       </c>
-      <c r="J31" s="59"/>
+      <c r="J31" s="58"/>
     </row>
     <row r="32" spans="2:30" x14ac:dyDescent="0.55000000000000004">
       <c r="G32" s="65" t="s">
         <v>57</v>
       </c>
       <c r="H32" s="65"/>
-      <c r="I32" s="58">
+      <c r="I32" s="57">
         <f>+D29+F29+H29+J29+L29+N29+P29+R29+T29+V29+X29</f>
         <v>2997.5899999999997</v>
       </c>
-      <c r="J32" s="59"/>
+      <c r="J32" s="58"/>
     </row>
     <row r="33" spans="3:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="I33" s="58">
+      <c r="I33" s="57">
         <f>I32-I31</f>
         <v>476.25999999999976</v>
       </c>
-      <c r="J33" s="59"/>
+      <c r="J33" s="58"/>
     </row>
     <row r="34" spans="3:17" x14ac:dyDescent="0.55000000000000004">
       <c r="C34" s="36">
@@ -9291,11 +9291,11 @@
         <v>64</v>
       </c>
       <c r="H36" s="42"/>
-      <c r="I36" s="66">
+      <c r="I36" s="67">
         <f>I35+I33</f>
         <v>2476.2599999999998</v>
       </c>
-      <c r="J36" s="66"/>
+      <c r="J36" s="67"/>
       <c r="M36" s="33"/>
     </row>
     <row r="40" spans="3:17" x14ac:dyDescent="0.55000000000000004">
@@ -9340,11 +9340,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="O2:P2"/>
     <mergeCell ref="Q2:R2"/>
     <mergeCell ref="S2:T2"/>
     <mergeCell ref="U2:V2"/>
@@ -9353,11 +9353,11 @@
     <mergeCell ref="I31:J31"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="W2:X2"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="54" orientation="landscape" r:id="rId1"/>
@@ -9391,54 +9391,54 @@
   <sheetData>
     <row r="1" spans="2:34" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="2" spans="2:34" ht="18.3" x14ac:dyDescent="0.7">
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="57"/>
-      <c r="E2" s="67" t="s">
+      <c r="D2" s="63"/>
+      <c r="E2" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="63"/>
-      <c r="G2" s="57" t="s">
+      <c r="F2" s="62"/>
+      <c r="G2" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57" t="s">
+      <c r="H2" s="63"/>
+      <c r="I2" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57" t="s">
+      <c r="J2" s="63"/>
+      <c r="K2" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="57"/>
-      <c r="M2" s="67" t="s">
+      <c r="L2" s="63"/>
+      <c r="M2" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="63"/>
-      <c r="O2" s="57" t="s">
+      <c r="N2" s="62"/>
+      <c r="O2" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="P2" s="57"/>
-      <c r="Q2" s="57" t="s">
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="R2" s="57"/>
-      <c r="S2" s="57" t="s">
+      <c r="R2" s="63"/>
+      <c r="S2" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="T2" s="57"/>
-      <c r="U2" s="57" t="s">
+      <c r="T2" s="63"/>
+      <c r="U2" s="63" t="s">
         <v>65</v>
       </c>
       <c r="V2" s="64"/>
-      <c r="W2" s="57" t="s">
+      <c r="W2" s="63" t="s">
         <v>66</v>
       </c>
       <c r="X2" s="64"/>
-      <c r="Y2" s="63" t="s">
+      <c r="Y2" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="Z2" s="57"/>
+      <c r="Z2" s="63"/>
     </row>
     <row r="3" spans="2:34" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="32" t="s">
@@ -11447,34 +11447,34 @@
       </c>
     </row>
     <row r="31" spans="2:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="F31" s="60" t="s">
+      <c r="F31" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="G31" s="61"/>
-      <c r="H31" s="62"/>
-      <c r="I31" s="58">
+      <c r="G31" s="60"/>
+      <c r="H31" s="61"/>
+      <c r="I31" s="57">
         <f>C29+E29+G29+I29+K29+M29+O29+Q29+S29+U29+W29</f>
         <v>2462.73</v>
       </c>
-      <c r="J31" s="59"/>
+      <c r="J31" s="58"/>
     </row>
     <row r="32" spans="2:30" x14ac:dyDescent="0.55000000000000004">
       <c r="G32" s="65" t="s">
         <v>57</v>
       </c>
       <c r="H32" s="65"/>
-      <c r="I32" s="58">
+      <c r="I32" s="57">
         <f>+D29+F29+H29+J29+L29+N29+P29+R29+T29+V29+X29</f>
         <v>1004.25</v>
       </c>
-      <c r="J32" s="59"/>
+      <c r="J32" s="58"/>
     </row>
     <row r="33" spans="3:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="I33" s="58">
+      <c r="I33" s="57">
         <f>I32-I31</f>
         <v>-1458.48</v>
       </c>
-      <c r="J33" s="59"/>
+      <c r="J33" s="58"/>
       <c r="Y33">
         <f>2167+183+5*10</f>
         <v>2400</v>
@@ -11570,11 +11570,11 @@
         <v>64</v>
       </c>
       <c r="H38" s="42"/>
-      <c r="I38" s="66">
+      <c r="I38" s="67">
         <f>I36+I33+J37</f>
         <v>322.7800000000002</v>
       </c>
-      <c r="J38" s="66"/>
+      <c r="J38" s="67"/>
       <c r="M38" s="33"/>
     </row>
     <row r="40" spans="3:25" x14ac:dyDescent="0.55000000000000004">
@@ -11846,16 +11846,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="U2:V2"/>
     <mergeCell ref="W2:X2"/>
     <mergeCell ref="Y2:Z2"/>
     <mergeCell ref="C2:D2"/>
@@ -11864,6 +11854,16 @@
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="M2:N2"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="I33:J33"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="54" orientation="landscape" r:id="rId1"/>
@@ -11875,10 +11875,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AH58"/>
+  <dimension ref="B1:AH60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V46" sqref="V46"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40:XFD40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -11901,54 +11901,54 @@
   <sheetData>
     <row r="1" spans="2:34" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="2" spans="2:34" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="63" t="s">
         <v>100</v>
       </c>
-      <c r="D2" s="57"/>
-      <c r="E2" s="67" t="s">
+      <c r="D2" s="63"/>
+      <c r="E2" s="66" t="s">
         <v>101</v>
       </c>
-      <c r="F2" s="63"/>
-      <c r="G2" s="57" t="s">
+      <c r="F2" s="62"/>
+      <c r="G2" s="63" t="s">
         <v>102</v>
       </c>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57" t="s">
+      <c r="H2" s="63"/>
+      <c r="I2" s="63" t="s">
         <v>103</v>
       </c>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57" t="s">
+      <c r="J2" s="63"/>
+      <c r="K2" s="63" t="s">
         <v>104</v>
       </c>
-      <c r="L2" s="57"/>
-      <c r="M2" s="67" t="s">
+      <c r="L2" s="63"/>
+      <c r="M2" s="66" t="s">
         <v>105</v>
       </c>
-      <c r="N2" s="63"/>
-      <c r="O2" s="57" t="s">
+      <c r="N2" s="62"/>
+      <c r="O2" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="P2" s="57"/>
-      <c r="Q2" s="57" t="s">
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63" t="s">
         <v>107</v>
       </c>
-      <c r="R2" s="57"/>
-      <c r="S2" s="57" t="s">
+      <c r="R2" s="63"/>
+      <c r="S2" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="T2" s="57"/>
-      <c r="U2" s="57" t="s">
+      <c r="T2" s="63"/>
+      <c r="U2" s="63" t="s">
         <v>108</v>
       </c>
       <c r="V2" s="64"/>
-      <c r="W2" s="57" t="s">
+      <c r="W2" s="63" t="s">
         <v>66</v>
       </c>
       <c r="X2" s="64"/>
-      <c r="Y2" s="63" t="s">
+      <c r="Y2" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="Z2" s="57"/>
+      <c r="Z2" s="63"/>
     </row>
     <row r="3" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B3" s="32" t="s">
@@ -13750,34 +13750,34 @@
       </c>
     </row>
     <row r="31" spans="2:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="F31" s="60" t="s">
+      <c r="F31" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="G31" s="61"/>
-      <c r="H31" s="62"/>
-      <c r="I31" s="58">
+      <c r="G31" s="60"/>
+      <c r="H31" s="61"/>
+      <c r="I31" s="57">
         <f>C29+E29+G29+I29+K29+M29+O29+Q29+S29+U29+W29</f>
         <v>1113</v>
       </c>
-      <c r="J31" s="59"/>
+      <c r="J31" s="58"/>
     </row>
     <row r="32" spans="2:30" x14ac:dyDescent="0.55000000000000004">
       <c r="G32" s="65" t="s">
         <v>57</v>
       </c>
       <c r="H32" s="65"/>
-      <c r="I32" s="58">
+      <c r="I32" s="57">
         <f>+D29+F29+H29+J29+L29+N29+P29+R29+T29+V29+X29</f>
         <v>472.5</v>
       </c>
-      <c r="J32" s="59"/>
+      <c r="J32" s="58"/>
     </row>
     <row r="33" spans="3:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="I33" s="58">
+      <c r="I33" s="57">
         <f>I32-I31</f>
         <v>-640.5</v>
       </c>
-      <c r="J33" s="59"/>
+      <c r="J33" s="58"/>
       <c r="Y33">
         <f>2167+183+5*10</f>
         <v>2400</v>
@@ -13866,318 +13866,305 @@
         <v>64</v>
       </c>
       <c r="H38" s="42"/>
-      <c r="I38" s="66">
+      <c r="I38" s="67">
         <f>I36+I33</f>
         <v>1361.09</v>
       </c>
-      <c r="J38" s="66"/>
+      <c r="J38" s="67"/>
       <c r="M38" s="33"/>
     </row>
-    <row r="40" spans="3:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="X40" s="55"/>
-    </row>
-    <row r="42" spans="3:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="C42" s="1">
+    <row r="44" spans="3:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="C44" s="1">
         <f>C29+E29+G29+I29</f>
         <v>463</v>
       </c>
-      <c r="D42" s="1">
+      <c r="D44" s="1">
         <f>D29+F29+H29+J29</f>
         <v>0</v>
       </c>
-      <c r="I42" s="1">
+      <c r="I44" s="1">
         <f>O29+K29+M29</f>
         <v>375</v>
       </c>
-      <c r="J42" s="1">
+      <c r="J44" s="1">
         <f>P29+L29+N29</f>
         <v>367.5</v>
       </c>
-      <c r="O42" s="1">
+      <c r="O44" s="1">
         <f>U29+Q29+S29</f>
         <v>275</v>
       </c>
-      <c r="P42" s="1">
+      <c r="P44" s="1">
         <f>V29+R29+T29</f>
         <v>105</v>
       </c>
     </row>
-    <row r="43" spans="3:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="D43" s="1">
-        <f>D42-C42</f>
+    <row r="45" spans="3:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="D45" s="1">
+        <f>D44-C44</f>
         <v>-463</v>
       </c>
-      <c r="J43" s="33">
-        <f>J42-I42</f>
+      <c r="J45" s="33">
+        <f>J44-I44</f>
         <v>-7.5</v>
       </c>
-      <c r="P43" s="33">
-        <f>P42-O42</f>
+      <c r="P45" s="33">
+        <f>P44-O44</f>
         <v>-170</v>
       </c>
     </row>
-    <row r="45" spans="3:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="V45" t="s">
+    <row r="47" spans="3:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="V47" t="s">
         <v>110</v>
-      </c>
-    </row>
-    <row r="46" spans="3:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="D46" t="s">
-        <v>88</v>
-      </c>
-      <c r="J46" t="s">
-        <v>111</v>
-      </c>
-      <c r="V46" t="s">
-        <v>89</v>
-      </c>
-      <c r="W46">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="47" spans="3:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="D47" t="s">
-        <v>90</v>
-      </c>
-      <c r="E47" t="s">
-        <v>91</v>
-      </c>
-      <c r="J47" t="s">
-        <v>90</v>
-      </c>
-      <c r="K47" t="s">
-        <v>112</v>
-      </c>
-      <c r="V47" t="s">
-        <v>12</v>
-      </c>
-      <c r="W47">
-        <v>6</v>
       </c>
     </row>
     <row r="48" spans="3:25" x14ac:dyDescent="0.55000000000000004">
       <c r="D48" t="s">
-        <v>92</v>
-      </c>
-      <c r="E48" s="1">
-        <f>SUM(V29)</f>
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="J48" t="s">
-        <v>92</v>
-      </c>
-      <c r="K48">
-        <v>3</v>
+        <v>111</v>
       </c>
       <c r="V48" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="W48">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="49" spans="4:23" x14ac:dyDescent="0.55000000000000004">
       <c r="D49" t="s">
+        <v>90</v>
+      </c>
+      <c r="E49" t="s">
+        <v>91</v>
+      </c>
+      <c r="J49" t="s">
+        <v>90</v>
+      </c>
+      <c r="K49" t="s">
+        <v>112</v>
+      </c>
+      <c r="V49" t="s">
         <v>12</v>
       </c>
-      <c r="E49" s="1">
-        <f>SUM(L29)</f>
-        <v>0</v>
-      </c>
-      <c r="J49" t="s">
-        <v>12</v>
-      </c>
-      <c r="K49">
-        <v>1</v>
-      </c>
-      <c r="V49" t="s">
-        <v>92</v>
-      </c>
       <c r="W49">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="50" spans="4:23" x14ac:dyDescent="0.55000000000000004">
       <c r="D50" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E50" s="1">
-        <f>SUM(D29)</f>
+        <f>SUM(V29)</f>
         <v>0</v>
       </c>
       <c r="J50" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K50">
+        <v>3</v>
+      </c>
+      <c r="V50" t="s">
+        <v>93</v>
+      </c>
+      <c r="W50">
         <v>1</v>
-      </c>
-      <c r="V50" t="s">
-        <v>9</v>
-      </c>
-      <c r="W50">
-        <v>2</v>
       </c>
     </row>
     <row r="51" spans="4:23" x14ac:dyDescent="0.55000000000000004">
       <c r="D51" t="s">
-        <v>95</v>
+        <v>12</v>
       </c>
       <c r="E51" s="1">
-        <f>SUM(F29)</f>
+        <f>SUM(L29)</f>
         <v>0</v>
       </c>
       <c r="J51" t="s">
-        <v>95</v>
+        <v>12</v>
       </c>
       <c r="K51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V51" t="s">
-        <v>11</v>
+        <v>92</v>
       </c>
       <c r="W51">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="4:23" x14ac:dyDescent="0.55000000000000004">
       <c r="D52" t="s">
+        <v>94</v>
+      </c>
+      <c r="E52" s="1">
+        <f>SUM(D29)</f>
+        <v>0</v>
+      </c>
+      <c r="J52" t="s">
+        <v>94</v>
+      </c>
+      <c r="K52">
+        <v>1</v>
+      </c>
+      <c r="V52" t="s">
+        <v>9</v>
+      </c>
+      <c r="W52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="4:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="D53" t="s">
+        <v>95</v>
+      </c>
+      <c r="E53" s="1">
+        <f>SUM(F29)</f>
+        <v>0</v>
+      </c>
+      <c r="J53" t="s">
+        <v>95</v>
+      </c>
+      <c r="K53">
+        <v>0</v>
+      </c>
+      <c r="V53" t="s">
+        <v>11</v>
+      </c>
+      <c r="W53">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="4:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="D54" t="s">
         <v>93</v>
       </c>
-      <c r="E52" s="1">
+      <c r="E54" s="1">
         <f>SUM(T29)</f>
         <v>105</v>
       </c>
-      <c r="J52" t="s">
+      <c r="J54" t="s">
         <v>93</v>
       </c>
-      <c r="K52">
+      <c r="K54">
         <v>1</v>
       </c>
-      <c r="V52" t="s">
+      <c r="V54" t="s">
         <v>96</v>
       </c>
-      <c r="W52">
+      <c r="W54">
         <v>3</v>
-      </c>
-    </row>
-    <row r="53" spans="4:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="D53" t="s">
-        <v>97</v>
-      </c>
-      <c r="E53" s="1">
-        <f>SUM(R29)</f>
-        <v>0</v>
-      </c>
-      <c r="J53" t="s">
-        <v>97</v>
-      </c>
-      <c r="K53">
-        <v>1</v>
-      </c>
-      <c r="V53" t="s">
-        <v>98</v>
-      </c>
-      <c r="W53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="4:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="D54" t="s">
-        <v>98</v>
-      </c>
-      <c r="E54" s="1">
-        <f>SUM(J29)</f>
-        <v>0</v>
-      </c>
-      <c r="J54" t="s">
-        <v>98</v>
-      </c>
-      <c r="K54">
-        <v>0</v>
-      </c>
-      <c r="V54" t="s">
-        <v>97</v>
-      </c>
-      <c r="W54">
-        <v>1</v>
       </c>
     </row>
     <row r="55" spans="4:23" x14ac:dyDescent="0.55000000000000004">
       <c r="D55" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E55" s="1">
-        <f>SUM(H29)</f>
+        <f>SUM(R29)</f>
         <v>0</v>
       </c>
       <c r="J55" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="K55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V55" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="W55">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="4:23" x14ac:dyDescent="0.55000000000000004">
       <c r="D56" t="s">
+        <v>98</v>
+      </c>
+      <c r="E56" s="1">
+        <f>SUM(J29)</f>
+        <v>0</v>
+      </c>
+      <c r="J56" t="s">
+        <v>98</v>
+      </c>
+      <c r="K56">
+        <v>0</v>
+      </c>
+      <c r="V56" t="s">
+        <v>97</v>
+      </c>
+      <c r="W56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="4:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="D57" t="s">
+        <v>89</v>
+      </c>
+      <c r="E57" s="1">
+        <f>SUM(H29)</f>
+        <v>0</v>
+      </c>
+      <c r="J57" t="s">
+        <v>89</v>
+      </c>
+      <c r="K57">
+        <v>0</v>
+      </c>
+      <c r="V57" t="s">
+        <v>94</v>
+      </c>
+      <c r="W57">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="4:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="D58" t="s">
         <v>96</v>
       </c>
-      <c r="E56" s="1">
+      <c r="E58" s="1">
         <f>SUM(N29)</f>
         <v>132.5</v>
       </c>
-      <c r="J56" t="s">
+      <c r="J58" t="s">
         <v>96</v>
       </c>
-      <c r="K56">
+      <c r="K58">
         <v>1</v>
       </c>
-      <c r="W56">
-        <f>SUM(W46:W55)</f>
+      <c r="W58">
+        <f>SUM(W48:W57)</f>
         <v>28</v>
       </c>
     </row>
-    <row r="57" spans="4:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="D57" t="s">
+    <row r="59" spans="4:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="D59" t="s">
         <v>9</v>
       </c>
-      <c r="E57" s="1">
+      <c r="E59" s="1">
         <f>SUM(P29)</f>
         <v>235</v>
       </c>
-      <c r="J57" t="s">
+      <c r="J59" t="s">
         <v>9</v>
       </c>
-      <c r="K57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="4:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="D58" t="s">
+      <c r="K59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="4:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="D60" t="s">
         <v>99</v>
       </c>
-      <c r="E58" s="1">
-        <f>SUM(E48:E57)</f>
+      <c r="E60" s="1">
+        <f>SUM(E50:E59)</f>
         <v>472.5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="U2:V2"/>
     <mergeCell ref="W2:X2"/>
     <mergeCell ref="Y2:Z2"/>
     <mergeCell ref="C2:D2"/>
@@ -14186,6 +14173,16 @@
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="M2:N2"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="I33:J33"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="54" orientation="landscape" r:id="rId1"/>
@@ -14202,6 +14199,14 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="3e1ffae5-f160-4019-9720-1b11bf1b81a3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002D8393059904904F9DB82DE4B9AFABF6" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f7bafc8adbaca2e93ffc3a1da3fd32d5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3e1ffae5-f160-4019-9720-1b11bf1b81a3" xmlns:ns4="21753bd8-bffc-4cd2-a328-982ee854c895" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f821f56a5d2247de677e71e73e5a99e" ns3:_="" ns4:_="">
     <xsd:import namespace="3e1ffae5-f160-4019-9720-1b11bf1b81a3"/>
@@ -14422,14 +14427,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="3e1ffae5-f160-4019-9720-1b11bf1b81a3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{948817D4-7F3F-493D-9D4C-B473DA03CC7E}">
   <ds:schemaRefs>
@@ -14439,6 +14436,16 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4D7A62A-0CB5-48B0-A73A-0A91BCC8EAEF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3e1ffae5-f160-4019-9720-1b11bf1b81a3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22BA772B-ABF0-4278-9CEF-D9160BBA9E07}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14457,16 +14464,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4D7A62A-0CB5-48B0-A73A-0A91BCC8EAEF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3e1ffae5-f160-4019-9720-1b11bf1b81a3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{0f7d30c2-cad0-4405-8153-25a6a3313da4}" enabled="1" method="Privileged" siteId="{6c637512-c417-4e78-9d62-b61258e4b619}" removed="0"/>

</xml_diff>

<commit_message>
Updating Some configs and data
</commit_message>
<xml_diff>
--- a/public/Data/HEMANPUNTERS.xlsx
+++ b/public/Data/HEMANPUNTERS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bturnor\source\repos\PersonalWork\seeMore\public\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB38CCA7-EA3E-4655-B27E-B8880BA1E5D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF6E930-B422-4A45-92FE-701588BBFF19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="86280" yWindow="45" windowWidth="29040" windowHeight="15720" firstSheet="5" activeTab="5" xr2:uid="{525E8989-1938-4309-A4CF-8F1D15E362FB}"/>
+    <workbookView xWindow="57480" yWindow="45" windowWidth="29040" windowHeight="15720" firstSheet="5" activeTab="5" xr2:uid="{525E8989-1938-4309-A4CF-8F1D15E362FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Punters club" sheetId="1" r:id="rId1"/>
@@ -985,9 +985,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1006,16 +1003,19 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3750,50 +3750,50 @@
   <sheetData>
     <row r="1" spans="2:27" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="2" spans="2:27" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57" t="s">
+      <c r="D2" s="63"/>
+      <c r="E2" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57" t="s">
+      <c r="F2" s="63"/>
+      <c r="G2" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57" t="s">
+      <c r="H2" s="63"/>
+      <c r="I2" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57" t="s">
+      <c r="J2" s="63"/>
+      <c r="K2" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="57"/>
-      <c r="M2" s="57" t="s">
+      <c r="L2" s="63"/>
+      <c r="M2" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="57"/>
-      <c r="O2" s="57" t="s">
+      <c r="N2" s="63"/>
+      <c r="O2" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="57"/>
-      <c r="Q2" s="57" t="s">
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="R2" s="57"/>
-      <c r="S2" s="57" t="s">
+      <c r="R2" s="63"/>
+      <c r="S2" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="T2" s="57"/>
-      <c r="U2" s="57" t="s">
+      <c r="T2" s="63"/>
+      <c r="U2" s="63" t="s">
         <v>27</v>
       </c>
       <c r="V2" s="64"/>
-      <c r="W2" s="63" t="s">
+      <c r="W2" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="X2" s="57"/>
+      <c r="X2" s="63"/>
     </row>
     <row r="3" spans="2:27" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B3" s="32" t="s">
@@ -5354,34 +5354,34 @@
       </c>
     </row>
     <row r="29" spans="2:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="F29" s="60" t="s">
+      <c r="F29" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="G29" s="61"/>
-      <c r="H29" s="62"/>
-      <c r="I29" s="58">
+      <c r="G29" s="60"/>
+      <c r="H29" s="61"/>
+      <c r="I29" s="57">
         <f>C27+E27+G27+I27+K27+M27+O27+Q27+S27+U27</f>
         <v>2469.42</v>
       </c>
-      <c r="J29" s="59"/>
+      <c r="J29" s="58"/>
     </row>
     <row r="30" spans="2:27" x14ac:dyDescent="0.55000000000000004">
       <c r="G30" s="65" t="s">
         <v>57</v>
       </c>
       <c r="H30" s="65"/>
-      <c r="I30" s="58">
+      <c r="I30" s="57">
         <f>+D27+F27+H27+J27+L27+N27+P27+R27+T27+V27</f>
         <v>1774.69</v>
       </c>
-      <c r="J30" s="59"/>
+      <c r="J30" s="58"/>
     </row>
     <row r="31" spans="2:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="I31" s="58">
+      <c r="I31" s="57">
         <f>I30-I29</f>
         <v>-694.73</v>
       </c>
-      <c r="J31" s="59"/>
+      <c r="J31" s="58"/>
     </row>
     <row r="32" spans="2:27" x14ac:dyDescent="0.55000000000000004">
       <c r="C32" s="1">
@@ -5430,11 +5430,11 @@
       </c>
     </row>
     <row r="34" spans="3:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="I34" s="59">
+      <c r="I34" s="58">
         <f>I33+I31</f>
         <v>505.27</v>
       </c>
-      <c r="J34" s="59"/>
+      <c r="J34" s="58"/>
     </row>
     <row r="38" spans="3:16" x14ac:dyDescent="0.55000000000000004">
       <c r="C38" s="1">
@@ -5478,6 +5478,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
     <mergeCell ref="I30:J30"/>
     <mergeCell ref="F29:H29"/>
     <mergeCell ref="I31:J31"/>
@@ -5490,11 +5495,6 @@
     <mergeCell ref="S2:T2"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="I29:J29"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5527,50 +5527,50 @@
   <sheetData>
     <row r="1" spans="2:27" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="2" spans="2:27" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57" t="s">
+      <c r="D2" s="63"/>
+      <c r="E2" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="57"/>
-      <c r="G2" s="67" t="s">
+      <c r="F2" s="63"/>
+      <c r="G2" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="57" t="s">
+      <c r="H2" s="62"/>
+      <c r="I2" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57" t="s">
+      <c r="J2" s="63"/>
+      <c r="K2" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="57"/>
-      <c r="M2" s="57" t="s">
+      <c r="L2" s="63"/>
+      <c r="M2" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="57"/>
-      <c r="O2" s="57" t="s">
+      <c r="N2" s="63"/>
+      <c r="O2" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="57"/>
-      <c r="Q2" s="57" t="s">
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="R2" s="57"/>
-      <c r="S2" s="57" t="s">
+      <c r="R2" s="63"/>
+      <c r="S2" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="T2" s="57"/>
-      <c r="U2" s="57" t="s">
+      <c r="T2" s="63"/>
+      <c r="U2" s="63" t="s">
         <v>27</v>
       </c>
       <c r="V2" s="64"/>
-      <c r="W2" s="63" t="s">
+      <c r="W2" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="X2" s="57"/>
+      <c r="X2" s="63"/>
     </row>
     <row r="3" spans="2:27" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B3" s="32" t="s">
@@ -6930,34 +6930,34 @@
       </c>
     </row>
     <row r="29" spans="2:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="F29" s="60" t="s">
+      <c r="F29" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="G29" s="61"/>
-      <c r="H29" s="62"/>
-      <c r="I29" s="58">
+      <c r="G29" s="60"/>
+      <c r="H29" s="61"/>
+      <c r="I29" s="57">
         <f>C27+E27+G27+I27+K27+M27+O27+Q27+S27+U27</f>
         <v>1788.24</v>
       </c>
-      <c r="J29" s="59"/>
+      <c r="J29" s="58"/>
     </row>
     <row r="30" spans="2:27" x14ac:dyDescent="0.55000000000000004">
       <c r="G30" s="65" t="s">
         <v>57</v>
       </c>
       <c r="H30" s="65"/>
-      <c r="I30" s="58">
+      <c r="I30" s="57">
         <f>+D27+F27+H27+J27+L27+N27+P27+R27+T27+V27</f>
         <v>2492.1999999999998</v>
       </c>
-      <c r="J30" s="59"/>
+      <c r="J30" s="58"/>
     </row>
     <row r="31" spans="2:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="I31" s="58">
+      <c r="I31" s="57">
         <f>I30-I29</f>
         <v>703.95999999999981</v>
       </c>
-      <c r="J31" s="59"/>
+      <c r="J31" s="58"/>
     </row>
     <row r="32" spans="2:27" x14ac:dyDescent="0.55000000000000004">
       <c r="C32" s="36">
@@ -7011,11 +7011,11 @@
         <v>64</v>
       </c>
       <c r="H34" s="42"/>
-      <c r="I34" s="66">
+      <c r="I34" s="67">
         <f>I33+I31</f>
         <v>1303.9599999999998</v>
       </c>
-      <c r="J34" s="66"/>
+      <c r="J34" s="67"/>
       <c r="M34" s="33"/>
     </row>
     <row r="38" spans="3:16" x14ac:dyDescent="0.55000000000000004">
@@ -7060,11 +7060,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="O2:P2"/>
     <mergeCell ref="Q2:R2"/>
     <mergeCell ref="S2:T2"/>
     <mergeCell ref="U2:V2"/>
@@ -7072,11 +7072,11 @@
     <mergeCell ref="F29:H29"/>
     <mergeCell ref="I29:J29"/>
     <mergeCell ref="M2:N2"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7110,54 +7110,54 @@
   <sheetData>
     <row r="1" spans="2:34" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="2" spans="2:34" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57" t="s">
+      <c r="D2" s="63"/>
+      <c r="E2" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57" t="s">
+      <c r="F2" s="63"/>
+      <c r="G2" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57" t="s">
+      <c r="H2" s="63"/>
+      <c r="I2" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57" t="s">
+      <c r="J2" s="63"/>
+      <c r="K2" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="57"/>
-      <c r="M2" s="57" t="s">
+      <c r="L2" s="63"/>
+      <c r="M2" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="N2" s="57"/>
-      <c r="O2" s="57" t="s">
+      <c r="N2" s="63"/>
+      <c r="O2" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="57"/>
-      <c r="Q2" s="57" t="s">
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="R2" s="57"/>
-      <c r="S2" s="57" t="s">
+      <c r="R2" s="63"/>
+      <c r="S2" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="T2" s="57"/>
-      <c r="U2" s="57" t="s">
+      <c r="T2" s="63"/>
+      <c r="U2" s="63" t="s">
         <v>65</v>
       </c>
       <c r="V2" s="64"/>
-      <c r="W2" s="57" t="s">
+      <c r="W2" s="63" t="s">
         <v>66</v>
       </c>
       <c r="X2" s="64"/>
-      <c r="Y2" s="63" t="s">
+      <c r="Y2" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="Z2" s="57"/>
+      <c r="Z2" s="63"/>
     </row>
     <row r="3" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B3" s="32" t="s">
@@ -9211,34 +9211,34 @@
       </c>
     </row>
     <row r="31" spans="2:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="F31" s="60" t="s">
+      <c r="F31" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="G31" s="61"/>
-      <c r="H31" s="62"/>
-      <c r="I31" s="58">
+      <c r="G31" s="60"/>
+      <c r="H31" s="61"/>
+      <c r="I31" s="57">
         <f>C29+E29+G29+I29+K29+M29+O29+Q29+S29+U29+W29</f>
         <v>2521.33</v>
       </c>
-      <c r="J31" s="59"/>
+      <c r="J31" s="58"/>
     </row>
     <row r="32" spans="2:30" x14ac:dyDescent="0.55000000000000004">
       <c r="G32" s="65" t="s">
         <v>57</v>
       </c>
       <c r="H32" s="65"/>
-      <c r="I32" s="58">
+      <c r="I32" s="57">
         <f>+D29+F29+H29+J29+L29+N29+P29+R29+T29+V29+X29</f>
         <v>2997.5899999999997</v>
       </c>
-      <c r="J32" s="59"/>
+      <c r="J32" s="58"/>
     </row>
     <row r="33" spans="3:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="I33" s="58">
+      <c r="I33" s="57">
         <f>I32-I31</f>
         <v>476.25999999999976</v>
       </c>
-      <c r="J33" s="59"/>
+      <c r="J33" s="58"/>
     </row>
     <row r="34" spans="3:17" x14ac:dyDescent="0.55000000000000004">
       <c r="C34" s="36">
@@ -9291,11 +9291,11 @@
         <v>64</v>
       </c>
       <c r="H36" s="42"/>
-      <c r="I36" s="66">
+      <c r="I36" s="67">
         <f>I35+I33</f>
         <v>2476.2599999999998</v>
       </c>
-      <c r="J36" s="66"/>
+      <c r="J36" s="67"/>
       <c r="M36" s="33"/>
     </row>
     <row r="40" spans="3:17" x14ac:dyDescent="0.55000000000000004">
@@ -9340,11 +9340,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="O2:P2"/>
     <mergeCell ref="Q2:R2"/>
     <mergeCell ref="S2:T2"/>
     <mergeCell ref="U2:V2"/>
@@ -9353,11 +9353,11 @@
     <mergeCell ref="I31:J31"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="W2:X2"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="54" orientation="landscape" r:id="rId1"/>
@@ -9391,54 +9391,54 @@
   <sheetData>
     <row r="1" spans="2:34" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="2" spans="2:34" ht="18.3" x14ac:dyDescent="0.7">
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="57"/>
-      <c r="E2" s="67" t="s">
+      <c r="D2" s="63"/>
+      <c r="E2" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="63"/>
-      <c r="G2" s="57" t="s">
+      <c r="F2" s="62"/>
+      <c r="G2" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57" t="s">
+      <c r="H2" s="63"/>
+      <c r="I2" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57" t="s">
+      <c r="J2" s="63"/>
+      <c r="K2" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="57"/>
-      <c r="M2" s="67" t="s">
+      <c r="L2" s="63"/>
+      <c r="M2" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="63"/>
-      <c r="O2" s="57" t="s">
+      <c r="N2" s="62"/>
+      <c r="O2" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="P2" s="57"/>
-      <c r="Q2" s="57" t="s">
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="R2" s="57"/>
-      <c r="S2" s="57" t="s">
+      <c r="R2" s="63"/>
+      <c r="S2" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="T2" s="57"/>
-      <c r="U2" s="57" t="s">
+      <c r="T2" s="63"/>
+      <c r="U2" s="63" t="s">
         <v>65</v>
       </c>
       <c r="V2" s="64"/>
-      <c r="W2" s="57" t="s">
+      <c r="W2" s="63" t="s">
         <v>66</v>
       </c>
       <c r="X2" s="64"/>
-      <c r="Y2" s="63" t="s">
+      <c r="Y2" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="Z2" s="57"/>
+      <c r="Z2" s="63"/>
     </row>
     <row r="3" spans="2:34" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="32" t="s">
@@ -11447,34 +11447,34 @@
       </c>
     </row>
     <row r="31" spans="2:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="F31" s="60" t="s">
+      <c r="F31" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="G31" s="61"/>
-      <c r="H31" s="62"/>
-      <c r="I31" s="58">
+      <c r="G31" s="60"/>
+      <c r="H31" s="61"/>
+      <c r="I31" s="57">
         <f>C29+E29+G29+I29+K29+M29+O29+Q29+S29+U29+W29</f>
         <v>2462.73</v>
       </c>
-      <c r="J31" s="59"/>
+      <c r="J31" s="58"/>
     </row>
     <row r="32" spans="2:30" x14ac:dyDescent="0.55000000000000004">
       <c r="G32" s="65" t="s">
         <v>57</v>
       </c>
       <c r="H32" s="65"/>
-      <c r="I32" s="58">
+      <c r="I32" s="57">
         <f>+D29+F29+H29+J29+L29+N29+P29+R29+T29+V29+X29</f>
         <v>1004.25</v>
       </c>
-      <c r="J32" s="59"/>
+      <c r="J32" s="58"/>
     </row>
     <row r="33" spans="3:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="I33" s="58">
+      <c r="I33" s="57">
         <f>I32-I31</f>
         <v>-1458.48</v>
       </c>
-      <c r="J33" s="59"/>
+      <c r="J33" s="58"/>
       <c r="Y33">
         <f>2167+183+5*10</f>
         <v>2400</v>
@@ -11570,11 +11570,11 @@
         <v>64</v>
       </c>
       <c r="H38" s="42"/>
-      <c r="I38" s="66">
+      <c r="I38" s="67">
         <f>I36+I33+J37</f>
         <v>322.7800000000002</v>
       </c>
-      <c r="J38" s="66"/>
+      <c r="J38" s="67"/>
       <c r="M38" s="33"/>
     </row>
     <row r="40" spans="3:25" x14ac:dyDescent="0.55000000000000004">
@@ -11846,16 +11846,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="U2:V2"/>
     <mergeCell ref="W2:X2"/>
     <mergeCell ref="Y2:Z2"/>
     <mergeCell ref="C2:D2"/>
@@ -11864,6 +11854,16 @@
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="M2:N2"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="I33:J33"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="54" orientation="landscape" r:id="rId1"/>
@@ -11878,7 +11878,7 @@
   <dimension ref="B1:AH58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="Q48" sqref="Q48"/>
+      <selection activeCell="M55" sqref="M55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -11901,54 +11901,54 @@
   <sheetData>
     <row r="1" spans="2:34" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="2" spans="2:34" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="63" t="s">
         <v>100</v>
       </c>
-      <c r="D2" s="57"/>
-      <c r="E2" s="67" t="s">
+      <c r="D2" s="63"/>
+      <c r="E2" s="66" t="s">
         <v>101</v>
       </c>
-      <c r="F2" s="63"/>
-      <c r="G2" s="57" t="s">
+      <c r="F2" s="62"/>
+      <c r="G2" s="63" t="s">
         <v>102</v>
       </c>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57" t="s">
+      <c r="H2" s="63"/>
+      <c r="I2" s="63" t="s">
         <v>103</v>
       </c>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57" t="s">
+      <c r="J2" s="63"/>
+      <c r="K2" s="63" t="s">
         <v>104</v>
       </c>
-      <c r="L2" s="57"/>
-      <c r="M2" s="67" t="s">
+      <c r="L2" s="63"/>
+      <c r="M2" s="66" t="s">
         <v>105</v>
       </c>
-      <c r="N2" s="63"/>
-      <c r="O2" s="57" t="s">
+      <c r="N2" s="62"/>
+      <c r="O2" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="P2" s="57"/>
-      <c r="Q2" s="57" t="s">
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63" t="s">
         <v>107</v>
       </c>
-      <c r="R2" s="57"/>
-      <c r="S2" s="57" t="s">
+      <c r="R2" s="63"/>
+      <c r="S2" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="T2" s="57"/>
-      <c r="U2" s="57" t="s">
+      <c r="T2" s="63"/>
+      <c r="U2" s="63" t="s">
         <v>108</v>
       </c>
       <c r="V2" s="64"/>
-      <c r="W2" s="57" t="s">
+      <c r="W2" s="63" t="s">
         <v>66</v>
       </c>
       <c r="X2" s="64"/>
-      <c r="Y2" s="63" t="s">
+      <c r="Y2" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="Z2" s="57"/>
+      <c r="Z2" s="63"/>
     </row>
     <row r="3" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B3" s="32" t="s">
@@ -13806,34 +13806,34 @@
       </c>
     </row>
     <row r="31" spans="2:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="F31" s="60" t="s">
+      <c r="F31" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="G31" s="61"/>
-      <c r="H31" s="62"/>
-      <c r="I31" s="58">
+      <c r="G31" s="60"/>
+      <c r="H31" s="61"/>
+      <c r="I31" s="57">
         <f>C29+E29+G29+I29+K29+M29+O29+Q29+S29+U29+W29</f>
         <v>1428</v>
       </c>
-      <c r="J31" s="59"/>
+      <c r="J31" s="58"/>
     </row>
     <row r="32" spans="2:30" x14ac:dyDescent="0.55000000000000004">
       <c r="G32" s="65" t="s">
         <v>57</v>
       </c>
       <c r="H32" s="65"/>
-      <c r="I32" s="58">
+      <c r="I32" s="57">
         <f>+D29+F29+H29+J29+L29+N29+P29+R29+T29+V29+X29</f>
         <v>572.5</v>
       </c>
-      <c r="J32" s="59"/>
+      <c r="J32" s="58"/>
     </row>
     <row r="33" spans="3:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="I33" s="58">
+      <c r="I33" s="57">
         <f>I32-I31</f>
         <v>-855.5</v>
       </c>
-      <c r="J33" s="59"/>
+      <c r="J33" s="58"/>
       <c r="Y33">
         <f>2167+183+5*10</f>
         <v>2400</v>
@@ -13922,11 +13922,11 @@
         <v>64</v>
       </c>
       <c r="H38" s="42"/>
-      <c r="I38" s="66">
+      <c r="I38" s="67">
         <f>I36+I33</f>
         <v>1146.0899999999999</v>
       </c>
-      <c r="J38" s="66"/>
+      <c r="J38" s="67"/>
       <c r="M38" s="33"/>
     </row>
     <row r="40" spans="3:25" x14ac:dyDescent="0.55000000000000004">
@@ -14170,7 +14170,7 @@
         <v>89</v>
       </c>
       <c r="K55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V55" t="s">
         <v>94</v>
@@ -14224,16 +14224,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="U2:V2"/>
     <mergeCell ref="W2:X2"/>
     <mergeCell ref="Y2:Z2"/>
     <mergeCell ref="C2:D2"/>
@@ -14242,6 +14232,16 @@
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="M2:N2"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="I33:J33"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="54" orientation="landscape" r:id="rId1"/>
@@ -14257,15 +14257,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002D8393059904904F9DB82DE4B9AFABF6" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f7bafc8adbaca2e93ffc3a1da3fd32d5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3e1ffae5-f160-4019-9720-1b11bf1b81a3" xmlns:ns4="21753bd8-bffc-4cd2-a328-982ee854c895" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f821f56a5d2247de677e71e73e5a99e" ns3:_="" ns4:_="">
     <xsd:import namespace="3e1ffae5-f160-4019-9720-1b11bf1b81a3"/>
@@ -14486,6 +14477,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4D7A62A-0CB5-48B0-A73A-0A91BCC8EAEF}">
   <ds:schemaRefs>
@@ -14497,14 +14497,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{948817D4-7F3F-493D-9D4C-B473DA03CC7E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22BA772B-ABF0-4278-9CEF-D9160BBA9E07}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14523,6 +14515,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{948817D4-7F3F-493D-9D4C-B473DA03CC7E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{0f7d30c2-cad0-4405-8153-25a6a3313da4}" enabled="1" method="Privileged" siteId="{6c637512-c417-4e78-9d62-b61258e4b619}" removed="0"/>

</xml_diff>

<commit_message>
updating data & Club History
</commit_message>
<xml_diff>
--- a/public/Data/HEMANPUNTERS.xlsx
+++ b/public/Data/HEMANPUNTERS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bturnor\source\repos\PersonalWork\seeMore\public\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF6E930-B422-4A45-92FE-701588BBFF19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5AED2F23-E1C7-409A-8524-9EE0DF085B3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="45" windowWidth="29040" windowHeight="15720" firstSheet="5" activeTab="5" xr2:uid="{525E8989-1938-4309-A4CF-8F1D15E362FB}"/>
+    <workbookView xWindow="2928" yWindow="2928" windowWidth="17280" windowHeight="9984" firstSheet="5" activeTab="5" xr2:uid="{525E8989-1938-4309-A4CF-8F1D15E362FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Punters club" sheetId="1" r:id="rId1"/>
@@ -395,10 +395,10 @@
     <t>OR</t>
   </si>
   <si>
-    <t>1 leg losses @ 1st July 2024</t>
+    <t>1 leg losses @ 15th July 2024</t>
   </si>
   <si>
-    <t>Strikes for 2024 Season at 25th June 2024</t>
+    <t>Strikes for 2024 Season at 15th July 2024</t>
   </si>
   <si>
     <t>Strikes</t>
@@ -11877,8 +11877,8 @@
   </sheetPr>
   <dimension ref="B1:AH58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="M55" sqref="M55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U21" sqref="U21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -12395,7 +12395,7 @@
       </c>
       <c r="AE8" s="44">
         <f>+E29+'Punters 2021'!I27+'Punters 2020'!G27+'Punters club'!J7+'Punters 2022'!E29</f>
-        <v>1058</v>
+        <v>1083</v>
       </c>
       <c r="AF8" s="44">
         <f>+F29+'Punters 2021'!J27+'Punters 2020'!H27+'Punters club'!K7+'Punters 2022'!F29</f>
@@ -12403,11 +12403,11 @@
       </c>
       <c r="AG8" s="50">
         <f t="shared" ref="AG8:AG16" si="3">+AF8-AE8</f>
-        <v>-38.230000000000018</v>
+        <v>-63.230000000000018</v>
       </c>
       <c r="AH8" s="47">
         <f t="shared" ref="AH8:AH16" si="4">(AF8-AE8)/AE8</f>
-        <v>-3.6134215500945199E-2</v>
+        <v>-5.8384118190212393E-2</v>
       </c>
     </row>
     <row r="9" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -12477,7 +12477,7 @@
       </c>
       <c r="AE9" s="44">
         <f>+I29+'Punters 2021'!K27+'Punters 2020'!E27+'Punters club'!J11+'Punters 2022'!G29</f>
-        <v>1026.48</v>
+        <v>1051.48</v>
       </c>
       <c r="AF9" s="44">
         <f>+J29+'Punters 2021'!L27+'Punters 2020'!F27+'Punters club'!K11+'Punters 2022'!H29</f>
@@ -12485,11 +12485,11 @@
       </c>
       <c r="AG9" s="50">
         <f t="shared" si="3"/>
-        <v>-65.080000000000041</v>
+        <v>-90.080000000000041</v>
       </c>
       <c r="AH9" s="47">
         <f t="shared" si="4"/>
-        <v>-6.3401137869223009E-2</v>
+        <v>-8.5669722676608245E-2</v>
       </c>
     </row>
     <row r="10" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -12633,7 +12633,7 @@
       </c>
       <c r="AE11" s="44">
         <f>+M29+'Punters 2021'!E27+'Punters 2020'!K27+'Punters 2022'!K29</f>
-        <v>783</v>
+        <v>808</v>
       </c>
       <c r="AF11" s="44">
         <f>+N29+'Punters 2021'!F27+'Punters 2020'!L27+'Punters 2022'!L29</f>
@@ -12641,11 +12641,11 @@
       </c>
       <c r="AG11" s="49">
         <f t="shared" si="3"/>
-        <v>-592.25</v>
+        <v>-617.25</v>
       </c>
       <c r="AH11" s="47">
         <f t="shared" si="4"/>
-        <v>-0.75638569604086847</v>
+        <v>-0.76392326732673266</v>
       </c>
     </row>
     <row r="12" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -12715,7 +12715,7 @@
       </c>
       <c r="AE12" s="44">
         <f>+C29+'Punters 2021'!S27+'Punters 2020'!S27+'Punters club'!J8+'Punters 2022'!M29</f>
-        <v>1104.96</v>
+        <v>1129.96</v>
       </c>
       <c r="AF12" s="44">
         <f>+D29+'Punters 2021'!T27+'Punters 2020'!T27+'Punters club'!K8+'Punters 2022'!N29</f>
@@ -12723,11 +12723,11 @@
       </c>
       <c r="AG12" s="49">
         <f t="shared" si="3"/>
-        <v>-540.63000000000011</v>
+        <v>-565.63000000000011</v>
       </c>
       <c r="AH12" s="47">
         <f t="shared" si="4"/>
-        <v>-0.48927562988705481</v>
+        <v>-0.50057524160147271</v>
       </c>
     </row>
     <row r="13" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -12872,7 +12872,7 @@
       </c>
       <c r="AE14" s="44">
         <f>+O29+'Punters 2021'!M27+'Punters 2020'!Q27+'Punters club'!J5+'Punters 2022'!Q29</f>
-        <v>1038</v>
+        <v>1063</v>
       </c>
       <c r="AF14" s="44">
         <f>+P29+'Punters 2021'!N27+'Punters 2020'!R27+'Punters club'!K5+'Punters 2022'!R29</f>
@@ -12880,11 +12880,11 @@
       </c>
       <c r="AG14" s="49">
         <f t="shared" si="3"/>
-        <v>-165.52999999999986</v>
+        <v>-190.52999999999986</v>
       </c>
       <c r="AH14" s="47">
         <f t="shared" si="4"/>
-        <v>-0.15947013487475903</v>
+        <v>-0.17923800564440251</v>
       </c>
     </row>
     <row r="15" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -12954,19 +12954,19 @@
       </c>
       <c r="AE15" s="44">
         <f>+K29+'Punters 2021'!C27+'Punters 2020'!C27+'Punters club'!J4+'Punters 2022'!S29</f>
-        <v>1042.7</v>
+        <v>1067.7</v>
       </c>
       <c r="AF15" s="44">
         <f>+L29+'Punters 2021'!D27+'Punters 2020'!D27+'Punters club'!K4+'Punters 2022'!T29</f>
-        <v>1514.84</v>
+        <v>1579.84</v>
       </c>
       <c r="AG15" s="50">
         <f t="shared" si="3"/>
-        <v>472.13999999999987</v>
+        <v>512.13999999999987</v>
       </c>
       <c r="AH15" s="45">
         <f t="shared" si="4"/>
-        <v>0.45280521722451317</v>
+        <v>0.47966657300739896</v>
       </c>
     </row>
     <row r="16" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -13032,7 +13032,7 @@
       </c>
       <c r="AE16" s="44">
         <f>+U29+'Punters 2022'!U29</f>
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="AF16" s="44">
         <f>+V29+'Punters 2022'!V29</f>
@@ -13040,11 +13040,11 @@
       </c>
       <c r="AG16" s="49">
         <f t="shared" si="3"/>
-        <v>-177.5</v>
+        <v>-182.5</v>
       </c>
       <c r="AH16" s="47">
         <f t="shared" si="4"/>
-        <v>-0.57258064516129037</v>
+        <v>-0.57936507936507942</v>
       </c>
     </row>
     <row r="17" spans="2:30" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -13266,7 +13266,7 @@
         <v>0</v>
       </c>
       <c r="U20" s="15">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="V20" s="20">
         <v>46.25</v>
@@ -13275,7 +13275,7 @@
       <c r="X20" s="20"/>
       <c r="Y20" s="17">
         <f t="shared" si="0"/>
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="Z20" s="35">
         <f t="shared" si="0"/>
@@ -13283,7 +13283,7 @@
       </c>
       <c r="AA20" s="1">
         <f t="shared" si="2"/>
-        <v>1428</v>
+        <v>1433</v>
       </c>
       <c r="AB20" s="1">
         <f t="shared" si="2"/>
@@ -13291,7 +13291,7 @@
       </c>
       <c r="AC20" s="1">
         <f t="shared" si="1"/>
-        <v>-855.5</v>
+        <v>-860.5</v>
       </c>
       <c r="AD20" s="1"/>
     </row>
@@ -13299,14 +13299,26 @@
       <c r="B21" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="16"/>
+      <c r="C21" s="15">
+        <v>25</v>
+      </c>
+      <c r="D21" s="16">
+        <v>0</v>
+      </c>
+      <c r="E21" s="17">
+        <v>25</v>
+      </c>
+      <c r="F21" s="16">
+        <v>0</v>
+      </c>
       <c r="G21" s="17"/>
       <c r="H21" s="16"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="16"/>
+      <c r="I21" s="17">
+        <v>25</v>
+      </c>
+      <c r="J21" s="16">
+        <v>0</v>
+      </c>
       <c r="K21" s="17"/>
       <c r="L21" s="16"/>
       <c r="M21" s="17"/>
@@ -13323,7 +13335,7 @@
       <c r="X21" s="20"/>
       <c r="Y21" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="Z21" s="35">
         <f t="shared" si="0"/>
@@ -13331,7 +13343,7 @@
       </c>
       <c r="AA21" s="1">
         <f t="shared" si="2"/>
-        <v>1428</v>
+        <v>1508</v>
       </c>
       <c r="AB21" s="1">
         <f t="shared" si="2"/>
@@ -13339,7 +13351,7 @@
       </c>
       <c r="AC21" s="1">
         <f t="shared" si="1"/>
-        <v>-855.5</v>
+        <v>-935.5</v>
       </c>
       <c r="AD21" s="1"/>
     </row>
@@ -13355,12 +13367,24 @@
       <c r="H22" s="16"/>
       <c r="I22" s="17"/>
       <c r="J22" s="16"/>
-      <c r="K22" s="17"/>
-      <c r="L22" s="16"/>
-      <c r="M22" s="17"/>
-      <c r="N22" s="16"/>
-      <c r="O22" s="17"/>
-      <c r="P22" s="16"/>
+      <c r="K22" s="17">
+        <v>25</v>
+      </c>
+      <c r="L22" s="16">
+        <v>65</v>
+      </c>
+      <c r="M22" s="17">
+        <v>25</v>
+      </c>
+      <c r="N22" s="16">
+        <v>0</v>
+      </c>
+      <c r="O22" s="17">
+        <v>25</v>
+      </c>
+      <c r="P22" s="16">
+        <v>0</v>
+      </c>
       <c r="Q22" s="17"/>
       <c r="R22" s="16"/>
       <c r="S22" s="17"/>
@@ -13371,23 +13395,23 @@
       <c r="X22" s="20"/>
       <c r="Y22" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="Z22" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="AA22" s="1">
         <f t="shared" ref="AA22:AB26" si="5">AA21+Y22</f>
-        <v>1428</v>
+        <v>1583</v>
       </c>
       <c r="AB22" s="1">
         <f t="shared" si="5"/>
-        <v>572.5</v>
+        <v>637.5</v>
       </c>
       <c r="AC22" s="1">
         <f t="shared" si="1"/>
-        <v>-855.5</v>
+        <v>-945.5</v>
       </c>
       <c r="AD22" s="1"/>
     </row>
@@ -13427,15 +13451,15 @@
       </c>
       <c r="AA23" s="1">
         <f t="shared" si="5"/>
-        <v>1428</v>
+        <v>1583</v>
       </c>
       <c r="AB23" s="1">
         <f t="shared" si="5"/>
-        <v>572.5</v>
+        <v>637.5</v>
       </c>
       <c r="AC23" s="1">
         <f t="shared" si="1"/>
-        <v>-855.5</v>
+        <v>-945.5</v>
       </c>
       <c r="AD23" s="1"/>
     </row>
@@ -13475,15 +13499,15 @@
       </c>
       <c r="AA24" s="1">
         <f t="shared" si="5"/>
-        <v>1428</v>
+        <v>1583</v>
       </c>
       <c r="AB24" s="1">
         <f t="shared" si="5"/>
-        <v>572.5</v>
+        <v>637.5</v>
       </c>
       <c r="AC24" s="1">
         <f t="shared" si="1"/>
-        <v>-855.5</v>
+        <v>-945.5</v>
       </c>
       <c r="AD24" s="1"/>
     </row>
@@ -13523,15 +13547,15 @@
       </c>
       <c r="AA25" s="1">
         <f t="shared" si="5"/>
-        <v>1428</v>
+        <v>1583</v>
       </c>
       <c r="AB25" s="1">
         <f t="shared" si="5"/>
-        <v>572.5</v>
+        <v>637.5</v>
       </c>
       <c r="AC25" s="1">
         <f t="shared" si="1"/>
-        <v>-855.5</v>
+        <v>-945.5</v>
       </c>
       <c r="AD25" s="1"/>
     </row>
@@ -13571,15 +13595,15 @@
       </c>
       <c r="AA26" s="1">
         <f t="shared" si="5"/>
-        <v>1428</v>
+        <v>1583</v>
       </c>
       <c r="AB26" s="1">
         <f t="shared" si="5"/>
-        <v>572.5</v>
+        <v>637.5</v>
       </c>
       <c r="AC26" s="1">
         <f t="shared" si="1"/>
-        <v>-855.5</v>
+        <v>-945.5</v>
       </c>
       <c r="AD26" s="1"/>
     </row>
@@ -13667,7 +13691,7 @@
       </c>
       <c r="C29" s="18">
         <f t="shared" ref="C29:Z29" si="7">SUM(C4:C28)</f>
-        <v>150</v>
+        <v>175</v>
       </c>
       <c r="D29" s="18">
         <f t="shared" si="7"/>
@@ -13675,7 +13699,7 @@
       </c>
       <c r="E29" s="18">
         <f t="shared" si="7"/>
-        <v>135</v>
+        <v>160</v>
       </c>
       <c r="F29" s="18">
         <f t="shared" si="7"/>
@@ -13691,7 +13715,7 @@
       </c>
       <c r="I29" s="18">
         <f t="shared" si="7"/>
-        <v>130</v>
+        <v>155</v>
       </c>
       <c r="J29" s="18">
         <f t="shared" si="7"/>
@@ -13699,15 +13723,15 @@
       </c>
       <c r="K29" s="18">
         <f t="shared" si="7"/>
-        <v>150</v>
+        <v>175</v>
       </c>
       <c r="L29" s="18">
         <f t="shared" si="7"/>
-        <v>53.75</v>
+        <v>118.75</v>
       </c>
       <c r="M29" s="18">
         <f t="shared" si="7"/>
-        <v>150</v>
+        <v>175</v>
       </c>
       <c r="N29" s="18">
         <f t="shared" si="7"/>
@@ -13715,7 +13739,7 @@
       </c>
       <c r="O29" s="18">
         <f t="shared" si="7"/>
-        <v>155</v>
+        <v>180</v>
       </c>
       <c r="P29" s="18">
         <f t="shared" si="7"/>
@@ -13739,7 +13763,7 @@
       </c>
       <c r="U29" s="18">
         <f t="shared" si="7"/>
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="V29" s="21">
         <f t="shared" si="7"/>
@@ -13755,11 +13779,11 @@
       </c>
       <c r="Y29" s="29">
         <f t="shared" si="7"/>
-        <v>1428</v>
+        <v>1583</v>
       </c>
       <c r="Z29" s="18">
         <f t="shared" si="7"/>
-        <v>572.5</v>
+        <v>637.5</v>
       </c>
       <c r="AA29" s="1"/>
     </row>
@@ -13782,15 +13806,15 @@
       </c>
       <c r="L30" s="28">
         <f>(L29-K29)/K29</f>
-        <v>-0.64166666666666672</v>
+        <v>-0.32142857142857145</v>
       </c>
       <c r="N30" s="28">
         <f>(N29-M29)/M29</f>
-        <v>-0.11666666666666667</v>
+        <v>-0.24285714285714285</v>
       </c>
       <c r="P30" s="28">
         <f>(P29-O29)/O29</f>
-        <v>0.5161290322580645</v>
+        <v>0.30555555555555558</v>
       </c>
       <c r="R30" s="28">
         <f>(R29-Q29)/Q29</f>
@@ -13802,7 +13826,7 @@
       </c>
       <c r="V30" s="28">
         <f>(V29-U29)/U29</f>
-        <v>-0.57954545454545459</v>
+        <v>-0.59782608695652173</v>
       </c>
     </row>
     <row r="31" spans="2:30" x14ac:dyDescent="0.55000000000000004">
@@ -13813,7 +13837,7 @@
       <c r="H31" s="61"/>
       <c r="I31" s="57">
         <f>C29+E29+G29+I29+K29+M29+O29+Q29+S29+U29+W29</f>
-        <v>1428</v>
+        <v>1583</v>
       </c>
       <c r="J31" s="58"/>
     </row>
@@ -13824,14 +13848,14 @@
       <c r="H32" s="65"/>
       <c r="I32" s="57">
         <f>+D29+F29+H29+J29+L29+N29+P29+R29+T29+V29+X29</f>
-        <v>572.5</v>
+        <v>637.5</v>
       </c>
       <c r="J32" s="58"/>
     </row>
     <row r="33" spans="3:25" x14ac:dyDescent="0.55000000000000004">
       <c r="I33" s="57">
         <f>I32-I31</f>
-        <v>-855.5</v>
+        <v>-945.5</v>
       </c>
       <c r="J33" s="58"/>
       <c r="Y33">
@@ -13842,7 +13866,7 @@
     <row r="34" spans="3:25" x14ac:dyDescent="0.55000000000000004">
       <c r="C34" s="36">
         <f>C29+E29+G29+I29</f>
-        <v>558</v>
+        <v>633</v>
       </c>
       <c r="D34" s="36">
         <f>D29+F29+H29+J29</f>
@@ -13850,23 +13874,23 @@
       </c>
       <c r="E34" s="37">
         <f>D34-C34</f>
-        <v>-558</v>
+        <v>-633</v>
       </c>
       <c r="I34" s="38">
         <f>O29+K29+M29</f>
-        <v>455</v>
+        <v>530</v>
       </c>
       <c r="J34" s="38">
         <f>P29+L29+N29</f>
-        <v>421.25</v>
+        <v>486.25</v>
       </c>
       <c r="K34" s="39">
         <f>J34-I34</f>
-        <v>-33.75</v>
+        <v>-43.75</v>
       </c>
       <c r="O34" s="40">
         <f>U29+Q29+S29</f>
-        <v>415</v>
+        <v>420</v>
       </c>
       <c r="P34" s="40">
         <f>V29+R29+T29</f>
@@ -13874,7 +13898,7 @@
       </c>
       <c r="Q34" s="41">
         <f>P34-O34</f>
-        <v>-263.75</v>
+        <v>-268.75</v>
       </c>
       <c r="X34" s="55"/>
       <c r="Y34">
@@ -13892,13 +13916,13 @@
       <c r="I35" s="38"/>
       <c r="J35" s="34">
         <f>(J34-I34)/I34</f>
-        <v>-7.4175824175824176E-2</v>
+        <v>-8.254716981132075E-2</v>
       </c>
       <c r="K35" s="39"/>
       <c r="O35" s="40"/>
       <c r="P35" s="34">
         <f>(P34-O34)/O34</f>
-        <v>-0.63554216867469882</v>
+        <v>-0.63988095238095233</v>
       </c>
       <c r="Q35" s="41"/>
       <c r="X35" s="55"/>
@@ -13924,7 +13948,7 @@
       <c r="H38" s="42"/>
       <c r="I38" s="67">
         <f>I36+I33</f>
-        <v>1146.0899999999999</v>
+        <v>1056.0899999999999</v>
       </c>
       <c r="J38" s="67"/>
       <c r="M38" s="33"/>
@@ -13935,7 +13959,7 @@
     <row r="42" spans="3:25" x14ac:dyDescent="0.55000000000000004">
       <c r="C42" s="1">
         <f>C29+E29+G29+I29</f>
-        <v>558</v>
+        <v>633</v>
       </c>
       <c r="D42" s="1">
         <f>D29+F29+H29+J29</f>
@@ -13943,15 +13967,15 @@
       </c>
       <c r="I42" s="1">
         <f>O29+K29+M29</f>
-        <v>455</v>
+        <v>530</v>
       </c>
       <c r="J42" s="1">
         <f>P29+L29+N29</f>
-        <v>421.25</v>
+        <v>486.25</v>
       </c>
       <c r="O42" s="1">
         <f>U29+Q29+S29</f>
-        <v>415</v>
+        <v>420</v>
       </c>
       <c r="P42" s="1">
         <f>V29+R29+T29</f>
@@ -13961,15 +13985,15 @@
     <row r="43" spans="3:25" x14ac:dyDescent="0.55000000000000004">
       <c r="D43" s="1">
         <f>D42-C42</f>
-        <v>-558</v>
+        <v>-633</v>
       </c>
       <c r="J43" s="33">
         <f>J42-I42</f>
-        <v>-33.75</v>
+        <v>-43.75</v>
       </c>
       <c r="P43" s="33">
         <f>P42-O42</f>
-        <v>-263.75</v>
+        <v>-268.75</v>
       </c>
     </row>
     <row r="45" spans="3:25" x14ac:dyDescent="0.55000000000000004">
@@ -14008,7 +14032,7 @@
         <v>12</v>
       </c>
       <c r="W47">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="48" spans="3:25" x14ac:dyDescent="0.55000000000000004">
@@ -14038,7 +14062,7 @@
       </c>
       <c r="E49" s="1">
         <f>SUM(L29)</f>
-        <v>53.75</v>
+        <v>118.75</v>
       </c>
       <c r="J49" t="s">
         <v>12</v>
@@ -14086,7 +14110,7 @@
         <v>95</v>
       </c>
       <c r="K51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V51" t="s">
         <v>11</v>
@@ -14195,7 +14219,7 @@
       </c>
       <c r="W56">
         <f>SUM(W46:W55)</f>
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="57" spans="4:23" x14ac:dyDescent="0.55000000000000004">
@@ -14219,7 +14243,7 @@
       </c>
       <c r="E58" s="1">
         <f>SUM(E48:E57)</f>
-        <v>572.5</v>
+        <v>637.5</v>
       </c>
     </row>
   </sheetData>
@@ -14249,14 +14273,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="3e1ffae5-f160-4019-9720-1b11bf1b81a3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002D8393059904904F9DB82DE4B9AFABF6" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f7bafc8adbaca2e93ffc3a1da3fd32d5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3e1ffae5-f160-4019-9720-1b11bf1b81a3" xmlns:ns4="21753bd8-bffc-4cd2-a328-982ee854c895" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f821f56a5d2247de677e71e73e5a99e" ns3:_="" ns4:_="">
     <xsd:import namespace="3e1ffae5-f160-4019-9720-1b11bf1b81a3"/>
@@ -14477,7 +14493,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -14486,17 +14502,15 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4D7A62A-0CB5-48B0-A73A-0A91BCC8EAEF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3e1ffae5-f160-4019-9720-1b11bf1b81a3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="3e1ffae5-f160-4019-9720-1b11bf1b81a3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22BA772B-ABF0-4278-9CEF-D9160BBA9E07}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14515,10 +14529,20 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{948817D4-7F3F-493D-9D4C-B473DA03CC7E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4D7A62A-0CB5-48B0-A73A-0A91BCC8EAEF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3e1ffae5-f160-4019-9720-1b11bf1b81a3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Adding new members and updates for 2025 season
</commit_message>
<xml_diff>
--- a/public/Data/HEMANPUNTERS.xlsx
+++ b/public/Data/HEMANPUNTERS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bturnor\source\repos\PersonalWork\seeMore\public\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5066772-1531-46B4-94FB-4DB64BE23E16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C081F570-F216-4560-8630-CB48449D33E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" firstSheet="5" activeTab="5" xr2:uid="{525E8989-1938-4309-A4CF-8F1D15E362FB}"/>
+    <workbookView xWindow="57480" yWindow="45" windowWidth="29040" windowHeight="15720" firstSheet="5" activeTab="6" xr2:uid="{525E8989-1938-4309-A4CF-8F1D15E362FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Punters club" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,8 @@
     <sheet name="Punters 2022" sheetId="7" r:id="rId4"/>
     <sheet name="Punters 2023" sheetId="8" r:id="rId5"/>
     <sheet name="Punters 2024" sheetId="9" r:id="rId6"/>
+    <sheet name="Punters 2025" sheetId="10" r:id="rId7"/>
+    <sheet name="1 Leg Losses 2025" sheetId="11" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -63,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="125">
   <si>
     <t>HE_MAN PUNTERS 2019</t>
   </si>
@@ -403,16 +405,52 @@
   <si>
     <t>Strikes</t>
   </si>
+  <si>
+    <t>Strikes for 2025 Season at 28 Jan 2025</t>
+  </si>
+  <si>
+    <t>1 leg losses</t>
+  </si>
+  <si>
+    <t>Punter</t>
+  </si>
+  <si>
+    <t>Bet Amount</t>
+  </si>
+  <si>
+    <t>Potential Winnings</t>
+  </si>
+  <si>
+    <t>C.STARKIE</t>
+  </si>
+  <si>
+    <t>C.PANO</t>
+  </si>
+  <si>
+    <t>D.MILEVSKI</t>
+  </si>
+  <si>
+    <t>cam</t>
+  </si>
+  <si>
+    <t>pano</t>
+  </si>
+  <si>
+    <t>Cam</t>
+  </si>
+  <si>
+    <t>Pano</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="166" formatCode="0.0%"/>
-    <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.0"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.0"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -503,7 +541,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -567,6 +605,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -871,55 +915,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -934,8 +978,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -945,30 +989,30 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -985,13 +1029,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1006,18 +1047,31 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3750,50 +3804,50 @@
   <sheetData>
     <row r="1" spans="2:27" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="2" spans="2:27" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57" t="s">
+      <c r="D2" s="63"/>
+      <c r="E2" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57" t="s">
+      <c r="F2" s="63"/>
+      <c r="G2" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57" t="s">
+      <c r="H2" s="63"/>
+      <c r="I2" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57" t="s">
+      <c r="J2" s="63"/>
+      <c r="K2" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="57"/>
-      <c r="M2" s="57" t="s">
+      <c r="L2" s="63"/>
+      <c r="M2" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="57"/>
-      <c r="O2" s="57" t="s">
+      <c r="N2" s="63"/>
+      <c r="O2" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="57"/>
-      <c r="Q2" s="57" t="s">
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="R2" s="57"/>
-      <c r="S2" s="57" t="s">
+      <c r="R2" s="63"/>
+      <c r="S2" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="T2" s="57"/>
-      <c r="U2" s="57" t="s">
+      <c r="T2" s="63"/>
+      <c r="U2" s="63" t="s">
         <v>27</v>
       </c>
       <c r="V2" s="64"/>
-      <c r="W2" s="63" t="s">
+      <c r="W2" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="X2" s="57"/>
+      <c r="X2" s="63"/>
     </row>
     <row r="3" spans="2:27" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B3" s="32" t="s">
@@ -5354,34 +5408,34 @@
       </c>
     </row>
     <row r="29" spans="2:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="F29" s="60" t="s">
+      <c r="F29" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="G29" s="61"/>
-      <c r="H29" s="62"/>
-      <c r="I29" s="58">
+      <c r="G29" s="60"/>
+      <c r="H29" s="61"/>
+      <c r="I29" s="57">
         <f>C27+E27+G27+I27+K27+M27+O27+Q27+S27+U27</f>
         <v>2469.42</v>
       </c>
-      <c r="J29" s="59"/>
+      <c r="J29" s="58"/>
     </row>
     <row r="30" spans="2:27" x14ac:dyDescent="0.55000000000000004">
       <c r="G30" s="65" t="s">
         <v>57</v>
       </c>
       <c r="H30" s="65"/>
-      <c r="I30" s="58">
+      <c r="I30" s="57">
         <f>+D27+F27+H27+J27+L27+N27+P27+R27+T27+V27</f>
         <v>1774.69</v>
       </c>
-      <c r="J30" s="59"/>
+      <c r="J30" s="58"/>
     </row>
     <row r="31" spans="2:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="I31" s="58">
+      <c r="I31" s="57">
         <f>I30-I29</f>
         <v>-694.73</v>
       </c>
-      <c r="J31" s="59"/>
+      <c r="J31" s="58"/>
     </row>
     <row r="32" spans="2:27" x14ac:dyDescent="0.55000000000000004">
       <c r="C32" s="1">
@@ -5430,11 +5484,11 @@
       </c>
     </row>
     <row r="34" spans="3:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="I34" s="59">
+      <c r="I34" s="58">
         <f>I33+I31</f>
         <v>505.27</v>
       </c>
-      <c r="J34" s="59"/>
+      <c r="J34" s="58"/>
     </row>
     <row r="38" spans="3:16" x14ac:dyDescent="0.55000000000000004">
       <c r="C38" s="1">
@@ -5478,6 +5532,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
     <mergeCell ref="I30:J30"/>
     <mergeCell ref="F29:H29"/>
     <mergeCell ref="I31:J31"/>
@@ -5490,11 +5549,6 @@
     <mergeCell ref="S2:T2"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="I29:J29"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5527,50 +5581,50 @@
   <sheetData>
     <row r="1" spans="2:27" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="2" spans="2:27" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57" t="s">
+      <c r="D2" s="63"/>
+      <c r="E2" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="57"/>
-      <c r="G2" s="67" t="s">
+      <c r="F2" s="63"/>
+      <c r="G2" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="57" t="s">
+      <c r="H2" s="62"/>
+      <c r="I2" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57" t="s">
+      <c r="J2" s="63"/>
+      <c r="K2" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="57"/>
-      <c r="M2" s="57" t="s">
+      <c r="L2" s="63"/>
+      <c r="M2" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="57"/>
-      <c r="O2" s="57" t="s">
+      <c r="N2" s="63"/>
+      <c r="O2" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="57"/>
-      <c r="Q2" s="57" t="s">
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="R2" s="57"/>
-      <c r="S2" s="57" t="s">
+      <c r="R2" s="63"/>
+      <c r="S2" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="T2" s="57"/>
-      <c r="U2" s="57" t="s">
+      <c r="T2" s="63"/>
+      <c r="U2" s="63" t="s">
         <v>27</v>
       </c>
       <c r="V2" s="64"/>
-      <c r="W2" s="63" t="s">
+      <c r="W2" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="X2" s="57"/>
+      <c r="X2" s="63"/>
     </row>
     <row r="3" spans="2:27" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B3" s="32" t="s">
@@ -6930,34 +6984,34 @@
       </c>
     </row>
     <row r="29" spans="2:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="F29" s="60" t="s">
+      <c r="F29" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="G29" s="61"/>
-      <c r="H29" s="62"/>
-      <c r="I29" s="58">
+      <c r="G29" s="60"/>
+      <c r="H29" s="61"/>
+      <c r="I29" s="57">
         <f>C27+E27+G27+I27+K27+M27+O27+Q27+S27+U27</f>
         <v>1788.24</v>
       </c>
-      <c r="J29" s="59"/>
+      <c r="J29" s="58"/>
     </row>
     <row r="30" spans="2:27" x14ac:dyDescent="0.55000000000000004">
       <c r="G30" s="65" t="s">
         <v>57</v>
       </c>
       <c r="H30" s="65"/>
-      <c r="I30" s="58">
+      <c r="I30" s="57">
         <f>+D27+F27+H27+J27+L27+N27+P27+R27+T27+V27</f>
         <v>2492.1999999999998</v>
       </c>
-      <c r="J30" s="59"/>
+      <c r="J30" s="58"/>
     </row>
     <row r="31" spans="2:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="I31" s="58">
+      <c r="I31" s="57">
         <f>I30-I29</f>
         <v>703.95999999999981</v>
       </c>
-      <c r="J31" s="59"/>
+      <c r="J31" s="58"/>
     </row>
     <row r="32" spans="2:27" x14ac:dyDescent="0.55000000000000004">
       <c r="C32" s="36">
@@ -7011,11 +7065,11 @@
         <v>64</v>
       </c>
       <c r="H34" s="42"/>
-      <c r="I34" s="66">
+      <c r="I34" s="67">
         <f>I33+I31</f>
         <v>1303.9599999999998</v>
       </c>
-      <c r="J34" s="66"/>
+      <c r="J34" s="67"/>
       <c r="M34" s="33"/>
     </row>
     <row r="38" spans="3:16" x14ac:dyDescent="0.55000000000000004">
@@ -7060,11 +7114,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="O2:P2"/>
     <mergeCell ref="Q2:R2"/>
     <mergeCell ref="S2:T2"/>
     <mergeCell ref="U2:V2"/>
@@ -7072,11 +7126,11 @@
     <mergeCell ref="F29:H29"/>
     <mergeCell ref="I29:J29"/>
     <mergeCell ref="M2:N2"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7092,7 +7146,7 @@
   <dimension ref="B1:AH41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+      <selection activeCell="AE7" sqref="AE7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -7110,54 +7164,54 @@
   <sheetData>
     <row r="1" spans="2:34" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="2" spans="2:34" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57" t="s">
+      <c r="D2" s="63"/>
+      <c r="E2" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57" t="s">
+      <c r="F2" s="63"/>
+      <c r="G2" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57" t="s">
+      <c r="H2" s="63"/>
+      <c r="I2" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57" t="s">
+      <c r="J2" s="63"/>
+      <c r="K2" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="57"/>
-      <c r="M2" s="57" t="s">
+      <c r="L2" s="63"/>
+      <c r="M2" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="N2" s="57"/>
-      <c r="O2" s="57" t="s">
+      <c r="N2" s="63"/>
+      <c r="O2" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="57"/>
-      <c r="Q2" s="57" t="s">
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="R2" s="57"/>
-      <c r="S2" s="57" t="s">
+      <c r="R2" s="63"/>
+      <c r="S2" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="T2" s="57"/>
-      <c r="U2" s="57" t="s">
+      <c r="T2" s="63"/>
+      <c r="U2" s="63" t="s">
         <v>65</v>
       </c>
       <c r="V2" s="64"/>
-      <c r="W2" s="57" t="s">
+      <c r="W2" s="63" t="s">
         <v>66</v>
       </c>
       <c r="X2" s="64"/>
-      <c r="Y2" s="63" t="s">
+      <c r="Y2" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="Z2" s="57"/>
+      <c r="Z2" s="63"/>
     </row>
     <row r="3" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B3" s="32" t="s">
@@ -9211,34 +9265,34 @@
       </c>
     </row>
     <row r="31" spans="2:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="F31" s="60" t="s">
+      <c r="F31" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="G31" s="61"/>
-      <c r="H31" s="62"/>
-      <c r="I31" s="58">
+      <c r="G31" s="60"/>
+      <c r="H31" s="61"/>
+      <c r="I31" s="57">
         <f>C29+E29+G29+I29+K29+M29+O29+Q29+S29+U29+W29</f>
         <v>2521.33</v>
       </c>
-      <c r="J31" s="59"/>
+      <c r="J31" s="58"/>
     </row>
     <row r="32" spans="2:30" x14ac:dyDescent="0.55000000000000004">
       <c r="G32" s="65" t="s">
         <v>57</v>
       </c>
       <c r="H32" s="65"/>
-      <c r="I32" s="58">
+      <c r="I32" s="57">
         <f>+D29+F29+H29+J29+L29+N29+P29+R29+T29+V29+X29</f>
         <v>2997.5899999999997</v>
       </c>
-      <c r="J32" s="59"/>
+      <c r="J32" s="58"/>
     </row>
     <row r="33" spans="3:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="I33" s="58">
+      <c r="I33" s="57">
         <f>I32-I31</f>
         <v>476.25999999999976</v>
       </c>
-      <c r="J33" s="59"/>
+      <c r="J33" s="58"/>
     </row>
     <row r="34" spans="3:17" x14ac:dyDescent="0.55000000000000004">
       <c r="C34" s="36">
@@ -9291,11 +9345,11 @@
         <v>64</v>
       </c>
       <c r="H36" s="42"/>
-      <c r="I36" s="66">
+      <c r="I36" s="67">
         <f>I35+I33</f>
         <v>2476.2599999999998</v>
       </c>
-      <c r="J36" s="66"/>
+      <c r="J36" s="67"/>
       <c r="M36" s="33"/>
     </row>
     <row r="40" spans="3:17" x14ac:dyDescent="0.55000000000000004">
@@ -9340,11 +9394,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="O2:P2"/>
     <mergeCell ref="Q2:R2"/>
     <mergeCell ref="S2:T2"/>
     <mergeCell ref="U2:V2"/>
@@ -9353,11 +9407,11 @@
     <mergeCell ref="I31:J31"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="W2:X2"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="54" orientation="landscape" r:id="rId1"/>
@@ -9372,7 +9426,7 @@
   <dimension ref="B1:AH58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+      <selection activeCell="AE16" sqref="AE16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -9391,54 +9445,54 @@
   <sheetData>
     <row r="1" spans="2:34" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="2" spans="2:34" ht="18.3" x14ac:dyDescent="0.7">
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="57"/>
-      <c r="E2" s="67" t="s">
+      <c r="D2" s="63"/>
+      <c r="E2" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="63"/>
-      <c r="G2" s="57" t="s">
+      <c r="F2" s="62"/>
+      <c r="G2" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57" t="s">
+      <c r="H2" s="63"/>
+      <c r="I2" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57" t="s">
+      <c r="J2" s="63"/>
+      <c r="K2" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="57"/>
-      <c r="M2" s="67" t="s">
+      <c r="L2" s="63"/>
+      <c r="M2" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="63"/>
-      <c r="O2" s="57" t="s">
+      <c r="N2" s="62"/>
+      <c r="O2" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="P2" s="57"/>
-      <c r="Q2" s="57" t="s">
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="R2" s="57"/>
-      <c r="S2" s="57" t="s">
+      <c r="R2" s="63"/>
+      <c r="S2" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="T2" s="57"/>
-      <c r="U2" s="57" t="s">
+      <c r="T2" s="63"/>
+      <c r="U2" s="63" t="s">
         <v>65</v>
       </c>
       <c r="V2" s="64"/>
-      <c r="W2" s="57" t="s">
+      <c r="W2" s="63" t="s">
         <v>66</v>
       </c>
       <c r="X2" s="64"/>
-      <c r="Y2" s="63" t="s">
+      <c r="Y2" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="Z2" s="57"/>
+      <c r="Z2" s="63"/>
     </row>
     <row r="3" spans="2:34" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="32" t="s">
@@ -11447,34 +11501,34 @@
       </c>
     </row>
     <row r="31" spans="2:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="F31" s="60" t="s">
+      <c r="F31" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="G31" s="61"/>
-      <c r="H31" s="62"/>
-      <c r="I31" s="58">
+      <c r="G31" s="60"/>
+      <c r="H31" s="61"/>
+      <c r="I31" s="57">
         <f>C29+E29+G29+I29+K29+M29+O29+Q29+S29+U29+W29</f>
         <v>2462.73</v>
       </c>
-      <c r="J31" s="59"/>
+      <c r="J31" s="58"/>
     </row>
     <row r="32" spans="2:30" x14ac:dyDescent="0.55000000000000004">
       <c r="G32" s="65" t="s">
         <v>57</v>
       </c>
       <c r="H32" s="65"/>
-      <c r="I32" s="58">
+      <c r="I32" s="57">
         <f>+D29+F29+H29+J29+L29+N29+P29+R29+T29+V29+X29</f>
         <v>1004.25</v>
       </c>
-      <c r="J32" s="59"/>
+      <c r="J32" s="58"/>
     </row>
     <row r="33" spans="3:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="I33" s="58">
+      <c r="I33" s="57">
         <f>I32-I31</f>
         <v>-1458.48</v>
       </c>
-      <c r="J33" s="59"/>
+      <c r="J33" s="58"/>
       <c r="Y33">
         <f>2167+183+5*10</f>
         <v>2400</v>
@@ -11570,11 +11624,11 @@
         <v>64</v>
       </c>
       <c r="H38" s="42"/>
-      <c r="I38" s="66">
+      <c r="I38" s="67">
         <f>I36+I33+J37</f>
         <v>322.7800000000002</v>
       </c>
-      <c r="J38" s="66"/>
+      <c r="J38" s="67"/>
       <c r="M38" s="33"/>
     </row>
     <row r="40" spans="3:25" x14ac:dyDescent="0.55000000000000004">
@@ -11846,16 +11900,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="U2:V2"/>
     <mergeCell ref="W2:X2"/>
     <mergeCell ref="Y2:Z2"/>
     <mergeCell ref="C2:D2"/>
@@ -11864,6 +11908,16 @@
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="M2:N2"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="I33:J33"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="54" orientation="landscape" r:id="rId1"/>
@@ -11877,8 +11931,8 @@
   </sheetPr>
   <dimension ref="B1:AH58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="Y27" sqref="Y27"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -11901,54 +11955,54 @@
   <sheetData>
     <row r="1" spans="2:34" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="2" spans="2:34" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="63" t="s">
         <v>100</v>
       </c>
-      <c r="D2" s="57"/>
-      <c r="E2" s="67" t="s">
+      <c r="D2" s="63"/>
+      <c r="E2" s="66" t="s">
         <v>101</v>
       </c>
-      <c r="F2" s="63"/>
-      <c r="G2" s="57" t="s">
+      <c r="F2" s="62"/>
+      <c r="G2" s="63" t="s">
         <v>102</v>
       </c>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57" t="s">
+      <c r="H2" s="63"/>
+      <c r="I2" s="63" t="s">
         <v>103</v>
       </c>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57" t="s">
+      <c r="J2" s="63"/>
+      <c r="K2" s="63" t="s">
         <v>104</v>
       </c>
-      <c r="L2" s="57"/>
-      <c r="M2" s="67" t="s">
+      <c r="L2" s="63"/>
+      <c r="M2" s="66" t="s">
         <v>105</v>
       </c>
-      <c r="N2" s="63"/>
-      <c r="O2" s="57" t="s">
+      <c r="N2" s="62"/>
+      <c r="O2" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="P2" s="57"/>
-      <c r="Q2" s="57" t="s">
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63" t="s">
         <v>107</v>
       </c>
-      <c r="R2" s="57"/>
-      <c r="S2" s="57" t="s">
+      <c r="R2" s="63"/>
+      <c r="S2" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="T2" s="57"/>
-      <c r="U2" s="57" t="s">
+      <c r="T2" s="63"/>
+      <c r="U2" s="63" t="s">
         <v>108</v>
       </c>
       <c r="V2" s="64"/>
-      <c r="W2" s="57" t="s">
+      <c r="W2" s="63" t="s">
         <v>66</v>
       </c>
       <c r="X2" s="64"/>
-      <c r="Y2" s="63" t="s">
+      <c r="Y2" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="Z2" s="57"/>
+      <c r="Z2" s="63"/>
     </row>
     <row r="3" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B3" s="32" t="s">
@@ -12316,20 +12370,20 @@
         <v>71</v>
       </c>
       <c r="AE7" s="44">
-        <f>+E29+'Punters 2021'!Q27+'Punters 2020'!M27+'Punters club'!J6+'Punters 2022'!C29</f>
-        <v>993</v>
+        <f>+E29+'Punters 2023'!AE7</f>
+        <v>1208</v>
       </c>
       <c r="AF7" s="44">
-        <f>+F29+'Punters 2021'!R27+'Punters 2020'!N27+'Punters club'!K6+'Punters 2022'!D29</f>
+        <f>+F29+'Punters 2023'!AF7</f>
         <v>542.6</v>
       </c>
       <c r="AG7" s="49">
         <f>+AF7-AE7</f>
-        <v>-450.4</v>
+        <v>-665.4</v>
       </c>
       <c r="AH7" s="47">
         <f>(AF7-AE7)/AE7</f>
-        <v>-0.4535750251762336</v>
+        <v>-0.55082781456953644</v>
       </c>
     </row>
     <row r="8" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -12394,20 +12448,20 @@
         <v>72</v>
       </c>
       <c r="AE8" s="44">
-        <f>+K29+'Punters 2021'!I27+'Punters 2020'!G27+'Punters club'!J7+'Punters 2022'!E29</f>
-        <v>1148</v>
+        <f>+K29+'Punters 2023'!AE8</f>
+        <v>1388</v>
       </c>
       <c r="AF8" s="44">
-        <f>+L29+'Punters 2021'!J27+'Punters 2020'!H27+'Punters club'!K7+'Punters 2022'!F29</f>
+        <f>+L29+'Punters 2023'!AF8</f>
         <v>1138.52</v>
       </c>
       <c r="AG8" s="50">
         <f t="shared" ref="AG8:AG16" si="3">+AF8-AE8</f>
-        <v>-9.4800000000000182</v>
+        <v>-249.48000000000002</v>
       </c>
       <c r="AH8" s="47">
         <f t="shared" ref="AH8:AH16" si="4">(AF8-AE8)/AE8</f>
-        <v>-8.2578397212543717E-3</v>
+        <v>-0.17974063400576371</v>
       </c>
     </row>
     <row r="9" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -12476,20 +12530,20 @@
         <v>73</v>
       </c>
       <c r="AE9" s="44">
-        <f>+M29+'Punters 2021'!K27+'Punters 2020'!E27+'Punters club'!J11+'Punters 2022'!G29</f>
-        <v>1126.48</v>
+        <f>+M29+'Punters 2023'!AE9</f>
+        <v>1366.48</v>
       </c>
       <c r="AF9" s="44">
-        <f>N29+'Punters 2021'!L27+'Punters 2020'!F27+'Punters club'!K11+'Punters 2022'!H29</f>
+        <f>N29+'Punters 2023'!AF9</f>
         <v>1093.9000000000001</v>
       </c>
       <c r="AG9" s="50">
         <f t="shared" si="3"/>
-        <v>-32.579999999999927</v>
+        <v>-272.57999999999993</v>
       </c>
       <c r="AH9" s="47">
         <f t="shared" si="4"/>
-        <v>-2.8921951565939855E-2</v>
+        <v>-0.19947602599379421</v>
       </c>
     </row>
     <row r="10" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -12554,20 +12608,20 @@
         <v>74</v>
       </c>
       <c r="AE10" s="44">
-        <f>+C29+'Punters 2021'!G27+'Punters 2020'!I27+'Punters club'!J10+'Punters 2022'!I29</f>
-        <v>1124.9000000000001</v>
+        <f>+C29+'Punters 2023'!AE10</f>
+        <v>1364.9</v>
       </c>
       <c r="AF10" s="44">
-        <f>+D29+'Punters 2021'!H27+'Punters 2020'!J27+'Punters club'!K10+'Punters 2022'!J29</f>
-        <v>1459.8999999999999</v>
+        <f>+D29+'Punters 2023'!AF10</f>
+        <v>1516.4499999999998</v>
       </c>
       <c r="AG10" s="50">
         <f t="shared" si="3"/>
-        <v>334.99999999999977</v>
+        <v>151.54999999999973</v>
       </c>
       <c r="AH10" s="45">
         <f t="shared" si="4"/>
-        <v>0.29780424926660126</v>
+        <v>0.11103377536815863</v>
       </c>
     </row>
     <row r="11" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -12632,20 +12686,20 @@
         <v>75</v>
       </c>
       <c r="AE11" s="44">
-        <f>+I29+'Punters 2021'!E27+'Punters 2020'!K27+'Punters 2022'!K29</f>
-        <v>838</v>
+        <f>+I29+'Punters 2023'!AE11</f>
+        <v>1073</v>
       </c>
       <c r="AF11" s="44">
-        <f>+J29+'Punters 2021'!F27+'Punters 2020'!L27+'Punters 2022'!L29</f>
+        <f>+J29+'Punters 2023'!AF11</f>
         <v>98.25</v>
       </c>
       <c r="AG11" s="49">
         <f t="shared" si="3"/>
-        <v>-739.75</v>
+        <v>-974.75</v>
       </c>
       <c r="AH11" s="47">
         <f t="shared" si="4"/>
-        <v>-0.88275656324582341</v>
+        <v>-0.9084342963653308</v>
       </c>
     </row>
     <row r="12" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -12714,20 +12768,20 @@
         <v>76</v>
       </c>
       <c r="AE12" s="44">
-        <f>+U29+'Punters 2021'!S27+'Punters 2020'!S27+'Punters club'!J8+'Punters 2022'!M29</f>
-        <v>1144.96</v>
+        <f>+U29+'Punters 2023'!AE12</f>
+        <v>1384.96</v>
       </c>
       <c r="AF12" s="44">
-        <f>+V29+'Punters 2021'!T27+'Punters 2020'!T27+'Punters club'!K8+'Punters 2022'!N29</f>
-        <v>610.57999999999993</v>
+        <f>+V29+'Punters 2023'!AF12</f>
+        <v>890.65999999999985</v>
       </c>
       <c r="AG12" s="49">
         <f t="shared" si="3"/>
-        <v>-534.38000000000011</v>
+        <v>-494.30000000000018</v>
       </c>
       <c r="AH12" s="47">
         <f t="shared" si="4"/>
-        <v>-0.46672372833985476</v>
+        <v>-0.35690561460258791</v>
       </c>
     </row>
     <row r="13" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -12792,20 +12846,20 @@
         <v>77</v>
       </c>
       <c r="AE13" s="44">
-        <f>+S29+'Punters 2021'!O27+'Punters 2020'!O27+'Punters club'!J9+'Punters 2022'!O29</f>
-        <v>1106.3400000000001</v>
+        <f>+S29+'Punters 2023'!AE13</f>
+        <v>1346.3400000000001</v>
       </c>
       <c r="AF13" s="44">
-        <f>+T29+'Punters 2021'!P27+'Punters 2020'!P27+'Punters club'!K9+'Punters 2022'!P29</f>
-        <v>346.40999999999997</v>
+        <f>+T29+'Punters 2023'!AF13</f>
+        <v>626.24</v>
       </c>
       <c r="AG13" s="49">
         <f t="shared" si="3"/>
-        <v>-759.93000000000018</v>
+        <v>-720.10000000000014</v>
       </c>
       <c r="AH13" s="47">
         <f t="shared" si="4"/>
-        <v>-0.68688649059059614</v>
+        <v>-0.5348574654247813</v>
       </c>
     </row>
     <row r="14" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -12871,20 +12925,20 @@
         <v>78</v>
       </c>
       <c r="AE14" s="44">
-        <f>+Q29+'Punters 2021'!M27+'Punters 2020'!Q27+'Punters club'!J5+'Punters 2022'!Q29</f>
-        <v>1113</v>
+        <f>+Q29+'Punters 2023'!AE14</f>
+        <v>1353</v>
       </c>
       <c r="AF14" s="44">
-        <f>+R29+'Punters 2021'!N27+'Punters 2020'!R27+'Punters club'!K5+'Punters 2022'!R29</f>
+        <f>+R29+'Punters 2023'!AF14</f>
         <v>637.47</v>
       </c>
       <c r="AG14" s="49">
         <f t="shared" si="3"/>
-        <v>-475.53</v>
+        <v>-715.53</v>
       </c>
       <c r="AH14" s="47">
         <f t="shared" si="4"/>
-        <v>-0.42725067385444743</v>
+        <v>-0.52884700665188467</v>
       </c>
     </row>
     <row r="15" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -12953,20 +13007,20 @@
         <v>79</v>
       </c>
       <c r="AE15" s="44">
-        <f>+O29+'Punters 2021'!C27+'Punters 2020'!C27+'Punters club'!J4+'Punters 2022'!S29</f>
-        <v>1122.7</v>
+        <f>+O29+'Punters 2023'!AE15</f>
+        <v>1362.7</v>
       </c>
       <c r="AF15" s="44">
-        <f>+P29+'Punters 2021'!D27+'Punters 2020'!D27+'Punters club'!K4+'Punters 2022'!T29</f>
+        <f>+P29+'Punters 2023'!AF15</f>
         <v>1696.09</v>
       </c>
       <c r="AG15" s="50">
         <f t="shared" si="3"/>
-        <v>573.38999999999987</v>
+        <v>333.38999999999987</v>
       </c>
       <c r="AH15" s="45">
         <f t="shared" si="4"/>
-        <v>0.5107241471452747</v>
+        <v>0.24465399574374394</v>
       </c>
     </row>
     <row r="16" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -13031,11 +13085,11 @@
         <v>80</v>
       </c>
       <c r="AE16" s="44">
-        <f>+G29+'Punters 2022'!U29+'Punters 2023'!U29</f>
+        <f>+G29+'Punters 2023'!AE16</f>
         <v>620</v>
       </c>
       <c r="AF16" s="44">
-        <f>+H29+'Punters 2022'!V29+'Punters 2023'!V29</f>
+        <f>+H29+'Punters 2023'!AF16</f>
         <v>151.25</v>
       </c>
       <c r="AG16" s="49">
@@ -13931,34 +13985,34 @@
       </c>
     </row>
     <row r="31" spans="2:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="F31" s="60" t="s">
+      <c r="F31" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="G31" s="61"/>
-      <c r="H31" s="62"/>
-      <c r="I31" s="58">
+      <c r="G31" s="60"/>
+      <c r="H31" s="61"/>
+      <c r="I31" s="57">
         <f>C29+E29+G29+I29+K29+M29+O29+Q29+S29+U29+W29</f>
         <v>2158</v>
       </c>
-      <c r="J31" s="59"/>
+      <c r="J31" s="58"/>
     </row>
     <row r="32" spans="2:30" x14ac:dyDescent="0.55000000000000004">
       <c r="G32" s="65" t="s">
         <v>57</v>
       </c>
       <c r="H32" s="65"/>
-      <c r="I32" s="58">
+      <c r="I32" s="57">
         <f>+D29+F29+H29+J29+L29+N29+P29+R29+T29+V29+X29</f>
         <v>709.26</v>
       </c>
-      <c r="J32" s="59"/>
+      <c r="J32" s="58"/>
     </row>
     <row r="33" spans="3:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="I33" s="58">
+      <c r="I33" s="57">
         <f>I32-I31</f>
         <v>-1448.74</v>
       </c>
-      <c r="J33" s="59"/>
+      <c r="J33" s="58"/>
       <c r="Y33">
         <f>2167+183+5*10</f>
         <v>2400</v>
@@ -14047,11 +14101,11 @@
         <v>64</v>
       </c>
       <c r="H38" s="42"/>
-      <c r="I38" s="66">
+      <c r="I38" s="67">
         <f>I36+I33</f>
         <v>552.84999999999991</v>
       </c>
-      <c r="J38" s="66"/>
+      <c r="J38" s="67"/>
       <c r="M38" s="33"/>
     </row>
     <row r="40" spans="3:25" x14ac:dyDescent="0.55000000000000004">
@@ -14346,9 +14400,2347 @@
         <f>SUM(E48:E57)</f>
         <v>709.26</v>
       </c>
+      <c r="K58">
+        <f>SUM(K48:K57)</f>
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="I33:J33"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="51" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEBD9F16-82B6-4065-BD66-A16405C0D139}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B1:AL60"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="1.68359375" customWidth="1"/>
+    <col min="2" max="2" width="5.68359375" customWidth="1"/>
+    <col min="3" max="3" width="7.83984375" customWidth="1"/>
+    <col min="4" max="4" width="9.15625" customWidth="1"/>
+    <col min="5" max="7" width="7.83984375" customWidth="1"/>
+    <col min="8" max="8" width="8.68359375" customWidth="1"/>
+    <col min="9" max="19" width="7.83984375" customWidth="1"/>
+    <col min="20" max="20" width="8.578125" customWidth="1"/>
+    <col min="21" max="23" width="7.83984375" customWidth="1"/>
+    <col min="24" max="24" width="8.83984375" customWidth="1"/>
+    <col min="25" max="25" width="9.41796875" customWidth="1"/>
+    <col min="26" max="26" width="9.68359375" customWidth="1"/>
+    <col min="29" max="29" width="10.41796875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.1015625" customWidth="1"/>
+    <col min="34" max="34" width="11" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="10.578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:38" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="W1" s="69"/>
+      <c r="X1" s="70"/>
+    </row>
+    <row r="2" spans="2:38" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="C2" s="63" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" s="63"/>
+      <c r="E2" s="66" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2" s="62"/>
+      <c r="G2" s="63" t="s">
+        <v>119</v>
+      </c>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63" t="s">
+        <v>120</v>
+      </c>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63" t="s">
+        <v>104</v>
+      </c>
+      <c r="L2" s="63"/>
+      <c r="M2" s="66" t="s">
+        <v>103</v>
+      </c>
+      <c r="N2" s="62"/>
+      <c r="O2" s="63" t="s">
+        <v>106</v>
+      </c>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63" t="s">
+        <v>107</v>
+      </c>
+      <c r="R2" s="63"/>
+      <c r="S2" s="63" t="s">
+        <v>100</v>
+      </c>
+      <c r="T2" s="63"/>
+      <c r="U2" s="63" t="s">
+        <v>108</v>
+      </c>
+      <c r="V2" s="64"/>
+      <c r="W2" s="63" t="s">
+        <v>102</v>
+      </c>
+      <c r="X2" s="64"/>
+      <c r="Y2" s="63" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z2" s="64"/>
+      <c r="AA2" s="66" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB2" s="68"/>
+      <c r="AC2" s="62" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD2" s="63"/>
+    </row>
+    <row r="3" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B3" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="M3" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="N3" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="O3" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="P3" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q3" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="R3" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="S3" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="T3" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="U3" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="V3" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="W3" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="X3" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y3" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z3" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA3" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB3" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC3" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD3" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE3" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF3" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG3" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH3" s="25"/>
+    </row>
+    <row r="4" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B4" s="54" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" s="12"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="13"/>
+      <c r="S4" s="14"/>
+      <c r="T4" s="13"/>
+      <c r="U4" s="12"/>
+      <c r="V4" s="19"/>
+      <c r="W4" s="12"/>
+      <c r="X4" s="19"/>
+      <c r="Y4" s="12"/>
+      <c r="Z4" s="19"/>
+      <c r="AA4" s="12"/>
+      <c r="AB4" s="19"/>
+      <c r="AC4" s="14">
+        <f>U4+S4+Q4+O4+M4+K4+I4+G4+E4+C4</f>
+        <v>0</v>
+      </c>
+      <c r="AD4" s="48">
+        <f>V4+T4+R4+P4+N4+L4+J4+H4+F4+D4</f>
+        <v>0</v>
+      </c>
+      <c r="AE4" s="1">
+        <f>AC4</f>
+        <v>0</v>
+      </c>
+      <c r="AF4" s="1">
+        <f>AD4</f>
+        <v>0</v>
+      </c>
+      <c r="AG4" s="1">
+        <f>AF4-AE4</f>
+        <v>0</v>
+      </c>
+      <c r="AH4" s="1"/>
+    </row>
+    <row r="5" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B5" s="54" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="15"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="17"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="17"/>
+      <c r="T5" s="16"/>
+      <c r="U5" s="15"/>
+      <c r="V5" s="20"/>
+      <c r="W5" s="15"/>
+      <c r="X5" s="20"/>
+      <c r="Y5" s="15"/>
+      <c r="Z5" s="20"/>
+      <c r="AA5" s="15"/>
+      <c r="AB5" s="20"/>
+      <c r="AC5" s="17">
+        <f>U5+S5+Q5+O5+M5+K5+I5+G5+E5+C5</f>
+        <v>0</v>
+      </c>
+      <c r="AD5" s="35">
+        <f>V5+T5+R5+P5+N5+L5+J5+H5+F5+D5</f>
+        <v>0</v>
+      </c>
+      <c r="AE5" s="1">
+        <f>AE4+AC5</f>
+        <v>0</v>
+      </c>
+      <c r="AF5" s="1">
+        <f>AF4+AD5</f>
+        <v>0</v>
+      </c>
+      <c r="AG5" s="1">
+        <f t="shared" ref="AG5:AG27" si="0">AF5-AE5</f>
+        <v>0</v>
+      </c>
+      <c r="AH5" s="1"/>
+    </row>
+    <row r="6" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B6" s="52" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="15"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="17"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="17"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="15"/>
+      <c r="V6" s="20"/>
+      <c r="W6" s="15"/>
+      <c r="X6" s="20"/>
+      <c r="Y6" s="15"/>
+      <c r="Z6" s="20"/>
+      <c r="AA6" s="15"/>
+      <c r="AB6" s="20"/>
+      <c r="AC6" s="17">
+        <f>U6+S6+Q6+O6+M6+K6+I6+G6+E6+C6</f>
+        <v>0</v>
+      </c>
+      <c r="AD6" s="35">
+        <f>V6+T6+R6+P6+N6+L6+J6+H6+F6+D6</f>
+        <v>0</v>
+      </c>
+      <c r="AE6" s="1">
+        <f t="shared" ref="AE6:AF21" si="1">AE5+AC6</f>
+        <v>0</v>
+      </c>
+      <c r="AF6" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AG6" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AH6" s="1"/>
+      <c r="AI6" s="43" t="s">
+        <v>67</v>
+      </c>
+      <c r="AJ6" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="AK6" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="AL6" s="43" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B7" s="51" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="15"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="16"/>
+      <c r="S7" s="17"/>
+      <c r="T7" s="16"/>
+      <c r="U7" s="15"/>
+      <c r="V7" s="20"/>
+      <c r="W7" s="15"/>
+      <c r="X7" s="20"/>
+      <c r="Y7" s="15"/>
+      <c r="Z7" s="20"/>
+      <c r="AA7" s="15"/>
+      <c r="AB7" s="20"/>
+      <c r="AC7" s="17">
+        <f>U7+S7+Q7+O7+M7+K7+I7+G7+E7+C7</f>
+        <v>0</v>
+      </c>
+      <c r="AD7" s="35">
+        <f>V7+T7+R7+P7+N7+L7+J7+H7+F7+D7</f>
+        <v>0</v>
+      </c>
+      <c r="AE7" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AF7" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AG7" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AH7" s="44" t="s">
+        <v>71</v>
+      </c>
+      <c r="AI7" s="44">
+        <f>+E29+'Punters 2023'!AE7</f>
+        <v>1003</v>
+      </c>
+      <c r="AJ7" s="44">
+        <f>+F29+'Punters 2023'!AF7</f>
+        <v>534</v>
+      </c>
+      <c r="AK7" s="49">
+        <f>+AJ7-AI7</f>
+        <v>-469</v>
+      </c>
+      <c r="AL7" s="47">
+        <f>(AJ7-AI7)/AI7</f>
+        <v>-0.46759720837487539</v>
+      </c>
+    </row>
+    <row r="8" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B8" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="15"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="17"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="17"/>
+      <c r="R8" s="16"/>
+      <c r="S8" s="17"/>
+      <c r="T8" s="16"/>
+      <c r="U8" s="15"/>
+      <c r="V8" s="20"/>
+      <c r="W8" s="15"/>
+      <c r="X8" s="20"/>
+      <c r="Y8" s="15"/>
+      <c r="Z8" s="20"/>
+      <c r="AA8" s="15"/>
+      <c r="AB8" s="20"/>
+      <c r="AC8" s="17">
+        <f>U8+S8+Q8+O8+M8+K8+I8+G8+E8+C8</f>
+        <v>0</v>
+      </c>
+      <c r="AD8" s="35">
+        <f>V8+T8+R8+P8+N8+L8+J8+H8+F8+D8</f>
+        <v>0</v>
+      </c>
+      <c r="AE8" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AF8" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AG8" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AH8" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="AI8" s="44">
+        <f>+K29+'Punters 2023'!AE8</f>
+        <v>1163</v>
+      </c>
+      <c r="AJ8" s="44">
+        <f>+L29+'Punters 2023'!AF8</f>
+        <v>1019.77</v>
+      </c>
+      <c r="AK8" s="50">
+        <f t="shared" ref="AK8:AK16" si="2">+AJ8-AI8</f>
+        <v>-143.23000000000002</v>
+      </c>
+      <c r="AL8" s="47">
+        <f t="shared" ref="AL8:AL16" si="3">(AJ8-AI8)/AI8</f>
+        <v>-0.12315563198624249</v>
+      </c>
+    </row>
+    <row r="9" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B9" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="15"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="17"/>
+      <c r="R9" s="16"/>
+      <c r="S9" s="17"/>
+      <c r="T9" s="16"/>
+      <c r="U9" s="15"/>
+      <c r="V9" s="20"/>
+      <c r="W9" s="15"/>
+      <c r="X9" s="20"/>
+      <c r="Y9" s="15"/>
+      <c r="Z9" s="20"/>
+      <c r="AA9" s="15"/>
+      <c r="AB9" s="20"/>
+      <c r="AC9" s="17">
+        <f>U9+S9+Q9+O9+M9+K9+I9+G9+E9+C9</f>
+        <v>0</v>
+      </c>
+      <c r="AD9" s="35">
+        <f>V9+T9+R9+P9+N9+L9+J9+H9+F9+D9</f>
+        <v>0</v>
+      </c>
+      <c r="AE9" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AF9" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AG9" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AH9" s="44" t="s">
+        <v>73</v>
+      </c>
+      <c r="AI9" s="44">
+        <f>+M29+'Punters 2023'!AE9</f>
+        <v>1136.48</v>
+      </c>
+      <c r="AJ9" s="44">
+        <f>N29+'Punters 2023'!AF9</f>
+        <v>961.4</v>
+      </c>
+      <c r="AK9" s="50">
+        <f t="shared" si="2"/>
+        <v>-175.08000000000004</v>
+      </c>
+      <c r="AL9" s="47">
+        <f t="shared" si="3"/>
+        <v>-0.15405462480641985</v>
+      </c>
+    </row>
+    <row r="10" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B10" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="15"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="17"/>
+      <c r="R10" s="16"/>
+      <c r="S10" s="17"/>
+      <c r="T10" s="16"/>
+      <c r="U10" s="15"/>
+      <c r="V10" s="20"/>
+      <c r="W10" s="15"/>
+      <c r="X10" s="20"/>
+      <c r="Y10" s="15"/>
+      <c r="Z10" s="20"/>
+      <c r="AA10" s="15"/>
+      <c r="AB10" s="20"/>
+      <c r="AC10" s="17">
+        <f>U10+S10+Q10+O10+M10+K10+I10+G10+E10+C10</f>
+        <v>0</v>
+      </c>
+      <c r="AD10" s="35">
+        <f>V10+T10+R10+P10+N10+L10+J10+H10+F10+D10</f>
+        <v>0</v>
+      </c>
+      <c r="AE10" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AF10" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AG10" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AH10" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="AI10" s="44">
+        <f>+C29+'Punters 2023'!AE10</f>
+        <v>1139.9000000000001</v>
+      </c>
+      <c r="AJ10" s="44">
+        <f>+D29+'Punters 2023'!AF10</f>
+        <v>1516.4499999999998</v>
+      </c>
+      <c r="AK10" s="50">
+        <f t="shared" si="2"/>
+        <v>376.54999999999973</v>
+      </c>
+      <c r="AL10" s="45">
+        <f t="shared" si="3"/>
+        <v>0.33033599438547212</v>
+      </c>
+    </row>
+    <row r="11" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B11" s="53" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="15"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="17"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="17"/>
+      <c r="R11" s="16"/>
+      <c r="S11" s="17"/>
+      <c r="T11" s="16"/>
+      <c r="U11" s="15"/>
+      <c r="V11" s="20"/>
+      <c r="W11" s="15"/>
+      <c r="X11" s="20"/>
+      <c r="Y11" s="15"/>
+      <c r="Z11" s="20"/>
+      <c r="AA11" s="15"/>
+      <c r="AB11" s="20"/>
+      <c r="AC11" s="17">
+        <f>U11+S11+Q11+O11+M11+K11+I11+G11+E11+C11</f>
+        <v>0</v>
+      </c>
+      <c r="AD11" s="35">
+        <f>V11+T11+R11+P11+N11+L11+J11+H11+F11+D11</f>
+        <v>0</v>
+      </c>
+      <c r="AE11" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AF11" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AG11" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AH11" s="44" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI11" s="44">
+        <f>+I29+'Punters 2023'!AE11</f>
+        <v>868</v>
+      </c>
+      <c r="AJ11" s="44">
+        <f>+J29+'Punters 2023'!AF11</f>
+        <v>58.25</v>
+      </c>
+      <c r="AK11" s="49">
+        <f t="shared" si="2"/>
+        <v>-809.75</v>
+      </c>
+      <c r="AL11" s="47">
+        <f t="shared" si="3"/>
+        <v>-0.93289170506912444</v>
+      </c>
+    </row>
+    <row r="12" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B12" s="52" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="15"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="17"/>
+      <c r="R12" s="16"/>
+      <c r="S12" s="17"/>
+      <c r="T12" s="16"/>
+      <c r="U12" s="15"/>
+      <c r="V12" s="20"/>
+      <c r="W12" s="15"/>
+      <c r="X12" s="20"/>
+      <c r="Y12" s="15"/>
+      <c r="Z12" s="20"/>
+      <c r="AA12" s="15"/>
+      <c r="AB12" s="20"/>
+      <c r="AC12" s="17">
+        <f>U12+S12+Q12+O12+M12+K12+I12+G12+E12+C12</f>
+        <v>0</v>
+      </c>
+      <c r="AD12" s="35">
+        <f>V12+T12+R12+P12+N12+L12+J12+H12+F12+D12</f>
+        <v>0</v>
+      </c>
+      <c r="AE12" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AF12" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AG12" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AH12" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="AI12" s="44">
+        <f>+U29+'Punters 2023'!AE12</f>
+        <v>1194.96</v>
+      </c>
+      <c r="AJ12" s="44">
+        <f>+V29+'Punters 2023'!AF12</f>
+        <v>844.40999999999985</v>
+      </c>
+      <c r="AK12" s="49">
+        <f t="shared" si="2"/>
+        <v>-350.55000000000018</v>
+      </c>
+      <c r="AL12" s="47">
+        <f t="shared" si="3"/>
+        <v>-0.29335709981924096</v>
+      </c>
+    </row>
+    <row r="13" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B13" s="51" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="15"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="17"/>
+      <c r="P13" s="16"/>
+      <c r="Q13" s="17"/>
+      <c r="R13" s="16"/>
+      <c r="S13" s="17"/>
+      <c r="T13" s="16"/>
+      <c r="U13" s="15"/>
+      <c r="V13" s="20"/>
+      <c r="W13" s="15"/>
+      <c r="X13" s="20"/>
+      <c r="Y13" s="15"/>
+      <c r="Z13" s="20"/>
+      <c r="AA13" s="15"/>
+      <c r="AB13" s="20"/>
+      <c r="AC13" s="17">
+        <f>U13+S13+Q13+O13+M13+K13+I13+G13+E13+C13</f>
+        <v>0</v>
+      </c>
+      <c r="AD13" s="35">
+        <f>V13+T13+R13+P13+N13+L13+J13+H13+F13+D13</f>
+        <v>0</v>
+      </c>
+      <c r="AE13" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AF13" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AG13" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AH13" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="AI13" s="44">
+        <f>+S29+'Punters 2023'!AE13</f>
+        <v>1121.3400000000001</v>
+      </c>
+      <c r="AJ13" s="44">
+        <f>+T29+'Punters 2023'!AF13</f>
+        <v>498.08</v>
+      </c>
+      <c r="AK13" s="49">
+        <f t="shared" si="2"/>
+        <v>-623.26000000000022</v>
+      </c>
+      <c r="AL13" s="47">
+        <f t="shared" si="3"/>
+        <v>-0.55581714734157361</v>
+      </c>
+    </row>
+    <row r="14" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B14" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="15"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="17"/>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="17"/>
+      <c r="R14" s="16"/>
+      <c r="S14" s="17"/>
+      <c r="T14" s="16"/>
+      <c r="U14" s="15"/>
+      <c r="V14" s="20"/>
+      <c r="W14" s="15"/>
+      <c r="X14" s="20"/>
+      <c r="Y14" s="15"/>
+      <c r="Z14" s="20"/>
+      <c r="AA14" s="15"/>
+      <c r="AB14" s="20"/>
+      <c r="AC14" s="17">
+        <f>U14+S14+Q14+O14+M14+K14+I14+G14+E14+C14</f>
+        <v>0</v>
+      </c>
+      <c r="AD14" s="35">
+        <f>V14+T14+R14+P14+N14+L14+J14+H14+F14+D14</f>
+        <v>0</v>
+      </c>
+      <c r="AE14" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AF14" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AG14" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AH14" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="AI14" s="44">
+        <f>+Q29+'Punters 2023'!AE14</f>
+        <v>1123</v>
+      </c>
+      <c r="AJ14" s="44">
+        <f>+R29+'Punters 2023'!AF14</f>
+        <v>637.47</v>
+      </c>
+      <c r="AK14" s="49">
+        <f t="shared" si="2"/>
+        <v>-485.53</v>
+      </c>
+      <c r="AL14" s="47">
+        <f t="shared" si="3"/>
+        <v>-0.4323508459483526</v>
+      </c>
+    </row>
+    <row r="15" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B15" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="15"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="17"/>
+      <c r="P15" s="16"/>
+      <c r="Q15" s="17"/>
+      <c r="R15" s="16"/>
+      <c r="S15" s="17"/>
+      <c r="T15" s="16"/>
+      <c r="U15" s="15"/>
+      <c r="V15" s="20"/>
+      <c r="W15" s="15"/>
+      <c r="X15" s="20"/>
+      <c r="Y15" s="15"/>
+      <c r="Z15" s="20"/>
+      <c r="AA15" s="15"/>
+      <c r="AB15" s="20"/>
+      <c r="AC15" s="17">
+        <f>U15+S15+Q15+O15+M15+K15+I15+G15+E15+C15</f>
+        <v>0</v>
+      </c>
+      <c r="AD15" s="35">
+        <f>V15+T15+R15+P15+N15+L15+J15+H15+F15+D15</f>
+        <v>0</v>
+      </c>
+      <c r="AE15" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AF15" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AG15" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AH15" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI15" s="44">
+        <f>+O29+'Punters 2023'!AE15</f>
+        <v>1132.7</v>
+      </c>
+      <c r="AJ15" s="44">
+        <f>+P29+'Punters 2023'!AF15</f>
+        <v>1461.09</v>
+      </c>
+      <c r="AK15" s="50">
+        <f t="shared" si="2"/>
+        <v>328.38999999999987</v>
+      </c>
+      <c r="AL15" s="45">
+        <f t="shared" si="3"/>
+        <v>0.28991789529442913</v>
+      </c>
+    </row>
+    <row r="16" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B16" s="51" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="15"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="17"/>
+      <c r="R16" s="16"/>
+      <c r="S16" s="17"/>
+      <c r="T16" s="16"/>
+      <c r="U16" s="15"/>
+      <c r="V16" s="20"/>
+      <c r="W16" s="15"/>
+      <c r="X16" s="20"/>
+      <c r="Y16" s="15"/>
+      <c r="Z16" s="20"/>
+      <c r="AA16" s="15"/>
+      <c r="AB16" s="20"/>
+      <c r="AC16" s="17">
+        <f>U16+S16+Q16+O16+M16+K16+I16+G16+E16+C16</f>
+        <v>0</v>
+      </c>
+      <c r="AD16" s="35">
+        <f>V16+T16+R16+P16+N16+L16+J16+H16+F16+D16</f>
+        <v>0</v>
+      </c>
+      <c r="AE16" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AF16" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AG16" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AH16" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI16" s="44">
+        <f>+G29+'Punters 2023'!AE16</f>
+        <v>427</v>
+      </c>
+      <c r="AJ16" s="44">
+        <f>+H29+'Punters 2023'!AF16</f>
+        <v>151.25</v>
+      </c>
+      <c r="AK16" s="49">
+        <f t="shared" si="2"/>
+        <v>-275.75</v>
+      </c>
+      <c r="AL16" s="47">
+        <f t="shared" si="3"/>
+        <v>-0.64578454332552693</v>
+      </c>
+    </row>
+    <row r="17" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B17" s="53" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="15"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="17"/>
+      <c r="R17" s="16"/>
+      <c r="S17" s="17"/>
+      <c r="T17" s="16"/>
+      <c r="U17" s="15"/>
+      <c r="V17" s="20"/>
+      <c r="W17" s="15"/>
+      <c r="X17" s="20"/>
+      <c r="Y17" s="15"/>
+      <c r="Z17" s="20"/>
+      <c r="AA17" s="15"/>
+      <c r="AB17" s="20"/>
+      <c r="AC17" s="17">
+        <f>U17+S17+Q17+O17+M17+K17+I17+G17+E17+C17</f>
+        <v>0</v>
+      </c>
+      <c r="AD17" s="35">
+        <f>V17+T17+R17+P17+N17+L17+J17+H17+F17+D17</f>
+        <v>0</v>
+      </c>
+      <c r="AE17" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AF17" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AG17" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AH17" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="AI17" s="71"/>
+      <c r="AJ17" s="71"/>
+      <c r="AK17" s="71"/>
+      <c r="AL17" s="71"/>
+    </row>
+    <row r="18" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B18" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="17"/>
+      <c r="P18" s="16"/>
+      <c r="Q18" s="17"/>
+      <c r="R18" s="16"/>
+      <c r="S18" s="17"/>
+      <c r="T18" s="16"/>
+      <c r="U18" s="15"/>
+      <c r="V18" s="20"/>
+      <c r="W18" s="15"/>
+      <c r="X18" s="20"/>
+      <c r="Y18" s="15"/>
+      <c r="Z18" s="20"/>
+      <c r="AA18" s="15"/>
+      <c r="AB18" s="20"/>
+      <c r="AC18" s="17">
+        <f>U18+S18+Q18+O18+M18+K18+I18+G18+E18+C18</f>
+        <v>0</v>
+      </c>
+      <c r="AD18" s="35">
+        <f>V18+T18+R18+P18+N18+L18+J18+H18+F18+D18</f>
+        <v>0</v>
+      </c>
+      <c r="AE18" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AF18" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AG18" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AH18" s="44" t="s">
+        <v>122</v>
+      </c>
+      <c r="AI18" s="71"/>
+      <c r="AJ18" s="71"/>
+      <c r="AK18" s="71"/>
+      <c r="AL18" s="71"/>
+    </row>
+    <row r="19" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B19" s="51" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="15"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="17"/>
+      <c r="P19" s="16"/>
+      <c r="Q19" s="17"/>
+      <c r="R19" s="16"/>
+      <c r="S19" s="17"/>
+      <c r="T19" s="16"/>
+      <c r="U19" s="15"/>
+      <c r="V19" s="20"/>
+      <c r="W19" s="15"/>
+      <c r="X19" s="20"/>
+      <c r="Y19" s="15"/>
+      <c r="Z19" s="20"/>
+      <c r="AA19" s="15"/>
+      <c r="AB19" s="20"/>
+      <c r="AC19" s="17">
+        <f>U19+S19+Q19+O19+M19+K19+I19+G19+E19+C19</f>
+        <v>0</v>
+      </c>
+      <c r="AD19" s="35">
+        <f>V19+T19+R19+P19+N19+L19+J19+H19+F19+D19</f>
+        <v>0</v>
+      </c>
+      <c r="AE19" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AF19" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AG19" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AH19" s="1"/>
+    </row>
+    <row r="20" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B20" s="53" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="15"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="17"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="17"/>
+      <c r="P20" s="16"/>
+      <c r="Q20" s="17"/>
+      <c r="R20" s="16"/>
+      <c r="S20" s="17"/>
+      <c r="T20" s="16"/>
+      <c r="U20" s="15"/>
+      <c r="V20" s="20"/>
+      <c r="W20" s="15"/>
+      <c r="X20" s="20"/>
+      <c r="Y20" s="15"/>
+      <c r="Z20" s="20"/>
+      <c r="AA20" s="15"/>
+      <c r="AB20" s="20"/>
+      <c r="AC20" s="17">
+        <f>U20+S20+Q20+O20+M20+K20+I20+G20+E20+C20</f>
+        <v>0</v>
+      </c>
+      <c r="AD20" s="35">
+        <f>V20+T20+R20+P20+N20+L20+J20+H20+F20+D20</f>
+        <v>0</v>
+      </c>
+      <c r="AE20" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AF20" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AG20" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AH20" s="1"/>
+    </row>
+    <row r="21" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B21" s="52" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="15"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="17"/>
+      <c r="N21" s="16"/>
+      <c r="O21" s="17"/>
+      <c r="P21" s="16"/>
+      <c r="Q21" s="17"/>
+      <c r="R21" s="16"/>
+      <c r="S21" s="17"/>
+      <c r="T21" s="16"/>
+      <c r="U21" s="15"/>
+      <c r="V21" s="20"/>
+      <c r="W21" s="15"/>
+      <c r="X21" s="20"/>
+      <c r="Y21" s="15"/>
+      <c r="Z21" s="20"/>
+      <c r="AA21" s="15"/>
+      <c r="AB21" s="20"/>
+      <c r="AC21" s="17">
+        <f>U21+S21+Q21+O21+M21+K21+I21+G21+E21+C21</f>
+        <v>0</v>
+      </c>
+      <c r="AD21" s="35">
+        <f>V21+T21+R21+P21+N21+L21+J21+H21+F21+D21</f>
+        <v>0</v>
+      </c>
+      <c r="AE21" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AF21" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AG21" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AH21" s="1"/>
+    </row>
+    <row r="22" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B22" s="51" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="15"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="17"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="17"/>
+      <c r="N22" s="16"/>
+      <c r="O22" s="17"/>
+      <c r="P22" s="16"/>
+      <c r="Q22" s="17"/>
+      <c r="R22" s="16"/>
+      <c r="S22" s="17"/>
+      <c r="T22" s="16"/>
+      <c r="U22" s="15"/>
+      <c r="V22" s="20"/>
+      <c r="W22" s="15"/>
+      <c r="X22" s="20"/>
+      <c r="Y22" s="15"/>
+      <c r="Z22" s="20"/>
+      <c r="AA22" s="15"/>
+      <c r="AB22" s="20"/>
+      <c r="AC22" s="17">
+        <f>U22+S22+Q22+O22+M22+K22+I22+G22+E22+C22</f>
+        <v>0</v>
+      </c>
+      <c r="AD22" s="16">
+        <f>V22+T22+R22+P22+N22+L22+J22+H22+F22+D22</f>
+        <v>0</v>
+      </c>
+      <c r="AE22" s="1">
+        <f t="shared" ref="AE22:AF27" si="4">AE21+AC22</f>
+        <v>0</v>
+      </c>
+      <c r="AF22" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AG22" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AH22" s="1"/>
+    </row>
+    <row r="23" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B23" s="53" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="15"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="16"/>
+      <c r="M23" s="17"/>
+      <c r="N23" s="16"/>
+      <c r="O23" s="17"/>
+      <c r="P23" s="16"/>
+      <c r="Q23" s="17"/>
+      <c r="R23" s="16"/>
+      <c r="S23" s="17"/>
+      <c r="T23" s="16"/>
+      <c r="U23" s="15"/>
+      <c r="V23" s="20"/>
+      <c r="W23" s="15"/>
+      <c r="X23" s="20"/>
+      <c r="Y23" s="15"/>
+      <c r="Z23" s="20"/>
+      <c r="AA23" s="15"/>
+      <c r="AB23" s="20"/>
+      <c r="AC23" s="17">
+        <f>U23+S23+Q23+O23+M23+K23+I23+G23+E23+C23</f>
+        <v>0</v>
+      </c>
+      <c r="AD23" s="16">
+        <f>V23+T23+R23+P23+N23+L23+J23+H23+F23+D23</f>
+        <v>0</v>
+      </c>
+      <c r="AE23" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AF23" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AG23" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AH23" s="1"/>
+    </row>
+    <row r="24" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B24" s="52" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="15"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="16"/>
+      <c r="M24" s="17"/>
+      <c r="N24" s="16"/>
+      <c r="O24" s="17"/>
+      <c r="P24" s="16"/>
+      <c r="Q24" s="17"/>
+      <c r="R24" s="16"/>
+      <c r="S24" s="17"/>
+      <c r="T24" s="16"/>
+      <c r="U24" s="15"/>
+      <c r="V24" s="20"/>
+      <c r="W24" s="15"/>
+      <c r="X24" s="20"/>
+      <c r="Y24" s="15"/>
+      <c r="Z24" s="20"/>
+      <c r="AA24" s="15"/>
+      <c r="AB24" s="20"/>
+      <c r="AC24" s="17">
+        <f>U24+S24+Q24+O24+M24+K24+I24+G24+E24+C24</f>
+        <v>0</v>
+      </c>
+      <c r="AD24" s="16">
+        <f>V24+T24+R24+P24+N24+L24+J24+H24+F24+D24</f>
+        <v>0</v>
+      </c>
+      <c r="AE24" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AF24" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AG24" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AH24" s="1"/>
+    </row>
+    <row r="25" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B25" s="51" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" s="15"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="17"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="17"/>
+      <c r="N25" s="16"/>
+      <c r="O25" s="17"/>
+      <c r="P25" s="16"/>
+      <c r="Q25" s="17"/>
+      <c r="R25" s="16"/>
+      <c r="S25" s="17"/>
+      <c r="T25" s="16"/>
+      <c r="U25" s="15"/>
+      <c r="V25" s="20"/>
+      <c r="W25" s="15"/>
+      <c r="X25" s="20"/>
+      <c r="Y25" s="15"/>
+      <c r="Z25" s="20"/>
+      <c r="AA25" s="15"/>
+      <c r="AB25" s="20"/>
+      <c r="AC25" s="17">
+        <f>U25+S25+Q25+O25+M25+K25+I25+G25+E25+C25</f>
+        <v>0</v>
+      </c>
+      <c r="AD25" s="16">
+        <f>V25+T25+R25+P25+N25+L25+J25+H25+F25+D25</f>
+        <v>0</v>
+      </c>
+      <c r="AE25" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AF25" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AG25" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AH25" s="1"/>
+    </row>
+    <row r="26" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B26" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" s="15"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="17"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="17"/>
+      <c r="N26" s="16"/>
+      <c r="O26" s="17"/>
+      <c r="P26" s="16"/>
+      <c r="Q26" s="17"/>
+      <c r="R26" s="16"/>
+      <c r="S26" s="17"/>
+      <c r="T26" s="16"/>
+      <c r="U26" s="15"/>
+      <c r="V26" s="20"/>
+      <c r="W26" s="15"/>
+      <c r="X26" s="20"/>
+      <c r="Y26" s="15"/>
+      <c r="Z26" s="20"/>
+      <c r="AA26" s="15"/>
+      <c r="AB26" s="20"/>
+      <c r="AC26" s="17">
+        <f>U26+S26+Q26+O26+M26+K26+I26+G26+E26+C26</f>
+        <v>0</v>
+      </c>
+      <c r="AD26" s="16">
+        <f>V26+T26+R26+P26+N26+L26+J26+H26+F26+D26</f>
+        <v>0</v>
+      </c>
+      <c r="AE26" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AF26" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AG26" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AH26" s="1"/>
+    </row>
+    <row r="27" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B27" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="15"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="17"/>
+      <c r="N27" s="16"/>
+      <c r="O27" s="17"/>
+      <c r="P27" s="16"/>
+      <c r="Q27" s="17"/>
+      <c r="R27" s="16"/>
+      <c r="S27" s="17"/>
+      <c r="T27" s="16"/>
+      <c r="U27" s="15"/>
+      <c r="V27" s="20"/>
+      <c r="W27" s="15"/>
+      <c r="X27" s="20"/>
+      <c r="Y27" s="15"/>
+      <c r="Z27" s="20"/>
+      <c r="AA27" s="15"/>
+      <c r="AB27" s="20"/>
+      <c r="AC27" s="17">
+        <f>U27+S27+Q27+O27+M27+K27+I27+G27+E27+C27+AA27</f>
+        <v>0</v>
+      </c>
+      <c r="AD27" s="16">
+        <f>V27+T27+R27+P27+N27+L27+J27+H27+F27+D27+AB27</f>
+        <v>0</v>
+      </c>
+      <c r="AE27" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AF27" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AG27" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AH27" s="1"/>
+    </row>
+    <row r="28" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B28" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28" s="15"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="17"/>
+      <c r="L28" s="16"/>
+      <c r="M28" s="17"/>
+      <c r="N28" s="16"/>
+      <c r="O28" s="17"/>
+      <c r="P28" s="16"/>
+      <c r="Q28" s="17"/>
+      <c r="R28" s="16"/>
+      <c r="S28" s="17"/>
+      <c r="T28" s="16"/>
+      <c r="U28" s="15"/>
+      <c r="V28" s="20"/>
+      <c r="W28" s="15"/>
+      <c r="X28" s="20"/>
+      <c r="Y28" s="15"/>
+      <c r="Z28" s="20"/>
+      <c r="AA28" s="15"/>
+      <c r="AB28" s="20"/>
+      <c r="AC28" s="17">
+        <f>U28+S28+Q28+O28+M28+K28+I28+G28+E28+C28</f>
+        <v>0</v>
+      </c>
+      <c r="AD28" s="16">
+        <f>V28+T28+R28+P28+N28+L28+J28+H28+F28+D28+AB28</f>
+        <v>0</v>
+      </c>
+      <c r="AE28" s="1"/>
+      <c r="AF28" s="1"/>
+      <c r="AG28" s="1"/>
+      <c r="AH28" s="1"/>
+    </row>
+    <row r="29" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B29" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="18">
+        <f t="shared" ref="C29:AD29" si="5">SUM(C4:C28)</f>
+        <v>0</v>
+      </c>
+      <c r="D29" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E29" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="F29" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G29" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H29" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I29" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J29" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K29" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L29" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M29" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N29" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O29" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P29" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q29" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="R29" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="S29" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T29" s="18">
+        <f>SUM(T4:T28)</f>
+        <v>0</v>
+      </c>
+      <c r="U29" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="V29" s="21">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="W29" s="18">
+        <f t="shared" ref="W29:X29" si="6">SUM(W4:W28)</f>
+        <v>0</v>
+      </c>
+      <c r="X29" s="21">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y29" s="18">
+        <f t="shared" ref="Y29:Z29" si="7">SUM(Y4:Y28)</f>
+        <v>0</v>
+      </c>
+      <c r="Z29" s="21">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AA29" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AB29" s="21">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AC29" s="29">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AD29" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AE29" s="1"/>
+    </row>
+    <row r="30" spans="2:38" x14ac:dyDescent="0.55000000000000004">
+      <c r="D30" s="56" t="e">
+        <f>(D29-C29)/C29</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F30" s="34" t="e">
+        <f>(F29-E29)/E29</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H30" s="34" t="e">
+        <f>(H29-G29)/G29</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J30" s="34" t="e">
+        <f>(J29-I29)/I29</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L30" s="28" t="e">
+        <f>(L29-K29)/K29</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N30" s="28" t="e">
+        <f>(N29-M29)/M29</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P30" s="28" t="e">
+        <f>(P29-O29)/O29</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R30" s="28" t="e">
+        <f>(R29-Q29)/Q29</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T30" s="22" t="e">
+        <f>(T29-S29)/S29</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V30" s="28" t="e">
+        <f>(V29-U29)/U29</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X30" s="28" t="e">
+        <f>(X29-W29)/W29</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Z30" s="28" t="e">
+        <f>(Z29-Y29)/Y29</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="31" spans="2:38" x14ac:dyDescent="0.55000000000000004">
+      <c r="F31" s="59" t="s">
+        <v>56</v>
+      </c>
+      <c r="G31" s="60"/>
+      <c r="H31" s="61"/>
+      <c r="I31" s="57">
+        <f>C29+E29+G29+I29+K29+M29+O29+Q29+S29+U29+AA29</f>
+        <v>0</v>
+      </c>
+      <c r="J31" s="58"/>
+    </row>
+    <row r="32" spans="2:38" x14ac:dyDescent="0.55000000000000004">
+      <c r="G32" s="65" t="s">
+        <v>57</v>
+      </c>
+      <c r="H32" s="65"/>
+      <c r="I32" s="57">
+        <f>+D29+F29+H29+J29+L29+N29+P29+R29+T29+V29+AB29</f>
+        <v>0</v>
+      </c>
+      <c r="J32" s="58"/>
+    </row>
+    <row r="33" spans="3:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="I33" s="57">
+        <f>I32-I31</f>
+        <v>0</v>
+      </c>
+      <c r="J33" s="58"/>
+      <c r="Y33">
+        <f>2167+183+5*10</f>
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="34" spans="3:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="C34" s="36">
+        <f>C29+E29+G29+I29</f>
+        <v>0</v>
+      </c>
+      <c r="D34" s="36">
+        <f>D29+F29+H29+J29</f>
+        <v>0</v>
+      </c>
+      <c r="E34" s="37">
+        <f>D34-C34</f>
+        <v>0</v>
+      </c>
+      <c r="I34" s="38">
+        <f>O29+K29+M29</f>
+        <v>0</v>
+      </c>
+      <c r="J34" s="38">
+        <f>P29+L29+N29</f>
+        <v>0</v>
+      </c>
+      <c r="K34" s="39">
+        <f>J34-I34</f>
+        <v>0</v>
+      </c>
+      <c r="O34" s="40">
+        <f>U29+Q29+S29</f>
+        <v>0</v>
+      </c>
+      <c r="P34" s="40">
+        <f>V29+R29+T29</f>
+        <v>0</v>
+      </c>
+      <c r="Q34" s="41">
+        <f>P34-O34</f>
+        <v>0</v>
+      </c>
+      <c r="X34" s="55"/>
+      <c r="Y34">
+        <f>15*10</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="35" spans="3:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="C35" s="36"/>
+      <c r="D35" s="34" t="e">
+        <f>(D34-C34)/C34</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E35" s="37"/>
+      <c r="I35" s="38"/>
+      <c r="J35" s="34" t="e">
+        <f>(J34-I34)/I34</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K35" s="39"/>
+      <c r="O35" s="40"/>
+      <c r="P35" s="34" t="e">
+        <f>(P34-O34)/O34</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q35" s="41"/>
+      <c r="X35" s="55"/>
+    </row>
+    <row r="36" spans="3:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="G36" t="s">
+        <v>58</v>
+      </c>
+      <c r="I36">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="37" spans="3:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="G37" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="3:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="G38" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="H38" s="42"/>
+      <c r="I38" s="67">
+        <f>I36+I33</f>
+        <v>2400</v>
+      </c>
+      <c r="J38" s="67"/>
+      <c r="M38" s="33"/>
+    </row>
+    <row r="40" spans="3:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="X40" s="55"/>
+    </row>
+    <row r="42" spans="3:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="C42" s="1">
+        <f>C29+E29+G29+I29</f>
+        <v>0</v>
+      </c>
+      <c r="D42" s="1">
+        <f>D29+F29+H29+J29</f>
+        <v>0</v>
+      </c>
+      <c r="I42" s="1">
+        <f>O29+K29+M29</f>
+        <v>0</v>
+      </c>
+      <c r="J42" s="1">
+        <f>P29+L29+N29</f>
+        <v>0</v>
+      </c>
+      <c r="O42" s="1">
+        <f>U29+Q29+S29</f>
+        <v>0</v>
+      </c>
+      <c r="P42" s="1">
+        <f>V29+R29+T29</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="3:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="D43" s="1">
+        <f>D42-C42</f>
+        <v>0</v>
+      </c>
+      <c r="J43" s="33">
+        <f>J42-I42</f>
+        <v>0</v>
+      </c>
+      <c r="P43" s="33">
+        <f>P42-O42</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="3:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="V45" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="46" spans="3:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="D46" t="s">
+        <v>88</v>
+      </c>
+      <c r="J46" t="s">
+        <v>113</v>
+      </c>
+      <c r="V46" t="s">
+        <v>89</v>
+      </c>
+      <c r="W46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="3:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="D47" t="s">
+        <v>90</v>
+      </c>
+      <c r="E47" t="s">
+        <v>91</v>
+      </c>
+      <c r="J47" t="s">
+        <v>90</v>
+      </c>
+      <c r="K47" t="s">
+        <v>112</v>
+      </c>
+      <c r="V47" t="s">
+        <v>12</v>
+      </c>
+      <c r="W47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="3:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="D48" t="s">
+        <v>92</v>
+      </c>
+      <c r="E48" s="1">
+        <f>SUM(V29)</f>
+        <v>0</v>
+      </c>
+      <c r="J48" t="s">
+        <v>92</v>
+      </c>
+      <c r="K48">
+        <v>2</v>
+      </c>
+      <c r="V48" t="s">
+        <v>93</v>
+      </c>
+      <c r="W48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="4:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="D49" t="s">
+        <v>12</v>
+      </c>
+      <c r="E49" s="1">
+        <f>SUM(L29)</f>
+        <v>0</v>
+      </c>
+      <c r="J49" t="s">
+        <v>12</v>
+      </c>
+      <c r="K49">
+        <v>0</v>
+      </c>
+      <c r="V49" t="s">
+        <v>92</v>
+      </c>
+      <c r="W49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="4:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="D50" t="s">
+        <v>94</v>
+      </c>
+      <c r="E50" s="1">
+        <f>SUM(T29)</f>
+        <v>0</v>
+      </c>
+      <c r="J50" t="s">
+        <v>94</v>
+      </c>
+      <c r="K50">
+        <v>0</v>
+      </c>
+      <c r="V50" t="s">
+        <v>9</v>
+      </c>
+      <c r="W50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="4:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="D51" t="s">
+        <v>95</v>
+      </c>
+      <c r="E51" s="1">
+        <f>SUM(F29)</f>
+        <v>0</v>
+      </c>
+      <c r="J51" t="s">
+        <v>95</v>
+      </c>
+      <c r="K51">
+        <v>0</v>
+      </c>
+      <c r="V51" t="s">
+        <v>11</v>
+      </c>
+      <c r="W51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="4:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="D52" t="s">
+        <v>93</v>
+      </c>
+      <c r="E52" s="1">
+        <f>SUM(J29)</f>
+        <v>0</v>
+      </c>
+      <c r="J52" t="s">
+        <v>93</v>
+      </c>
+      <c r="K52">
+        <v>0</v>
+      </c>
+      <c r="V52" t="s">
+        <v>96</v>
+      </c>
+      <c r="W52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="4:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="D53" t="s">
+        <v>97</v>
+      </c>
+      <c r="E53" s="1">
+        <f>SUM(R29)</f>
+        <v>0</v>
+      </c>
+      <c r="J53" t="s">
+        <v>97</v>
+      </c>
+      <c r="K53">
+        <v>0</v>
+      </c>
+      <c r="V53" t="s">
+        <v>98</v>
+      </c>
+      <c r="W53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="4:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="D54" t="s">
+        <v>98</v>
+      </c>
+      <c r="E54" s="1">
+        <f>SUM(N29)</f>
+        <v>0</v>
+      </c>
+      <c r="J54" t="s">
+        <v>98</v>
+      </c>
+      <c r="K54">
+        <v>1</v>
+      </c>
+      <c r="V54" t="s">
+        <v>97</v>
+      </c>
+      <c r="W54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="4:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="D55" t="s">
+        <v>89</v>
+      </c>
+      <c r="E55" s="1">
+        <f>SUM(X29)</f>
+        <v>0</v>
+      </c>
+      <c r="J55" t="s">
+        <v>89</v>
+      </c>
+      <c r="K55">
+        <v>0</v>
+      </c>
+      <c r="V55" t="s">
+        <v>94</v>
+      </c>
+      <c r="W55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="4:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="D56" t="s">
+        <v>96</v>
+      </c>
+      <c r="E56" s="1">
+        <f>SUM(Z29)</f>
+        <v>0</v>
+      </c>
+      <c r="J56" t="s">
+        <v>96</v>
+      </c>
+      <c r="K56">
+        <v>0</v>
+      </c>
+      <c r="W56">
+        <f>SUM(W46:W55)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="4:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="D57" t="s">
+        <v>123</v>
+      </c>
+      <c r="E57" s="1">
+        <f>SUM(D29)</f>
+        <v>0</v>
+      </c>
+      <c r="J57" t="s">
+        <v>123</v>
+      </c>
+      <c r="K57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="4:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="D58" t="s">
+        <v>124</v>
+      </c>
+      <c r="E58" s="1">
+        <f>SUM(H29)</f>
+        <v>0</v>
+      </c>
+      <c r="J58" t="s">
+        <v>124</v>
+      </c>
+      <c r="K58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="4:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="D59" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59" s="1">
+        <f>SUM(P29)</f>
+        <v>0</v>
+      </c>
+      <c r="J59" t="s">
+        <v>9</v>
+      </c>
+      <c r="K59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="4:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="D60" t="s">
+        <v>99</v>
+      </c>
+      <c r="E60" s="1">
+        <f>SUM(E48:E59)</f>
+        <v>0</v>
+      </c>
+      <c r="K60">
+        <f>SUM(K48:K59)</f>
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="21">
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="Y2:Z2"/>
     <mergeCell ref="F31:H31"/>
     <mergeCell ref="I31:J31"/>
     <mergeCell ref="G32:H32"/>
@@ -14359,8 +16751,8 @@
     <mergeCell ref="Q2:R2"/>
     <mergeCell ref="S2:T2"/>
     <mergeCell ref="U2:V2"/>
-    <mergeCell ref="W2:X2"/>
-    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="AA2:AB2"/>
+    <mergeCell ref="AC2:AD2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:H2"/>
@@ -14369,11 +16761,59 @@
     <mergeCell ref="M2:N2"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="54" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="51" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B9A81C0-C60A-48E0-A96A-1599E0795A8C}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="10.05078125" customWidth="1"/>
+    <col min="2" max="2" width="13.3125" customWidth="1"/>
+    <col min="3" max="3" width="20.41796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="3e1ffae5-f160-4019-9720-1b11bf1b81a3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002D8393059904904F9DB82DE4B9AFABF6" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f7bafc8adbaca2e93ffc3a1da3fd32d5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3e1ffae5-f160-4019-9720-1b11bf1b81a3" xmlns:ns4="21753bd8-bffc-4cd2-a328-982ee854c895" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f821f56a5d2247de677e71e73e5a99e" ns3:_="" ns4:_="">
     <xsd:import namespace="3e1ffae5-f160-4019-9720-1b11bf1b81a3"/>
@@ -14594,24 +17034,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="3e1ffae5-f160-4019-9720-1b11bf1b81a3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{948817D4-7F3F-493D-9D4C-B473DA03CC7E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4D7A62A-0CB5-48B0-A73A-0A91BCC8EAEF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="21753bd8-bffc-4cd2-a328-982ee854c895"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="3e1ffae5-f160-4019-9720-1b11bf1b81a3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22BA772B-ABF0-4278-9CEF-D9160BBA9E07}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14630,24 +17078,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4D7A62A-0CB5-48B0-A73A-0A91BCC8EAEF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3e1ffae5-f160-4019-9720-1b11bf1b81a3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{948817D4-7F3F-493D-9D4C-B473DA03CC7E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{0f7d30c2-cad0-4405-8153-25a6a3313da4}" enabled="1" method="Privileged" siteId="{6c637512-c417-4e78-9d62-b61258e4b619}" removed="0"/>

</xml_diff>

<commit_message>
Updating Leaderboard and strikes
</commit_message>
<xml_diff>
--- a/public/Data/HEMANPUNTERS.xlsx
+++ b/public/Data/HEMANPUNTERS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bturnor\source\repos\PersonalWork\seeMore\public\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C081F570-F216-4560-8630-CB48449D33E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{969DCC44-5C42-46E9-ABCE-C083CB393636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="45" windowWidth="29040" windowHeight="15720" firstSheet="5" activeTab="6" xr2:uid="{525E8989-1938-4309-A4CF-8F1D15E362FB}"/>
+    <workbookView xWindow="57480" yWindow="45" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="6" xr2:uid="{525E8989-1938-4309-A4CF-8F1D15E362FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Punters club" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="125">
   <si>
     <t>HE_MAN PUNTERS 2019</t>
   </si>
@@ -436,10 +436,10 @@
     <t>pano</t>
   </si>
   <si>
-    <t>Cam</t>
+    <t>Pano</t>
   </si>
   <si>
-    <t>Pano</t>
+    <t>Cam</t>
   </si>
 </sst>
 </file>
@@ -1029,6 +1029,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1047,22 +1051,16 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1071,7 +1069,9 @@
     <xf numFmtId="0" fontId="7" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1088,6 +1088,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3804,50 +3808,50 @@
   <sheetData>
     <row r="1" spans="2:27" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="2" spans="2:27" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63" t="s">
+      <c r="D2" s="58"/>
+      <c r="E2" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63" t="s">
+      <c r="F2" s="58"/>
+      <c r="G2" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63" t="s">
+      <c r="H2" s="58"/>
+      <c r="I2" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="63"/>
-      <c r="K2" s="63" t="s">
+      <c r="J2" s="58"/>
+      <c r="K2" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="63"/>
-      <c r="M2" s="63" t="s">
+      <c r="L2" s="58"/>
+      <c r="M2" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="63"/>
-      <c r="O2" s="63" t="s">
+      <c r="N2" s="58"/>
+      <c r="O2" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="63" t="s">
+      <c r="P2" s="58"/>
+      <c r="Q2" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="R2" s="63"/>
-      <c r="S2" s="63" t="s">
+      <c r="R2" s="58"/>
+      <c r="S2" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="T2" s="63"/>
-      <c r="U2" s="63" t="s">
+      <c r="T2" s="58"/>
+      <c r="U2" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="V2" s="64"/>
-      <c r="W2" s="62" t="s">
+      <c r="V2" s="65"/>
+      <c r="W2" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="X2" s="63"/>
+      <c r="X2" s="58"/>
     </row>
     <row r="3" spans="2:27" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B3" s="32" t="s">
@@ -5408,34 +5412,34 @@
       </c>
     </row>
     <row r="29" spans="2:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="F29" s="59" t="s">
+      <c r="F29" s="61" t="s">
         <v>56</v>
       </c>
-      <c r="G29" s="60"/>
-      <c r="H29" s="61"/>
-      <c r="I29" s="57">
+      <c r="G29" s="62"/>
+      <c r="H29" s="63"/>
+      <c r="I29" s="59">
         <f>C27+E27+G27+I27+K27+M27+O27+Q27+S27+U27</f>
         <v>2469.42</v>
       </c>
-      <c r="J29" s="58"/>
+      <c r="J29" s="60"/>
     </row>
     <row r="30" spans="2:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="G30" s="65" t="s">
+      <c r="G30" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="H30" s="65"/>
-      <c r="I30" s="57">
+      <c r="H30" s="66"/>
+      <c r="I30" s="59">
         <f>+D27+F27+H27+J27+L27+N27+P27+R27+T27+V27</f>
         <v>1774.69</v>
       </c>
-      <c r="J30" s="58"/>
+      <c r="J30" s="60"/>
     </row>
     <row r="31" spans="2:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="I31" s="57">
+      <c r="I31" s="59">
         <f>I30-I29</f>
         <v>-694.73</v>
       </c>
-      <c r="J31" s="58"/>
+      <c r="J31" s="60"/>
     </row>
     <row r="32" spans="2:27" x14ac:dyDescent="0.55000000000000004">
       <c r="C32" s="1">
@@ -5484,11 +5488,11 @@
       </c>
     </row>
     <row r="34" spans="3:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="I34" s="58">
+      <c r="I34" s="60">
         <f>I33+I31</f>
         <v>505.27</v>
       </c>
-      <c r="J34" s="58"/>
+      <c r="J34" s="60"/>
     </row>
     <row r="38" spans="3:16" x14ac:dyDescent="0.55000000000000004">
       <c r="C38" s="1">
@@ -5532,11 +5536,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
     <mergeCell ref="I30:J30"/>
     <mergeCell ref="F29:H29"/>
     <mergeCell ref="I31:J31"/>
@@ -5549,6 +5548,11 @@
     <mergeCell ref="S2:T2"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="I29:J29"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5581,50 +5585,50 @@
   <sheetData>
     <row r="1" spans="2:27" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="2" spans="2:27" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63" t="s">
+      <c r="D2" s="58"/>
+      <c r="E2" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="63"/>
-      <c r="G2" s="66" t="s">
+      <c r="F2" s="58"/>
+      <c r="G2" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="62"/>
-      <c r="I2" s="63" t="s">
+      <c r="H2" s="64"/>
+      <c r="I2" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="63"/>
-      <c r="K2" s="63" t="s">
+      <c r="J2" s="58"/>
+      <c r="K2" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="63"/>
-      <c r="M2" s="63" t="s">
+      <c r="L2" s="58"/>
+      <c r="M2" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="63"/>
-      <c r="O2" s="63" t="s">
+      <c r="N2" s="58"/>
+      <c r="O2" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="63" t="s">
+      <c r="P2" s="58"/>
+      <c r="Q2" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="R2" s="63"/>
-      <c r="S2" s="63" t="s">
+      <c r="R2" s="58"/>
+      <c r="S2" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="T2" s="63"/>
-      <c r="U2" s="63" t="s">
+      <c r="T2" s="58"/>
+      <c r="U2" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="V2" s="64"/>
-      <c r="W2" s="62" t="s">
+      <c r="V2" s="65"/>
+      <c r="W2" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="X2" s="63"/>
+      <c r="X2" s="58"/>
     </row>
     <row r="3" spans="2:27" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B3" s="32" t="s">
@@ -6984,34 +6988,34 @@
       </c>
     </row>
     <row r="29" spans="2:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="F29" s="59" t="s">
+      <c r="F29" s="61" t="s">
         <v>56</v>
       </c>
-      <c r="G29" s="60"/>
-      <c r="H29" s="61"/>
-      <c r="I29" s="57">
+      <c r="G29" s="62"/>
+      <c r="H29" s="63"/>
+      <c r="I29" s="59">
         <f>C27+E27+G27+I27+K27+M27+O27+Q27+S27+U27</f>
         <v>1788.24</v>
       </c>
-      <c r="J29" s="58"/>
+      <c r="J29" s="60"/>
     </row>
     <row r="30" spans="2:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="G30" s="65" t="s">
+      <c r="G30" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="H30" s="65"/>
-      <c r="I30" s="57">
+      <c r="H30" s="66"/>
+      <c r="I30" s="59">
         <f>+D27+F27+H27+J27+L27+N27+P27+R27+T27+V27</f>
         <v>2492.1999999999998</v>
       </c>
-      <c r="J30" s="58"/>
+      <c r="J30" s="60"/>
     </row>
     <row r="31" spans="2:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="I31" s="57">
+      <c r="I31" s="59">
         <f>I30-I29</f>
         <v>703.95999999999981</v>
       </c>
-      <c r="J31" s="58"/>
+      <c r="J31" s="60"/>
     </row>
     <row r="32" spans="2:27" x14ac:dyDescent="0.55000000000000004">
       <c r="C32" s="36">
@@ -7114,11 +7118,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
     <mergeCell ref="Q2:R2"/>
     <mergeCell ref="S2:T2"/>
     <mergeCell ref="U2:V2"/>
@@ -7126,11 +7130,11 @@
     <mergeCell ref="F29:H29"/>
     <mergeCell ref="I29:J29"/>
     <mergeCell ref="M2:N2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="O2:P2"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7164,54 +7168,54 @@
   <sheetData>
     <row r="1" spans="2:34" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="2" spans="2:34" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63" t="s">
+      <c r="D2" s="58"/>
+      <c r="E2" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63" t="s">
+      <c r="F2" s="58"/>
+      <c r="G2" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63" t="s">
+      <c r="H2" s="58"/>
+      <c r="I2" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="63"/>
-      <c r="K2" s="63" t="s">
+      <c r="J2" s="58"/>
+      <c r="K2" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="63"/>
-      <c r="M2" s="63" t="s">
+      <c r="L2" s="58"/>
+      <c r="M2" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="N2" s="63"/>
-      <c r="O2" s="63" t="s">
+      <c r="N2" s="58"/>
+      <c r="O2" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="63" t="s">
+      <c r="P2" s="58"/>
+      <c r="Q2" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="R2" s="63"/>
-      <c r="S2" s="63" t="s">
+      <c r="R2" s="58"/>
+      <c r="S2" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="T2" s="63"/>
-      <c r="U2" s="63" t="s">
+      <c r="T2" s="58"/>
+      <c r="U2" s="58" t="s">
         <v>65</v>
       </c>
-      <c r="V2" s="64"/>
-      <c r="W2" s="63" t="s">
+      <c r="V2" s="65"/>
+      <c r="W2" s="58" t="s">
         <v>66</v>
       </c>
-      <c r="X2" s="64"/>
-      <c r="Y2" s="62" t="s">
+      <c r="X2" s="65"/>
+      <c r="Y2" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="Z2" s="63"/>
+      <c r="Z2" s="58"/>
     </row>
     <row r="3" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B3" s="32" t="s">
@@ -9265,34 +9269,34 @@
       </c>
     </row>
     <row r="31" spans="2:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="F31" s="59" t="s">
+      <c r="F31" s="61" t="s">
         <v>56</v>
       </c>
-      <c r="G31" s="60"/>
-      <c r="H31" s="61"/>
-      <c r="I31" s="57">
+      <c r="G31" s="62"/>
+      <c r="H31" s="63"/>
+      <c r="I31" s="59">
         <f>C29+E29+G29+I29+K29+M29+O29+Q29+S29+U29+W29</f>
         <v>2521.33</v>
       </c>
-      <c r="J31" s="58"/>
+      <c r="J31" s="60"/>
     </row>
     <row r="32" spans="2:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="G32" s="65" t="s">
+      <c r="G32" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="H32" s="65"/>
-      <c r="I32" s="57">
+      <c r="H32" s="66"/>
+      <c r="I32" s="59">
         <f>+D29+F29+H29+J29+L29+N29+P29+R29+T29+V29+X29</f>
         <v>2997.5899999999997</v>
       </c>
-      <c r="J32" s="58"/>
+      <c r="J32" s="60"/>
     </row>
     <row r="33" spans="3:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="I33" s="57">
+      <c r="I33" s="59">
         <f>I32-I31</f>
         <v>476.25999999999976</v>
       </c>
-      <c r="J33" s="58"/>
+      <c r="J33" s="60"/>
     </row>
     <row r="34" spans="3:17" x14ac:dyDescent="0.55000000000000004">
       <c r="C34" s="36">
@@ -9394,11 +9398,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
     <mergeCell ref="Q2:R2"/>
     <mergeCell ref="S2:T2"/>
     <mergeCell ref="U2:V2"/>
@@ -9407,11 +9411,11 @@
     <mergeCell ref="I31:J31"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="W2:X2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="O2:P2"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="54" orientation="landscape" r:id="rId1"/>
@@ -9445,54 +9449,54 @@
   <sheetData>
     <row r="1" spans="2:34" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="2" spans="2:34" ht="18.3" x14ac:dyDescent="0.7">
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="63"/>
-      <c r="E2" s="66" t="s">
+      <c r="D2" s="58"/>
+      <c r="E2" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="62"/>
-      <c r="G2" s="63" t="s">
+      <c r="F2" s="64"/>
+      <c r="G2" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63" t="s">
+      <c r="H2" s="58"/>
+      <c r="I2" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="63"/>
-      <c r="K2" s="63" t="s">
+      <c r="J2" s="58"/>
+      <c r="K2" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="63"/>
-      <c r="M2" s="66" t="s">
+      <c r="L2" s="58"/>
+      <c r="M2" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="62"/>
-      <c r="O2" s="63" t="s">
+      <c r="N2" s="64"/>
+      <c r="O2" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="63" t="s">
+      <c r="P2" s="58"/>
+      <c r="Q2" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="R2" s="63"/>
-      <c r="S2" s="63" t="s">
+      <c r="R2" s="58"/>
+      <c r="S2" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="T2" s="63"/>
-      <c r="U2" s="63" t="s">
+      <c r="T2" s="58"/>
+      <c r="U2" s="58" t="s">
         <v>65</v>
       </c>
-      <c r="V2" s="64"/>
-      <c r="W2" s="63" t="s">
+      <c r="V2" s="65"/>
+      <c r="W2" s="58" t="s">
         <v>66</v>
       </c>
-      <c r="X2" s="64"/>
-      <c r="Y2" s="62" t="s">
+      <c r="X2" s="65"/>
+      <c r="Y2" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="Z2" s="63"/>
+      <c r="Z2" s="58"/>
     </row>
     <row r="3" spans="2:34" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="32" t="s">
@@ -11501,34 +11505,34 @@
       </c>
     </row>
     <row r="31" spans="2:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="F31" s="59" t="s">
+      <c r="F31" s="61" t="s">
         <v>56</v>
       </c>
-      <c r="G31" s="60"/>
-      <c r="H31" s="61"/>
-      <c r="I31" s="57">
+      <c r="G31" s="62"/>
+      <c r="H31" s="63"/>
+      <c r="I31" s="59">
         <f>C29+E29+G29+I29+K29+M29+O29+Q29+S29+U29+W29</f>
         <v>2462.73</v>
       </c>
-      <c r="J31" s="58"/>
+      <c r="J31" s="60"/>
     </row>
     <row r="32" spans="2:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="G32" s="65" t="s">
+      <c r="G32" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="H32" s="65"/>
-      <c r="I32" s="57">
+      <c r="H32" s="66"/>
+      <c r="I32" s="59">
         <f>+D29+F29+H29+J29+L29+N29+P29+R29+T29+V29+X29</f>
         <v>1004.25</v>
       </c>
-      <c r="J32" s="58"/>
+      <c r="J32" s="60"/>
     </row>
     <row r="33" spans="3:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="I33" s="57">
+      <c r="I33" s="59">
         <f>I32-I31</f>
         <v>-1458.48</v>
       </c>
-      <c r="J33" s="58"/>
+      <c r="J33" s="60"/>
       <c r="Y33">
         <f>2167+183+5*10</f>
         <v>2400</v>
@@ -11900,6 +11904,16 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
     <mergeCell ref="W2:X2"/>
     <mergeCell ref="Y2:Z2"/>
     <mergeCell ref="C2:D2"/>
@@ -11908,16 +11922,6 @@
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="M2:N2"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="I33:J33"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="54" orientation="landscape" r:id="rId1"/>
@@ -11955,54 +11959,54 @@
   <sheetData>
     <row r="1" spans="2:34" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="2" spans="2:34" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="58" t="s">
         <v>100</v>
       </c>
-      <c r="D2" s="63"/>
-      <c r="E2" s="66" t="s">
+      <c r="D2" s="58"/>
+      <c r="E2" s="68" t="s">
         <v>101</v>
       </c>
-      <c r="F2" s="62"/>
-      <c r="G2" s="63" t="s">
+      <c r="F2" s="64"/>
+      <c r="G2" s="58" t="s">
         <v>102</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63" t="s">
+      <c r="H2" s="58"/>
+      <c r="I2" s="58" t="s">
         <v>103</v>
       </c>
-      <c r="J2" s="63"/>
-      <c r="K2" s="63" t="s">
+      <c r="J2" s="58"/>
+      <c r="K2" s="58" t="s">
         <v>104</v>
       </c>
-      <c r="L2" s="63"/>
-      <c r="M2" s="66" t="s">
+      <c r="L2" s="58"/>
+      <c r="M2" s="68" t="s">
         <v>105</v>
       </c>
-      <c r="N2" s="62"/>
-      <c r="O2" s="63" t="s">
+      <c r="N2" s="64"/>
+      <c r="O2" s="58" t="s">
         <v>106</v>
       </c>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="63" t="s">
+      <c r="P2" s="58"/>
+      <c r="Q2" s="58" t="s">
         <v>107</v>
       </c>
-      <c r="R2" s="63"/>
-      <c r="S2" s="63" t="s">
+      <c r="R2" s="58"/>
+      <c r="S2" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="T2" s="63"/>
-      <c r="U2" s="63" t="s">
+      <c r="T2" s="58"/>
+      <c r="U2" s="58" t="s">
         <v>108</v>
       </c>
-      <c r="V2" s="64"/>
-      <c r="W2" s="63" t="s">
+      <c r="V2" s="65"/>
+      <c r="W2" s="58" t="s">
         <v>66</v>
       </c>
-      <c r="X2" s="64"/>
-      <c r="Y2" s="62" t="s">
+      <c r="X2" s="65"/>
+      <c r="Y2" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="Z2" s="63"/>
+      <c r="Z2" s="58"/>
     </row>
     <row r="3" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B3" s="32" t="s">
@@ -13985,34 +13989,34 @@
       </c>
     </row>
     <row r="31" spans="2:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="F31" s="59" t="s">
+      <c r="F31" s="61" t="s">
         <v>56</v>
       </c>
-      <c r="G31" s="60"/>
-      <c r="H31" s="61"/>
-      <c r="I31" s="57">
+      <c r="G31" s="62"/>
+      <c r="H31" s="63"/>
+      <c r="I31" s="59">
         <f>C29+E29+G29+I29+K29+M29+O29+Q29+S29+U29+W29</f>
         <v>2158</v>
       </c>
-      <c r="J31" s="58"/>
+      <c r="J31" s="60"/>
     </row>
     <row r="32" spans="2:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="G32" s="65" t="s">
+      <c r="G32" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="H32" s="65"/>
-      <c r="I32" s="57">
+      <c r="H32" s="66"/>
+      <c r="I32" s="59">
         <f>+D29+F29+H29+J29+L29+N29+P29+R29+T29+V29+X29</f>
         <v>709.26</v>
       </c>
-      <c r="J32" s="58"/>
+      <c r="J32" s="60"/>
     </row>
     <row r="33" spans="3:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="I33" s="57">
+      <c r="I33" s="59">
         <f>I32-I31</f>
         <v>-1448.74</v>
       </c>
-      <c r="J33" s="58"/>
+      <c r="J33" s="60"/>
       <c r="Y33">
         <f>2167+183+5*10</f>
         <v>2400</v>
@@ -14407,6 +14411,16 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
     <mergeCell ref="W2:X2"/>
     <mergeCell ref="Y2:Z2"/>
     <mergeCell ref="C2:D2"/>
@@ -14415,16 +14429,6 @@
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="M2:N2"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="I33:J33"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="51" orientation="landscape" r:id="rId1"/>
@@ -14438,8 +14442,8 @@
   </sheetPr>
   <dimension ref="B1:AL60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W59" sqref="W59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -14467,62 +14471,62 @@
       <c r="X1" s="70"/>
     </row>
     <row r="2" spans="2:38" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="58" t="s">
         <v>118</v>
       </c>
-      <c r="D2" s="63"/>
-      <c r="E2" s="66" t="s">
+      <c r="D2" s="58"/>
+      <c r="E2" s="68" t="s">
         <v>101</v>
       </c>
-      <c r="F2" s="62"/>
-      <c r="G2" s="63" t="s">
+      <c r="F2" s="64"/>
+      <c r="G2" s="58" t="s">
         <v>119</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63" t="s">
+      <c r="H2" s="58"/>
+      <c r="I2" s="58" t="s">
         <v>120</v>
       </c>
-      <c r="J2" s="63"/>
-      <c r="K2" s="63" t="s">
+      <c r="J2" s="58"/>
+      <c r="K2" s="58" t="s">
         <v>104</v>
       </c>
-      <c r="L2" s="63"/>
-      <c r="M2" s="66" t="s">
+      <c r="L2" s="58"/>
+      <c r="M2" s="68" t="s">
         <v>103</v>
       </c>
-      <c r="N2" s="62"/>
-      <c r="O2" s="63" t="s">
+      <c r="N2" s="64"/>
+      <c r="O2" s="58" t="s">
         <v>106</v>
       </c>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="63" t="s">
+      <c r="P2" s="58"/>
+      <c r="Q2" s="58" t="s">
         <v>107</v>
       </c>
-      <c r="R2" s="63"/>
-      <c r="S2" s="63" t="s">
+      <c r="R2" s="58"/>
+      <c r="S2" s="58" t="s">
         <v>100</v>
       </c>
-      <c r="T2" s="63"/>
-      <c r="U2" s="63" t="s">
+      <c r="T2" s="58"/>
+      <c r="U2" s="58" t="s">
         <v>108</v>
       </c>
-      <c r="V2" s="64"/>
-      <c r="W2" s="63" t="s">
+      <c r="V2" s="65"/>
+      <c r="W2" s="58" t="s">
         <v>102</v>
       </c>
-      <c r="X2" s="64"/>
-      <c r="Y2" s="63" t="s">
+      <c r="X2" s="65"/>
+      <c r="Y2" s="58" t="s">
         <v>105</v>
       </c>
-      <c r="Z2" s="64"/>
-      <c r="AA2" s="66" t="s">
+      <c r="Z2" s="65"/>
+      <c r="AA2" s="68" t="s">
         <v>66</v>
       </c>
-      <c r="AB2" s="68"/>
-      <c r="AC2" s="62" t="s">
+      <c r="AB2" s="71"/>
+      <c r="AC2" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="AD2" s="63"/>
+      <c r="AD2" s="58"/>
     </row>
     <row r="3" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B3" s="32" t="s">
@@ -14654,11 +14658,11 @@
       <c r="AA4" s="12"/>
       <c r="AB4" s="19"/>
       <c r="AC4" s="14">
-        <f>U4+S4+Q4+O4+M4+K4+I4+G4+E4+C4</f>
+        <f t="shared" ref="AC4:AC26" si="0">U4+S4+Q4+O4+M4+K4+I4+G4+E4+C4</f>
         <v>0</v>
       </c>
       <c r="AD4" s="48">
-        <f>V4+T4+R4+P4+N4+L4+J4+H4+F4+D4</f>
+        <f t="shared" ref="AD4:AD26" si="1">V4+T4+R4+P4+N4+L4+J4+H4+F4+D4</f>
         <v>0</v>
       </c>
       <c r="AE4" s="1">
@@ -14706,11 +14710,11 @@
       <c r="AA5" s="15"/>
       <c r="AB5" s="20"/>
       <c r="AC5" s="17">
-        <f>U5+S5+Q5+O5+M5+K5+I5+G5+E5+C5</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AD5" s="35">
-        <f>V5+T5+R5+P5+N5+L5+J5+H5+F5+D5</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE5" s="1">
@@ -14722,7 +14726,7 @@
         <v>0</v>
       </c>
       <c r="AG5" s="1">
-        <f t="shared" ref="AG5:AG27" si="0">AF5-AE5</f>
+        <f t="shared" ref="AG5:AG27" si="2">AF5-AE5</f>
         <v>0</v>
       </c>
       <c r="AH5" s="1"/>
@@ -14758,23 +14762,23 @@
       <c r="AA6" s="15"/>
       <c r="AB6" s="20"/>
       <c r="AC6" s="17">
-        <f>U6+S6+Q6+O6+M6+K6+I6+G6+E6+C6</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AD6" s="35">
-        <f>V6+T6+R6+P6+N6+L6+J6+H6+F6+D6</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE6" s="1">
-        <f t="shared" ref="AE6:AF21" si="1">AE5+AC6</f>
+        <f t="shared" ref="AE6:AF21" si="3">AE5+AC6</f>
         <v>0</v>
       </c>
       <c r="AF6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AG6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH6" s="1"/>
@@ -14822,23 +14826,23 @@
       <c r="AA7" s="15"/>
       <c r="AB7" s="20"/>
       <c r="AC7" s="17">
-        <f>U7+S7+Q7+O7+M7+K7+I7+G7+E7+C7</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AD7" s="35">
-        <f>V7+T7+R7+P7+N7+L7+J7+H7+F7+D7</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AG7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH7" s="44" t="s">
@@ -14892,23 +14896,23 @@
       <c r="AA8" s="15"/>
       <c r="AB8" s="20"/>
       <c r="AC8" s="17">
-        <f>U8+S8+Q8+O8+M8+K8+I8+G8+E8+C8</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AD8" s="35">
-        <f>V8+T8+R8+P8+N8+L8+J8+H8+F8+D8</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AG8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH8" s="44" t="s">
@@ -14923,11 +14927,11 @@
         <v>1019.77</v>
       </c>
       <c r="AK8" s="50">
-        <f t="shared" ref="AK8:AK16" si="2">+AJ8-AI8</f>
+        <f t="shared" ref="AK8:AK16" si="4">+AJ8-AI8</f>
         <v>-143.23000000000002</v>
       </c>
       <c r="AL8" s="47">
-        <f t="shared" ref="AL8:AL16" si="3">(AJ8-AI8)/AI8</f>
+        <f t="shared" ref="AL8:AL16" si="5">(AJ8-AI8)/AI8</f>
         <v>-0.12315563198624249</v>
       </c>
     </row>
@@ -14962,23 +14966,23 @@
       <c r="AA9" s="15"/>
       <c r="AB9" s="20"/>
       <c r="AC9" s="17">
-        <f>U9+S9+Q9+O9+M9+K9+I9+G9+E9+C9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AD9" s="35">
-        <f>V9+T9+R9+P9+N9+L9+J9+H9+F9+D9</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AG9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH9" s="44" t="s">
@@ -14993,11 +14997,11 @@
         <v>961.4</v>
       </c>
       <c r="AK9" s="50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-175.08000000000004</v>
       </c>
       <c r="AL9" s="47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-0.15405462480641985</v>
       </c>
     </row>
@@ -15032,23 +15036,23 @@
       <c r="AA10" s="15"/>
       <c r="AB10" s="20"/>
       <c r="AC10" s="17">
-        <f>U10+S10+Q10+O10+M10+K10+I10+G10+E10+C10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AD10" s="35">
-        <f>V10+T10+R10+P10+N10+L10+J10+H10+F10+D10</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AG10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH10" s="44" t="s">
@@ -15063,11 +15067,11 @@
         <v>1516.4499999999998</v>
       </c>
       <c r="AK10" s="50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>376.54999999999973</v>
       </c>
       <c r="AL10" s="45">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.33033599438547212</v>
       </c>
     </row>
@@ -15102,23 +15106,23 @@
       <c r="AA11" s="15"/>
       <c r="AB11" s="20"/>
       <c r="AC11" s="17">
-        <f>U11+S11+Q11+O11+M11+K11+I11+G11+E11+C11</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AD11" s="35">
-        <f>V11+T11+R11+P11+N11+L11+J11+H11+F11+D11</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AG11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH11" s="44" t="s">
@@ -15133,11 +15137,11 @@
         <v>58.25</v>
       </c>
       <c r="AK11" s="49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-809.75</v>
       </c>
       <c r="AL11" s="47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-0.93289170506912444</v>
       </c>
     </row>
@@ -15172,23 +15176,23 @@
       <c r="AA12" s="15"/>
       <c r="AB12" s="20"/>
       <c r="AC12" s="17">
-        <f>U12+S12+Q12+O12+M12+K12+I12+G12+E12+C12</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AD12" s="35">
-        <f>V12+T12+R12+P12+N12+L12+J12+H12+F12+D12</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AG12" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH12" s="44" t="s">
@@ -15203,11 +15207,11 @@
         <v>844.40999999999985</v>
       </c>
       <c r="AK12" s="49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-350.55000000000018</v>
       </c>
       <c r="AL12" s="47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-0.29335709981924096</v>
       </c>
     </row>
@@ -15242,23 +15246,23 @@
       <c r="AA13" s="15"/>
       <c r="AB13" s="20"/>
       <c r="AC13" s="17">
-        <f>U13+S13+Q13+O13+M13+K13+I13+G13+E13+C13</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AD13" s="35">
-        <f>V13+T13+R13+P13+N13+L13+J13+H13+F13+D13</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AG13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH13" s="44" t="s">
@@ -15273,11 +15277,11 @@
         <v>498.08</v>
       </c>
       <c r="AK13" s="49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-623.26000000000022</v>
       </c>
       <c r="AL13" s="47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-0.55581714734157361</v>
       </c>
     </row>
@@ -15312,23 +15316,23 @@
       <c r="AA14" s="15"/>
       <c r="AB14" s="20"/>
       <c r="AC14" s="17">
-        <f>U14+S14+Q14+O14+M14+K14+I14+G14+E14+C14</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AD14" s="35">
-        <f>V14+T14+R14+P14+N14+L14+J14+H14+F14+D14</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AG14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH14" s="44" t="s">
@@ -15343,11 +15347,11 @@
         <v>637.47</v>
       </c>
       <c r="AK14" s="49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-485.53</v>
       </c>
       <c r="AL14" s="47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-0.4323508459483526</v>
       </c>
     </row>
@@ -15382,23 +15386,23 @@
       <c r="AA15" s="15"/>
       <c r="AB15" s="20"/>
       <c r="AC15" s="17">
-        <f>U15+S15+Q15+O15+M15+K15+I15+G15+E15+C15</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AD15" s="35">
-        <f>V15+T15+R15+P15+N15+L15+J15+H15+F15+D15</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AG15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH15" s="44" t="s">
@@ -15413,11 +15417,11 @@
         <v>1461.09</v>
       </c>
       <c r="AK15" s="50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>328.38999999999987</v>
       </c>
       <c r="AL15" s="45">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.28991789529442913</v>
       </c>
     </row>
@@ -15452,23 +15456,23 @@
       <c r="AA16" s="15"/>
       <c r="AB16" s="20"/>
       <c r="AC16" s="17">
-        <f>U16+S16+Q16+O16+M16+K16+I16+G16+E16+C16</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AD16" s="35">
-        <f>V16+T16+R16+P16+N16+L16+J16+H16+F16+D16</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AG16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH16" s="44" t="s">
@@ -15483,11 +15487,11 @@
         <v>151.25</v>
       </c>
       <c r="AK16" s="49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-275.75</v>
       </c>
       <c r="AL16" s="47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-0.64578454332552693</v>
       </c>
     </row>
@@ -15522,32 +15526,32 @@
       <c r="AA17" s="15"/>
       <c r="AB17" s="20"/>
       <c r="AC17" s="17">
-        <f>U17+S17+Q17+O17+M17+K17+I17+G17+E17+C17</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AD17" s="35">
-        <f>V17+T17+R17+P17+N17+L17+J17+H17+F17+D17</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE17" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF17" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AG17" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH17" s="44" t="s">
         <v>121</v>
       </c>
-      <c r="AI17" s="71"/>
-      <c r="AJ17" s="71"/>
-      <c r="AK17" s="71"/>
-      <c r="AL17" s="71"/>
+      <c r="AI17" s="57"/>
+      <c r="AJ17" s="57"/>
+      <c r="AK17" s="57"/>
+      <c r="AL17" s="57"/>
     </row>
     <row r="18" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B18" s="52" t="s">
@@ -15580,32 +15584,32 @@
       <c r="AA18" s="15"/>
       <c r="AB18" s="20"/>
       <c r="AC18" s="17">
-        <f>U18+S18+Q18+O18+M18+K18+I18+G18+E18+C18</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AD18" s="35">
-        <f>V18+T18+R18+P18+N18+L18+J18+H18+F18+D18</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AG18" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH18" s="44" t="s">
         <v>122</v>
       </c>
-      <c r="AI18" s="71"/>
-      <c r="AJ18" s="71"/>
-      <c r="AK18" s="71"/>
-      <c r="AL18" s="71"/>
+      <c r="AI18" s="57"/>
+      <c r="AJ18" s="57"/>
+      <c r="AK18" s="57"/>
+      <c r="AL18" s="57"/>
     </row>
     <row r="19" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B19" s="51" t="s">
@@ -15638,23 +15642,23 @@
       <c r="AA19" s="15"/>
       <c r="AB19" s="20"/>
       <c r="AC19" s="17">
-        <f>U19+S19+Q19+O19+M19+K19+I19+G19+E19+C19</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AD19" s="35">
-        <f>V19+T19+R19+P19+N19+L19+J19+H19+F19+D19</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AG19" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH19" s="1"/>
@@ -15690,23 +15694,23 @@
       <c r="AA20" s="15"/>
       <c r="AB20" s="20"/>
       <c r="AC20" s="17">
-        <f>U20+S20+Q20+O20+M20+K20+I20+G20+E20+C20</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AD20" s="35">
-        <f>V20+T20+R20+P20+N20+L20+J20+H20+F20+D20</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE20" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF20" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AG20" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH20" s="1"/>
@@ -15742,23 +15746,23 @@
       <c r="AA21" s="15"/>
       <c r="AB21" s="20"/>
       <c r="AC21" s="17">
-        <f>U21+S21+Q21+O21+M21+K21+I21+G21+E21+C21</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AD21" s="35">
-        <f>V21+T21+R21+P21+N21+L21+J21+H21+F21+D21</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE21" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF21" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AG21" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH21" s="1"/>
@@ -15794,23 +15798,23 @@
       <c r="AA22" s="15"/>
       <c r="AB22" s="20"/>
       <c r="AC22" s="17">
-        <f>U22+S22+Q22+O22+M22+K22+I22+G22+E22+C22</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AD22" s="16">
-        <f>V22+T22+R22+P22+N22+L22+J22+H22+F22+D22</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE22" s="1">
-        <f t="shared" ref="AE22:AF27" si="4">AE21+AC22</f>
+        <f t="shared" ref="AE22:AF27" si="6">AE21+AC22</f>
         <v>0</v>
       </c>
       <c r="AF22" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AG22" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH22" s="1"/>
@@ -15846,23 +15850,23 @@
       <c r="AA23" s="15"/>
       <c r="AB23" s="20"/>
       <c r="AC23" s="17">
-        <f>U23+S23+Q23+O23+M23+K23+I23+G23+E23+C23</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AD23" s="16">
-        <f>V23+T23+R23+P23+N23+L23+J23+H23+F23+D23</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE23" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AF23" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AG23" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH23" s="1"/>
@@ -15898,23 +15902,23 @@
       <c r="AA24" s="15"/>
       <c r="AB24" s="20"/>
       <c r="AC24" s="17">
-        <f>U24+S24+Q24+O24+M24+K24+I24+G24+E24+C24</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AD24" s="16">
-        <f>V24+T24+R24+P24+N24+L24+J24+H24+F24+D24</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE24" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AF24" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AG24" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH24" s="1"/>
@@ -15950,23 +15954,23 @@
       <c r="AA25" s="15"/>
       <c r="AB25" s="20"/>
       <c r="AC25" s="17">
-        <f>U25+S25+Q25+O25+M25+K25+I25+G25+E25+C25</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AD25" s="16">
-        <f>V25+T25+R25+P25+N25+L25+J25+H25+F25+D25</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE25" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AF25" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AG25" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH25" s="1"/>
@@ -16002,23 +16006,23 @@
       <c r="AA26" s="15"/>
       <c r="AB26" s="20"/>
       <c r="AC26" s="17">
-        <f>U26+S26+Q26+O26+M26+K26+I26+G26+E26+C26</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AD26" s="16">
-        <f>V26+T26+R26+P26+N26+L26+J26+H26+F26+D26</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE26" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AF26" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AG26" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH26" s="1"/>
@@ -16062,15 +16066,15 @@
         <v>0</v>
       </c>
       <c r="AE27" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AF27" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AG27" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH27" s="1"/>
@@ -16123,71 +16127,71 @@
         <v>55</v>
       </c>
       <c r="C29" s="18">
-        <f t="shared" ref="C29:AD29" si="5">SUM(C4:C28)</f>
+        <f t="shared" ref="C29:AD29" si="7">SUM(C4:C28)</f>
         <v>0</v>
       </c>
       <c r="D29" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="E29" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F29" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G29" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H29" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="I29" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J29" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K29" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L29" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M29" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N29" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="O29" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P29" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Q29" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="R29" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="S29" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T29" s="18">
@@ -16195,43 +16199,43 @@
         <v>0</v>
       </c>
       <c r="U29" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V29" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="W29" s="18">
-        <f t="shared" ref="W29:X29" si="6">SUM(W4:W28)</f>
+        <f t="shared" ref="W29:X29" si="8">SUM(W4:W28)</f>
         <v>0</v>
       </c>
       <c r="X29" s="21">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Y29" s="18">
-        <f t="shared" ref="Y29:Z29" si="7">SUM(Y4:Y28)</f>
+        <f t="shared" ref="Y29:Z29" si="9">SUM(Y4:Y28)</f>
         <v>0</v>
       </c>
       <c r="Z29" s="21">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AA29" s="18">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AA29" s="18">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
       <c r="AB29" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AC29" s="29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AD29" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AE29" s="1"/>
@@ -16287,34 +16291,34 @@
       </c>
     </row>
     <row r="31" spans="2:38" x14ac:dyDescent="0.55000000000000004">
-      <c r="F31" s="59" t="s">
+      <c r="F31" s="61" t="s">
         <v>56</v>
       </c>
-      <c r="G31" s="60"/>
-      <c r="H31" s="61"/>
-      <c r="I31" s="57">
+      <c r="G31" s="62"/>
+      <c r="H31" s="63"/>
+      <c r="I31" s="59">
         <f>C29+E29+G29+I29+K29+M29+O29+Q29+S29+U29+AA29</f>
         <v>0</v>
       </c>
-      <c r="J31" s="58"/>
+      <c r="J31" s="60"/>
     </row>
     <row r="32" spans="2:38" x14ac:dyDescent="0.55000000000000004">
-      <c r="G32" s="65" t="s">
+      <c r="G32" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="H32" s="65"/>
-      <c r="I32" s="57">
+      <c r="H32" s="66"/>
+      <c r="I32" s="59">
         <f>+D29+F29+H29+J29+L29+N29+P29+R29+T29+V29+AB29</f>
         <v>0</v>
       </c>
-      <c r="J32" s="58"/>
+      <c r="J32" s="60"/>
     </row>
     <row r="33" spans="3:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="I33" s="57">
+      <c r="I33" s="59">
         <f>I32-I31</f>
         <v>0</v>
       </c>
-      <c r="J33" s="58"/>
+      <c r="J33" s="60"/>
       <c r="Y33">
         <f>2167+183+5*10</f>
         <v>2400</v>
@@ -16389,12 +16393,7 @@
         <v>58</v>
       </c>
       <c r="I36">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="37" spans="3:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="G37" t="s">
-        <v>85</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="38" spans="3:25" x14ac:dyDescent="0.55000000000000004">
@@ -16404,7 +16403,7 @@
       <c r="H38" s="42"/>
       <c r="I38" s="67">
         <f>I36+I33</f>
-        <v>2400</v>
+        <v>0.05</v>
       </c>
       <c r="J38" s="67"/>
       <c r="M38" s="33"/>
@@ -16503,7 +16502,7 @@
         <v>92</v>
       </c>
       <c r="K48">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V48" t="s">
         <v>93</v>
@@ -16538,7 +16537,7 @@
         <v>94</v>
       </c>
       <c r="E50" s="1">
-        <f>SUM(T29)</f>
+        <f>SUM(D29)</f>
         <v>0</v>
       </c>
       <c r="J50" t="s">
@@ -16580,14 +16579,14 @@
         <v>93</v>
       </c>
       <c r="E52" s="1">
-        <f>SUM(J29)</f>
+        <f>SUM(T29)</f>
         <v>0</v>
       </c>
       <c r="J52" t="s">
         <v>93</v>
       </c>
       <c r="K52">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V52" t="s">
         <v>96</v>
@@ -16622,7 +16621,7 @@
         <v>98</v>
       </c>
       <c r="E54" s="1">
-        <f>SUM(N29)</f>
+        <f>SUM(J29)</f>
         <v>0</v>
       </c>
       <c r="J54" t="s">
@@ -16643,7 +16642,7 @@
         <v>89</v>
       </c>
       <c r="E55" s="1">
-        <f>SUM(X29)</f>
+        <f>SUM(H29)</f>
         <v>0</v>
       </c>
       <c r="J55" t="s">
@@ -16664,7 +16663,7 @@
         <v>96</v>
       </c>
       <c r="E56" s="1">
-        <f>SUM(Z29)</f>
+        <f>SUM(N29)</f>
         <v>0</v>
       </c>
       <c r="J56" t="s">
@@ -16673,8 +16672,10 @@
       <c r="K56">
         <v>0</v>
       </c>
+      <c r="V56" t="s">
+        <v>123</v>
+      </c>
       <c r="W56">
-        <f>SUM(W46:W55)</f>
         <v>0</v>
       </c>
     </row>
@@ -16683,13 +16684,19 @@
         <v>123</v>
       </c>
       <c r="E57" s="1">
-        <f>SUM(D29)</f>
+        <f>SUM(H29)</f>
         <v>0</v>
       </c>
       <c r="J57" t="s">
         <v>123</v>
       </c>
       <c r="K57">
+        <v>0</v>
+      </c>
+      <c r="V57" t="s">
+        <v>124</v>
+      </c>
+      <c r="W57">
         <v>0</v>
       </c>
     </row>
@@ -16698,13 +16705,20 @@
         <v>124</v>
       </c>
       <c r="E58" s="1">
-        <f>SUM(H29)</f>
+        <f>SUM(D29)</f>
         <v>0</v>
       </c>
       <c r="J58" t="s">
         <v>124</v>
       </c>
       <c r="K58">
+        <v>1</v>
+      </c>
+      <c r="V58" t="s">
+        <v>99</v>
+      </c>
+      <c r="W58">
+        <f>SUM(W46:W57)</f>
         <v>0</v>
       </c>
     </row>
@@ -16731,26 +16745,16 @@
         <f>SUM(E48:E59)</f>
         <v>0</v>
       </c>
+      <c r="J60" t="s">
+        <v>99</v>
+      </c>
       <c r="K60">
         <f>SUM(K48:K59)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="W1:X1"/>
-    <mergeCell ref="W2:X2"/>
-    <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="U2:V2"/>
     <mergeCell ref="AA2:AB2"/>
     <mergeCell ref="AC2:AD2"/>
     <mergeCell ref="C2:D2"/>
@@ -16759,6 +16763,19 @@
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="M2:N2"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="51" orientation="landscape" r:id="rId1"/>
@@ -16797,23 +16814,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="3e1ffae5-f160-4019-9720-1b11bf1b81a3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002D8393059904904F9DB82DE4B9AFABF6" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f7bafc8adbaca2e93ffc3a1da3fd32d5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3e1ffae5-f160-4019-9720-1b11bf1b81a3" xmlns:ns4="21753bd8-bffc-4cd2-a328-982ee854c895" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f821f56a5d2247de677e71e73e5a99e" ns3:_="" ns4:_="">
     <xsd:import namespace="3e1ffae5-f160-4019-9720-1b11bf1b81a3"/>
@@ -17034,32 +17034,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{948817D4-7F3F-493D-9D4C-B473DA03CC7E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="3e1ffae5-f160-4019-9720-1b11bf1b81a3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4D7A62A-0CB5-48B0-A73A-0A91BCC8EAEF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="21753bd8-bffc-4cd2-a328-982ee854c895"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="3e1ffae5-f160-4019-9720-1b11bf1b81a3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22BA772B-ABF0-4278-9CEF-D9160BBA9E07}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17078,6 +17070,31 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4D7A62A-0CB5-48B0-A73A-0A91BCC8EAEF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="21753bd8-bffc-4cd2-a328-982ee854c895"/>
+    <ds:schemaRef ds:uri="3e1ffae5-f160-4019-9720-1b11bf1b81a3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{948817D4-7F3F-493D-9D4C-B473DA03CC7E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{0f7d30c2-cad0-4405-8153-25a6a3313da4}" enabled="1" method="Privileged" siteId="{6c637512-c417-4e78-9d62-b61258e4b619}" removed="0"/>

</xml_diff>

<commit_message>
Spreadsheet update and current betting group highlighted fix
</commit_message>
<xml_diff>
--- a/public/Data/HEMANPUNTERS.xlsx
+++ b/public/Data/HEMANPUNTERS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bturnor\source\repos\PersonalWork\seeMore\public\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1FA3CF68-9C40-440C-844B-AF52595A73EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{309339B6-8538-4FF3-B869-690A10D76FA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="45" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="6" xr2:uid="{525E8989-1938-4309-A4CF-8F1D15E362FB}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" firstSheet="6" activeTab="6" xr2:uid="{525E8989-1938-4309-A4CF-8F1D15E362FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Punters club" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="149">
   <si>
     <t>HE_MAN PUNTERS 2019</t>
   </si>
@@ -421,9 +421,6 @@
     <t>pano</t>
   </si>
   <si>
-    <t>1 leg losses as at 17th March 2025</t>
-  </si>
-  <si>
     <t>Pano</t>
   </si>
   <si>
@@ -466,7 +463,55 @@
     <t>Eagles Suns under 167.5, total 185</t>
   </si>
   <si>
-    <t>Strikes for 2025 Season at 24 Mar 2025</t>
+    <t>Cripps 22/25 touches</t>
+  </si>
+  <si>
+    <t>Jarrod Berry 17/20 touches</t>
+  </si>
+  <si>
+    <t>Wilkie 13/20 touches</t>
+  </si>
+  <si>
+    <t>Nathan O'Driscoll 12/20 touches</t>
+  </si>
+  <si>
+    <t>Liverpool lost to Fulham</t>
+  </si>
+  <si>
+    <t>Chad Warner 10/20 touches</t>
+  </si>
+  <si>
+    <t>Stringer 0 goals, needed 2</t>
+  </si>
+  <si>
+    <t>Sean Woodson to win</t>
+  </si>
+  <si>
+    <t>Colby McKercher 8/15 touches</t>
+  </si>
+  <si>
+    <t>Moose</t>
+  </si>
+  <si>
+    <t>Swikowski 6/15 touches</t>
+  </si>
+  <si>
+    <t>Scotty</t>
+  </si>
+  <si>
+    <t>Logan Morris 0/2 goals</t>
+  </si>
+  <si>
+    <t>Strikes for 2025 Season at 28 April 2025</t>
+  </si>
+  <si>
+    <t>Sandro Tonali shot on target</t>
+  </si>
+  <si>
+    <t>Willie Rioli 1/2 goals</t>
+  </si>
+  <si>
+    <t>1 leg losses as at 28 April 2025</t>
   </si>
 </sst>
 </file>
@@ -1243,6 +1288,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
@@ -14592,7 +14641,7 @@
   <dimension ref="B1:AL60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="N58" sqref="N58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -15019,20 +15068,44 @@
       </c>
       <c r="C7" s="15"/>
       <c r="D7" s="16"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="16"/>
+      <c r="E7" s="17">
+        <v>5</v>
+      </c>
+      <c r="F7" s="16">
+        <v>0</v>
+      </c>
       <c r="G7" s="17"/>
       <c r="H7" s="16"/>
       <c r="I7" s="17"/>
       <c r="J7" s="16"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="17"/>
-      <c r="P7" s="16"/>
-      <c r="Q7" s="17"/>
-      <c r="R7" s="16"/>
+      <c r="K7" s="17">
+        <f>10+7.5+5+2.5</f>
+        <v>25</v>
+      </c>
+      <c r="L7" s="16">
+        <v>0</v>
+      </c>
+      <c r="M7" s="17">
+        <f>5+10+5</f>
+        <v>20</v>
+      </c>
+      <c r="N7" s="16">
+        <v>0</v>
+      </c>
+      <c r="O7" s="17">
+        <f>5+5+5+5+5</f>
+        <v>25</v>
+      </c>
+      <c r="P7" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="17">
+        <f>5+10+5+5</f>
+        <v>25</v>
+      </c>
+      <c r="R7" s="16">
+        <v>0</v>
+      </c>
       <c r="S7" s="17"/>
       <c r="T7" s="16"/>
       <c r="U7" s="15"/>
@@ -15045,7 +15118,7 @@
       <c r="AB7" s="20"/>
       <c r="AC7" s="17">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AD7" s="35">
         <f t="shared" si="3"/>
@@ -15053,7 +15126,7 @@
       </c>
       <c r="AE7" s="1">
         <f t="shared" si="4"/>
-        <v>390</v>
+        <v>490</v>
       </c>
       <c r="AF7" s="1">
         <f t="shared" si="4"/>
@@ -15061,14 +15134,14 @@
       </c>
       <c r="AG7" s="1">
         <f t="shared" si="1"/>
-        <v>8.7599999999999909</v>
+        <v>-91.240000000000009</v>
       </c>
       <c r="AH7" s="44" t="s">
         <v>71</v>
       </c>
       <c r="AI7" s="44">
         <f>+E29+'Punters 2023'!AE7</f>
-        <v>1048</v>
+        <v>1078</v>
       </c>
       <c r="AJ7" s="44">
         <f>+F29+'Punters 2023'!AF7</f>
@@ -15076,11 +15149,11 @@
       </c>
       <c r="AK7" s="49">
         <f>+AJ7-AI7</f>
-        <v>-514</v>
+        <v>-544</v>
       </c>
       <c r="AL7" s="47">
         <f>(AJ7-AI7)/AI7</f>
-        <v>-0.49045801526717558</v>
+        <v>-0.50463821892393323</v>
       </c>
     </row>
     <row r="8" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -15103,42 +15176,58 @@
       <c r="P8" s="16"/>
       <c r="Q8" s="17"/>
       <c r="R8" s="16"/>
-      <c r="S8" s="17"/>
-      <c r="T8" s="16"/>
-      <c r="U8" s="15"/>
-      <c r="V8" s="20"/>
-      <c r="W8" s="15"/>
-      <c r="X8" s="20"/>
-      <c r="Y8" s="15"/>
-      <c r="Z8" s="20"/>
+      <c r="S8" s="17">
+        <v>25</v>
+      </c>
+      <c r="T8" s="16">
+        <v>0</v>
+      </c>
+      <c r="U8" s="15">
+        <v>25</v>
+      </c>
+      <c r="V8" s="20">
+        <v>0</v>
+      </c>
+      <c r="W8" s="15">
+        <v>25</v>
+      </c>
+      <c r="X8" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="15">
+        <v>25</v>
+      </c>
+      <c r="Z8" s="20">
+        <v>1.65</v>
+      </c>
       <c r="AA8" s="15"/>
       <c r="AB8" s="20"/>
       <c r="AC8" s="17">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AD8" s="35">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1.65</v>
       </c>
       <c r="AE8" s="1">
         <f t="shared" si="4"/>
-        <v>390</v>
+        <v>590</v>
       </c>
       <c r="AF8" s="1">
         <f t="shared" si="4"/>
-        <v>398.76</v>
+        <v>400.40999999999997</v>
       </c>
       <c r="AG8" s="1">
         <f t="shared" si="1"/>
-        <v>8.7599999999999909</v>
+        <v>-189.59000000000003</v>
       </c>
       <c r="AH8" s="44" t="s">
         <v>72</v>
       </c>
       <c r="AI8" s="44">
         <f>+K29+'Punters 2023'!AE8</f>
-        <v>1188</v>
+        <v>1238</v>
       </c>
       <c r="AJ8" s="44">
         <f>+L29+'Punters 2023'!AF8</f>
@@ -15146,25 +15235,41 @@
       </c>
       <c r="AK8" s="50">
         <f t="shared" ref="AK8:AK16" si="5">+AJ8-AI8</f>
-        <v>-168.23000000000002</v>
+        <v>-218.23000000000002</v>
       </c>
       <c r="AL8" s="47">
         <f t="shared" ref="AL8:AL16" si="6">(AJ8-AI8)/AI8</f>
-        <v>-0.14160774410774413</v>
+        <v>-0.17627625201938613</v>
       </c>
     </row>
     <row r="9" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B9" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="16"/>
+      <c r="C9" s="15">
+        <v>30</v>
+      </c>
+      <c r="D9" s="16">
+        <v>0</v>
+      </c>
+      <c r="E9" s="17">
+        <v>25</v>
+      </c>
+      <c r="F9" s="16">
+        <v>0</v>
+      </c>
+      <c r="G9" s="17">
+        <v>25</v>
+      </c>
+      <c r="H9" s="16">
+        <v>0</v>
+      </c>
+      <c r="I9" s="17">
+        <v>25</v>
+      </c>
+      <c r="J9" s="16">
+        <v>0</v>
+      </c>
       <c r="K9" s="17"/>
       <c r="L9" s="16"/>
       <c r="M9" s="17"/>
@@ -15185,7 +15290,7 @@
       <c r="AB9" s="20"/>
       <c r="AC9" s="17">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="AD9" s="35">
         <f t="shared" si="3"/>
@@ -15193,22 +15298,22 @@
       </c>
       <c r="AE9" s="1">
         <f t="shared" si="4"/>
-        <v>390</v>
+        <v>695</v>
       </c>
       <c r="AF9" s="1">
         <f t="shared" si="4"/>
-        <v>398.76</v>
+        <v>400.40999999999997</v>
       </c>
       <c r="AG9" s="1">
         <f t="shared" si="1"/>
-        <v>8.7599999999999909</v>
+        <v>-294.59000000000003</v>
       </c>
       <c r="AH9" s="44" t="s">
         <v>73</v>
       </c>
       <c r="AI9" s="44">
         <f>+M29+'Punters 2023'!AE9</f>
-        <v>1161.48</v>
+        <v>1211.48</v>
       </c>
       <c r="AJ9" s="44">
         <f>N29+'Punters 2023'!AF9</f>
@@ -15216,11 +15321,11 @@
       </c>
       <c r="AK9" s="50">
         <f t="shared" si="5"/>
-        <v>-200.08000000000004</v>
+        <v>-250.08000000000004</v>
       </c>
       <c r="AL9" s="47">
         <f t="shared" si="6"/>
-        <v>-0.17226297482522301</v>
+        <v>-0.20642519893023412</v>
       </c>
     </row>
     <row r="10" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -15235,14 +15340,31 @@
       <c r="H10" s="16"/>
       <c r="I10" s="17"/>
       <c r="J10" s="16"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="16"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="16"/>
-      <c r="Q10" s="17"/>
-      <c r="R10" s="16"/>
+      <c r="K10" s="17">
+        <v>25</v>
+      </c>
+      <c r="L10" s="16">
+        <v>0</v>
+      </c>
+      <c r="M10" s="17">
+        <f>5+10+5+10</f>
+        <v>30</v>
+      </c>
+      <c r="N10" s="16">
+        <v>0</v>
+      </c>
+      <c r="O10" s="17">
+        <v>25</v>
+      </c>
+      <c r="P10" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="17">
+        <v>25</v>
+      </c>
+      <c r="R10" s="16">
+        <v>0</v>
+      </c>
       <c r="S10" s="17"/>
       <c r="T10" s="16"/>
       <c r="U10" s="15"/>
@@ -15255,7 +15377,7 @@
       <c r="AB10" s="20"/>
       <c r="AC10" s="17">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="AD10" s="35">
         <f t="shared" si="3"/>
@@ -15263,22 +15385,22 @@
       </c>
       <c r="AE10" s="1">
         <f t="shared" si="4"/>
-        <v>390</v>
+        <v>800</v>
       </c>
       <c r="AF10" s="1">
         <f t="shared" si="4"/>
-        <v>398.76</v>
+        <v>400.40999999999997</v>
       </c>
       <c r="AG10" s="1">
         <f t="shared" si="1"/>
-        <v>8.7599999999999909</v>
+        <v>-399.59000000000003</v>
       </c>
       <c r="AH10" s="44" t="s">
         <v>74</v>
       </c>
       <c r="AI10" s="44">
         <f>+C29+'Punters 2023'!AE10</f>
-        <v>1184.9000000000001</v>
+        <v>1214.9000000000001</v>
       </c>
       <c r="AJ10" s="44">
         <f>+D29+'Punters 2023'!AF10</f>
@@ -15286,11 +15408,11 @@
       </c>
       <c r="AK10" s="50">
         <f t="shared" si="5"/>
-        <v>331.54999999999973</v>
+        <v>301.54999999999973</v>
       </c>
       <c r="AL10" s="45">
         <f t="shared" si="6"/>
-        <v>0.27981264241708137</v>
+        <v>0.24820972919581835</v>
       </c>
     </row>
     <row r="11" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -15313,42 +15435,59 @@
       <c r="P11" s="16"/>
       <c r="Q11" s="17"/>
       <c r="R11" s="16"/>
-      <c r="S11" s="17"/>
-      <c r="T11" s="16"/>
-      <c r="U11" s="15"/>
-      <c r="V11" s="20"/>
-      <c r="W11" s="15"/>
-      <c r="X11" s="20"/>
-      <c r="Y11" s="15"/>
-      <c r="Z11" s="20"/>
+      <c r="S11" s="17">
+        <v>25</v>
+      </c>
+      <c r="T11" s="16">
+        <v>78.61</v>
+      </c>
+      <c r="U11" s="15">
+        <v>20</v>
+      </c>
+      <c r="V11" s="20">
+        <v>0</v>
+      </c>
+      <c r="W11" s="15">
+        <v>25</v>
+      </c>
+      <c r="X11" s="20">
+        <f>33.75+32.5</f>
+        <v>66.25</v>
+      </c>
+      <c r="Y11" s="15">
+        <v>25</v>
+      </c>
+      <c r="Z11" s="20">
+        <v>83.75</v>
+      </c>
       <c r="AA11" s="15"/>
       <c r="AB11" s="20"/>
       <c r="AC11" s="17">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="AD11" s="35">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>228.61</v>
       </c>
       <c r="AE11" s="1">
         <f t="shared" si="4"/>
-        <v>390</v>
+        <v>895</v>
       </c>
       <c r="AF11" s="1">
         <f t="shared" si="4"/>
-        <v>398.76</v>
+        <v>629.02</v>
       </c>
       <c r="AG11" s="1">
         <f t="shared" si="1"/>
-        <v>8.7599999999999909</v>
+        <v>-265.98</v>
       </c>
       <c r="AH11" s="44" t="s">
         <v>75</v>
       </c>
       <c r="AI11" s="44">
         <f>+I29+'Punters 2023'!AE11</f>
-        <v>918</v>
+        <v>943</v>
       </c>
       <c r="AJ11" s="44">
         <f>+J29+'Punters 2023'!AF11</f>
@@ -15356,11 +15495,11 @@
       </c>
       <c r="AK11" s="49">
         <f t="shared" si="5"/>
-        <v>-859.75</v>
+        <v>-884.75</v>
       </c>
       <c r="AL11" s="47">
         <f t="shared" si="6"/>
-        <v>-0.93654684095860563</v>
+        <v>-0.93822905620360553</v>
       </c>
     </row>
     <row r="12" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -15403,22 +15542,22 @@
       </c>
       <c r="AE12" s="1">
         <f t="shared" si="4"/>
-        <v>390</v>
+        <v>895</v>
       </c>
       <c r="AF12" s="1">
         <f t="shared" si="4"/>
-        <v>398.76</v>
+        <v>629.02</v>
       </c>
       <c r="AG12" s="1">
         <f t="shared" si="1"/>
-        <v>8.7599999999999909</v>
+        <v>-265.98</v>
       </c>
       <c r="AH12" s="44" t="s">
         <v>76</v>
       </c>
       <c r="AI12" s="44">
         <f>+U29+'Punters 2023'!AE12</f>
-        <v>1219.96</v>
+        <v>1264.96</v>
       </c>
       <c r="AJ12" s="44">
         <f>+V29+'Punters 2023'!AF12</f>
@@ -15426,11 +15565,11 @@
       </c>
       <c r="AK12" s="49">
         <f t="shared" si="5"/>
-        <v>-375.55000000000018</v>
+        <v>-420.55000000000018</v>
       </c>
       <c r="AL12" s="47">
         <f t="shared" si="6"/>
-        <v>-0.30783796190039031</v>
+        <v>-0.33246110548950175</v>
       </c>
     </row>
     <row r="13" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -15473,34 +15612,34 @@
       </c>
       <c r="AE13" s="1">
         <f t="shared" si="4"/>
-        <v>390</v>
+        <v>895</v>
       </c>
       <c r="AF13" s="1">
         <f t="shared" si="4"/>
-        <v>398.76</v>
+        <v>629.02</v>
       </c>
       <c r="AG13" s="1">
         <f t="shared" si="1"/>
-        <v>8.7599999999999909</v>
+        <v>-265.98</v>
       </c>
       <c r="AH13" s="44" t="s">
         <v>77</v>
       </c>
       <c r="AI13" s="44">
         <f>+S29+'Punters 2023'!AE13</f>
-        <v>1146.3400000000001</v>
+        <v>1196.3400000000001</v>
       </c>
       <c r="AJ13" s="44">
         <f>+T29+'Punters 2023'!AF13</f>
-        <v>688.07999999999993</v>
+        <v>766.69</v>
       </c>
       <c r="AK13" s="49">
         <f t="shared" si="5"/>
-        <v>-458.26000000000022</v>
+        <v>-429.65000000000009</v>
       </c>
       <c r="AL13" s="47">
         <f t="shared" si="6"/>
-        <v>-0.39975923373519212</v>
+        <v>-0.35913703462226459</v>
       </c>
     </row>
     <row r="14" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -15543,22 +15682,22 @@
       </c>
       <c r="AE14" s="1">
         <f t="shared" si="4"/>
-        <v>390</v>
+        <v>895</v>
       </c>
       <c r="AF14" s="1">
         <f t="shared" si="4"/>
-        <v>398.76</v>
+        <v>629.02</v>
       </c>
       <c r="AG14" s="1">
         <f t="shared" si="1"/>
-        <v>8.7599999999999909</v>
+        <v>-265.98</v>
       </c>
       <c r="AH14" s="44" t="s">
         <v>78</v>
       </c>
       <c r="AI14" s="44">
         <f>+Q29+'Punters 2023'!AE14</f>
-        <v>1148</v>
+        <v>1198</v>
       </c>
       <c r="AJ14" s="44">
         <f>+R29+'Punters 2023'!AF14</f>
@@ -15566,11 +15705,11 @@
       </c>
       <c r="AK14" s="49">
         <f t="shared" si="5"/>
-        <v>-510.53</v>
+        <v>-560.53</v>
       </c>
       <c r="AL14" s="47">
         <f t="shared" si="6"/>
-        <v>-0.44471254355400697</v>
+        <v>-0.4678881469115192</v>
       </c>
     </row>
     <row r="15" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -15613,22 +15752,22 @@
       </c>
       <c r="AE15" s="1">
         <f t="shared" si="4"/>
-        <v>390</v>
+        <v>895</v>
       </c>
       <c r="AF15" s="1">
         <f t="shared" si="4"/>
-        <v>398.76</v>
+        <v>629.02</v>
       </c>
       <c r="AG15" s="1">
         <f t="shared" si="1"/>
-        <v>8.7599999999999909</v>
+        <v>-265.98</v>
       </c>
       <c r="AH15" s="44" t="s">
         <v>79</v>
       </c>
       <c r="AI15" s="44">
         <f>+O29+'Punters 2023'!AE15</f>
-        <v>1157.7</v>
+        <v>1207.7</v>
       </c>
       <c r="AJ15" s="44">
         <f>+P29+'Punters 2023'!AF15</f>
@@ -15636,11 +15775,11 @@
       </c>
       <c r="AK15" s="50">
         <f t="shared" si="5"/>
-        <v>412.76999999999975</v>
+        <v>362.76999999999975</v>
       </c>
       <c r="AL15" s="45">
         <f t="shared" si="6"/>
-        <v>0.35654314589271807</v>
+        <v>0.30038088929369855</v>
       </c>
     </row>
     <row r="16" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -15683,22 +15822,22 @@
       </c>
       <c r="AE16" s="1">
         <f t="shared" si="4"/>
-        <v>390</v>
+        <v>895</v>
       </c>
       <c r="AF16" s="1">
         <f t="shared" si="4"/>
-        <v>398.76</v>
+        <v>629.02</v>
       </c>
       <c r="AG16" s="1">
         <f t="shared" si="1"/>
-        <v>8.7599999999999909</v>
+        <v>-265.98</v>
       </c>
       <c r="AH16" s="44" t="s">
         <v>80</v>
       </c>
       <c r="AI16" s="44">
         <f>+G29+'Punters 2023'!AE16</f>
-        <v>477</v>
+        <v>502</v>
       </c>
       <c r="AJ16" s="44">
         <f>+H29+'Punters 2023'!AF16</f>
@@ -15706,11 +15845,11 @@
       </c>
       <c r="AK16" s="49">
         <f t="shared" si="5"/>
-        <v>-325.75</v>
+        <v>-350.75</v>
       </c>
       <c r="AL16" s="47">
         <f t="shared" si="6"/>
-        <v>-0.68291404612159334</v>
+        <v>-0.69870517928286857</v>
       </c>
     </row>
     <row r="17" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -15753,15 +15892,15 @@
       </c>
       <c r="AE17" s="1">
         <f t="shared" si="4"/>
-        <v>390</v>
+        <v>895</v>
       </c>
       <c r="AF17" s="1">
         <f t="shared" si="4"/>
-        <v>398.76</v>
+        <v>629.02</v>
       </c>
       <c r="AG17" s="1">
         <f t="shared" si="1"/>
-        <v>8.7599999999999909</v>
+        <v>-265.98</v>
       </c>
       <c r="AH17" s="44" t="s">
         <v>116</v>
@@ -15811,15 +15950,15 @@
       </c>
       <c r="AE18" s="1">
         <f t="shared" si="4"/>
-        <v>390</v>
+        <v>895</v>
       </c>
       <c r="AF18" s="1">
         <f t="shared" si="4"/>
-        <v>398.76</v>
+        <v>629.02</v>
       </c>
       <c r="AG18" s="1">
         <f t="shared" si="1"/>
-        <v>8.7599999999999909</v>
+        <v>-265.98</v>
       </c>
       <c r="AH18" s="44" t="s">
         <v>117</v>
@@ -15869,15 +16008,15 @@
       </c>
       <c r="AE19" s="1">
         <f t="shared" si="4"/>
-        <v>390</v>
+        <v>895</v>
       </c>
       <c r="AF19" s="1">
         <f t="shared" si="4"/>
-        <v>398.76</v>
+        <v>629.02</v>
       </c>
       <c r="AG19" s="1">
         <f t="shared" si="1"/>
-        <v>8.7599999999999909</v>
+        <v>-265.98</v>
       </c>
       <c r="AH19" s="1"/>
     </row>
@@ -15921,15 +16060,15 @@
       </c>
       <c r="AE20" s="1">
         <f t="shared" si="4"/>
-        <v>390</v>
+        <v>895</v>
       </c>
       <c r="AF20" s="1">
         <f t="shared" si="4"/>
-        <v>398.76</v>
+        <v>629.02</v>
       </c>
       <c r="AG20" s="1">
         <f t="shared" si="1"/>
-        <v>8.7599999999999909</v>
+        <v>-265.98</v>
       </c>
       <c r="AH20" s="1"/>
     </row>
@@ -15973,15 +16112,15 @@
       </c>
       <c r="AE21" s="1">
         <f t="shared" si="4"/>
-        <v>390</v>
+        <v>895</v>
       </c>
       <c r="AF21" s="1">
         <f t="shared" si="4"/>
-        <v>398.76</v>
+        <v>629.02</v>
       </c>
       <c r="AG21" s="1">
         <f t="shared" si="1"/>
-        <v>8.7599999999999909</v>
+        <v>-265.98</v>
       </c>
       <c r="AH21" s="1"/>
     </row>
@@ -16025,15 +16164,15 @@
       </c>
       <c r="AE22" s="1">
         <f t="shared" ref="AE22:AF27" si="7">AE21+AC22</f>
-        <v>390</v>
+        <v>895</v>
       </c>
       <c r="AF22" s="1">
         <f t="shared" si="7"/>
-        <v>398.76</v>
+        <v>629.02</v>
       </c>
       <c r="AG22" s="1">
         <f t="shared" si="1"/>
-        <v>8.7599999999999909</v>
+        <v>-265.98</v>
       </c>
       <c r="AH22" s="1"/>
     </row>
@@ -16077,15 +16216,15 @@
       </c>
       <c r="AE23" s="1">
         <f t="shared" si="7"/>
-        <v>390</v>
+        <v>895</v>
       </c>
       <c r="AF23" s="1">
         <f t="shared" si="7"/>
-        <v>398.76</v>
+        <v>629.02</v>
       </c>
       <c r="AG23" s="1">
         <f t="shared" si="1"/>
-        <v>8.7599999999999909</v>
+        <v>-265.98</v>
       </c>
       <c r="AH23" s="1"/>
     </row>
@@ -16129,15 +16268,15 @@
       </c>
       <c r="AE24" s="1">
         <f t="shared" si="7"/>
-        <v>390</v>
+        <v>895</v>
       </c>
       <c r="AF24" s="1">
         <f t="shared" si="7"/>
-        <v>398.76</v>
+        <v>629.02</v>
       </c>
       <c r="AG24" s="1">
         <f t="shared" si="1"/>
-        <v>8.7599999999999909</v>
+        <v>-265.98</v>
       </c>
       <c r="AH24" s="1"/>
     </row>
@@ -16181,15 +16320,15 @@
       </c>
       <c r="AE25" s="1">
         <f t="shared" si="7"/>
-        <v>390</v>
+        <v>895</v>
       </c>
       <c r="AF25" s="1">
         <f t="shared" si="7"/>
-        <v>398.76</v>
+        <v>629.02</v>
       </c>
       <c r="AG25" s="1">
         <f t="shared" si="1"/>
-        <v>8.7599999999999909</v>
+        <v>-265.98</v>
       </c>
       <c r="AH25" s="1"/>
     </row>
@@ -16233,15 +16372,15 @@
       </c>
       <c r="AE26" s="1">
         <f t="shared" si="7"/>
-        <v>390</v>
+        <v>895</v>
       </c>
       <c r="AF26" s="1">
         <f t="shared" si="7"/>
-        <v>398.76</v>
+        <v>629.02</v>
       </c>
       <c r="AG26" s="1">
         <f t="shared" si="1"/>
-        <v>8.7599999999999909</v>
+        <v>-265.98</v>
       </c>
       <c r="AH26" s="1"/>
     </row>
@@ -16285,15 +16424,15 @@
       </c>
       <c r="AE27" s="1">
         <f t="shared" si="7"/>
-        <v>390</v>
+        <v>895</v>
       </c>
       <c r="AF27" s="1">
         <f t="shared" si="7"/>
-        <v>398.76</v>
+        <v>629.02</v>
       </c>
       <c r="AG27" s="1">
         <f t="shared" si="1"/>
-        <v>8.7599999999999909</v>
+        <v>-265.98</v>
       </c>
       <c r="AH27" s="1"/>
     </row>
@@ -16346,7 +16485,7 @@
       </c>
       <c r="C29" s="18">
         <f t="shared" ref="C29:AD29" si="8">SUM(C4:C28)</f>
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="D29" s="18">
         <f t="shared" si="8"/>
@@ -16354,7 +16493,7 @@
       </c>
       <c r="E29" s="18">
         <f t="shared" si="8"/>
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="F29" s="18">
         <f t="shared" si="8"/>
@@ -16362,7 +16501,7 @@
       </c>
       <c r="G29" s="18">
         <f t="shared" si="8"/>
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="H29" s="18">
         <f t="shared" si="8"/>
@@ -16370,7 +16509,7 @@
       </c>
       <c r="I29" s="18">
         <f t="shared" si="8"/>
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="J29" s="18">
         <f t="shared" si="8"/>
@@ -16378,7 +16517,7 @@
       </c>
       <c r="K29" s="18">
         <f t="shared" si="8"/>
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="L29" s="18">
         <f t="shared" si="8"/>
@@ -16386,7 +16525,7 @@
       </c>
       <c r="M29" s="18">
         <f t="shared" si="8"/>
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="N29" s="18">
         <f t="shared" si="8"/>
@@ -16394,7 +16533,7 @@
       </c>
       <c r="O29" s="18">
         <f t="shared" si="8"/>
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="P29" s="18">
         <f t="shared" si="8"/>
@@ -16402,7 +16541,7 @@
       </c>
       <c r="Q29" s="18">
         <f t="shared" si="8"/>
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="R29" s="18">
         <f t="shared" si="8"/>
@@ -16410,15 +16549,15 @@
       </c>
       <c r="S29" s="18">
         <f t="shared" si="8"/>
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="T29" s="18">
         <f>SUM(T4:T28)</f>
-        <v>190</v>
+        <v>268.61</v>
       </c>
       <c r="U29" s="18">
         <f t="shared" si="8"/>
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="V29" s="21">
         <f t="shared" si="8"/>
@@ -16426,19 +16565,19 @@
       </c>
       <c r="W29" s="18">
         <f t="shared" ref="W29:X29" si="9">SUM(W4:W28)</f>
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="X29" s="21">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>66.25</v>
       </c>
       <c r="Y29" s="18">
         <f t="shared" ref="Y29:Z29" si="10">SUM(Y4:Y28)</f>
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="Z29" s="21">
         <f t="shared" si="10"/>
-        <v>99.38</v>
+        <v>184.78</v>
       </c>
       <c r="AA29" s="18">
         <f t="shared" si="8"/>
@@ -16450,11 +16589,11 @@
       </c>
       <c r="AC29" s="29">
         <f t="shared" si="8"/>
-        <v>390</v>
+        <v>895</v>
       </c>
       <c r="AD29" s="18">
         <f t="shared" si="8"/>
-        <v>398.76</v>
+        <v>629.02</v>
       </c>
       <c r="AE29" s="1"/>
     </row>
@@ -16485,7 +16624,7 @@
       </c>
       <c r="P30" s="28">
         <f>(P29-O29)/O29</f>
-        <v>3.3752</v>
+        <v>0.45839999999999992</v>
       </c>
       <c r="R30" s="28">
         <f>(R29-Q29)/Q29</f>
@@ -16493,7 +16632,7 @@
       </c>
       <c r="T30" s="22">
         <f>(T29-S29)/S29</f>
-        <v>6.6</v>
+        <v>2.581466666666667</v>
       </c>
       <c r="V30" s="28">
         <f>(V29-U29)/U29</f>
@@ -16501,11 +16640,11 @@
       </c>
       <c r="X30" s="28">
         <f>(X29-W29)/W29</f>
-        <v>-1</v>
+        <v>-0.11666666666666667</v>
       </c>
       <c r="Z30" s="28">
         <f>(Z29-Y29)/Y29</f>
-        <v>2.9751999999999996</v>
+        <v>1.4637333333333333</v>
       </c>
     </row>
     <row r="31" spans="2:38" x14ac:dyDescent="0.55000000000000004">
@@ -16516,7 +16655,7 @@
       <c r="H31" s="66"/>
       <c r="I31" s="62">
         <f>C29+E29+G29+I29+K29+M29+O29+Q29+S29+U29+AA29+W29+Y29</f>
-        <v>390</v>
+        <v>895</v>
       </c>
       <c r="J31" s="63"/>
     </row>
@@ -16527,14 +16666,14 @@
       <c r="H32" s="70"/>
       <c r="I32" s="62">
         <f>+D29+F29+H29+J29+L29+N29+P29+R29+T29+V29+AB29+X29+Z29</f>
-        <v>398.76</v>
+        <v>629.02</v>
       </c>
       <c r="J32" s="63"/>
     </row>
     <row r="33" spans="3:25" x14ac:dyDescent="0.55000000000000004">
       <c r="I33" s="62">
         <f>I32-I31</f>
-        <v>8.7599999999999909</v>
+        <v>-265.98</v>
       </c>
       <c r="J33" s="63"/>
       <c r="Y33">
@@ -16545,7 +16684,7 @@
     <row r="34" spans="3:25" x14ac:dyDescent="0.55000000000000004">
       <c r="C34" s="36">
         <f>C29+E29+G29+I29</f>
-        <v>190</v>
+        <v>300</v>
       </c>
       <c r="D34" s="36">
         <f>D29+F29+H29+J29</f>
@@ -16553,11 +16692,11 @@
       </c>
       <c r="E34" s="37">
         <f>D34-C34</f>
-        <v>-190</v>
+        <v>-300</v>
       </c>
       <c r="I34" s="38">
         <f>O29+K29+M29+Q29</f>
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="J34" s="38">
         <f>P29+L29+N29</f>
@@ -16565,19 +16704,19 @@
       </c>
       <c r="K34" s="39">
         <f>J34-I34</f>
-        <v>9.3799999999999955</v>
+        <v>-190.62</v>
       </c>
       <c r="O34" s="40">
         <f>U29+W29+Y29+S29</f>
-        <v>100</v>
+        <v>295</v>
       </c>
       <c r="P34" s="40">
         <f>V29+X29+T29+Z29</f>
-        <v>289.38</v>
+        <v>519.64</v>
       </c>
       <c r="Q34" s="41">
         <f>P34-O34</f>
-        <v>189.38</v>
+        <v>224.64</v>
       </c>
       <c r="X34" s="55"/>
       <c r="Y34">
@@ -16595,13 +16734,13 @@
       <c r="I35" s="38"/>
       <c r="J35" s="34">
         <f>(J34-I34)/I34</f>
-        <v>9.3799999999999953E-2</v>
+        <v>-0.63539999999999996</v>
       </c>
       <c r="K35" s="39"/>
       <c r="O35" s="40"/>
       <c r="P35" s="34">
         <f>(P34-O34)/O34</f>
-        <v>1.8937999999999999</v>
+        <v>0.76149152542372878</v>
       </c>
       <c r="Q35" s="41"/>
       <c r="X35" s="55"/>
@@ -16621,7 +16760,7 @@
       <c r="H38" s="42"/>
       <c r="I38" s="72">
         <f>I36+I33</f>
-        <v>2408.8100000000004</v>
+        <v>2134.0700000000002</v>
       </c>
       <c r="J38" s="72"/>
       <c r="M38" s="33"/>
@@ -16632,7 +16771,7 @@
     <row r="42" spans="3:25" x14ac:dyDescent="0.55000000000000004">
       <c r="C42" s="1">
         <f>C29+E29+G29+I29</f>
-        <v>190</v>
+        <v>300</v>
       </c>
       <c r="D42" s="1">
         <f>D29+F29+H29+J29</f>
@@ -16640,7 +16779,7 @@
       </c>
       <c r="I42" s="1">
         <f>O29+K29+M29</f>
-        <v>75</v>
+        <v>225</v>
       </c>
       <c r="J42" s="1">
         <f>P29+L29+N29</f>
@@ -16648,30 +16787,30 @@
       </c>
       <c r="O42" s="1">
         <f>U29+Q29+S29</f>
-        <v>75</v>
+        <v>220</v>
       </c>
       <c r="P42" s="1">
         <f>V29+R29+T29</f>
-        <v>190</v>
+        <v>268.61</v>
       </c>
     </row>
     <row r="43" spans="3:25" x14ac:dyDescent="0.55000000000000004">
       <c r="D43" s="1">
         <f>D42-C42</f>
-        <v>-190</v>
+        <v>-300</v>
       </c>
       <c r="J43" s="33">
         <f>J42-I42</f>
-        <v>34.379999999999995</v>
+        <v>-115.62</v>
       </c>
       <c r="P43" s="33">
         <f>P42-O42</f>
-        <v>115</v>
+        <v>48.610000000000014</v>
       </c>
     </row>
     <row r="45" spans="3:25" x14ac:dyDescent="0.55000000000000004">
       <c r="V45" t="s">
-        <v>118</v>
+        <v>148</v>
       </c>
     </row>
     <row r="46" spans="3:25" x14ac:dyDescent="0.55000000000000004">
@@ -16679,13 +16818,13 @@
         <v>88</v>
       </c>
       <c r="J46" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="V46" t="s">
         <v>89</v>
       </c>
       <c r="W46">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="3:25" x14ac:dyDescent="0.55000000000000004">
@@ -16705,7 +16844,7 @@
         <v>12</v>
       </c>
       <c r="W47">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="3:25" x14ac:dyDescent="0.55000000000000004">
@@ -16726,7 +16865,7 @@
         <v>93</v>
       </c>
       <c r="W48">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="4:23" x14ac:dyDescent="0.55000000000000004">
@@ -16756,7 +16895,7 @@
       </c>
       <c r="E50" s="1">
         <f>SUM(T29)</f>
-        <v>190</v>
+        <v>268.61</v>
       </c>
       <c r="J50" t="s">
         <v>94</v>
@@ -16768,7 +16907,7 @@
         <v>9</v>
       </c>
       <c r="W50">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="4:23" x14ac:dyDescent="0.55000000000000004">
@@ -16783,13 +16922,13 @@
         <v>95</v>
       </c>
       <c r="K51">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V51" t="s">
         <v>11</v>
       </c>
       <c r="W51">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="4:23" x14ac:dyDescent="0.55000000000000004">
@@ -16810,7 +16949,7 @@
         <v>96</v>
       </c>
       <c r="W52">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53" spans="4:23" x14ac:dyDescent="0.55000000000000004">
@@ -16825,7 +16964,7 @@
         <v>97</v>
       </c>
       <c r="K53">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V53" t="s">
         <v>98</v>
@@ -16852,7 +16991,7 @@
         <v>97</v>
       </c>
       <c r="W54">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="55" spans="4:23" x14ac:dyDescent="0.55000000000000004">
@@ -16861,7 +17000,7 @@
       </c>
       <c r="E55" s="1">
         <f>SUM(X29)</f>
-        <v>0</v>
+        <v>66.25</v>
       </c>
       <c r="J55" t="s">
         <v>89</v>
@@ -16882,7 +17021,7 @@
       </c>
       <c r="E56" s="1">
         <f>SUM(Z29)</f>
-        <v>99.38</v>
+        <v>184.78</v>
       </c>
       <c r="J56" t="s">
         <v>96</v>
@@ -16891,28 +17030,28 @@
         <v>0</v>
       </c>
       <c r="V56" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="W56">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="4:23" x14ac:dyDescent="0.55000000000000004">
       <c r="D57" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E57" s="1">
         <f>SUM(H29)</f>
         <v>0</v>
       </c>
       <c r="J57" t="s">
+        <v>118</v>
+      </c>
+      <c r="K57">
+        <v>0</v>
+      </c>
+      <c r="V57" t="s">
         <v>119</v>
-      </c>
-      <c r="K57">
-        <v>0</v>
-      </c>
-      <c r="V57" t="s">
-        <v>120</v>
       </c>
       <c r="W57">
         <v>0</v>
@@ -16920,24 +17059,24 @@
     </row>
     <row r="58" spans="4:23" x14ac:dyDescent="0.55000000000000004">
       <c r="D58" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E58" s="1">
         <f>SUM(D29)</f>
         <v>0</v>
       </c>
       <c r="J58" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K58">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V58" t="s">
         <v>99</v>
       </c>
       <c r="W58">
         <f>SUM(W46:W57)</f>
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="59" spans="4:23" x14ac:dyDescent="0.55000000000000004">
@@ -16961,14 +17100,14 @@
       </c>
       <c r="E60" s="1">
         <f>SUM(E48:E59)</f>
-        <v>398.76</v>
+        <v>629.02</v>
       </c>
       <c r="J60" t="s">
         <v>99</v>
       </c>
       <c r="K60">
         <f>SUM(K48:K59)</f>
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -17002,7 +17141,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B9A81C0-C60A-48E0-A96A-1599E0795A8C}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
@@ -17018,16 +17157,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" t="s">
         <v>121</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>122</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>123</v>
-      </c>
-      <c r="D1" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -17035,13 +17174,13 @@
         <v>97</v>
       </c>
       <c r="B2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C2" s="60">
         <v>376.63</v>
       </c>
       <c r="D2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -17049,13 +17188,13 @@
         <v>93</v>
       </c>
       <c r="B3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C3" s="60">
         <v>236.2</v>
       </c>
       <c r="D3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -17069,7 +17208,7 @@
         <v>375.45</v>
       </c>
       <c r="D4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -17083,7 +17222,7 @@
         <v>82.5</v>
       </c>
       <c r="D5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -17097,7 +17236,7 @@
         <v>163.13</v>
       </c>
       <c r="D6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -17111,7 +17250,7 @@
         <v>70</v>
       </c>
       <c r="D7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -17125,7 +17264,189 @@
         <v>110</v>
       </c>
       <c r="D8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="61">
+        <v>10</v>
+      </c>
+      <c r="C9" s="61">
+        <v>77</v>
+      </c>
+      <c r="D9" t="s">
         <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>97</v>
+      </c>
+      <c r="B10" s="61">
+        <v>5</v>
+      </c>
+      <c r="C10" s="61">
+        <v>125</v>
+      </c>
+      <c r="D10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>97</v>
+      </c>
+      <c r="B11" s="61">
+        <v>10</v>
+      </c>
+      <c r="C11" s="61">
+        <v>150</v>
+      </c>
+      <c r="D11" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" s="61">
+        <v>5</v>
+      </c>
+      <c r="C12" s="60">
+        <v>72.5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13" s="60">
+        <v>2.5</v>
+      </c>
+      <c r="C13" s="60">
+        <v>46.3</v>
+      </c>
+      <c r="D13" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" s="61">
+        <v>5</v>
+      </c>
+      <c r="C14" s="61">
+        <v>30</v>
+      </c>
+      <c r="D14" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B15" s="61">
+        <v>5</v>
+      </c>
+      <c r="C15" s="61">
+        <v>60</v>
+      </c>
+      <c r="D15" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>118</v>
+      </c>
+      <c r="B16" s="61">
+        <v>25</v>
+      </c>
+      <c r="C16" s="60">
+        <v>411.75</v>
+      </c>
+      <c r="D16" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>93</v>
+      </c>
+      <c r="B17" s="61">
+        <v>5</v>
+      </c>
+      <c r="C17" s="60">
+        <v>79.67</v>
+      </c>
+      <c r="D17" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>141</v>
+      </c>
+      <c r="B18" s="61">
+        <v>5</v>
+      </c>
+      <c r="C18" s="61">
+        <v>60</v>
+      </c>
+      <c r="D18" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
+        <v>143</v>
+      </c>
+      <c r="B19" s="61">
+        <v>5</v>
+      </c>
+      <c r="C19" s="61">
+        <v>140</v>
+      </c>
+      <c r="D19" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
+        <v>96</v>
+      </c>
+      <c r="B20" s="61">
+        <v>5</v>
+      </c>
+      <c r="C20" s="61">
+        <v>20</v>
+      </c>
+      <c r="D20" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" s="61">
+        <v>5</v>
+      </c>
+      <c r="C21" s="60">
+        <v>43.75</v>
+      </c>
+      <c r="D21" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -17401,16 +17722,16 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4D7A62A-0CB5-48B0-A73A-0A91BCC8EAEF}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="21753bd8-bffc-4cd2-a328-982ee854c895"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="3e1ffae5-f160-4019-9720-1b11bf1b81a3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Updating Spreadsheet with latest
</commit_message>
<xml_diff>
--- a/public/Data/HEMANPUNTERS.xlsx
+++ b/public/Data/HEMANPUNTERS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bturnor\source\repos\PersonalWork\seeMore\public\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C020696A-46D5-4352-8593-37B7F73EB871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6A576FA9-1E9D-4FAA-B5D5-E17305E717D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" firstSheet="6" activeTab="6" xr2:uid="{525E8989-1938-4309-A4CF-8F1D15E362FB}"/>
+    <workbookView xWindow="1344" yWindow="2502" windowWidth="17100" windowHeight="9900" firstSheet="6" activeTab="6" xr2:uid="{525E8989-1938-4309-A4CF-8F1D15E362FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Punters club" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="172">
   <si>
     <t>HE_MAN PUNTERS 2019</t>
   </si>
@@ -421,10 +421,10 @@
     <t>pano</t>
   </si>
   <si>
-    <t>1 leg losses as at 16 June 2025</t>
+    <t>1 leg losses as at 23 July 2025</t>
   </si>
   <si>
-    <t>Strikes for 2025 Season at 10 June 2025</t>
+    <t>Strikes for 2025 Season at 24 July 2025</t>
   </si>
   <si>
     <t>Pano</t>
@@ -496,7 +496,7 @@
     <t>Colby McKercher 8/15 touches</t>
   </si>
   <si>
-    <t>Swikowski 6/15 touches</t>
+    <t>Switkowski 6/15 touches</t>
   </si>
   <si>
     <t>Logan Morris 0/2 goals</t>
@@ -563,6 +563,24 @@
   </si>
   <si>
     <t>Cody Brundage KO/TKO???</t>
+  </si>
+  <si>
+    <t>Max gawn 14/15 touches</t>
+  </si>
+  <si>
+    <t>Caleb Serong most disposals</t>
+  </si>
+  <si>
+    <t>Petracca 23/24 disposals</t>
+  </si>
+  <si>
+    <t>MucCluggage 18/25.5 disposals</t>
+  </si>
+  <si>
+    <t>Herbie Farnworth anytime try scorer</t>
+  </si>
+  <si>
+    <t>GWS Essendon over 171.5, total 160</t>
   </si>
 </sst>
 </file>
@@ -1282,9 +1300,6 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1303,16 +1318,25 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="12" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1328,12 +1352,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4068,50 +4086,50 @@
   <sheetData>
     <row r="1" spans="2:27" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="2" spans="2:27" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="C2" s="62" t="s">
+      <c r="C2" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62" t="s">
+      <c r="D2" s="68"/>
+      <c r="E2" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62" t="s">
+      <c r="F2" s="68"/>
+      <c r="G2" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62" t="s">
+      <c r="H2" s="68"/>
+      <c r="I2" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62" t="s">
+      <c r="J2" s="68"/>
+      <c r="K2" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="62"/>
-      <c r="M2" s="62" t="s">
+      <c r="L2" s="68"/>
+      <c r="M2" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="62"/>
-      <c r="O2" s="62" t="s">
+      <c r="N2" s="68"/>
+      <c r="O2" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="62"/>
-      <c r="Q2" s="62" t="s">
-        <v>25</v>
-      </c>
-      <c r="R2" s="62"/>
-      <c r="S2" s="62" t="s">
+      <c r="P2" s="68"/>
+      <c r="Q2" s="68" t="s">
+        <v>25</v>
+      </c>
+      <c r="R2" s="68"/>
+      <c r="S2" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="T2" s="62"/>
-      <c r="U2" s="62" t="s">
+      <c r="T2" s="68"/>
+      <c r="U2" s="68" t="s">
         <v>27</v>
       </c>
       <c r="V2" s="69"/>
-      <c r="W2" s="68" t="s">
+      <c r="W2" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="X2" s="62"/>
+      <c r="X2" s="68"/>
     </row>
     <row r="3" spans="2:27" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B3" s="32" t="s">
@@ -5672,34 +5690,34 @@
       </c>
     </row>
     <row r="29" spans="2:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="F29" s="65" t="s">
+      <c r="F29" s="64" t="s">
         <v>56</v>
       </c>
-      <c r="G29" s="66"/>
-      <c r="H29" s="67"/>
-      <c r="I29" s="63">
+      <c r="G29" s="65"/>
+      <c r="H29" s="66"/>
+      <c r="I29" s="62">
         <f>C27+E27+G27+I27+K27+M27+O27+Q27+S27+U27</f>
         <v>2469.42</v>
       </c>
-      <c r="J29" s="64"/>
+      <c r="J29" s="63"/>
     </row>
     <row r="30" spans="2:27" x14ac:dyDescent="0.55000000000000004">
       <c r="G30" s="70" t="s">
         <v>57</v>
       </c>
       <c r="H30" s="70"/>
-      <c r="I30" s="63">
+      <c r="I30" s="62">
         <f>+D27+F27+H27+J27+L27+N27+P27+R27+T27+V27</f>
         <v>1774.69</v>
       </c>
-      <c r="J30" s="64"/>
+      <c r="J30" s="63"/>
     </row>
     <row r="31" spans="2:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="I31" s="63">
+      <c r="I31" s="62">
         <f>I30-I29</f>
         <v>-694.73</v>
       </c>
-      <c r="J31" s="64"/>
+      <c r="J31" s="63"/>
     </row>
     <row r="32" spans="2:27" x14ac:dyDescent="0.55000000000000004">
       <c r="C32" s="1">
@@ -5748,11 +5766,11 @@
       </c>
     </row>
     <row r="34" spans="3:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="I34" s="64">
+      <c r="I34" s="63">
         <f>I33+I31</f>
         <v>505.27</v>
       </c>
-      <c r="J34" s="64"/>
+      <c r="J34" s="63"/>
     </row>
     <row r="38" spans="3:16" x14ac:dyDescent="0.55000000000000004">
       <c r="C38" s="1">
@@ -5796,6 +5814,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
     <mergeCell ref="I30:J30"/>
     <mergeCell ref="F29:H29"/>
     <mergeCell ref="I31:J31"/>
@@ -5808,11 +5831,6 @@
     <mergeCell ref="S2:T2"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="I29:J29"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5845,50 +5863,50 @@
   <sheetData>
     <row r="1" spans="2:27" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="2" spans="2:27" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="C2" s="62" t="s">
+      <c r="C2" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62" t="s">
+      <c r="D2" s="68"/>
+      <c r="E2" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="62"/>
-      <c r="G2" s="72" t="s">
+      <c r="F2" s="68"/>
+      <c r="G2" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="68"/>
-      <c r="I2" s="62" t="s">
+      <c r="H2" s="67"/>
+      <c r="I2" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62" t="s">
+      <c r="J2" s="68"/>
+      <c r="K2" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="62"/>
-      <c r="M2" s="62" t="s">
-        <v>25</v>
-      </c>
-      <c r="N2" s="62"/>
-      <c r="O2" s="62" t="s">
+      <c r="L2" s="68"/>
+      <c r="M2" s="68" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="68"/>
+      <c r="O2" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="62"/>
-      <c r="Q2" s="62" t="s">
+      <c r="P2" s="68"/>
+      <c r="Q2" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="R2" s="62"/>
-      <c r="S2" s="62" t="s">
+      <c r="R2" s="68"/>
+      <c r="S2" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="T2" s="62"/>
-      <c r="U2" s="62" t="s">
+      <c r="T2" s="68"/>
+      <c r="U2" s="68" t="s">
         <v>27</v>
       </c>
       <c r="V2" s="69"/>
-      <c r="W2" s="68" t="s">
+      <c r="W2" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="X2" s="62"/>
+      <c r="X2" s="68"/>
     </row>
     <row r="3" spans="2:27" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B3" s="32" t="s">
@@ -7248,34 +7266,34 @@
       </c>
     </row>
     <row r="29" spans="2:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="F29" s="65" t="s">
+      <c r="F29" s="64" t="s">
         <v>56</v>
       </c>
-      <c r="G29" s="66"/>
-      <c r="H29" s="67"/>
-      <c r="I29" s="63">
+      <c r="G29" s="65"/>
+      <c r="H29" s="66"/>
+      <c r="I29" s="62">
         <f>C27+E27+G27+I27+K27+M27+O27+Q27+S27+U27</f>
         <v>1788.24</v>
       </c>
-      <c r="J29" s="64"/>
+      <c r="J29" s="63"/>
     </row>
     <row r="30" spans="2:27" x14ac:dyDescent="0.55000000000000004">
       <c r="G30" s="70" t="s">
         <v>57</v>
       </c>
       <c r="H30" s="70"/>
-      <c r="I30" s="63">
+      <c r="I30" s="62">
         <f>+D27+F27+H27+J27+L27+N27+P27+R27+T27+V27</f>
         <v>2492.1999999999998</v>
       </c>
-      <c r="J30" s="64"/>
+      <c r="J30" s="63"/>
     </row>
     <row r="31" spans="2:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="I31" s="63">
+      <c r="I31" s="62">
         <f>I30-I29</f>
         <v>703.95999999999981</v>
       </c>
-      <c r="J31" s="64"/>
+      <c r="J31" s="63"/>
     </row>
     <row r="32" spans="2:27" x14ac:dyDescent="0.55000000000000004">
       <c r="C32" s="36">
@@ -7329,11 +7347,11 @@
         <v>64</v>
       </c>
       <c r="H34" s="42"/>
-      <c r="I34" s="71">
+      <c r="I34" s="72">
         <f>I33+I31</f>
         <v>1303.9599999999998</v>
       </c>
-      <c r="J34" s="71"/>
+      <c r="J34" s="72"/>
       <c r="M34" s="33"/>
     </row>
     <row r="38" spans="3:16" x14ac:dyDescent="0.55000000000000004">
@@ -7378,11 +7396,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="O2:P2"/>
     <mergeCell ref="Q2:R2"/>
     <mergeCell ref="S2:T2"/>
     <mergeCell ref="U2:V2"/>
@@ -7390,11 +7408,11 @@
     <mergeCell ref="F29:H29"/>
     <mergeCell ref="I29:J29"/>
     <mergeCell ref="M2:N2"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7428,54 +7446,54 @@
   <sheetData>
     <row r="1" spans="2:34" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="2" spans="2:34" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="C2" s="62" t="s">
+      <c r="C2" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62" t="s">
+      <c r="D2" s="68"/>
+      <c r="E2" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62" t="s">
+      <c r="F2" s="68"/>
+      <c r="G2" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62" t="s">
+      <c r="H2" s="68"/>
+      <c r="I2" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62" t="s">
+      <c r="J2" s="68"/>
+      <c r="K2" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="62"/>
-      <c r="M2" s="62" t="s">
+      <c r="L2" s="68"/>
+      <c r="M2" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="N2" s="62"/>
-      <c r="O2" s="62" t="s">
+      <c r="N2" s="68"/>
+      <c r="O2" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="62"/>
-      <c r="Q2" s="62" t="s">
-        <v>25</v>
-      </c>
-      <c r="R2" s="62"/>
-      <c r="S2" s="62" t="s">
+      <c r="P2" s="68"/>
+      <c r="Q2" s="68" t="s">
+        <v>25</v>
+      </c>
+      <c r="R2" s="68"/>
+      <c r="S2" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="T2" s="62"/>
-      <c r="U2" s="62" t="s">
+      <c r="T2" s="68"/>
+      <c r="U2" s="68" t="s">
         <v>65</v>
       </c>
       <c r="V2" s="69"/>
-      <c r="W2" s="62" t="s">
+      <c r="W2" s="68" t="s">
         <v>66</v>
       </c>
       <c r="X2" s="69"/>
-      <c r="Y2" s="68" t="s">
+      <c r="Y2" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="Z2" s="62"/>
+      <c r="Z2" s="68"/>
     </row>
     <row r="3" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B3" s="32" t="s">
@@ -9529,34 +9547,34 @@
       </c>
     </row>
     <row r="31" spans="2:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="F31" s="65" t="s">
+      <c r="F31" s="64" t="s">
         <v>56</v>
       </c>
-      <c r="G31" s="66"/>
-      <c r="H31" s="67"/>
-      <c r="I31" s="63">
+      <c r="G31" s="65"/>
+      <c r="H31" s="66"/>
+      <c r="I31" s="62">
         <f>C29+E29+G29+I29+K29+M29+O29+Q29+S29+U29+W29</f>
         <v>2521.33</v>
       </c>
-      <c r="J31" s="64"/>
+      <c r="J31" s="63"/>
     </row>
     <row r="32" spans="2:30" x14ac:dyDescent="0.55000000000000004">
       <c r="G32" s="70" t="s">
         <v>57</v>
       </c>
       <c r="H32" s="70"/>
-      <c r="I32" s="63">
+      <c r="I32" s="62">
         <f>+D29+F29+H29+J29+L29+N29+P29+R29+T29+V29+X29</f>
         <v>2997.5899999999997</v>
       </c>
-      <c r="J32" s="64"/>
+      <c r="J32" s="63"/>
     </row>
     <row r="33" spans="3:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="I33" s="63">
+      <c r="I33" s="62">
         <f>I32-I31</f>
         <v>476.25999999999976</v>
       </c>
-      <c r="J33" s="64"/>
+      <c r="J33" s="63"/>
     </row>
     <row r="34" spans="3:17" x14ac:dyDescent="0.55000000000000004">
       <c r="C34" s="36">
@@ -9609,11 +9627,11 @@
         <v>64</v>
       </c>
       <c r="H36" s="42"/>
-      <c r="I36" s="71">
+      <c r="I36" s="72">
         <f>I35+I33</f>
         <v>2476.2599999999998</v>
       </c>
-      <c r="J36" s="71"/>
+      <c r="J36" s="72"/>
       <c r="M36" s="33"/>
     </row>
     <row r="40" spans="3:17" x14ac:dyDescent="0.55000000000000004">
@@ -9658,11 +9676,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="O2:P2"/>
     <mergeCell ref="Q2:R2"/>
     <mergeCell ref="S2:T2"/>
     <mergeCell ref="U2:V2"/>
@@ -9671,11 +9689,11 @@
     <mergeCell ref="I31:J31"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="W2:X2"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="54" orientation="landscape" r:id="rId1"/>
@@ -9709,54 +9727,54 @@
   <sheetData>
     <row r="1" spans="2:34" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="2" spans="2:34" ht="18.3" x14ac:dyDescent="0.7">
-      <c r="C2" s="62" t="s">
+      <c r="C2" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="62"/>
-      <c r="E2" s="72" t="s">
+      <c r="D2" s="68"/>
+      <c r="E2" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="68"/>
-      <c r="G2" s="62" t="s">
+      <c r="F2" s="67"/>
+      <c r="G2" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62" t="s">
+      <c r="H2" s="68"/>
+      <c r="I2" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62" t="s">
+      <c r="J2" s="68"/>
+      <c r="K2" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="62"/>
-      <c r="M2" s="72" t="s">
+      <c r="L2" s="68"/>
+      <c r="M2" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="68"/>
-      <c r="O2" s="62" t="s">
-        <v>25</v>
-      </c>
-      <c r="P2" s="62"/>
-      <c r="Q2" s="62" t="s">
+      <c r="N2" s="67"/>
+      <c r="O2" s="68" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2" s="68"/>
+      <c r="Q2" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="R2" s="62"/>
-      <c r="S2" s="62" t="s">
+      <c r="R2" s="68"/>
+      <c r="S2" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="T2" s="62"/>
-      <c r="U2" s="62" t="s">
+      <c r="T2" s="68"/>
+      <c r="U2" s="68" t="s">
         <v>65</v>
       </c>
       <c r="V2" s="69"/>
-      <c r="W2" s="62" t="s">
+      <c r="W2" s="68" t="s">
         <v>66</v>
       </c>
       <c r="X2" s="69"/>
-      <c r="Y2" s="68" t="s">
+      <c r="Y2" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="Z2" s="62"/>
+      <c r="Z2" s="68"/>
     </row>
     <row r="3" spans="2:34" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="32" t="s">
@@ -11765,34 +11783,34 @@
       </c>
     </row>
     <row r="31" spans="2:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="F31" s="65" t="s">
+      <c r="F31" s="64" t="s">
         <v>56</v>
       </c>
-      <c r="G31" s="66"/>
-      <c r="H31" s="67"/>
-      <c r="I31" s="63">
+      <c r="G31" s="65"/>
+      <c r="H31" s="66"/>
+      <c r="I31" s="62">
         <f>C29+E29+G29+I29+K29+M29+O29+Q29+S29+U29+W29</f>
         <v>2462.73</v>
       </c>
-      <c r="J31" s="64"/>
+      <c r="J31" s="63"/>
     </row>
     <row r="32" spans="2:30" x14ac:dyDescent="0.55000000000000004">
       <c r="G32" s="70" t="s">
         <v>57</v>
       </c>
       <c r="H32" s="70"/>
-      <c r="I32" s="63">
+      <c r="I32" s="62">
         <f>+D29+F29+H29+J29+L29+N29+P29+R29+T29+V29+X29</f>
         <v>1004.25</v>
       </c>
-      <c r="J32" s="64"/>
+      <c r="J32" s="63"/>
     </row>
     <row r="33" spans="3:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="I33" s="63">
+      <c r="I33" s="62">
         <f>I32-I31</f>
         <v>-1458.48</v>
       </c>
-      <c r="J33" s="64"/>
+      <c r="J33" s="63"/>
       <c r="Y33">
         <f>2167+183+5*10</f>
         <v>2400</v>
@@ -11888,11 +11906,11 @@
         <v>64</v>
       </c>
       <c r="H38" s="42"/>
-      <c r="I38" s="71">
+      <c r="I38" s="72">
         <f>I36+I33+J37</f>
         <v>322.7800000000002</v>
       </c>
-      <c r="J38" s="71"/>
+      <c r="J38" s="72"/>
       <c r="M38" s="33"/>
     </row>
     <row r="40" spans="3:25" x14ac:dyDescent="0.55000000000000004">
@@ -12164,16 +12182,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="U2:V2"/>
     <mergeCell ref="W2:X2"/>
     <mergeCell ref="Y2:Z2"/>
     <mergeCell ref="C2:D2"/>
@@ -12182,6 +12190,16 @@
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="M2:N2"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="I33:J33"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="54" orientation="landscape" r:id="rId1"/>
@@ -12219,54 +12237,54 @@
   <sheetData>
     <row r="1" spans="2:34" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="2" spans="2:34" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="C2" s="62" t="s">
+      <c r="C2" s="68" t="s">
         <v>100</v>
       </c>
-      <c r="D2" s="62"/>
-      <c r="E2" s="72" t="s">
+      <c r="D2" s="68"/>
+      <c r="E2" s="71" t="s">
         <v>101</v>
       </c>
-      <c r="F2" s="68"/>
-      <c r="G2" s="62" t="s">
+      <c r="F2" s="67"/>
+      <c r="G2" s="68" t="s">
         <v>102</v>
       </c>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62" t="s">
+      <c r="H2" s="68"/>
+      <c r="I2" s="68" t="s">
         <v>103</v>
       </c>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62" t="s">
+      <c r="J2" s="68"/>
+      <c r="K2" s="68" t="s">
         <v>104</v>
       </c>
-      <c r="L2" s="62"/>
-      <c r="M2" s="72" t="s">
+      <c r="L2" s="68"/>
+      <c r="M2" s="71" t="s">
         <v>105</v>
       </c>
-      <c r="N2" s="68"/>
-      <c r="O2" s="62" t="s">
+      <c r="N2" s="67"/>
+      <c r="O2" s="68" t="s">
         <v>106</v>
       </c>
-      <c r="P2" s="62"/>
-      <c r="Q2" s="62" t="s">
+      <c r="P2" s="68"/>
+      <c r="Q2" s="68" t="s">
         <v>107</v>
       </c>
-      <c r="R2" s="62"/>
-      <c r="S2" s="62" t="s">
+      <c r="R2" s="68"/>
+      <c r="S2" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="T2" s="62"/>
-      <c r="U2" s="62" t="s">
+      <c r="T2" s="68"/>
+      <c r="U2" s="68" t="s">
         <v>108</v>
       </c>
       <c r="V2" s="69"/>
-      <c r="W2" s="62" t="s">
+      <c r="W2" s="68" t="s">
         <v>66</v>
       </c>
       <c r="X2" s="69"/>
-      <c r="Y2" s="68" t="s">
+      <c r="Y2" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="Z2" s="62"/>
+      <c r="Z2" s="68"/>
     </row>
     <row r="3" spans="2:34" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B3" s="32" t="s">
@@ -14249,34 +14267,34 @@
       </c>
     </row>
     <row r="31" spans="2:30" x14ac:dyDescent="0.55000000000000004">
-      <c r="F31" s="65" t="s">
+      <c r="F31" s="64" t="s">
         <v>56</v>
       </c>
-      <c r="G31" s="66"/>
-      <c r="H31" s="67"/>
-      <c r="I31" s="63">
+      <c r="G31" s="65"/>
+      <c r="H31" s="66"/>
+      <c r="I31" s="62">
         <f>C29+E29+G29+I29+K29+M29+O29+Q29+S29+U29+W29</f>
         <v>2158</v>
       </c>
-      <c r="J31" s="64"/>
+      <c r="J31" s="63"/>
     </row>
     <row r="32" spans="2:30" x14ac:dyDescent="0.55000000000000004">
       <c r="G32" s="70" t="s">
         <v>57</v>
       </c>
       <c r="H32" s="70"/>
-      <c r="I32" s="63">
+      <c r="I32" s="62">
         <f>+D29+F29+H29+J29+L29+N29+P29+R29+T29+V29+X29</f>
         <v>709.26</v>
       </c>
-      <c r="J32" s="64"/>
+      <c r="J32" s="63"/>
     </row>
     <row r="33" spans="3:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="I33" s="63">
+      <c r="I33" s="62">
         <f>I32-I31</f>
         <v>-1448.74</v>
       </c>
-      <c r="J33" s="64"/>
+      <c r="J33" s="63"/>
       <c r="Y33">
         <f>2167+183+5*10</f>
         <v>2400</v>
@@ -14365,11 +14383,11 @@
         <v>64</v>
       </c>
       <c r="H38" s="42"/>
-      <c r="I38" s="71">
+      <c r="I38" s="72">
         <f>I36+I33</f>
         <v>552.84999999999991</v>
       </c>
-      <c r="J38" s="71"/>
+      <c r="J38" s="72"/>
       <c r="M38" s="33"/>
     </row>
     <row r="40" spans="3:25" x14ac:dyDescent="0.55000000000000004">
@@ -14671,16 +14689,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="U2:V2"/>
     <mergeCell ref="W2:X2"/>
     <mergeCell ref="Y2:Z2"/>
     <mergeCell ref="C2:D2"/>
@@ -14689,6 +14697,16 @@
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="M2:N2"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="I33:J33"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="51" orientation="landscape" r:id="rId1"/>
@@ -14702,8 +14720,8 @@
   </sheetPr>
   <dimension ref="B1:AL60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="N51" sqref="N51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -14728,66 +14746,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:38" ht="7.5" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="W1" s="73"/>
-      <c r="X1" s="74"/>
+      <c r="W1" s="75"/>
+      <c r="X1" s="76"/>
     </row>
     <row r="2" spans="2:38" ht="18.3" x14ac:dyDescent="0.7">
-      <c r="C2" s="62" t="s">
+      <c r="C2" s="68" t="s">
         <v>113</v>
       </c>
-      <c r="D2" s="62"/>
-      <c r="E2" s="72" t="s">
+      <c r="D2" s="68"/>
+      <c r="E2" s="71" t="s">
         <v>101</v>
       </c>
-      <c r="F2" s="68"/>
-      <c r="G2" s="62" t="s">
+      <c r="F2" s="67"/>
+      <c r="G2" s="68" t="s">
         <v>114</v>
       </c>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62" t="s">
+      <c r="H2" s="68"/>
+      <c r="I2" s="68" t="s">
         <v>115</v>
       </c>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62" t="s">
+      <c r="J2" s="68"/>
+      <c r="K2" s="68" t="s">
         <v>104</v>
       </c>
-      <c r="L2" s="62"/>
-      <c r="M2" s="72" t="s">
+      <c r="L2" s="68"/>
+      <c r="M2" s="71" t="s">
         <v>103</v>
       </c>
-      <c r="N2" s="68"/>
-      <c r="O2" s="62" t="s">
+      <c r="N2" s="67"/>
+      <c r="O2" s="68" t="s">
         <v>106</v>
       </c>
-      <c r="P2" s="62"/>
-      <c r="Q2" s="62" t="s">
+      <c r="P2" s="68"/>
+      <c r="Q2" s="68" t="s">
         <v>107</v>
       </c>
-      <c r="R2" s="62"/>
-      <c r="S2" s="62" t="s">
+      <c r="R2" s="68"/>
+      <c r="S2" s="68" t="s">
         <v>100</v>
       </c>
-      <c r="T2" s="62"/>
-      <c r="U2" s="62" t="s">
+      <c r="T2" s="68"/>
+      <c r="U2" s="68" t="s">
         <v>108</v>
       </c>
-      <c r="V2" s="72"/>
-      <c r="W2" s="75" t="s">
+      <c r="V2" s="71"/>
+      <c r="W2" s="77" t="s">
         <v>102</v>
       </c>
-      <c r="X2" s="76"/>
-      <c r="Y2" s="75" t="s">
+      <c r="X2" s="78"/>
+      <c r="Y2" s="77" t="s">
         <v>105</v>
       </c>
-      <c r="Z2" s="77"/>
-      <c r="AA2" s="78" t="s">
+      <c r="Z2" s="79"/>
+      <c r="AA2" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="AB2" s="79"/>
-      <c r="AC2" s="68" t="s">
+      <c r="AB2" s="74"/>
+      <c r="AC2" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="AD2" s="62"/>
+      <c r="AD2" s="68"/>
     </row>
     <row r="3" spans="2:38" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="32" t="s">
@@ -15204,7 +15222,7 @@
       </c>
       <c r="AI7" s="44">
         <f>+E29+'Punters 2023'!AE7</f>
-        <v>1153</v>
+        <v>1168</v>
       </c>
       <c r="AJ7" s="44">
         <f>+F29+'Punters 2023'!AF7</f>
@@ -15212,11 +15230,11 @@
       </c>
       <c r="AK7" s="49">
         <f>+AJ7-AI7</f>
-        <v>-619</v>
+        <v>-634</v>
       </c>
       <c r="AL7" s="47">
         <f>(AJ7-AI7)/AI7</f>
-        <v>-0.53686036426712924</v>
+        <v>-0.5428082191780822</v>
       </c>
     </row>
     <row r="8" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -15290,7 +15308,7 @@
       </c>
       <c r="AI8" s="44">
         <f>+K29+'Punters 2023'!AE8</f>
-        <v>1305.5</v>
+        <v>1338</v>
       </c>
       <c r="AJ8" s="44">
         <f>+L29+'Punters 2023'!AF8</f>
@@ -15298,11 +15316,11 @@
       </c>
       <c r="AK8" s="50">
         <f t="shared" ref="AK8:AK16" si="5">+AJ8-AI8</f>
-        <v>-285.73</v>
+        <v>-318.23</v>
       </c>
       <c r="AL8" s="47">
         <f t="shared" ref="AL8:AL16" si="6">(AJ8-AI8)/AI8</f>
-        <v>-0.21886633473764844</v>
+        <v>-0.23784005979073244</v>
       </c>
     </row>
     <row r="9" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -15376,7 +15394,7 @@
       </c>
       <c r="AI9" s="44">
         <f>+M29+'Punters 2023'!AE9</f>
-        <v>1286.48</v>
+        <v>1306.48</v>
       </c>
       <c r="AJ9" s="44">
         <f>N29+'Punters 2023'!AF9</f>
@@ -15384,11 +15402,11 @@
       </c>
       <c r="AK9" s="50">
         <f t="shared" si="5"/>
-        <v>-325.08000000000004</v>
+        <v>-345.08000000000004</v>
       </c>
       <c r="AL9" s="47">
         <f t="shared" si="6"/>
-        <v>-0.25268950935887075</v>
+        <v>-0.26412956953034111</v>
       </c>
     </row>
     <row r="10" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -15463,19 +15481,19 @@
       </c>
       <c r="AI10" s="44">
         <f>+C29+'Punters 2023'!AE10</f>
-        <v>1289.9000000000001</v>
+        <v>1314.9</v>
       </c>
       <c r="AJ10" s="44">
         <f>+D29+'Punters 2023'!AF10</f>
-        <v>1596.4499999999998</v>
+        <v>1641.4499999999998</v>
       </c>
       <c r="AK10" s="50">
         <f t="shared" si="5"/>
-        <v>306.54999999999973</v>
+        <v>326.54999999999973</v>
       </c>
       <c r="AL10" s="45">
         <f t="shared" si="6"/>
-        <v>0.23765408171176036</v>
+        <v>0.24834588181610748</v>
       </c>
     </row>
     <row r="11" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -15550,7 +15568,7 @@
       </c>
       <c r="AI11" s="44">
         <f>+I29+'Punters 2023'!AE11</f>
-        <v>1018</v>
+        <v>1043</v>
       </c>
       <c r="AJ11" s="44">
         <f>+J29+'Punters 2023'!AF11</f>
@@ -15558,11 +15576,11 @@
       </c>
       <c r="AK11" s="49">
         <f t="shared" si="5"/>
-        <v>-776.4</v>
+        <v>-801.4</v>
       </c>
       <c r="AL11" s="47">
         <f t="shared" si="6"/>
-        <v>-0.76267190569744592</v>
+        <v>-0.76836049856184085</v>
       </c>
     </row>
     <row r="12" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -15632,7 +15650,7 @@
       </c>
       <c r="AI12" s="44">
         <f>+U29+'Punters 2023'!AE12</f>
-        <v>1319.96</v>
+        <v>1369.96</v>
       </c>
       <c r="AJ12" s="44">
         <f>+V29+'Punters 2023'!AF12</f>
@@ -15640,11 +15658,11 @@
       </c>
       <c r="AK12" s="49">
         <f t="shared" si="5"/>
-        <v>-475.55000000000018</v>
+        <v>-525.55000000000018</v>
       </c>
       <c r="AL12" s="47">
         <f t="shared" si="6"/>
-        <v>-0.36027606897178716</v>
+        <v>-0.38362433939677082</v>
       </c>
     </row>
     <row r="13" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -15722,7 +15740,7 @@
       </c>
       <c r="AI13" s="44">
         <f>+S29+'Punters 2023'!AE13</f>
-        <v>1246.3400000000001</v>
+        <v>1296.3400000000001</v>
       </c>
       <c r="AJ13" s="44">
         <f>+T29+'Punters 2023'!AF13</f>
@@ -15730,11 +15748,11 @@
       </c>
       <c r="AK13" s="49">
         <f t="shared" si="5"/>
-        <v>-479.65000000000009</v>
+        <v>-529.65000000000009</v>
       </c>
       <c r="AL13" s="47">
         <f t="shared" si="6"/>
-        <v>-0.3848468315226985</v>
+        <v>-0.40857336809787559</v>
       </c>
     </row>
     <row r="14" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -15808,7 +15826,7 @@
       </c>
       <c r="AI14" s="44">
         <f>+Q29+'Punters 2023'!AE14</f>
-        <v>1273</v>
+        <v>1298</v>
       </c>
       <c r="AJ14" s="44">
         <f>+R29+'Punters 2023'!AF14</f>
@@ -15816,11 +15834,11 @@
       </c>
       <c r="AK14" s="49">
         <f t="shared" si="5"/>
-        <v>-635.53</v>
+        <v>-660.53</v>
       </c>
       <c r="AL14" s="47">
         <f t="shared" si="6"/>
-        <v>-0.49923802042419479</v>
+        <v>-0.50888289676425269</v>
       </c>
     </row>
     <row r="15" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -15894,7 +15912,7 @@
       </c>
       <c r="AI15" s="44">
         <f>+O29+'Punters 2023'!AE15</f>
-        <v>1277.7</v>
+        <v>1307.7</v>
       </c>
       <c r="AJ15" s="44">
         <f>+P29+'Punters 2023'!AF15</f>
@@ -15902,11 +15920,11 @@
       </c>
       <c r="AK15" s="50">
         <f t="shared" si="5"/>
-        <v>414.64999999999986</v>
+        <v>384.64999999999986</v>
       </c>
       <c r="AL15" s="45">
         <f t="shared" si="6"/>
-        <v>0.32452844955779903</v>
+        <v>0.29414238739772108</v>
       </c>
     </row>
     <row r="16" spans="2:38" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -15980,7 +15998,7 @@
       </c>
       <c r="AI16" s="44">
         <f>+G29+'Punters 2023'!AE16</f>
-        <v>577</v>
+        <v>603</v>
       </c>
       <c r="AJ16" s="44">
         <f>+H29+'Punters 2023'!AF16</f>
@@ -15988,11 +16006,11 @@
       </c>
       <c r="AK16" s="49">
         <f t="shared" si="5"/>
-        <v>-425.75</v>
+        <v>-451.75</v>
       </c>
       <c r="AL16" s="47">
         <f t="shared" si="6"/>
-        <v>-0.73786828422876949</v>
+        <v>-0.74917081260364837</v>
       </c>
     </row>
     <row r="17" spans="2:38" x14ac:dyDescent="0.55000000000000004">
@@ -16070,19 +16088,19 @@
       </c>
       <c r="AI17" s="44">
         <f>+C29</f>
-        <v>150</v>
+        <v>175</v>
       </c>
       <c r="AJ17" s="44">
         <f>+D29</f>
-        <v>80</v>
+        <v>125</v>
       </c>
       <c r="AK17" s="49">
         <f t="shared" ref="AK17:AK18" si="7">+AJ17-AI17</f>
-        <v>-70</v>
+        <v>-50</v>
       </c>
       <c r="AL17" s="47">
         <f t="shared" ref="AL17:AL18" si="8">(AJ17-AI17)/AI17</f>
-        <v>-0.46666666666666667</v>
+        <v>-0.2857142857142857</v>
       </c>
     </row>
     <row r="18" spans="2:38" x14ac:dyDescent="0.55000000000000004">
@@ -16157,7 +16175,7 @@
       </c>
       <c r="AI18" s="44">
         <f>+G29</f>
-        <v>150</v>
+        <v>176</v>
       </c>
       <c r="AJ18" s="44">
         <f>+H29</f>
@@ -16165,7 +16183,7 @@
       </c>
       <c r="AK18" s="49">
         <f t="shared" si="7"/>
-        <v>-150</v>
+        <v>-176</v>
       </c>
       <c r="AL18" s="47">
         <f t="shared" si="8"/>
@@ -16252,27 +16270,51 @@
       <c r="H20" s="16"/>
       <c r="I20" s="17"/>
       <c r="J20" s="16"/>
-      <c r="K20" s="17"/>
-      <c r="L20" s="16"/>
+      <c r="K20" s="17">
+        <v>7.5</v>
+      </c>
+      <c r="L20" s="16">
+        <v>0</v>
+      </c>
       <c r="M20" s="17"/>
       <c r="N20" s="16"/>
-      <c r="O20" s="17"/>
-      <c r="P20" s="16"/>
+      <c r="O20" s="17">
+        <v>5</v>
+      </c>
+      <c r="P20" s="16">
+        <v>0</v>
+      </c>
       <c r="Q20" s="17"/>
       <c r="R20" s="16"/>
-      <c r="S20" s="17"/>
-      <c r="T20" s="16"/>
-      <c r="U20" s="15"/>
-      <c r="V20" s="20"/>
-      <c r="W20" s="15"/>
-      <c r="X20" s="20"/>
-      <c r="Y20" s="15"/>
-      <c r="Z20" s="20"/>
+      <c r="S20" s="17">
+        <v>25</v>
+      </c>
+      <c r="T20" s="16">
+        <v>0</v>
+      </c>
+      <c r="U20" s="15">
+        <v>25</v>
+      </c>
+      <c r="V20" s="20">
+        <v>0</v>
+      </c>
+      <c r="W20" s="15">
+        <v>25</v>
+      </c>
+      <c r="X20" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="15">
+        <v>25</v>
+      </c>
+      <c r="Z20" s="20">
+        <v>0</v>
+      </c>
       <c r="AA20" s="15"/>
       <c r="AB20" s="20"/>
       <c r="AC20" s="17">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>112.5</v>
       </c>
       <c r="AD20" s="35">
         <f t="shared" si="3"/>
@@ -16280,7 +16322,7 @@
       </c>
       <c r="AE20" s="1">
         <f t="shared" si="4"/>
-        <v>1687.5</v>
+        <v>1800</v>
       </c>
       <c r="AF20" s="1">
         <f t="shared" si="4"/>
@@ -16288,7 +16330,7 @@
       </c>
       <c r="AG20" s="1">
         <f t="shared" si="1"/>
-        <v>-673.25</v>
+        <v>-785.75</v>
       </c>
       <c r="AH20" s="1"/>
     </row>
@@ -16296,14 +16338,33 @@
       <c r="B21" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="16"/>
+      <c r="C21" s="15">
+        <f>6+5+4.5+4.5</f>
+        <v>20</v>
+      </c>
+      <c r="D21" s="16">
+        <v>45</v>
+      </c>
+      <c r="E21" s="17">
+        <v>15</v>
+      </c>
+      <c r="F21" s="16">
+        <v>0</v>
+      </c>
+      <c r="G21" s="17">
+        <f>10+1+5+10</f>
+        <v>26</v>
+      </c>
+      <c r="H21" s="16">
+        <v>0</v>
+      </c>
+      <c r="I21" s="17">
+        <f>5+5+5</f>
+        <v>15</v>
+      </c>
+      <c r="J21" s="16">
+        <v>0</v>
+      </c>
       <c r="K21" s="17"/>
       <c r="L21" s="16"/>
       <c r="M21" s="17"/>
@@ -16324,23 +16385,23 @@
       <c r="AB21" s="20"/>
       <c r="AC21" s="17">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="AD21" s="35">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="AE21" s="1">
         <f t="shared" si="4"/>
-        <v>1687.5</v>
+        <v>1876</v>
       </c>
       <c r="AF21" s="1">
         <f t="shared" si="4"/>
-        <v>1014.25</v>
+        <v>1059.25</v>
       </c>
       <c r="AG21" s="1">
         <f t="shared" si="1"/>
-        <v>-673.25</v>
+        <v>-816.75</v>
       </c>
       <c r="AH21" s="1"/>
     </row>
@@ -16348,22 +16409,42 @@
       <c r="B22" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="15"/>
-      <c r="D22" s="16"/>
+      <c r="C22" s="15">
+        <v>5</v>
+      </c>
+      <c r="D22" s="16">
+        <v>0</v>
+      </c>
       <c r="E22" s="17"/>
       <c r="F22" s="16"/>
       <c r="G22" s="17"/>
       <c r="H22" s="16"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="17"/>
-      <c r="L22" s="16"/>
+      <c r="I22" s="17">
+        <v>10</v>
+      </c>
+      <c r="J22" s="16">
+        <v>0</v>
+      </c>
+      <c r="K22" s="17">
+        <v>17.5</v>
+      </c>
+      <c r="L22" s="16">
+        <v>0</v>
+      </c>
       <c r="M22" s="17"/>
       <c r="N22" s="16"/>
-      <c r="O22" s="17"/>
-      <c r="P22" s="16"/>
-      <c r="Q22" s="17"/>
-      <c r="R22" s="16"/>
+      <c r="O22" s="17">
+        <v>25</v>
+      </c>
+      <c r="P22" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="17">
+        <v>25</v>
+      </c>
+      <c r="R22" s="16">
+        <v>0</v>
+      </c>
       <c r="S22" s="17"/>
       <c r="T22" s="16"/>
       <c r="U22" s="15"/>
@@ -16376,7 +16457,7 @@
       <c r="AB22" s="20"/>
       <c r="AC22" s="17">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>82.5</v>
       </c>
       <c r="AD22" s="35">
         <f t="shared" si="3"/>
@@ -16384,15 +16465,15 @@
       </c>
       <c r="AE22" s="1">
         <f t="shared" ref="AE22:AF27" si="9">AE21+AC22</f>
-        <v>1687.5</v>
+        <v>1958.5</v>
       </c>
       <c r="AF22" s="1">
         <f t="shared" si="9"/>
-        <v>1014.25</v>
+        <v>1059.25</v>
       </c>
       <c r="AG22" s="1">
         <f t="shared" si="1"/>
-        <v>-673.25</v>
+        <v>-899.25</v>
       </c>
       <c r="AH22" s="1"/>
     </row>
@@ -16408,43 +16489,67 @@
       <c r="H23" s="16"/>
       <c r="I23" s="17"/>
       <c r="J23" s="16"/>
-      <c r="K23" s="17"/>
-      <c r="L23" s="16"/>
-      <c r="M23" s="17"/>
-      <c r="N23" s="16"/>
+      <c r="K23" s="17">
+        <v>7.5</v>
+      </c>
+      <c r="L23" s="16">
+        <v>0</v>
+      </c>
+      <c r="M23" s="17">
+        <v>20</v>
+      </c>
+      <c r="N23" s="16">
+        <v>0</v>
+      </c>
       <c r="O23" s="17"/>
       <c r="P23" s="16"/>
       <c r="Q23" s="17"/>
       <c r="R23" s="16"/>
-      <c r="S23" s="17"/>
-      <c r="T23" s="16"/>
-      <c r="U23" s="15"/>
-      <c r="V23" s="20"/>
-      <c r="W23" s="15"/>
-      <c r="X23" s="20"/>
-      <c r="Y23" s="15"/>
-      <c r="Z23" s="20"/>
+      <c r="S23" s="17">
+        <v>25</v>
+      </c>
+      <c r="T23" s="16">
+        <v>0</v>
+      </c>
+      <c r="U23" s="15">
+        <v>25</v>
+      </c>
+      <c r="V23" s="20">
+        <v>0</v>
+      </c>
+      <c r="W23" s="15">
+        <v>25</v>
+      </c>
+      <c r="X23" s="20">
+        <v>69.83</v>
+      </c>
+      <c r="Y23" s="15">
+        <v>27</v>
+      </c>
+      <c r="Z23" s="20">
+        <v>0</v>
+      </c>
       <c r="AA23" s="15"/>
       <c r="AB23" s="20"/>
       <c r="AC23" s="17">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>129.5</v>
       </c>
       <c r="AD23" s="35">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>69.83</v>
       </c>
       <c r="AE23" s="1">
         <f t="shared" si="9"/>
-        <v>1687.5</v>
+        <v>2088</v>
       </c>
       <c r="AF23" s="1">
         <f t="shared" si="9"/>
-        <v>1014.25</v>
+        <v>1129.08</v>
       </c>
       <c r="AG23" s="1">
         <f t="shared" si="1"/>
-        <v>-673.25</v>
+        <v>-958.92000000000007</v>
       </c>
       <c r="AH23" s="1"/>
     </row>
@@ -16488,15 +16593,15 @@
       </c>
       <c r="AE24" s="1">
         <f t="shared" si="9"/>
-        <v>1687.5</v>
+        <v>2088</v>
       </c>
       <c r="AF24" s="1">
         <f t="shared" si="9"/>
-        <v>1014.25</v>
+        <v>1129.08</v>
       </c>
       <c r="AG24" s="1">
         <f t="shared" si="1"/>
-        <v>-673.25</v>
+        <v>-958.92000000000007</v>
       </c>
       <c r="AH24" s="1"/>
     </row>
@@ -16540,15 +16645,15 @@
       </c>
       <c r="AE25" s="1">
         <f t="shared" si="9"/>
-        <v>1687.5</v>
+        <v>2088</v>
       </c>
       <c r="AF25" s="1">
         <f t="shared" si="9"/>
-        <v>1014.25</v>
+        <v>1129.08</v>
       </c>
       <c r="AG25" s="1">
         <f t="shared" si="1"/>
-        <v>-673.25</v>
+        <v>-958.92000000000007</v>
       </c>
       <c r="AH25" s="1"/>
     </row>
@@ -16592,15 +16697,15 @@
       </c>
       <c r="AE26" s="1">
         <f t="shared" si="9"/>
-        <v>1687.5</v>
+        <v>2088</v>
       </c>
       <c r="AF26" s="1">
         <f t="shared" si="9"/>
-        <v>1014.25</v>
+        <v>1129.08</v>
       </c>
       <c r="AG26" s="1">
         <f t="shared" si="1"/>
-        <v>-673.25</v>
+        <v>-958.92000000000007</v>
       </c>
       <c r="AH26" s="1"/>
     </row>
@@ -16644,15 +16749,15 @@
       </c>
       <c r="AE27" s="1">
         <f t="shared" si="9"/>
-        <v>1687.5</v>
+        <v>2088</v>
       </c>
       <c r="AF27" s="1">
         <f t="shared" si="9"/>
-        <v>1014.25</v>
+        <v>1129.08</v>
       </c>
       <c r="AG27" s="1">
         <f t="shared" si="1"/>
-        <v>-673.25</v>
+        <v>-958.92000000000007</v>
       </c>
       <c r="AH27" s="1"/>
     </row>
@@ -16705,15 +16810,15 @@
       </c>
       <c r="C29" s="18">
         <f t="shared" ref="C29:AD29" si="10">SUM(C4:C28)</f>
-        <v>150</v>
+        <v>175</v>
       </c>
       <c r="D29" s="18">
         <f t="shared" si="10"/>
-        <v>80</v>
+        <v>125</v>
       </c>
       <c r="E29" s="18">
         <f t="shared" si="10"/>
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="F29" s="18">
         <f t="shared" si="10"/>
@@ -16721,7 +16826,7 @@
       </c>
       <c r="G29" s="18">
         <f t="shared" si="10"/>
-        <v>150</v>
+        <v>176</v>
       </c>
       <c r="H29" s="18">
         <f t="shared" si="10"/>
@@ -16729,7 +16834,7 @@
       </c>
       <c r="I29" s="18">
         <f t="shared" si="10"/>
-        <v>150</v>
+        <v>175</v>
       </c>
       <c r="J29" s="18">
         <f t="shared" si="10"/>
@@ -16737,7 +16842,7 @@
       </c>
       <c r="K29" s="18">
         <f t="shared" si="10"/>
-        <v>142.5</v>
+        <v>175</v>
       </c>
       <c r="L29" s="18">
         <f t="shared" si="10"/>
@@ -16745,7 +16850,7 @@
       </c>
       <c r="M29" s="18">
         <f t="shared" si="10"/>
-        <v>150</v>
+        <v>170</v>
       </c>
       <c r="N29" s="18">
         <f t="shared" si="10"/>
@@ -16753,7 +16858,7 @@
       </c>
       <c r="O29" s="18">
         <f t="shared" si="10"/>
-        <v>145</v>
+        <v>175</v>
       </c>
       <c r="P29" s="18">
         <f t="shared" si="10"/>
@@ -16761,7 +16866,7 @@
       </c>
       <c r="Q29" s="18">
         <f t="shared" si="10"/>
-        <v>150</v>
+        <v>175</v>
       </c>
       <c r="R29" s="18">
         <f t="shared" si="10"/>
@@ -16769,7 +16874,7 @@
       </c>
       <c r="S29" s="18">
         <f t="shared" si="10"/>
-        <v>125</v>
+        <v>175</v>
       </c>
       <c r="T29" s="18">
         <f>SUM(T4:T28)</f>
@@ -16777,7 +16882,7 @@
       </c>
       <c r="U29" s="18">
         <f t="shared" si="10"/>
-        <v>125</v>
+        <v>175</v>
       </c>
       <c r="V29" s="21">
         <f t="shared" si="10"/>
@@ -16785,15 +16890,15 @@
       </c>
       <c r="W29" s="18">
         <f t="shared" ref="W29:X29" si="11">SUM(W4:W28)</f>
-        <v>125</v>
+        <v>175</v>
       </c>
       <c r="X29" s="21">
         <f t="shared" si="11"/>
-        <v>66.25</v>
+        <v>136.07999999999998</v>
       </c>
       <c r="Y29" s="18">
         <f t="shared" ref="Y29:Z29" si="12">SUM(Y4:Y28)</f>
-        <v>125</v>
+        <v>177</v>
       </c>
       <c r="Z29" s="21">
         <f t="shared" si="12"/>
@@ -16809,18 +16914,18 @@
       </c>
       <c r="AC29" s="29">
         <f t="shared" si="10"/>
-        <v>1687.5</v>
+        <v>2088</v>
       </c>
       <c r="AD29" s="18">
         <f t="shared" si="10"/>
-        <v>1014.25</v>
+        <v>1129.08</v>
       </c>
       <c r="AE29" s="1"/>
     </row>
     <row r="30" spans="2:38" x14ac:dyDescent="0.55000000000000004">
       <c r="D30" s="56">
         <f>(D29-C29)/C29</f>
-        <v>-0.46666666666666667</v>
+        <v>-0.2857142857142857</v>
       </c>
       <c r="F30" s="34">
         <f>(F29-E29)/E29</f>
@@ -16832,7 +16937,7 @@
       </c>
       <c r="J30" s="34">
         <f>(J29-I29)/I29</f>
-        <v>0.2223333333333333</v>
+        <v>4.7714285714285681E-2</v>
       </c>
       <c r="L30" s="28">
         <f>(L29-K29)/K29</f>
@@ -16844,7 +16949,7 @@
       </c>
       <c r="P30" s="28">
         <f>(P29-O29)/O29</f>
-        <v>0.59489655172413791</v>
+        <v>0.32148571428571421</v>
       </c>
       <c r="R30" s="28">
         <f>(R29-Q29)/Q29</f>
@@ -16852,7 +16957,7 @@
       </c>
       <c r="T30" s="22">
         <f>(T29-S29)/S29</f>
-        <v>1.1488800000000001</v>
+        <v>0.53491428571428579</v>
       </c>
       <c r="V30" s="28">
         <f>(V29-U29)/U29</f>
@@ -16860,42 +16965,42 @@
       </c>
       <c r="X30" s="28">
         <f>(X29-W29)/W29</f>
-        <v>-0.47</v>
+        <v>-0.2224000000000001</v>
       </c>
       <c r="Z30" s="28">
         <f>(Z29-Y29)/Y29</f>
-        <v>0.47824</v>
+        <v>4.3954802259887009E-2</v>
       </c>
     </row>
     <row r="31" spans="2:38" x14ac:dyDescent="0.55000000000000004">
-      <c r="F31" s="65" t="s">
+      <c r="F31" s="64" t="s">
         <v>56</v>
       </c>
-      <c r="G31" s="66"/>
-      <c r="H31" s="67"/>
-      <c r="I31" s="63">
+      <c r="G31" s="65"/>
+      <c r="H31" s="66"/>
+      <c r="I31" s="62">
         <f>C29+E29+G29+I29+K29+M29+O29+Q29+S29+U29+AA29+W29+Y29</f>
-        <v>1687.5</v>
-      </c>
-      <c r="J31" s="64"/>
+        <v>2088</v>
+      </c>
+      <c r="J31" s="63"/>
     </row>
     <row r="32" spans="2:38" x14ac:dyDescent="0.55000000000000004">
       <c r="G32" s="70" t="s">
         <v>57</v>
       </c>
       <c r="H32" s="70"/>
-      <c r="I32" s="63">
+      <c r="I32" s="62">
         <f>+D29+F29+H29+J29+L29+N29+P29+R29+T29+V29+AB29+X29+Z29</f>
-        <v>1014.25</v>
-      </c>
-      <c r="J32" s="64"/>
+        <v>1129.08</v>
+      </c>
+      <c r="J32" s="63"/>
     </row>
     <row r="33" spans="3:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="I33" s="63">
+      <c r="I33" s="62">
         <f>I32-I31</f>
-        <v>-673.25</v>
-      </c>
-      <c r="J33" s="64"/>
+        <v>-958.92000000000007</v>
+      </c>
+      <c r="J33" s="63"/>
       <c r="Y33">
         <f>2167+183+5*10</f>
         <v>2400</v>
@@ -16904,19 +17009,19 @@
     <row r="34" spans="3:25" x14ac:dyDescent="0.55000000000000004">
       <c r="C34" s="36">
         <f>C29+E29+G29+I29</f>
-        <v>600</v>
+        <v>691</v>
       </c>
       <c r="D34" s="36">
         <f>D29+F29+H29+J29</f>
-        <v>263.35000000000002</v>
+        <v>308.35000000000002</v>
       </c>
       <c r="E34" s="37">
         <f>D34-C34</f>
-        <v>-336.65</v>
+        <v>-382.65</v>
       </c>
       <c r="I34" s="38">
         <f>O29+K29+M29+Q29</f>
-        <v>587.5</v>
+        <v>695</v>
       </c>
       <c r="J34" s="38">
         <f>P29+L29+N29</f>
@@ -16924,19 +17029,19 @@
       </c>
       <c r="K34" s="39">
         <f>J34-I34</f>
-        <v>-356.24</v>
+        <v>-463.74</v>
       </c>
       <c r="O34" s="40">
         <f>U29+W29+Y29+S29</f>
-        <v>500</v>
+        <v>702</v>
       </c>
       <c r="P34" s="40">
         <f>V29+X29+T29+Z29</f>
-        <v>519.64</v>
+        <v>589.47</v>
       </c>
       <c r="Q34" s="41">
         <f>P34-O34</f>
-        <v>19.639999999999986</v>
+        <v>-112.52999999999997</v>
       </c>
       <c r="X34" s="55"/>
       <c r="Y34">
@@ -16948,19 +17053,19 @@
       <c r="C35" s="36"/>
       <c r="D35" s="34">
         <f>(D34-C34)/C34</f>
-        <v>-0.56108333333333327</v>
+        <v>-0.55376266280752529</v>
       </c>
       <c r="E35" s="37"/>
       <c r="I35" s="38"/>
       <c r="J35" s="34">
         <f>(J34-I34)/I34</f>
-        <v>-0.60636595744680855</v>
+        <v>-0.66725179856115113</v>
       </c>
       <c r="K35" s="39"/>
       <c r="O35" s="40"/>
       <c r="P35" s="34">
         <f>(P34-O34)/O34</f>
-        <v>3.9279999999999975E-2</v>
+        <v>-0.16029914529914527</v>
       </c>
       <c r="Q35" s="41"/>
       <c r="X35" s="55"/>
@@ -16978,11 +17083,11 @@
         <v>64</v>
       </c>
       <c r="H38" s="42"/>
-      <c r="I38" s="71">
+      <c r="I38" s="72">
         <f>I36+I33</f>
-        <v>1726.8000000000002</v>
-      </c>
-      <c r="J38" s="71"/>
+        <v>1441.13</v>
+      </c>
+      <c r="J38" s="72"/>
       <c r="M38" s="33"/>
     </row>
     <row r="40" spans="3:25" x14ac:dyDescent="0.55000000000000004">
@@ -16991,15 +17096,15 @@
     <row r="42" spans="3:25" x14ac:dyDescent="0.55000000000000004">
       <c r="C42" s="1">
         <f>C29+E29+G29+I29</f>
-        <v>600</v>
+        <v>691</v>
       </c>
       <c r="D42" s="1">
         <f>D29+F29+H29+J29</f>
-        <v>263.35000000000002</v>
+        <v>308.35000000000002</v>
       </c>
       <c r="I42" s="1">
         <f>O29+K29+M29</f>
-        <v>437.5</v>
+        <v>520</v>
       </c>
       <c r="J42" s="1">
         <f>P29+L29+N29</f>
@@ -17007,7 +17112,7 @@
       </c>
       <c r="O42" s="1">
         <f>U29+Q29+S29</f>
-        <v>400</v>
+        <v>525</v>
       </c>
       <c r="P42" s="1">
         <f>V29+R29+T29</f>
@@ -17017,15 +17122,15 @@
     <row r="43" spans="3:25" x14ac:dyDescent="0.55000000000000004">
       <c r="D43" s="1">
         <f>D42-C42</f>
-        <v>-336.65</v>
+        <v>-382.65</v>
       </c>
       <c r="J43" s="33">
         <f>J42-I42</f>
-        <v>-206.24</v>
+        <v>-288.74</v>
       </c>
       <c r="P43" s="33">
         <f>P42-O42</f>
-        <v>-131.38999999999999</v>
+        <v>-256.39</v>
       </c>
     </row>
     <row r="45" spans="3:25" x14ac:dyDescent="0.55000000000000004">
@@ -17044,7 +17149,7 @@
         <v>89</v>
       </c>
       <c r="W46">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47" spans="3:25" x14ac:dyDescent="0.55000000000000004">
@@ -17064,7 +17169,7 @@
         <v>12</v>
       </c>
       <c r="W47">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="3:25" x14ac:dyDescent="0.55000000000000004">
@@ -17127,7 +17232,7 @@
         <v>9</v>
       </c>
       <c r="W50">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51" spans="4:23" x14ac:dyDescent="0.55000000000000004">
@@ -17148,7 +17253,7 @@
         <v>11</v>
       </c>
       <c r="W51">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="4:23" x14ac:dyDescent="0.55000000000000004">
@@ -17184,7 +17289,7 @@
         <v>97</v>
       </c>
       <c r="K53">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="V53" t="s">
         <v>98</v>
@@ -17220,7 +17325,7 @@
       </c>
       <c r="E55" s="1">
         <f>SUM(X29)</f>
-        <v>66.25</v>
+        <v>136.07999999999998</v>
       </c>
       <c r="J55" t="s">
         <v>89</v>
@@ -17232,7 +17337,7 @@
         <v>94</v>
       </c>
       <c r="W55">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="56" spans="4:23" x14ac:dyDescent="0.55000000000000004">
@@ -17247,7 +17352,7 @@
         <v>96</v>
       </c>
       <c r="K56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V56" t="s">
         <v>120</v>
@@ -17268,7 +17373,7 @@
         <v>120</v>
       </c>
       <c r="K57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V57" t="s">
         <v>121</v>
@@ -17283,7 +17388,7 @@
       </c>
       <c r="E58" s="1">
         <f>SUM(D29)</f>
-        <v>80</v>
+        <v>125</v>
       </c>
       <c r="J58" t="s">
         <v>121</v>
@@ -17296,7 +17401,7 @@
       </c>
       <c r="W58">
         <f>SUM(W46:W57)</f>
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="59" spans="4:23" x14ac:dyDescent="0.55000000000000004">
@@ -17320,18 +17425,31 @@
       </c>
       <c r="E60" s="1">
         <f>SUM(E48:E59)</f>
-        <v>1014.25</v>
+        <v>1129.08</v>
       </c>
       <c r="J60" t="s">
         <v>99</v>
       </c>
       <c r="K60">
         <f>SUM(K48:K59)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="O2:P2"/>
     <mergeCell ref="AA2:AB2"/>
     <mergeCell ref="AC2:AD2"/>
     <mergeCell ref="C2:D2"/>
@@ -17340,19 +17458,6 @@
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="M2:N2"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="W1:X1"/>
-    <mergeCell ref="W2:X2"/>
-    <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="U2:V2"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="51" orientation="landscape" r:id="rId1"/>
@@ -17361,10 +17466,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B9A81C0-C60A-48E0-A96A-1599E0795A8C}">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -17414,7 +17519,7 @@
       </c>
       <c r="F2">
         <f t="shared" ref="F2:F12" si="0">IF(COUNTIF(A:A, E2)=0, "", SUMIF(A:A, E2, C:C))</f>
-        <v>410.13</v>
+        <v>563.88</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -17435,7 +17540,7 @@
       </c>
       <c r="F3">
         <f t="shared" si="0"/>
-        <v>351.25</v>
+        <v>612.5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -17540,7 +17645,7 @@
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>401.8</v>
+        <v>508.55</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -17624,7 +17729,7 @@
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
-        <v>159.37</v>
+        <v>264.37</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -17642,7 +17747,7 @@
       </c>
       <c r="F13" s="61">
         <f>SUM(F1:F12)</f>
-        <v>5420.63</v>
+        <v>6047.38</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -17979,6 +18084,104 @@
       </c>
       <c r="D37" t="s">
         <v>165</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" t="s">
+        <v>94</v>
+      </c>
+      <c r="B38" t="s">
+        <v>152</v>
+      </c>
+      <c r="C38" s="60">
+        <v>95</v>
+      </c>
+      <c r="D38" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" t="s">
+        <v>12</v>
+      </c>
+      <c r="B39" s="59">
+        <v>7.5</v>
+      </c>
+      <c r="C39" s="59">
+        <v>63.75</v>
+      </c>
+      <c r="D39" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" t="s">
+        <v>89</v>
+      </c>
+      <c r="B40" s="60">
+        <v>7</v>
+      </c>
+      <c r="C40" s="59">
+        <v>106.75</v>
+      </c>
+      <c r="D40" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" t="s">
+        <v>11</v>
+      </c>
+      <c r="B41" s="60">
+        <v>15</v>
+      </c>
+      <c r="C41" s="59">
+        <v>157.5</v>
+      </c>
+      <c r="D41" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" t="s">
+        <v>9</v>
+      </c>
+      <c r="B42" s="60">
+        <v>10</v>
+      </c>
+      <c r="C42" s="60">
+        <v>105</v>
+      </c>
+      <c r="D42" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" t="s">
+        <v>94</v>
+      </c>
+      <c r="B43" s="60">
+        <v>5</v>
+      </c>
+      <c r="C43" s="59">
+        <v>166.25</v>
+      </c>
+      <c r="D43" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" s="59">
+        <v>7.5</v>
+      </c>
+      <c r="C44" s="60">
+        <v>90</v>
+      </c>
+      <c r="D44" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -17987,6 +18190,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="3e1ffae5-f160-4019-9720-1b11bf1b81a3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002D8393059904904F9DB82DE4B9AFABF6" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f7bafc8adbaca2e93ffc3a1da3fd32d5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3e1ffae5-f160-4019-9720-1b11bf1b81a3" xmlns:ns4="21753bd8-bffc-4cd2-a328-982ee854c895" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f821f56a5d2247de677e71e73e5a99e" ns3:_="" ns4:_="">
     <xsd:import namespace="3e1ffae5-f160-4019-9720-1b11bf1b81a3"/>
@@ -18207,14 +18418,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="3e1ffae5-f160-4019-9720-1b11bf1b81a3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -18225,6 +18428,16 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4D7A62A-0CB5-48B0-A73A-0A91BCC8EAEF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3e1ffae5-f160-4019-9720-1b11bf1b81a3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22BA772B-ABF0-4278-9CEF-D9160BBA9E07}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18243,23 +18456,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4D7A62A-0CB5-48B0-A73A-0A91BCC8EAEF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="3e1ffae5-f160-4019-9720-1b11bf1b81a3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="21753bd8-bffc-4cd2-a328-982ee854c895"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{948817D4-7F3F-493D-9D4C-B473DA03CC7E}">
   <ds:schemaRefs>

</xml_diff>